<commit_message>
Penambahan API, Penambahan Model, Penambahan Helper, Update Data API Catalogue, Update Store Procedure
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -30,6 +30,79 @@
             <charset val="1"/>
           </rPr>
           <t>API ini hanya boleh dijalankan melalui instance class, tidak melalui Call API (karena akan menghasilkan error disebabkan tidak dikenalnya APIWebToken)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Internal API
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>digunakan oleh \App\Helpers\ZhtHelper\General\Helper_JavaScript::getSyntaxFunc_DOMInputFileContent</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal API
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">digunakan oleh \App\Helpers\ZhtHelper\General\Helper_JavaScript::getSyntaxFunc_DOMInputFileContent
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Internal API
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>digunakan oleh \App\Helpers\ZhtHelper\General\Helper_JavaScript::getSyntaxFunc_DOMInputFileContent</t>
         </r>
       </text>
     </comment>
@@ -2710,7 +2783,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2790,6 +2863,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3590,10 +3676,10 @@
   <dimension ref="A1:L490"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Penambahan dan Update Data PickList getCombinedBudgetOwner dan getCombinedBudgetSection
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -3257,12 +3257,6 @@
     <t>dataPickList.project.getProject</t>
   </si>
   <si>
-    <t>dataPickList.master.getBudgetOrigin</t>
-  </si>
-  <si>
-    <t>Mendapatkan Data Picklist Asal Anggaran</t>
-  </si>
-  <si>
     <t>Mendapatkan Data Picklist Project</t>
   </si>
   <si>
@@ -3288,6 +3282,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mendapatkan Daftar Pekerjaan Item Seksi Proyek </t>
+  </si>
+  <si>
+    <t>dataPickList.budgeting.getCombinedBudgetSection</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Picklist Seksi Anggaran Gabungan</t>
   </si>
 </sst>
 </file>
@@ -4159,10 +4159,10 @@
   <dimension ref="A1:L578"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C316" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B331" sqref="B331"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4401,10 +4401,10 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="7" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="29">
@@ -4419,38 +4419,38 @@
       <c r="J12" s="20"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>979</v>
+      </c>
       <c r="D13" s="35"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="55"/>
+      <c r="E13" s="29">
+        <v>44480</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>624</v>
+      </c>
       <c r="G13" s="35"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="35"/>
-      <c r="B14" s="7" t="s">
-        <v>969</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>970</v>
-      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="35"/>
-      <c r="E14" s="29">
-        <v>44420</v>
-      </c>
-      <c r="F14" s="53" t="s">
-        <v>624</v>
-      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
       <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4472,7 +4472,7 @@
         <v>968</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="29">
@@ -4490,10 +4490,10 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>974</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>976</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="29">
@@ -4511,10 +4511,10 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>975</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>977</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="29">
@@ -11342,10 +11342,10 @@
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="35"/>
       <c r="B331" s="7" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D331" s="35"/>
       <c r="E331" s="29">
@@ -16727,7 +16727,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F4:F6 F9 F21:F23 F34:F35 F37 F39:F41 F74:F80 F83:F88 F147:F151 F153:F157 F159:F165 F167:F169 F181 F183:F201 F248:F250 F252:F256 F295:F300 F302:F303 F326:F327 F329:F331 F338:F343 F345:F346 F402:F410 F413:F415 F417 F419:F423 F425:F428 F430:F431 F441:F446 F448:F450 F459:F460 F178:F179 F462 F464:F465 F508:F510 F512:F516 F435:F439 F519:F523 F525:F527 F137:F140 F567:F570 F305:F324 F397:F400 F334:F336 F142:F144 F572:F574 F71 F50:F69 F48 F28:F31 F293 F26 F90:F97 F285:F286 F259:F261 F171:F176 F452:F457 F348:F353 F356:F395 F44 F16:F18 F14 F99:F135 F529:F565 F467:F506 F263:F283 F203:F246 F355 F12" numberStoredAsText="1"/>
+    <ignoredError sqref="F4:F6 F9 F21:F23 F34:F35 F37 F39:F41 F74:F80 F83:F88 F147:F151 F153:F157 F159:F165 F167:F169 F181 F183:F201 F248:F250 F252:F256 F295:F300 F302:F303 F326:F327 F329:F331 F338:F343 F345:F346 F402:F410 F413:F415 F417 F419:F423 F425:F428 F430:F431 F441:F446 F448:F450 F459:F460 F178:F179 F462 F464:F465 F508:F510 F512:F516 F435:F439 F519:F523 F525:F527 F137:F140 F567:F570 F305:F324 F397:F400 F334:F336 F142:F144 F572:F574 F71 F50:F69 F48 F28:F31 F293 F26 F90:F97 F285:F286 F259:F261 F171:F176 F452:F457 F348:F353 F356:F395 F44 F16:F18 F99:F135 F529:F565 F467:F506 F263:F283 F203:F246 F355 F12:F13" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Penambahan dan Update API transaction.read.dataRecord.project.getProjectSectionItemWork
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4171,10 +4171,10 @@
   <dimension ref="A1:L580"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C291" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C303" sqref="C303"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4530,7 +4530,7 @@
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="29">
-        <v>44474</v>
+        <v>44481</v>
       </c>
       <c r="F18" s="53" t="s">
         <v>624</v>
@@ -11403,7 +11403,7 @@
       </c>
       <c r="D333" s="35"/>
       <c r="E333" s="29">
-        <v>44474</v>
+        <v>44481</v>
       </c>
       <c r="F333" s="53" t="s">
         <v>624</v>

</xml_diff>

<commit_message>
Penambahan dan Update Model
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4198,7 +4198,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C289" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C304" sqref="C304"/>
+      <selection pane="bottomRight" activeCell="E305" sqref="E305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -10770,7 +10770,7 @@
       </c>
       <c r="D304" s="35"/>
       <c r="E304" s="29">
-        <v>44486</v>
+        <v>44487</v>
       </c>
       <c r="F304" s="53" t="s">
         <v>624</v>

</xml_diff>

<commit_message>
Update Pertanggal 1 Desember 2021
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -3236,12 +3236,6 @@
     <t>Mendapatkan Data Picklist Project</t>
   </si>
   <si>
-    <t>dataPickList.budgeting.getCombinedBudgetOwner</t>
-  </si>
-  <si>
-    <t>Mendapatkan Data Picklist Pemilik Anggaran Gabungan</t>
-  </si>
-  <si>
     <t>dataPickList.project.getProjectSectionItem</t>
   </si>
   <si>
@@ -3266,15 +3260,9 @@
     <t>Mendapatkan Data Picklist Seksi Anggaran Gabungan</t>
   </si>
   <si>
-    <t>transaction.read.dataList.budgeting.getCombinedBudgetOwner</t>
-  </si>
-  <si>
     <t>transaction.read.dataList.budgeting.getCombinedBudgetSection</t>
   </si>
   <si>
-    <t>Mendapatkan Daftar Pemilik Anggaran Gabungan</t>
-  </si>
-  <si>
     <t>Mendapatkan Daftar Seksi Anggaran Gabungan</t>
   </si>
   <si>
@@ -3456,6 +3444,18 @@
   </si>
   <si>
     <t>Mendapatkan Data Picklist Akun Bank</t>
+  </si>
+  <si>
+    <t>dataPickList.budgeting.getCombinedBudget</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Picklist Anggaran Gabungan</t>
+  </si>
+  <si>
+    <t>transaction.read.dataList.budgeting.getCombinedBudget</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Anggaran Gabungan</t>
   </si>
 </sst>
 </file>
@@ -4323,7 +4323,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4562,10 +4562,10 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="7" t="s">
-        <v>962</v>
+        <v>1032</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>963</v>
+        <v>1033</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="29">
@@ -4583,10 +4583,10 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="29">
@@ -4617,10 +4617,10 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="7" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="29">
@@ -4651,10 +4651,10 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="7" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="29">
@@ -4672,10 +4672,10 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="7" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="29">
@@ -4706,10 +4706,10 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="7" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="29">
@@ -4761,10 +4761,10 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>964</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>966</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="29">
@@ -4782,10 +4782,10 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>965</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>967</v>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="29">
@@ -5264,10 +5264,10 @@
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="7" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="D50" s="35"/>
       <c r="E50" s="29">
@@ -5285,10 +5285,10 @@
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="7" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="D51" s="35"/>
       <c r="E51" s="29">
@@ -6393,10 +6393,10 @@
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
       <c r="B109" s="7" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="D109" s="35"/>
       <c r="E109" s="29">
@@ -6414,10 +6414,10 @@
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="35"/>
       <c r="B110" s="7" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="D110" s="35"/>
       <c r="E110" s="29">
@@ -8721,10 +8721,10 @@
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="7" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="29">
@@ -8746,10 +8746,10 @@
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
       <c r="B214" s="7" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="D214" s="35"/>
       <c r="E214" s="29">
@@ -8784,10 +8784,10 @@
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="7" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="D216" s="35"/>
       <c r="E216" s="29">
@@ -8805,10 +8805,10 @@
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
       <c r="B217" s="7" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="D217" s="35"/>
       <c r="E217" s="29">
@@ -10242,10 +10242,10 @@
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="35"/>
       <c r="B278" s="7" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="D278" s="35"/>
       <c r="E278" s="29">
@@ -10263,10 +10263,10 @@
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="35"/>
       <c r="B279" s="7" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="D279" s="35"/>
       <c r="E279" s="29">
@@ -11112,7 +11112,7 @@
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="35"/>
       <c r="B316" s="7" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="C316" s="4" t="s">
         <v>472</v>
@@ -11133,7 +11133,7 @@
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="35"/>
       <c r="B317" s="7" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="C317" s="4" t="s">
         <v>473</v>
@@ -11154,10 +11154,10 @@
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="35"/>
       <c r="B318" s="7" t="s">
-        <v>972</v>
+        <v>1034</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>974</v>
+        <v>1035</v>
       </c>
       <c r="D318" s="35"/>
       <c r="E318" s="29">
@@ -11175,10 +11175,10 @@
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="35"/>
       <c r="B319" s="7" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="D319" s="35"/>
       <c r="E319" s="29">
@@ -11264,10 +11264,10 @@
     <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="35"/>
       <c r="B324" s="7" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="D324" s="35"/>
       <c r="E324" s="29">
@@ -11298,10 +11298,10 @@
     <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="35"/>
       <c r="B326" s="7" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="D326" s="35"/>
       <c r="E326" s="29">
@@ -11319,10 +11319,10 @@
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="35"/>
       <c r="B327" s="7" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="D327" s="35"/>
       <c r="E327" s="29">
@@ -11853,10 +11853,10 @@
     <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="35"/>
       <c r="B349" s="7" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="D349" s="35"/>
       <c r="E349" s="29">
@@ -11971,10 +11971,10 @@
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="35"/>
       <c r="B355" s="7" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C355" s="4" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D355" s="35"/>
       <c r="E355" s="29">
@@ -12178,7 +12178,7 @@
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="35"/>
       <c r="B366" s="7" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="C366" s="4" t="s">
         <v>475</v>
@@ -12199,7 +12199,7 @@
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="35"/>
       <c r="B367" s="7" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="C367" s="4" t="s">
         <v>476</v>
@@ -12427,10 +12427,10 @@
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="35"/>
       <c r="B379" s="7" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="D379" s="35"/>
       <c r="E379" s="29">
@@ -12452,10 +12452,10 @@
     <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="35"/>
       <c r="B380" s="7" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="D380" s="35"/>
       <c r="E380" s="29">
@@ -12490,10 +12490,10 @@
     <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="35"/>
       <c r="B382" s="7" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
       <c r="D382" s="35"/>
       <c r="E382" s="29">
@@ -12511,10 +12511,10 @@
     <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="35"/>
       <c r="B383" s="7" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="C383" s="4" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
       <c r="D383" s="35"/>
       <c r="E383" s="29">
@@ -14925,10 +14925,10 @@
     <row r="494" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A494" s="35"/>
       <c r="B494" s="7" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="D494" s="35"/>
       <c r="E494" s="29">
@@ -14950,10 +14950,10 @@
     <row r="495" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A495" s="35"/>
       <c r="B495" s="7" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="C495" s="4" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="D495" s="35"/>
       <c r="E495" s="29">
@@ -14988,10 +14988,10 @@
     <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497" s="35"/>
       <c r="B497" s="7" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="D497" s="35"/>
       <c r="E497" s="29">
@@ -15009,10 +15009,10 @@
     <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498" s="35"/>
       <c r="B498" s="7" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="D498" s="35"/>
       <c r="E498" s="29">
@@ -16464,10 +16464,10 @@
     <row r="561" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A561" s="35"/>
       <c r="B561" s="7" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="C561" s="14" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="D561" s="35"/>
       <c r="E561" s="29">
@@ -16485,10 +16485,10 @@
     <row r="562" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A562" s="35"/>
       <c r="B562" s="7" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="C562" s="14" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="D562" s="35"/>
       <c r="E562" s="29">

</xml_diff>

<commit_message>
Update Pertanggal 14 Desember 2021 11:34:58
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -2069,12 +2069,6 @@
     <t>2021-06-31</t>
   </si>
   <si>
-    <t>transaction.delete.budgeting.setBudgetExpenseCeiling</t>
-  </si>
-  <si>
-    <t>transaction.delete.budgeting.setBudgetExpenseCeilingObjects</t>
-  </si>
-  <si>
     <t>Menghapus Data Pagu Anggaran Belanja</t>
   </si>
   <si>
@@ -3456,6 +3450,12 @@
   </si>
   <si>
     <t>Mendapatkan Daftar Anggaran Gabungan</t>
+  </si>
+  <si>
+    <t>transaction.delete.budgeting.setBudgetExpenseLineCeiling</t>
+  </si>
+  <si>
+    <t>transaction.delete.budgeting.setBudgetExpenseLineCeilingObjects</t>
   </si>
 </sst>
 </file>
@@ -4320,10 +4320,10 @@
   <dimension ref="A1:L612"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C166" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4562,10 +4562,10 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35"/>
       <c r="B12" s="7" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="29">
@@ -4583,10 +4583,10 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="29">
@@ -4617,10 +4617,10 @@
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="7" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="29">
@@ -4651,10 +4651,10 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="7" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>1028</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>1030</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="29">
@@ -4672,10 +4672,10 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="7" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>1029</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>1031</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="29">
@@ -4706,10 +4706,10 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="7" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="29">
@@ -4740,10 +4740,10 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
       <c r="B22" s="7" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D22" s="35"/>
       <c r="E22" s="29">
@@ -4761,10 +4761,10 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="7" t="s">
+        <v>960</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>962</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>964</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="29">
@@ -4782,10 +4782,10 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>963</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>965</v>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="29">
@@ -4930,10 +4930,10 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="7" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D32" s="35"/>
       <c r="E32" s="29">
@@ -4964,10 +4964,10 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="35"/>
       <c r="B34" s="7" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="29">
@@ -4985,10 +4985,10 @@
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
       <c r="B35" s="7" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="29">
@@ -5006,10 +5006,10 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
       <c r="B36" s="7" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D36" s="35"/>
       <c r="E36" s="29">
@@ -5027,10 +5027,10 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
       <c r="B37" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>809</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>811</v>
       </c>
       <c r="D37" s="35"/>
       <c r="E37" s="29">
@@ -5264,10 +5264,10 @@
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="7" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="D50" s="35"/>
       <c r="E50" s="29">
@@ -5285,10 +5285,10 @@
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="7" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D51" s="35"/>
       <c r="E51" s="29">
@@ -5332,10 +5332,10 @@
     <row r="54" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="37"/>
       <c r="B54" s="13" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D54" s="37"/>
       <c r="E54" s="29">
@@ -5392,10 +5392,10 @@
     <row r="58" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="37"/>
       <c r="B58" s="13" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D58" s="37"/>
       <c r="E58" s="29">
@@ -5426,10 +5426,10 @@
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
       <c r="B60" s="7" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D60" s="35"/>
       <c r="E60" s="29">
@@ -5447,10 +5447,10 @@
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="35"/>
       <c r="B61" s="7" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D61" s="35"/>
       <c r="E61" s="29">
@@ -5468,10 +5468,10 @@
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="35"/>
       <c r="B62" s="7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D62" s="35"/>
       <c r="E62" s="29">
@@ -5489,10 +5489,10 @@
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="35"/>
       <c r="B63" s="7" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D63" s="35"/>
       <c r="E63" s="29">
@@ -5510,10 +5510,10 @@
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="35"/>
       <c r="B64" s="7" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D64" s="35"/>
       <c r="E64" s="29">
@@ -5531,10 +5531,10 @@
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="35"/>
       <c r="B65" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D65" s="35"/>
       <c r="E65" s="29">
@@ -5552,10 +5552,10 @@
     <row r="66" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37"/>
       <c r="B66" s="13" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D66" s="37"/>
       <c r="E66" s="29">
@@ -5573,10 +5573,10 @@
     <row r="67" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
       <c r="B67" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="29">
@@ -5594,10 +5594,10 @@
     <row r="68" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="37"/>
       <c r="B68" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D68" s="37"/>
       <c r="E68" s="29">
@@ -5615,10 +5615,10 @@
     <row r="69" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="37"/>
       <c r="B69" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D69" s="37"/>
       <c r="E69" s="29">
@@ -5636,10 +5636,10 @@
     <row r="70" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="37"/>
       <c r="B70" s="13" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D70" s="37"/>
       <c r="E70" s="29">
@@ -5657,10 +5657,10 @@
     <row r="71" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="37"/>
       <c r="B71" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D71" s="37"/>
       <c r="E71" s="29">
@@ -5678,10 +5678,10 @@
     <row r="72" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="37"/>
       <c r="B72" s="13" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D72" s="37"/>
       <c r="E72" s="29">
@@ -5699,10 +5699,10 @@
     <row r="73" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="37"/>
       <c r="B73" s="13" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D73" s="37"/>
       <c r="E73" s="29">
@@ -5722,10 +5722,10 @@
         <v>2</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D74" s="37"/>
       <c r="E74" s="29">
@@ -5743,10 +5743,10 @@
     <row r="75" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="37"/>
       <c r="B75" s="13" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D75" s="37"/>
       <c r="E75" s="29">
@@ -5764,10 +5764,10 @@
     <row r="76" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="37"/>
       <c r="B76" s="13" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D76" s="37"/>
       <c r="E76" s="29">
@@ -5785,10 +5785,10 @@
     <row r="77" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="37"/>
       <c r="B77" s="13" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D77" s="37"/>
       <c r="E77" s="29">
@@ -5806,10 +5806,10 @@
     <row r="78" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="37"/>
       <c r="B78" s="13" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D78" s="37"/>
       <c r="E78" s="29">
@@ -5827,10 +5827,10 @@
     <row r="79" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="37"/>
       <c r="B79" s="13" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D79" s="37"/>
       <c r="E79" s="29">
@@ -5861,10 +5861,10 @@
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="35"/>
       <c r="B81" s="7" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D81" s="35"/>
       <c r="E81" s="29">
@@ -6296,10 +6296,10 @@
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="35"/>
       <c r="B104" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="C104" s="4" t="s">
         <v>828</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>830</v>
       </c>
       <c r="D104" s="35"/>
       <c r="E104" s="29">
@@ -6317,10 +6317,10 @@
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="35"/>
       <c r="B105" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="C105" s="4" t="s">
         <v>829</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>831</v>
       </c>
       <c r="D105" s="35"/>
       <c r="E105" s="29">
@@ -6338,10 +6338,10 @@
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="35"/>
       <c r="B106" s="7" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D106" s="35"/>
       <c r="E106" s="29">
@@ -6359,10 +6359,10 @@
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="35"/>
       <c r="B107" s="7" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D107" s="35"/>
       <c r="E107" s="29">
@@ -6393,10 +6393,10 @@
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="35"/>
       <c r="B109" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C109" s="14" t="s">
         <v>1004</v>
-      </c>
-      <c r="C109" s="14" t="s">
-        <v>1006</v>
       </c>
       <c r="D109" s="35"/>
       <c r="E109" s="29">
@@ -6414,10 +6414,10 @@
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="35"/>
       <c r="B110" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C110" s="14" t="s">
         <v>1005</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>1007</v>
       </c>
       <c r="D110" s="35"/>
       <c r="E110" s="29">
@@ -6462,10 +6462,10 @@
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="35"/>
       <c r="B112" s="13" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="29">
@@ -6594,10 +6594,10 @@
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="35"/>
       <c r="B118" s="7" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D118" s="35"/>
       <c r="E118" s="29">
@@ -6615,10 +6615,10 @@
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="35"/>
       <c r="B119" s="7" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D119" s="35"/>
       <c r="E119" s="29">
@@ -6636,10 +6636,10 @@
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="35"/>
       <c r="B120" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D120" s="35"/>
       <c r="E120" s="29">
@@ -6657,10 +6657,10 @@
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="35"/>
       <c r="B121" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D121" s="35"/>
       <c r="E121" s="29">
@@ -6678,10 +6678,10 @@
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="35"/>
       <c r="B122" s="7" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D122" s="35"/>
       <c r="E122" s="29">
@@ -6699,10 +6699,10 @@
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="35"/>
       <c r="B123" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="C123" s="4" t="s">
         <v>916</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>918</v>
       </c>
       <c r="D123" s="35"/>
       <c r="E123" s="29">
@@ -6720,10 +6720,10 @@
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="35"/>
       <c r="B124" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="C124" s="4" t="s">
         <v>917</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>919</v>
       </c>
       <c r="D124" s="35"/>
       <c r="E124" s="29">
@@ -6867,10 +6867,10 @@
     <row r="131" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="37"/>
       <c r="B131" s="13" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D131" s="37"/>
       <c r="E131" s="29">
@@ -7315,10 +7315,10 @@
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="35"/>
       <c r="B149" s="7" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D149" s="35"/>
       <c r="E149" s="29">
@@ -7336,10 +7336,10 @@
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="35"/>
       <c r="B150" s="7" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D150" s="35"/>
       <c r="E150" s="29">
@@ -7357,10 +7357,10 @@
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="35"/>
       <c r="B151" s="7" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D151" s="35"/>
       <c r="E151" s="29">
@@ -7378,10 +7378,10 @@
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="35"/>
       <c r="B152" s="7" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D152" s="35"/>
       <c r="E152" s="29">
@@ -7412,10 +7412,10 @@
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="35"/>
       <c r="B154" s="7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D154" s="35"/>
       <c r="E154" s="29">
@@ -7433,10 +7433,10 @@
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="35"/>
       <c r="B155" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D155" s="35"/>
       <c r="E155" s="29">
@@ -7454,10 +7454,10 @@
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="35"/>
       <c r="B156" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D156" s="35"/>
       <c r="E156" s="29">
@@ -7821,14 +7821,14 @@
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="35"/>
       <c r="B173" s="7" t="s">
-        <v>624</v>
+        <v>451</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>626</v>
+        <v>452</v>
       </c>
       <c r="D173" s="35"/>
       <c r="E173" s="29">
-        <v>44378</v>
+        <v>44362</v>
       </c>
       <c r="F173" s="53" t="s">
         <v>618</v>
@@ -7842,14 +7842,14 @@
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="35"/>
       <c r="B174" s="7" t="s">
-        <v>625</v>
+        <v>463</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>627</v>
+        <v>464</v>
       </c>
       <c r="D174" s="35"/>
       <c r="E174" s="29">
-        <v>44378</v>
+        <v>44362</v>
       </c>
       <c r="F174" s="53" t="s">
         <v>618</v>
@@ -7863,14 +7863,14 @@
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="35"/>
       <c r="B175" s="7" t="s">
-        <v>451</v>
+        <v>1034</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>452</v>
+        <v>624</v>
       </c>
       <c r="D175" s="35"/>
       <c r="E175" s="29">
-        <v>44362</v>
+        <v>44378</v>
       </c>
       <c r="F175" s="53" t="s">
         <v>618</v>
@@ -7884,14 +7884,14 @@
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="35"/>
       <c r="B176" s="7" t="s">
-        <v>463</v>
+        <v>1035</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>464</v>
+        <v>625</v>
       </c>
       <c r="D176" s="35"/>
       <c r="E176" s="29">
-        <v>44362</v>
+        <v>44378</v>
       </c>
       <c r="F176" s="53" t="s">
         <v>618</v>
@@ -7946,7 +7946,7 @@
         <v>201</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D179" s="35"/>
       <c r="E179" s="29">
@@ -7968,10 +7968,10 @@
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="35"/>
       <c r="B180" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="C180" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="C180" s="4" t="s">
-        <v>631</v>
       </c>
       <c r="D180" s="35"/>
       <c r="E180" s="29">
@@ -7989,10 +7989,10 @@
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="35"/>
       <c r="B181" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="C181" s="4" t="s">
         <v>630</v>
-      </c>
-      <c r="C181" s="4" t="s">
-        <v>632</v>
       </c>
       <c r="D181" s="35"/>
       <c r="E181" s="29">
@@ -8023,10 +8023,10 @@
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="35"/>
       <c r="B183" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="C183" s="4" t="s">
         <v>633</v>
-      </c>
-      <c r="C183" s="4" t="s">
-        <v>635</v>
       </c>
       <c r="D183" s="35"/>
       <c r="E183" s="29">
@@ -8048,10 +8048,10 @@
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="35"/>
       <c r="B184" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="C184" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="C184" s="4" t="s">
-        <v>636</v>
       </c>
       <c r="D184" s="35"/>
       <c r="E184" s="29">
@@ -8073,10 +8073,10 @@
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="35"/>
       <c r="B185" s="7" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D185" s="35"/>
       <c r="E185" s="29">
@@ -8094,10 +8094,10 @@
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="35"/>
       <c r="B186" s="7" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D186" s="35"/>
       <c r="E186" s="29">
@@ -8115,10 +8115,10 @@
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="35"/>
       <c r="B187" s="7" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D187" s="35"/>
       <c r="E187" s="29">
@@ -8136,10 +8136,10 @@
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="35"/>
       <c r="B188" s="7" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D188" s="35"/>
       <c r="E188" s="29">
@@ -8721,10 +8721,10 @@
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="7" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="29">
@@ -8746,10 +8746,10 @@
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
       <c r="B214" s="7" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D214" s="35"/>
       <c r="E214" s="29">
@@ -8784,10 +8784,10 @@
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="35"/>
       <c r="B216" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C216" s="4" t="s">
         <v>1016</v>
-      </c>
-      <c r="C216" s="4" t="s">
-        <v>1018</v>
       </c>
       <c r="D216" s="35"/>
       <c r="E216" s="29">
@@ -8805,10 +8805,10 @@
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="35"/>
       <c r="B217" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C217" s="4" t="s">
         <v>1017</v>
-      </c>
-      <c r="C217" s="4" t="s">
-        <v>1019</v>
       </c>
       <c r="D217" s="35"/>
       <c r="E217" s="29">
@@ -8851,10 +8851,10 @@
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="35"/>
       <c r="B219" s="7" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D219" s="35"/>
       <c r="E219" s="29">
@@ -9051,10 +9051,10 @@
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="35"/>
       <c r="B227" s="7" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D227" s="35"/>
       <c r="E227" s="29">
@@ -9072,10 +9072,10 @@
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="35"/>
       <c r="B228" s="7" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D228" s="35"/>
       <c r="E228" s="29">
@@ -9147,10 +9147,10 @@
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="35"/>
       <c r="B231" s="7" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D231" s="35"/>
       <c r="E231" s="29">
@@ -9172,10 +9172,10 @@
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="35"/>
       <c r="B232" s="7" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D232" s="35"/>
       <c r="E232" s="29">
@@ -9397,10 +9397,10 @@
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="35"/>
       <c r="B241" s="7" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="D241" s="35"/>
       <c r="E241" s="29">
@@ -9722,10 +9722,10 @@
     <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="35"/>
       <c r="B254" s="7" t="s">
+        <v>892</v>
+      </c>
+      <c r="C254" s="4" t="s">
         <v>894</v>
-      </c>
-      <c r="C254" s="4" t="s">
-        <v>896</v>
       </c>
       <c r="D254" s="35"/>
       <c r="E254" s="29">
@@ -9743,10 +9743,10 @@
     <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="35"/>
       <c r="B255" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="C255" s="4" t="s">
         <v>895</v>
-      </c>
-      <c r="C255" s="4" t="s">
-        <v>897</v>
       </c>
       <c r="D255" s="35"/>
       <c r="E255" s="29">
@@ -9977,10 +9977,10 @@
     <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="35"/>
       <c r="B265" s="7" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D265" s="35"/>
       <c r="E265" s="29">
@@ -10166,10 +10166,10 @@
     <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="35"/>
       <c r="B274" s="7" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="D274" s="35"/>
       <c r="E274" s="29">
@@ -10187,10 +10187,10 @@
     <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="35"/>
       <c r="B275" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="C275" s="4" t="s">
         <v>840</v>
-      </c>
-      <c r="C275" s="4" t="s">
-        <v>842</v>
       </c>
       <c r="D275" s="35"/>
       <c r="E275" s="29">
@@ -10208,10 +10208,10 @@
     <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="35"/>
       <c r="B276" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="C276" s="4" t="s">
         <v>841</v>
-      </c>
-      <c r="C276" s="4" t="s">
-        <v>843</v>
       </c>
       <c r="D276" s="35"/>
       <c r="E276" s="29">
@@ -10242,10 +10242,10 @@
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="35"/>
       <c r="B278" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="C278" s="4" t="s">
         <v>1000</v>
-      </c>
-      <c r="C278" s="4" t="s">
-        <v>1002</v>
       </c>
       <c r="D278" s="35"/>
       <c r="E278" s="29">
@@ -10263,10 +10263,10 @@
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="35"/>
       <c r="B279" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="C279" s="4" t="s">
         <v>1001</v>
-      </c>
-      <c r="C279" s="4" t="s">
-        <v>1003</v>
       </c>
       <c r="D279" s="35"/>
       <c r="E279" s="29">
@@ -10311,10 +10311,10 @@
     <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="35"/>
       <c r="B281" s="7" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D281" s="35"/>
       <c r="E281" s="29">
@@ -10858,10 +10858,10 @@
     <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="35"/>
       <c r="B302" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D302" s="35"/>
       <c r="E302" s="29">
@@ -10879,10 +10879,10 @@
     <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="35"/>
       <c r="B303" s="7" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D303" s="35"/>
       <c r="E303" s="29">
@@ -10926,10 +10926,10 @@
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="35"/>
       <c r="B306" s="7" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D306" s="35"/>
       <c r="E306" s="29"/>
@@ -10943,10 +10943,10 @@
     <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="35"/>
       <c r="B307" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="C307" s="4" t="s">
         <v>817</v>
-      </c>
-      <c r="C307" s="4" t="s">
-        <v>819</v>
       </c>
       <c r="D307" s="35"/>
       <c r="E307" s="29"/>
@@ -10960,10 +10960,10 @@
     <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="35"/>
       <c r="B308" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="C308" s="4" t="s">
         <v>818</v>
-      </c>
-      <c r="C308" s="4" t="s">
-        <v>820</v>
       </c>
       <c r="D308" s="35"/>
       <c r="E308" s="29"/>
@@ -10977,10 +10977,10 @@
     <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="35"/>
       <c r="B309" s="7" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D309" s="35"/>
       <c r="E309" s="29"/>
@@ -10994,10 +10994,10 @@
     <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="35"/>
       <c r="B310" s="7" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D310" s="35"/>
       <c r="E310" s="29">
@@ -11112,7 +11112,7 @@
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="35"/>
       <c r="B316" s="7" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="C316" s="4" t="s">
         <v>472</v>
@@ -11133,7 +11133,7 @@
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="35"/>
       <c r="B317" s="7" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C317" s="4" t="s">
         <v>473</v>
@@ -11154,10 +11154,10 @@
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="35"/>
       <c r="B318" s="7" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D318" s="35"/>
       <c r="E318" s="29">
@@ -11175,10 +11175,10 @@
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="35"/>
       <c r="B319" s="7" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D319" s="35"/>
       <c r="E319" s="29">
@@ -11264,10 +11264,10 @@
     <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="35"/>
       <c r="B324" s="7" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D324" s="35"/>
       <c r="E324" s="29">
@@ -11298,10 +11298,10 @@
     <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="35"/>
       <c r="B326" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C326" s="4" t="s">
         <v>1012</v>
-      </c>
-      <c r="C326" s="4" t="s">
-        <v>1014</v>
       </c>
       <c r="D326" s="35"/>
       <c r="E326" s="29">
@@ -11319,10 +11319,10 @@
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="35"/>
       <c r="B327" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C327" s="4" t="s">
         <v>1013</v>
-      </c>
-      <c r="C327" s="4" t="s">
-        <v>1015</v>
       </c>
       <c r="D327" s="35"/>
       <c r="E327" s="29">
@@ -11415,10 +11415,10 @@
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="35"/>
       <c r="B331" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D331" s="35"/>
       <c r="E331" s="29">
@@ -11853,10 +11853,10 @@
     <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="35"/>
       <c r="B349" s="7" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D349" s="35"/>
       <c r="E349" s="29">
@@ -11971,10 +11971,10 @@
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="35"/>
       <c r="B355" s="7" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C355" s="4" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D355" s="35"/>
       <c r="E355" s="29">
@@ -12178,7 +12178,7 @@
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="35"/>
       <c r="B366" s="7" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C366" s="4" t="s">
         <v>475</v>
@@ -12199,7 +12199,7 @@
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="35"/>
       <c r="B367" s="7" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="C367" s="4" t="s">
         <v>476</v>
@@ -12291,7 +12291,7 @@
         <v>552</v>
       </c>
       <c r="C372" s="4" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D372" s="35"/>
       <c r="E372" s="29">
@@ -12312,7 +12312,7 @@
         <v>551</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D373" s="35"/>
       <c r="E373" s="29">
@@ -12330,10 +12330,10 @@
     <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="35"/>
       <c r="B374" s="7" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D374" s="35"/>
       <c r="E374" s="29">
@@ -12351,10 +12351,10 @@
     <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="35"/>
       <c r="B375" s="7" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D375" s="35"/>
       <c r="E375" s="29">
@@ -12372,10 +12372,10 @@
     <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="35"/>
       <c r="B376" s="7" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="D376" s="35"/>
       <c r="E376" s="29">
@@ -12393,10 +12393,10 @@
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="35"/>
       <c r="B377" s="7" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C377" s="4" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D377" s="35"/>
       <c r="E377" s="29">
@@ -12427,10 +12427,10 @@
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="35"/>
       <c r="B379" s="7" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D379" s="35"/>
       <c r="E379" s="29">
@@ -12452,10 +12452,10 @@
     <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="35"/>
       <c r="B380" s="7" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C380" s="4" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D380" s="35"/>
       <c r="E380" s="29">
@@ -12490,10 +12490,10 @@
     <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="35"/>
       <c r="B382" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C382" s="4" t="s">
         <v>1024</v>
-      </c>
-      <c r="C382" s="4" t="s">
-        <v>1026</v>
       </c>
       <c r="D382" s="35"/>
       <c r="E382" s="29">
@@ -12511,10 +12511,10 @@
     <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="35"/>
       <c r="B383" s="7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C383" s="4" t="s">
         <v>1025</v>
-      </c>
-      <c r="C383" s="4" t="s">
-        <v>1027</v>
       </c>
       <c r="D383" s="35"/>
       <c r="E383" s="29">
@@ -12557,10 +12557,10 @@
     <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="35"/>
       <c r="B385" s="7" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="D385" s="35"/>
       <c r="E385" s="29">
@@ -12699,10 +12699,10 @@
     <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="35"/>
       <c r="B391" s="7" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="D391" s="35"/>
       <c r="E391" s="29">
@@ -12724,10 +12724,10 @@
     <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="35"/>
       <c r="B392" s="7" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C392" s="4" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D392" s="35"/>
       <c r="E392" s="29">
@@ -12745,10 +12745,10 @@
     <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="35"/>
       <c r="B393" s="7" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C393" s="4" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D393" s="35"/>
       <c r="E393" s="29">
@@ -12795,10 +12795,10 @@
     <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="35"/>
       <c r="B395" s="7" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C395" s="4" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="D395" s="35"/>
       <c r="E395" s="29">
@@ -12820,10 +12820,10 @@
     <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="35"/>
       <c r="B396" s="7" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D396" s="35"/>
       <c r="E396" s="29">
@@ -12845,10 +12845,10 @@
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="35"/>
       <c r="B397" s="7" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D397" s="35"/>
       <c r="E397" s="29">
@@ -13020,10 +13020,10 @@
     <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" s="35"/>
       <c r="B404" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="C404" s="4" t="s">
         <v>721</v>
-      </c>
-      <c r="C404" s="4" t="s">
-        <v>723</v>
       </c>
       <c r="D404" s="35"/>
       <c r="E404" s="29">
@@ -13045,10 +13045,10 @@
     <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="35"/>
       <c r="B405" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="C405" s="4" t="s">
         <v>722</v>
-      </c>
-      <c r="C405" s="4" t="s">
-        <v>724</v>
       </c>
       <c r="D405" s="35"/>
       <c r="E405" s="29">
@@ -13070,10 +13070,10 @@
     <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" s="35"/>
       <c r="B406" s="7" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="D406" s="35"/>
       <c r="E406" s="29">
@@ -13091,10 +13091,10 @@
     <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" s="35"/>
       <c r="B407" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="C407" s="4" t="s">
         <v>850</v>
-      </c>
-      <c r="C407" s="4" t="s">
-        <v>852</v>
       </c>
       <c r="D407" s="35"/>
       <c r="E407" s="29">
@@ -13112,10 +13112,10 @@
     <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" s="35"/>
       <c r="B408" s="7" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C408" s="4" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D408" s="35"/>
       <c r="E408" s="29">
@@ -13133,10 +13133,10 @@
     <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A409" s="35"/>
       <c r="B409" s="7" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="C409" s="4" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D409" s="35"/>
       <c r="E409" s="29">
@@ -13179,10 +13179,10 @@
     <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" s="35"/>
       <c r="B411" s="7" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D411" s="35"/>
       <c r="E411" s="29">
@@ -13204,10 +13204,10 @@
     <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A412" s="35"/>
       <c r="B412" s="7" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D412" s="35"/>
       <c r="E412" s="29">
@@ -13225,10 +13225,10 @@
     <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" s="35"/>
       <c r="B413" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="C413" s="4" t="s">
         <v>717</v>
-      </c>
-      <c r="C413" s="4" t="s">
-        <v>719</v>
       </c>
       <c r="D413" s="35"/>
       <c r="E413" s="29">
@@ -13246,10 +13246,10 @@
     <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="35"/>
       <c r="B414" s="7" t="s">
+        <v>716</v>
+      </c>
+      <c r="C414" s="4" t="s">
         <v>718</v>
-      </c>
-      <c r="C414" s="4" t="s">
-        <v>720</v>
       </c>
       <c r="D414" s="35"/>
       <c r="E414" s="29">
@@ -13367,10 +13367,10 @@
     <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419" s="35"/>
       <c r="B419" s="7" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="D419" s="35"/>
       <c r="E419" s="29">
@@ -13388,10 +13388,10 @@
     <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420" s="35"/>
       <c r="B420" s="7" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C420" s="4" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D420" s="35"/>
       <c r="E420" s="29">
@@ -13522,10 +13522,10 @@
     <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="35"/>
       <c r="B426" s="7" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C426" s="4" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D426" s="35"/>
       <c r="E426" s="29">
@@ -13543,10 +13543,10 @@
     <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="35"/>
       <c r="B427" s="7" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D427" s="35"/>
       <c r="E427" s="29">
@@ -13698,7 +13698,7 @@
         <v>538</v>
       </c>
       <c r="C435" s="4" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D435" s="35"/>
       <c r="E435" s="29">
@@ -13726,7 +13726,7 @@
         <v>539</v>
       </c>
       <c r="C436" s="4" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D436" s="35"/>
       <c r="E436" s="29">
@@ -13754,7 +13754,7 @@
         <v>541</v>
       </c>
       <c r="C437" s="4" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D437" s="35"/>
       <c r="E437" s="29">
@@ -13782,7 +13782,7 @@
         <v>542</v>
       </c>
       <c r="C438" s="4" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D438" s="35"/>
       <c r="E438" s="29">
@@ -13807,10 +13807,10 @@
     <row r="439" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A439" s="35"/>
       <c r="B439" s="13" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C439" s="14" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D439" s="35"/>
       <c r="E439" s="29">
@@ -13937,10 +13937,10 @@
     <row r="446" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A446" s="35"/>
       <c r="B446" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C446" s="4" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D446" s="35"/>
       <c r="E446" s="29">
@@ -14295,10 +14295,10 @@
     <row r="464" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A464" s="35"/>
       <c r="B464" s="7" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C464" s="4" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D464" s="35"/>
       <c r="E464" s="29">
@@ -14320,10 +14320,10 @@
     <row r="465" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A465" s="35"/>
       <c r="B465" s="7" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C465" s="4" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D465" s="35"/>
       <c r="E465" s="29">
@@ -14345,10 +14345,10 @@
     <row r="466" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A466" s="35"/>
       <c r="B466" s="7" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C466" s="4" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D466" s="35"/>
       <c r="E466" s="29">
@@ -14370,10 +14370,10 @@
     <row r="467" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A467" s="35"/>
       <c r="B467" s="7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C467" s="4" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D467" s="35"/>
       <c r="E467" s="29">
@@ -14395,10 +14395,10 @@
     <row r="468" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A468" s="35"/>
       <c r="B468" s="7" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C468" s="4" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D468" s="35"/>
       <c r="E468" s="29">
@@ -14433,10 +14433,10 @@
     <row r="470" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A470" s="35"/>
       <c r="B470" s="7" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C470" s="4" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D470" s="35"/>
       <c r="E470" s="29">
@@ -14475,10 +14475,10 @@
     <row r="472" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A472" s="35"/>
       <c r="B472" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C472" s="4" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D472" s="35"/>
       <c r="E472" s="29">
@@ -14496,10 +14496,10 @@
     <row r="473" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A473" s="35"/>
       <c r="B473" s="7" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D473" s="35"/>
       <c r="E473" s="29">
@@ -14572,10 +14572,10 @@
     <row r="477" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A477" s="35"/>
       <c r="B477" s="7" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D477" s="35"/>
       <c r="E477" s="29">
@@ -14597,10 +14597,10 @@
     <row r="478" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A478" s="35"/>
       <c r="B478" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D478" s="35"/>
       <c r="E478" s="29">
@@ -14618,10 +14618,10 @@
     <row r="479" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A479" s="35"/>
       <c r="B479" s="7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D479" s="35"/>
       <c r="E479" s="29">
@@ -14652,10 +14652,10 @@
     <row r="481" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A481" s="35"/>
       <c r="B481" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="C481" s="4" t="s">
         <v>651</v>
-      </c>
-      <c r="C481" s="4" t="s">
-        <v>653</v>
       </c>
       <c r="D481" s="35"/>
       <c r="E481" s="29">
@@ -14677,10 +14677,10 @@
     <row r="482" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A482" s="35"/>
       <c r="B482" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="C482" s="4" t="s">
         <v>652</v>
-      </c>
-      <c r="C482" s="4" t="s">
-        <v>654</v>
       </c>
       <c r="D482" s="35"/>
       <c r="E482" s="29">
@@ -14702,10 +14702,10 @@
     <row r="483" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A483" s="35"/>
       <c r="B483" s="7" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D483" s="35"/>
       <c r="E483" s="29">
@@ -14723,10 +14723,10 @@
     <row r="484" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A484" s="35"/>
       <c r="B484" s="7" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D484" s="35"/>
       <c r="E484" s="29">
@@ -14744,10 +14744,10 @@
     <row r="485" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A485" s="35"/>
       <c r="B485" s="7" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D485" s="35"/>
       <c r="E485" s="29">
@@ -14765,10 +14765,10 @@
     <row r="486" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A486" s="35"/>
       <c r="B486" s="7" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D486" s="35"/>
       <c r="E486" s="29">
@@ -14799,10 +14799,10 @@
     <row r="488" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A488" s="35"/>
       <c r="B488" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="C488" s="4" t="s">
         <v>655</v>
-      </c>
-      <c r="C488" s="4" t="s">
-        <v>657</v>
       </c>
       <c r="D488" s="35"/>
       <c r="E488" s="29">
@@ -14824,10 +14824,10 @@
     <row r="489" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A489" s="35"/>
       <c r="B489" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="C489" s="4" t="s">
         <v>656</v>
-      </c>
-      <c r="C489" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="D489" s="35"/>
       <c r="E489" s="29">
@@ -14862,10 +14862,10 @@
     <row r="491" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A491" s="35"/>
       <c r="B491" s="7" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D491" s="35"/>
       <c r="E491" s="29">
@@ -14900,10 +14900,10 @@
     <row r="493" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A493" s="35"/>
       <c r="B493" s="7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D493" s="35"/>
       <c r="E493" s="29">
@@ -14925,10 +14925,10 @@
     <row r="494" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A494" s="35"/>
       <c r="B494" s="7" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C494" s="4" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="D494" s="35"/>
       <c r="E494" s="29">
@@ -14950,10 +14950,10 @@
     <row r="495" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A495" s="35"/>
       <c r="B495" s="7" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C495" s="4" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D495" s="35"/>
       <c r="E495" s="29">
@@ -14988,10 +14988,10 @@
     <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497" s="35"/>
       <c r="B497" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C497" s="4" t="s">
         <v>1020</v>
-      </c>
-      <c r="C497" s="4" t="s">
-        <v>1022</v>
       </c>
       <c r="D497" s="35"/>
       <c r="E497" s="29">
@@ -15009,10 +15009,10 @@
     <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498" s="35"/>
       <c r="B498" s="7" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C498" s="4" t="s">
         <v>1021</v>
-      </c>
-      <c r="C498" s="4" t="s">
-        <v>1023</v>
       </c>
       <c r="D498" s="35"/>
       <c r="E498" s="29">
@@ -15055,10 +15055,10 @@
     <row r="500" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A500" s="35"/>
       <c r="B500" s="7" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D500" s="35"/>
       <c r="E500" s="29">
@@ -15230,10 +15230,10 @@
     <row r="507" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A507" s="35"/>
       <c r="B507" s="7" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C507" s="4" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D507" s="35"/>
       <c r="E507" s="29">
@@ -15301,10 +15301,10 @@
     <row r="510" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A510" s="35"/>
       <c r="B510" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="C510" s="4" t="s">
         <v>936</v>
-      </c>
-      <c r="C510" s="4" t="s">
-        <v>938</v>
       </c>
       <c r="D510" s="35"/>
       <c r="E510" s="29">
@@ -15326,10 +15326,10 @@
     <row r="511" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A511" s="35"/>
       <c r="B511" s="7" t="s">
+        <v>935</v>
+      </c>
+      <c r="C511" s="4" t="s">
         <v>937</v>
-      </c>
-      <c r="C511" s="4" t="s">
-        <v>939</v>
       </c>
       <c r="D511" s="35"/>
       <c r="E511" s="29">
@@ -15547,10 +15547,10 @@
     <row r="520" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A520" s="35"/>
       <c r="B520" s="7" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C520" s="4" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D520" s="35"/>
       <c r="E520" s="29">
@@ -15675,7 +15675,7 @@
         <v>163</v>
       </c>
       <c r="C525" s="4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D525" s="35"/>
       <c r="E525" s="29">
@@ -15700,7 +15700,7 @@
         <v>164</v>
       </c>
       <c r="C526" s="4" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D526" s="35"/>
       <c r="E526" s="29">
@@ -15725,7 +15725,7 @@
         <v>165</v>
       </c>
       <c r="C527" s="4" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D527" s="35"/>
       <c r="E527" s="29">
@@ -15750,7 +15750,7 @@
         <v>166</v>
       </c>
       <c r="C528" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D528" s="35"/>
       <c r="E528" s="29">
@@ -15775,7 +15775,7 @@
         <v>167</v>
       </c>
       <c r="C529" s="4" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D529" s="35"/>
       <c r="E529" s="29">
@@ -15800,7 +15800,7 @@
         <v>168</v>
       </c>
       <c r="C530" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D530" s="35"/>
       <c r="E530" s="29">
@@ -15825,7 +15825,7 @@
         <v>169</v>
       </c>
       <c r="C531" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="D531" s="35"/>
       <c r="E531" s="29">
@@ -15847,10 +15847,10 @@
     <row r="532" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A532" s="35"/>
       <c r="B532" s="7" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C532" s="4" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D532" s="35"/>
       <c r="E532" s="29">
@@ -15871,7 +15871,7 @@
         <v>170</v>
       </c>
       <c r="C533" s="4" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D533" s="35"/>
       <c r="E533" s="29">
@@ -15896,7 +15896,7 @@
         <v>171</v>
       </c>
       <c r="C534" s="4" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D534" s="35"/>
       <c r="E534" s="29">
@@ -15921,7 +15921,7 @@
         <v>172</v>
       </c>
       <c r="C535" s="4" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="D535" s="35"/>
       <c r="E535" s="29">
@@ -15946,7 +15946,7 @@
         <v>173</v>
       </c>
       <c r="C536" s="4" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D536" s="35"/>
       <c r="E536" s="29">
@@ -15971,7 +15971,7 @@
         <v>174</v>
       </c>
       <c r="C537" s="4" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D537" s="35"/>
       <c r="E537" s="29">
@@ -15996,7 +15996,7 @@
         <v>175</v>
       </c>
       <c r="C538" s="4" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D538" s="35"/>
       <c r="E538" s="29">
@@ -16034,7 +16034,7 @@
         <v>176</v>
       </c>
       <c r="C540" s="4" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="D540" s="35"/>
       <c r="E540" s="29">
@@ -16059,7 +16059,7 @@
         <v>196</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D541" s="35"/>
       <c r="E541" s="29">
@@ -16081,10 +16081,10 @@
     <row r="542" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A542" s="35"/>
       <c r="B542" s="7" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C542" s="4" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D542" s="35"/>
       <c r="E542" s="29">
@@ -16119,10 +16119,10 @@
     <row r="544" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A544" s="35"/>
       <c r="B544" s="7" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C544" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D544" s="35"/>
       <c r="E544" s="29">
@@ -16144,10 +16144,10 @@
     <row r="545" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A545" s="35"/>
       <c r="B545" s="7" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C545" s="4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D545" s="35"/>
       <c r="E545" s="29">
@@ -16169,10 +16169,10 @@
     <row r="546" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A546" s="35"/>
       <c r="B546" s="7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C546" s="4" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D546" s="35"/>
       <c r="E546" s="29">
@@ -16194,10 +16194,10 @@
     <row r="547" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A547" s="35"/>
       <c r="B547" s="7" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C547" s="4" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D547" s="35"/>
       <c r="E547" s="29">
@@ -16219,10 +16219,10 @@
     <row r="548" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A548" s="35"/>
       <c r="B548" s="7" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C548" s="4" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D548" s="35"/>
       <c r="E548" s="29">
@@ -16291,10 +16291,10 @@
     <row r="552" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A552" s="35"/>
       <c r="B552" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="C552" s="4" t="s">
         <v>693</v>
-      </c>
-      <c r="C552" s="4" t="s">
-        <v>695</v>
       </c>
       <c r="D552" s="35"/>
       <c r="E552" s="29">
@@ -16312,10 +16312,10 @@
     <row r="553" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A553" s="35"/>
       <c r="B553" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="C553" s="4" t="s">
         <v>694</v>
-      </c>
-      <c r="C553" s="4" t="s">
-        <v>696</v>
       </c>
       <c r="D553" s="35"/>
       <c r="E553" s="29">
@@ -16464,10 +16464,10 @@
     <row r="561" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A561" s="35"/>
       <c r="B561" s="7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C561" s="14" t="s">
         <v>1008</v>
-      </c>
-      <c r="C561" s="14" t="s">
-        <v>1010</v>
       </c>
       <c r="D561" s="35"/>
       <c r="E561" s="29">
@@ -16485,10 +16485,10 @@
     <row r="562" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A562" s="35"/>
       <c r="B562" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C562" s="14" t="s">
         <v>1009</v>
-      </c>
-      <c r="C562" s="14" t="s">
-        <v>1011</v>
       </c>
       <c r="D562" s="35"/>
       <c r="E562" s="29">
@@ -16531,10 +16531,10 @@
     <row r="564" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A564" s="35"/>
       <c r="B564" s="13" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C564" s="14" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D564" s="35"/>
       <c r="E564" s="29">
@@ -16661,10 +16661,10 @@
     <row r="570" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A570" s="35"/>
       <c r="B570" s="7" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="C570" s="4" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="D570" s="35"/>
       <c r="E570" s="29">
@@ -16682,10 +16682,10 @@
     <row r="571" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A571" s="35"/>
       <c r="B571" s="7" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C571" s="4" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D571" s="35"/>
       <c r="E571" s="29">
@@ -16703,10 +16703,10 @@
     <row r="572" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A572" s="35"/>
       <c r="B572" s="7" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C572" s="4" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D572" s="35"/>
       <c r="E572" s="29">
@@ -16724,10 +16724,10 @@
     <row r="573" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A573" s="35"/>
       <c r="B573" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C573" s="4" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D573" s="35"/>
       <c r="E573" s="29">
@@ -16745,10 +16745,10 @@
     <row r="574" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A574" s="35"/>
       <c r="B574" s="7" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="C574" s="4" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D574" s="35"/>
       <c r="E574" s="29">
@@ -16766,10 +16766,10 @@
     <row r="575" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A575" s="35"/>
       <c r="B575" s="7" t="s">
+        <v>920</v>
+      </c>
+      <c r="C575" s="4" t="s">
         <v>922</v>
-      </c>
-      <c r="C575" s="4" t="s">
-        <v>924</v>
       </c>
       <c r="D575" s="35"/>
       <c r="E575" s="29">
@@ -16787,10 +16787,10 @@
     <row r="576" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A576" s="35"/>
       <c r="B576" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="C576" s="4" t="s">
         <v>923</v>
-      </c>
-      <c r="C576" s="4" t="s">
-        <v>925</v>
       </c>
       <c r="D576" s="35"/>
       <c r="E576" s="29">
@@ -16934,10 +16934,10 @@
     <row r="583" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A583" s="37"/>
       <c r="B583" s="13" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C583" s="14" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D583" s="37"/>
       <c r="E583" s="31">
@@ -17360,10 +17360,10 @@
     <row r="601" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A601" s="35"/>
       <c r="B601" s="7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D601" s="35"/>
       <c r="E601" s="29">
@@ -17381,10 +17381,10 @@
     <row r="602" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A602" s="35"/>
       <c r="B602" s="7" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C602" s="4" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D602" s="35"/>
       <c r="E602" s="29">
@@ -17402,10 +17402,10 @@
     <row r="603" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A603" s="35"/>
       <c r="B603" s="7" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="C603" s="4" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D603" s="35"/>
       <c r="E603" s="29">
@@ -17423,10 +17423,10 @@
     <row r="604" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A604" s="35"/>
       <c r="B604" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C604" s="4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D604" s="35"/>
       <c r="E604" s="29">
@@ -17457,10 +17457,10 @@
     <row r="606" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A606" s="35"/>
       <c r="B606" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C606" s="4" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D606" s="35"/>
       <c r="E606" s="29">
@@ -17478,10 +17478,10 @@
     <row r="607" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A607" s="35"/>
       <c r="B607" s="7" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="C607" s="4" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D607" s="35"/>
       <c r="E607" s="29">
@@ -17499,10 +17499,10 @@
     <row r="608" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A608" s="35"/>
       <c r="B608" s="7" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C608" s="4" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D608" s="35"/>
       <c r="E608" s="29">
@@ -17570,7 +17570,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F4:F6 F9 F27:F29 F40:F41 F43 F45:F47 F84:F90 F93:F98 F159:F163 F165:F169 F171:F177 F179:F181 F193 F263:F265 F267:F271 F324 F349:F351 F353:F355 F369:F370 F431:F439 F442:F444 F446 F448:F452 F454:F457 F459:F460 F470:F475 F477:F479 F488:F489 F190:F191 F491 F493:F495 F540:F542 F544:F548 F464:F468 F551:F555 F557:F559 F149:F152 F601:F604 F328:F347 F426:F429 F358:F360 F154:F156 F606:F608 F81 F60:F79 F58 F34:F37 F310 F32 F100:F107 F302:F303 F274:F276 F183:F188 F481:F486 F372:F377 F54 F22:F24 F111:F147 F563:F599 F499:F538 F280:F300 F218:F261 F384:F424 F12:F13 F20 F318:F319 F50:F51 F379:F380 F321:F322 F15 F195:F214 F362:F367 F312:F313 F314:F315 F316:F317 F278:F279 F109:F110 F561:F562 F326:F327 F216:F217 F497:F498 F382:F383 F17:F19" numberStoredAsText="1"/>
+    <ignoredError sqref="F4:F6 F9 F27:F29 F40:F41 F43 F45:F47 F84:F90 F93:F98 F159:F163 F165:F169 F177 F179:F181 F193 F263:F265 F267:F271 F324 F349:F351 F353:F355 F369:F370 F431:F439 F442:F444 F446 F448:F452 F454:F457 F459:F460 F470:F475 F477:F479 F488:F489 F190:F191 F491 F493:F495 F540:F542 F544:F548 F464:F468 F551:F555 F557:F559 F149:F152 F601:F604 F426:F429 F358:F360 F154:F156 F606:F608 F81 F60:F79 F58 F34:F37 F310 F32 F100:F107 F302:F303 F274:F276 F183:F188 F481:F486 F372:F377 F54 F22:F24 F12:F13 F50:F51 F379:F380 F321:F322 F15 F195:F214 F362:F367 F312:F319 F278:F300 F109:F147 F561:F599 F326:F347 F216:F261 F497:F538 F382:F424 F17:F20 F171:F172 F173:F174 F175:F176" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Pertanggal 22 Desember 2021 17:22:04
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4356,10 +4356,10 @@
   <dimension ref="A1:L618"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4625,7 +4625,9 @@
         <v>1039</v>
       </c>
       <c r="D13" s="35"/>
-      <c r="E13" s="29"/>
+      <c r="E13" s="29">
+        <v>44550</v>
+      </c>
       <c r="F13" s="53" t="s">
         <v>618</v>
       </c>
@@ -4644,7 +4646,9 @@
         <v>1047</v>
       </c>
       <c r="D14" s="35"/>
-      <c r="E14" s="29"/>
+      <c r="E14" s="29">
+        <v>44551</v>
+      </c>
       <c r="F14" s="53" t="s">
         <v>618</v>
       </c>
@@ -4663,7 +4667,9 @@
         <v>1041</v>
       </c>
       <c r="D15" s="35"/>
-      <c r="E15" s="29"/>
+      <c r="E15" s="29">
+        <v>44551</v>
+      </c>
       <c r="F15" s="53" t="s">
         <v>618</v>
       </c>
@@ -4682,7 +4688,9 @@
         <v>1043</v>
       </c>
       <c r="D16" s="35"/>
-      <c r="E16" s="29"/>
+      <c r="E16" s="29">
+        <v>44552</v>
+      </c>
       <c r="F16" s="53" t="s">
         <v>618</v>
       </c>
@@ -4701,7 +4709,9 @@
         <v>1045</v>
       </c>
       <c r="D17" s="35"/>
-      <c r="E17" s="29"/>
+      <c r="E17" s="29">
+        <v>44552</v>
+      </c>
       <c r="F17" s="53" t="s">
         <v>618</v>
       </c>

</xml_diff>

<commit_message>
Update Pertanggal 24 Desember 2021 17:41:52
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="1054">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -3504,6 +3504,12 @@
   </si>
   <si>
     <t>Mendapatkan Data Picklist Departemen Organisasi</t>
+  </si>
+  <si>
+    <t>transaction.update.budgeting.setBudget</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Anggaran</t>
   </si>
 </sst>
 </file>
@@ -4365,13 +4371,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L620"/>
+  <dimension ref="A1:L621"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C556" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="B616" sqref="B616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -16486,14 +16492,14 @@
     <row r="559" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A559" s="35"/>
       <c r="B559" s="7" t="s">
-        <v>458</v>
+        <v>1052</v>
       </c>
       <c r="C559" s="4" t="s">
-        <v>460</v>
+        <v>1053</v>
       </c>
       <c r="D559" s="35"/>
       <c r="E559" s="29">
-        <v>44363</v>
+        <v>44554</v>
       </c>
       <c r="F559" s="53" t="s">
         <v>618</v>
@@ -16507,14 +16513,14 @@
     <row r="560" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A560" s="35"/>
       <c r="B560" s="7" t="s">
-        <v>691</v>
+        <v>458</v>
       </c>
       <c r="C560" s="4" t="s">
-        <v>693</v>
+        <v>460</v>
       </c>
       <c r="D560" s="35"/>
       <c r="E560" s="29">
-        <v>44365</v>
+        <v>44363</v>
       </c>
       <c r="F560" s="53" t="s">
         <v>618</v>
@@ -16528,10 +16534,10 @@
     <row r="561" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A561" s="35"/>
       <c r="B561" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C561" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D561" s="35"/>
       <c r="E561" s="29">
@@ -16549,14 +16555,14 @@
     <row r="562" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A562" s="35"/>
       <c r="B562" s="7" t="s">
-        <v>447</v>
+        <v>692</v>
       </c>
       <c r="C562" s="4" t="s">
-        <v>448</v>
+        <v>694</v>
       </c>
       <c r="D562" s="35"/>
       <c r="E562" s="29">
-        <v>44362</v>
+        <v>44365</v>
       </c>
       <c r="F562" s="53" t="s">
         <v>618</v>
@@ -16570,14 +16576,14 @@
     <row r="563" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A563" s="35"/>
       <c r="B563" s="7" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="C563" s="4" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="D563" s="35"/>
       <c r="E563" s="29">
-        <v>44363</v>
+        <v>44362</v>
       </c>
       <c r="F563" s="53" t="s">
         <v>618</v>
@@ -16588,51 +16594,51 @@
       <c r="J563" s="20"/>
       <c r="K563" s="35"/>
     </row>
-    <row r="564" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A564" s="35"/>
-      <c r="B564" s="11"/>
-      <c r="C564" s="12"/>
+      <c r="B564" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C564" s="4" t="s">
+        <v>461</v>
+      </c>
       <c r="D564" s="35"/>
-      <c r="E564" s="32"/>
-      <c r="F564" s="55"/>
+      <c r="E564" s="29">
+        <v>44363</v>
+      </c>
+      <c r="F564" s="53" t="s">
+        <v>618</v>
+      </c>
       <c r="G564" s="35"/>
-      <c r="H564" s="32"/>
-      <c r="I564" s="23"/>
-      <c r="J564" s="24"/>
+      <c r="H564" s="29"/>
+      <c r="I564" s="19"/>
+      <c r="J564" s="20"/>
       <c r="K564" s="35"/>
     </row>
-    <row r="565" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A565" s="35"/>
-      <c r="B565" s="7" t="s">
-        <v>405</v>
-      </c>
-      <c r="C565" s="4" t="s">
-        <v>406</v>
-      </c>
+      <c r="B565" s="11"/>
+      <c r="C565" s="12"/>
       <c r="D565" s="35"/>
-      <c r="E565" s="29">
-        <v>44250</v>
-      </c>
-      <c r="F565" s="53" t="s">
-        <v>618</v>
-      </c>
+      <c r="E565" s="32"/>
+      <c r="F565" s="55"/>
       <c r="G565" s="35"/>
-      <c r="H565" s="29"/>
-      <c r="I565" s="19"/>
-      <c r="J565" s="20"/>
+      <c r="H565" s="32"/>
+      <c r="I565" s="23"/>
+      <c r="J565" s="24"/>
       <c r="K565" s="35"/>
     </row>
     <row r="566" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A566" s="35"/>
       <c r="B566" s="7" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="C566" s="4" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D566" s="35"/>
       <c r="E566" s="29">
-        <v>44382</v>
+        <v>44250</v>
       </c>
       <c r="F566" s="53" t="s">
         <v>618</v>
@@ -16646,14 +16652,14 @@
     <row r="567" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A567" s="35"/>
       <c r="B567" s="7" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="C567" s="4" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="D567" s="35"/>
       <c r="E567" s="29">
-        <v>44250</v>
+        <v>44382</v>
       </c>
       <c r="F567" s="53" t="s">
         <v>618</v>
@@ -16664,47 +16670,47 @@
       <c r="J567" s="20"/>
       <c r="K567" s="35"/>
     </row>
-    <row r="568" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A568" s="35"/>
-      <c r="B568" s="11"/>
-      <c r="C568" s="12"/>
+      <c r="B568" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C568" s="4" t="s">
+        <v>408</v>
+      </c>
       <c r="D568" s="35"/>
-      <c r="E568" s="32"/>
-      <c r="F568" s="55"/>
+      <c r="E568" s="29">
+        <v>44250</v>
+      </c>
+      <c r="F568" s="53" t="s">
+        <v>618</v>
+      </c>
       <c r="G568" s="35"/>
-      <c r="H568" s="32"/>
-      <c r="I568" s="23"/>
-      <c r="J568" s="24"/>
+      <c r="H568" s="29"/>
+      <c r="I568" s="19"/>
+      <c r="J568" s="20"/>
       <c r="K568" s="35"/>
     </row>
-    <row r="569" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A569" s="35"/>
-      <c r="B569" s="7" t="s">
-        <v>1006</v>
-      </c>
-      <c r="C569" s="14" t="s">
-        <v>1008</v>
-      </c>
+      <c r="B569" s="11"/>
+      <c r="C569" s="12"/>
       <c r="D569" s="35"/>
-      <c r="E569" s="29">
-        <v>44525</v>
-      </c>
-      <c r="F569" s="53" t="s">
-        <v>618</v>
-      </c>
+      <c r="E569" s="32"/>
+      <c r="F569" s="55"/>
       <c r="G569" s="35"/>
-      <c r="H569" s="29"/>
-      <c r="I569" s="19"/>
-      <c r="J569" s="20"/>
+      <c r="H569" s="32"/>
+      <c r="I569" s="23"/>
+      <c r="J569" s="24"/>
       <c r="K569" s="35"/>
     </row>
     <row r="570" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A570" s="35"/>
       <c r="B570" s="7" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C570" s="14" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D570" s="35"/>
       <c r="E570" s="29">
@@ -16722,60 +16728,60 @@
     <row r="571" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A571" s="35"/>
       <c r="B571" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C571" s="4" t="s">
-        <v>85</v>
+        <v>1007</v>
+      </c>
+      <c r="C571" s="14" t="s">
+        <v>1009</v>
       </c>
       <c r="D571" s="35"/>
       <c r="E571" s="29">
-        <v>44148</v>
+        <v>44525</v>
       </c>
       <c r="F571" s="53" t="s">
         <v>618</v>
       </c>
       <c r="G571" s="35"/>
       <c r="H571" s="29"/>
-      <c r="I571" s="19">
-        <v>1</v>
-      </c>
-      <c r="J571" s="20">
-        <v>0</v>
-      </c>
+      <c r="I571" s="19"/>
+      <c r="J571" s="20"/>
       <c r="K571" s="35"/>
     </row>
     <row r="572" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A572" s="35"/>
-      <c r="B572" s="13" t="s">
-        <v>946</v>
-      </c>
-      <c r="C572" s="14" t="s">
-        <v>947</v>
+      <c r="B572" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C572" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="D572" s="35"/>
       <c r="E572" s="29">
-        <v>44420</v>
+        <v>44148</v>
       </c>
       <c r="F572" s="53" t="s">
         <v>618</v>
       </c>
       <c r="G572" s="35"/>
       <c r="H572" s="29"/>
-      <c r="I572" s="19"/>
-      <c r="J572" s="20"/>
+      <c r="I572" s="19">
+        <v>1</v>
+      </c>
+      <c r="J572" s="20">
+        <v>0</v>
+      </c>
       <c r="K572" s="35"/>
     </row>
     <row r="573" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A573" s="35"/>
-      <c r="B573" s="7" t="s">
-        <v>585</v>
-      </c>
-      <c r="C573" s="4" t="s">
-        <v>586</v>
+      <c r="B573" s="13" t="s">
+        <v>946</v>
+      </c>
+      <c r="C573" s="14" t="s">
+        <v>947</v>
       </c>
       <c r="D573" s="35"/>
       <c r="E573" s="29">
-        <v>44377</v>
+        <v>44420</v>
       </c>
       <c r="F573" s="53" t="s">
         <v>618</v>
@@ -16789,10 +16795,10 @@
     <row r="574" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A574" s="35"/>
       <c r="B574" s="7" t="s">
-        <v>291</v>
+        <v>585</v>
       </c>
       <c r="C574" s="4" t="s">
-        <v>293</v>
+        <v>586</v>
       </c>
       <c r="D574" s="35"/>
       <c r="E574" s="29">
@@ -16810,10 +16816,10 @@
     <row r="575" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A575" s="35"/>
       <c r="B575" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C575" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D575" s="35"/>
       <c r="E575" s="29">
@@ -16831,60 +16837,60 @@
     <row r="576" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A576" s="35"/>
       <c r="B576" s="7" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="C576" s="4" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D576" s="35"/>
       <c r="E576" s="29">
-        <v>44172</v>
+        <v>44377</v>
       </c>
       <c r="F576" s="53" t="s">
         <v>618</v>
       </c>
       <c r="G576" s="35"/>
       <c r="H576" s="29"/>
-      <c r="I576" s="19">
-        <v>1</v>
-      </c>
-      <c r="J576" s="20">
-        <v>0</v>
-      </c>
+      <c r="I576" s="19"/>
+      <c r="J576" s="20"/>
       <c r="K576" s="35"/>
     </row>
     <row r="577" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A577" s="35"/>
       <c r="B577" s="7" t="s">
-        <v>615</v>
+        <v>285</v>
       </c>
       <c r="C577" s="4" t="s">
-        <v>616</v>
+        <v>286</v>
       </c>
       <c r="D577" s="35"/>
       <c r="E577" s="29">
-        <v>44378</v>
+        <v>44172</v>
       </c>
       <c r="F577" s="53" t="s">
         <v>618</v>
       </c>
       <c r="G577" s="35"/>
       <c r="H577" s="29"/>
-      <c r="I577" s="19"/>
-      <c r="J577" s="20"/>
+      <c r="I577" s="19">
+        <v>1</v>
+      </c>
+      <c r="J577" s="20">
+        <v>0</v>
+      </c>
       <c r="K577" s="35"/>
     </row>
     <row r="578" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A578" s="35"/>
       <c r="B578" s="7" t="s">
-        <v>854</v>
+        <v>615</v>
       </c>
       <c r="C578" s="4" t="s">
-        <v>904</v>
+        <v>616</v>
       </c>
       <c r="D578" s="35"/>
       <c r="E578" s="29">
-        <v>44406</v>
+        <v>44378</v>
       </c>
       <c r="F578" s="53" t="s">
         <v>618</v>
@@ -16898,14 +16904,14 @@
     <row r="579" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A579" s="35"/>
       <c r="B579" s="7" t="s">
-        <v>888</v>
+        <v>854</v>
       </c>
       <c r="C579" s="4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D579" s="35"/>
       <c r="E579" s="29">
-        <v>44407</v>
+        <v>44406</v>
       </c>
       <c r="F579" s="53" t="s">
         <v>618</v>
@@ -16919,14 +16925,14 @@
     <row r="580" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A580" s="35"/>
       <c r="B580" s="7" t="s">
-        <v>924</v>
+        <v>888</v>
       </c>
       <c r="C580" s="4" t="s">
-        <v>925</v>
+        <v>905</v>
       </c>
       <c r="D580" s="35"/>
       <c r="E580" s="29">
-        <v>44411</v>
+        <v>44407</v>
       </c>
       <c r="F580" s="53" t="s">
         <v>618</v>
@@ -16940,10 +16946,10 @@
     <row r="581" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A581" s="35"/>
       <c r="B581" s="7" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C581" s="4" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D581" s="35"/>
       <c r="E581" s="29">
@@ -16961,14 +16967,14 @@
     <row r="582" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A582" s="35"/>
       <c r="B582" s="7" t="s">
-        <v>889</v>
+        <v>926</v>
       </c>
       <c r="C582" s="4" t="s">
-        <v>906</v>
+        <v>927</v>
       </c>
       <c r="D582" s="35"/>
       <c r="E582" s="29">
-        <v>44406</v>
+        <v>44411</v>
       </c>
       <c r="F582" s="53" t="s">
         <v>618</v>
@@ -16982,14 +16988,14 @@
     <row r="583" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A583" s="35"/>
       <c r="B583" s="7" t="s">
-        <v>920</v>
+        <v>889</v>
       </c>
       <c r="C583" s="4" t="s">
-        <v>922</v>
+        <v>906</v>
       </c>
       <c r="D583" s="35"/>
       <c r="E583" s="29">
-        <v>44411</v>
+        <v>44406</v>
       </c>
       <c r="F583" s="53" t="s">
         <v>618</v>
@@ -17003,10 +17009,10 @@
     <row r="584" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A584" s="35"/>
       <c r="B584" s="7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C584" s="4" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D584" s="35"/>
       <c r="E584" s="29">
@@ -17024,14 +17030,14 @@
     <row r="585" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A585" s="35"/>
       <c r="B585" s="7" t="s">
-        <v>569</v>
+        <v>921</v>
       </c>
       <c r="C585" s="4" t="s">
-        <v>575</v>
+        <v>923</v>
       </c>
       <c r="D585" s="35"/>
       <c r="E585" s="29">
-        <v>44376</v>
+        <v>44411</v>
       </c>
       <c r="F585" s="53" t="s">
         <v>618</v>
@@ -17045,10 +17051,10 @@
     <row r="586" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A586" s="35"/>
       <c r="B586" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C586" s="4" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D586" s="35"/>
       <c r="E586" s="29">
@@ -17066,10 +17072,10 @@
     <row r="587" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A587" s="35"/>
       <c r="B587" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C587" s="4" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D587" s="35"/>
       <c r="E587" s="29">
@@ -17087,10 +17093,10 @@
     <row r="588" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A588" s="35"/>
       <c r="B588" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C588" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D588" s="35"/>
       <c r="E588" s="29">
@@ -17108,10 +17114,10 @@
     <row r="589" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A589" s="35"/>
       <c r="B589" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C589" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D589" s="35"/>
       <c r="E589" s="29">
@@ -17129,10 +17135,10 @@
     <row r="590" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A590" s="35"/>
       <c r="B590" s="7" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="C590" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D590" s="35"/>
       <c r="E590" s="29">
@@ -17147,42 +17153,38 @@
       <c r="J590" s="20"/>
       <c r="K590" s="35"/>
     </row>
-    <row r="591" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A591" s="37"/>
-      <c r="B591" s="13" t="s">
-        <v>852</v>
-      </c>
-      <c r="C591" s="14" t="s">
-        <v>853</v>
-      </c>
-      <c r="D591" s="37"/>
-      <c r="E591" s="31">
-        <v>44406</v>
+    <row r="591" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A591" s="35"/>
+      <c r="B591" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="C591" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="D591" s="35"/>
+      <c r="E591" s="29">
+        <v>44376</v>
       </c>
       <c r="F591" s="53" t="s">
         <v>618</v>
       </c>
-      <c r="G591" s="37"/>
-      <c r="H591" s="31"/>
-      <c r="I591" s="19">
-        <v>1</v>
-      </c>
-      <c r="J591" s="20">
-        <v>0</v>
-      </c>
-      <c r="K591" s="37"/>
+      <c r="G591" s="35"/>
+      <c r="H591" s="29"/>
+      <c r="I591" s="19"/>
+      <c r="J591" s="20"/>
+      <c r="K591" s="35"/>
     </row>
     <row r="592" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A592" s="37"/>
       <c r="B592" s="13" t="s">
-        <v>335</v>
+        <v>852</v>
       </c>
       <c r="C592" s="14" t="s">
-        <v>339</v>
+        <v>853</v>
       </c>
       <c r="D592" s="37"/>
       <c r="E592" s="31">
-        <v>44176</v>
+        <v>44406</v>
       </c>
       <c r="F592" s="53" t="s">
         <v>618</v>
@@ -17200,10 +17202,10 @@
     <row r="593" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A593" s="37"/>
       <c r="B593" s="13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C593" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D593" s="37"/>
       <c r="E593" s="31">
@@ -17225,10 +17227,10 @@
     <row r="594" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A594" s="37"/>
       <c r="B594" s="13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C594" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D594" s="37"/>
       <c r="E594" s="31">
@@ -17250,10 +17252,10 @@
     <row r="595" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A595" s="37"/>
       <c r="B595" s="13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C595" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D595" s="37"/>
       <c r="E595" s="31">
@@ -17274,32 +17276,36 @@
     </row>
     <row r="596" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A596" s="37"/>
-      <c r="B596" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="C596" s="4" t="s">
-        <v>400</v>
+      <c r="B596" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C596" s="14" t="s">
+        <v>342</v>
       </c>
       <c r="D596" s="37"/>
       <c r="E596" s="31">
-        <v>44245</v>
+        <v>44176</v>
       </c>
       <c r="F596" s="53" t="s">
         <v>618</v>
       </c>
       <c r="G596" s="37"/>
       <c r="H596" s="31"/>
-      <c r="I596" s="19"/>
-      <c r="J596" s="20"/>
+      <c r="I596" s="19">
+        <v>1</v>
+      </c>
+      <c r="J596" s="20">
+        <v>0</v>
+      </c>
       <c r="K596" s="37"/>
     </row>
     <row r="597" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="37"/>
       <c r="B597" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C597" s="4" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D597" s="37"/>
       <c r="E597" s="31">
@@ -17317,10 +17323,10 @@
     <row r="598" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="37"/>
       <c r="B598" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C598" s="4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D598" s="37"/>
       <c r="E598" s="31">
@@ -17335,38 +17341,34 @@
       <c r="J598" s="20"/>
       <c r="K598" s="37"/>
     </row>
-    <row r="599" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A599" s="35"/>
+    <row r="599" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A599" s="37"/>
       <c r="B599" s="7" t="s">
-        <v>319</v>
+        <v>402</v>
       </c>
       <c r="C599" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="D599" s="35"/>
-      <c r="E599" s="29">
-        <v>44175</v>
+        <v>403</v>
+      </c>
+      <c r="D599" s="37"/>
+      <c r="E599" s="31">
+        <v>44245</v>
       </c>
       <c r="F599" s="53" t="s">
         <v>618</v>
       </c>
-      <c r="G599" s="35"/>
-      <c r="H599" s="29"/>
-      <c r="I599" s="19">
-        <v>1</v>
-      </c>
-      <c r="J599" s="20">
-        <v>0</v>
-      </c>
-      <c r="K599" s="35"/>
+      <c r="G599" s="37"/>
+      <c r="H599" s="31"/>
+      <c r="I599" s="19"/>
+      <c r="J599" s="20"/>
+      <c r="K599" s="37"/>
     </row>
     <row r="600" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A600" s="35"/>
       <c r="B600" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C600" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D600" s="35"/>
       <c r="E600" s="29">
@@ -17388,10 +17390,10 @@
     <row r="601" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A601" s="35"/>
       <c r="B601" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D601" s="35"/>
       <c r="E601" s="29">
@@ -17413,10 +17415,10 @@
     <row r="602" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A602" s="35"/>
       <c r="B602" s="7" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="C602" s="4" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="D602" s="35"/>
       <c r="E602" s="29">
@@ -17438,10 +17440,10 @@
     <row r="603" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A603" s="35"/>
       <c r="B603" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C603" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D603" s="35"/>
       <c r="E603" s="29">
@@ -17463,10 +17465,10 @@
     <row r="604" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A604" s="35"/>
       <c r="B604" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C604" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D604" s="35"/>
       <c r="E604" s="29">
@@ -17488,14 +17490,14 @@
     <row r="605" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A605" s="35"/>
       <c r="B605" s="7" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="C605" s="4" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="D605" s="35"/>
       <c r="E605" s="29">
-        <v>44173</v>
+        <v>44175</v>
       </c>
       <c r="F605" s="53" t="s">
         <v>618</v>
@@ -17513,10 +17515,10 @@
     <row r="606" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A606" s="35"/>
       <c r="B606" s="7" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C606" s="4" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D606" s="35"/>
       <c r="E606" s="29">
@@ -17538,10 +17540,10 @@
     <row r="607" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A607" s="35"/>
       <c r="B607" s="7" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C607" s="4" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="D607" s="35"/>
       <c r="E607" s="29">
@@ -17560,47 +17562,51 @@
       </c>
       <c r="K607" s="35"/>
     </row>
-    <row r="608" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A608" s="35"/>
-      <c r="B608" s="11"/>
-      <c r="C608" s="12"/>
+      <c r="B608" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C608" s="4" t="s">
+        <v>296</v>
+      </c>
       <c r="D608" s="35"/>
-      <c r="E608" s="32"/>
-      <c r="F608" s="55"/>
+      <c r="E608" s="29">
+        <v>44173</v>
+      </c>
+      <c r="F608" s="53" t="s">
+        <v>618</v>
+      </c>
       <c r="G608" s="35"/>
-      <c r="H608" s="32"/>
-      <c r="I608" s="23"/>
-      <c r="J608" s="24"/>
+      <c r="H608" s="29"/>
+      <c r="I608" s="19">
+        <v>1</v>
+      </c>
+      <c r="J608" s="20">
+        <v>0</v>
+      </c>
       <c r="K608" s="35"/>
     </row>
-    <row r="609" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A609" s="35"/>
-      <c r="B609" s="7" t="s">
-        <v>703</v>
-      </c>
-      <c r="C609" s="4" t="s">
-        <v>707</v>
-      </c>
+      <c r="B609" s="11"/>
+      <c r="C609" s="12"/>
       <c r="D609" s="35"/>
-      <c r="E609" s="29">
-        <v>44382</v>
-      </c>
-      <c r="F609" s="53" t="s">
-        <v>618</v>
-      </c>
+      <c r="E609" s="32"/>
+      <c r="F609" s="55"/>
       <c r="G609" s="35"/>
-      <c r="H609" s="29"/>
-      <c r="I609" s="19"/>
-      <c r="J609" s="20"/>
+      <c r="H609" s="32"/>
+      <c r="I609" s="23"/>
+      <c r="J609" s="24"/>
       <c r="K609" s="35"/>
     </row>
     <row r="610" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A610" s="35"/>
       <c r="B610" s="7" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C610" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D610" s="35"/>
       <c r="E610" s="29">
@@ -17618,10 +17624,10 @@
     <row r="611" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A611" s="35"/>
       <c r="B611" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C611" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D611" s="35"/>
       <c r="E611" s="29">
@@ -17639,10 +17645,10 @@
     <row r="612" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A612" s="35"/>
       <c r="B612" s="7" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C612" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D612" s="35"/>
       <c r="E612" s="29">
@@ -17657,47 +17663,47 @@
       <c r="J612" s="20"/>
       <c r="K612" s="35"/>
     </row>
-    <row r="613" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A613" s="35"/>
-      <c r="B613" s="11"/>
-      <c r="C613" s="12"/>
+      <c r="B613" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="C613" s="4" t="s">
+        <v>710</v>
+      </c>
       <c r="D613" s="35"/>
-      <c r="E613" s="32"/>
-      <c r="F613" s="55"/>
+      <c r="E613" s="29">
+        <v>44382</v>
+      </c>
+      <c r="F613" s="53" t="s">
+        <v>618</v>
+      </c>
       <c r="G613" s="35"/>
-      <c r="H613" s="32"/>
-      <c r="I613" s="23"/>
-      <c r="J613" s="24"/>
+      <c r="H613" s="29"/>
+      <c r="I613" s="19"/>
+      <c r="J613" s="20"/>
       <c r="K613" s="35"/>
     </row>
-    <row r="614" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A614" s="35"/>
-      <c r="B614" s="7" t="s">
-        <v>743</v>
-      </c>
-      <c r="C614" s="4" t="s">
-        <v>740</v>
-      </c>
+      <c r="B614" s="11"/>
+      <c r="C614" s="12"/>
       <c r="D614" s="35"/>
-      <c r="E614" s="29">
-        <v>44384</v>
-      </c>
-      <c r="F614" s="53" t="s">
-        <v>618</v>
-      </c>
+      <c r="E614" s="32"/>
+      <c r="F614" s="55"/>
       <c r="G614" s="35"/>
-      <c r="H614" s="29"/>
-      <c r="I614" s="19"/>
-      <c r="J614" s="20"/>
+      <c r="H614" s="32"/>
+      <c r="I614" s="23"/>
+      <c r="J614" s="24"/>
       <c r="K614" s="35"/>
     </row>
     <row r="615" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A615" s="35"/>
       <c r="B615" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C615" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D615" s="35"/>
       <c r="E615" s="29">
@@ -17715,10 +17721,10 @@
     <row r="616" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A616" s="35"/>
       <c r="B616" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C616" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D616" s="35"/>
       <c r="E616" s="29">
@@ -17733,48 +17739,69 @@
       <c r="J616" s="20"/>
       <c r="K616" s="35"/>
     </row>
-    <row r="617" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="617" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A617" s="35"/>
-      <c r="B617" s="8"/>
-      <c r="C617" s="6"/>
+      <c r="B617" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="C617" s="4" t="s">
+        <v>742</v>
+      </c>
       <c r="D617" s="35"/>
-      <c r="E617" s="33"/>
-      <c r="F617" s="56"/>
+      <c r="E617" s="29">
+        <v>44384</v>
+      </c>
+      <c r="F617" s="53" t="s">
+        <v>618</v>
+      </c>
       <c r="G617" s="35"/>
-      <c r="H617" s="33"/>
-      <c r="I617" s="25"/>
-      <c r="J617" s="26"/>
+      <c r="H617" s="29"/>
+      <c r="I617" s="19"/>
+      <c r="J617" s="20"/>
       <c r="K617" s="35"/>
     </row>
-    <row r="618" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A618" s="35"/>
-      <c r="B618" s="38"/>
-      <c r="C618" s="39"/>
+      <c r="B618" s="8"/>
+      <c r="C618" s="6"/>
       <c r="D618" s="35"/>
-      <c r="E618" s="40"/>
-      <c r="F618" s="50"/>
+      <c r="E618" s="33"/>
+      <c r="F618" s="56"/>
       <c r="G618" s="35"/>
-      <c r="H618" s="40"/>
-      <c r="I618" s="41"/>
-      <c r="J618" s="41"/>
+      <c r="H618" s="33"/>
+      <c r="I618" s="25"/>
+      <c r="J618" s="26"/>
       <c r="K618" s="35"/>
     </row>
-    <row r="620" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A620" s="35"/>
-      <c r="B620" s="7" t="s">
+    <row r="619" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A619" s="35"/>
+      <c r="B619" s="38"/>
+      <c r="C619" s="39"/>
+      <c r="D619" s="35"/>
+      <c r="E619" s="40"/>
+      <c r="F619" s="50"/>
+      <c r="G619" s="35"/>
+      <c r="H619" s="40"/>
+      <c r="I619" s="41"/>
+      <c r="J619" s="41"/>
+      <c r="K619" s="35"/>
+    </row>
+    <row r="621" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A621" s="35"/>
+      <c r="B621" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="C620" s="4" t="s">
+      <c r="C621" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="D620" s="35"/>
-      <c r="E620" s="29"/>
-      <c r="F620" s="53"/>
-      <c r="G620" s="35"/>
-      <c r="H620" s="29"/>
-      <c r="I620" s="19"/>
-      <c r="J620" s="20"/>
-      <c r="K620" s="35"/>
+      <c r="D621" s="35"/>
+      <c r="E621" s="29"/>
+      <c r="F621" s="53"/>
+      <c r="G621" s="35"/>
+      <c r="H621" s="29"/>
+      <c r="I621" s="19"/>
+      <c r="J621" s="20"/>
+      <c r="K621" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -17786,7 +17813,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F4:F6 F9 F34:F36 F47:F48 F50 F52:F54 F91:F97 F100:F105 F166:F170 F172:F176 F186:F188 F200 F270:F272 F274:F278 F331 F357:F359 F361:F363 F377:F378 F439:F447 F450:F452 F454 F456:F460 F462:F465 F467:F468 F478:F483 F485:F487 F496:F497 F197:F198 F499 F501:F503 F548:F550 F552:F556 F472:F476 F559:F563 F565:F567 F156:F159 F609:F612 F434:F437 F366:F368 F161:F163 F614:F616 F88 F67:F86 F65 F41:F44 F317 F39 F107:F114 F309:F310 F281:F283 F190:F195 F489:F494 F380:F385 F61 F29:F31 F57:F58 F387:F388 F328:F329 F21:F22 F202:F221 F370:F375 F319:F326 F285:F307 F116:F154 F569:F607 F334:F355 F223:F268 F505:F546 F390:F432 F24:F27 F178:F184 F14:F19 F12:F13" numberStoredAsText="1"/>
+    <ignoredError sqref="F4:F6 F9 F34:F36 F47:F48 F50 F52:F54 F91:F97 F100:F105 F166:F170 F172:F176 F186:F188 F200 F270:F272 F274:F278 F331 F357:F359 F361:F363 F377:F378 F439:F447 F450:F452 F454 F456:F460 F462:F465 F467:F468 F478:F483 F485:F487 F496:F497 F197:F198 F499 F501:F503 F548:F550 F552:F556 F472:F476 F560:F564 F566:F568 F156:F159 F610:F613 F434:F437 F366:F368 F161:F163 F615:F617 F88 F67:F86 F65 F41:F44 F317 F39 F107:F114 F309:F310 F281:F283 F190:F195 F489:F494 F380:F385 F61 F29:F31 F57:F58 F387:F388 F328:F329 F21:F22 F202:F221 F370:F375 F319:F326 F285:F307 F116:F154 F570:F608 F334:F355 F223:F268 F505:F546 F390:F432 F24:F27 F178:F184 F12:F19 F559" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Pertanggal 16 Maret 2022 22:26
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="5820"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="5820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
+    <sheet name="Classification" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="1333">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -4387,6 +4388,135 @@
   <si>
     <t>Mendapatkan Data Picklist Jenis Pajak</t>
   </si>
+  <si>
+    <t>authentication</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>dataPickList</t>
+  </si>
+  <si>
+    <t>environmant</t>
+  </si>
+  <si>
+    <t>fileHandling</t>
+  </si>
+  <si>
+    <t>instruction</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>scheduler</t>
+  </si>
+  <si>
+    <t>transacation</t>
+  </si>
+  <si>
+    <t>userAction</t>
+  </si>
+  <si>
+    <t>►</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>approval</t>
+  </si>
+  <si>
+    <t>cancelation</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>Menangani Aksi dari Pengguna</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>Menangani perintah instruksi</t>
+  </si>
+  <si>
+    <t>►Instruksi pada alat</t>
+  </si>
+  <si>
+    <t>►Instruksi pada server</t>
+  </si>
+  <si>
+    <t>►Pengesahan dokumen</t>
+  </si>
+  <si>
+    <t>►Pembatalan dokumen</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>&lt;Modul Name&gt; ►set...</t>
+  </si>
+  <si>
+    <t>undelete</t>
+  </si>
+  <si>
+    <t>Menangani Transaksi Record pada Tabel</t>
+  </si>
+  <si>
+    <t>hide</t>
+  </si>
+  <si>
+    <t>initialize</t>
+  </si>
+  <si>
+    <t>►Inisialisasi kumpulan data</t>
+  </si>
+  <si>
+    <t>synchronize</t>
+  </si>
+  <si>
+    <t>►Sinkronisasi kumpulan data</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>dataList</t>
+  </si>
+  <si>
+    <t>dataRecord</t>
+  </si>
+  <si>
+    <t>►Pembacaan data tertentu</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>►Menampilkan data tertentu</t>
+  </si>
+  <si>
+    <t>►Pembatalan penghapusan data tertentu</t>
+  </si>
+  <si>
+    <t>►Pembacaan daftar kumpulan data</t>
+  </si>
+  <si>
+    <t>►Penyembunyian data tertentu</t>
+  </si>
+  <si>
+    <t>►Pembuatan data baru tertentu</t>
+  </si>
+  <si>
+    <t>►Penghapusan data tertentu</t>
+  </si>
 </sst>
 </file>
 
@@ -4395,7 +4525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4481,6 +4611,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4734,7 +4870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4942,6 +5078,19 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5249,11 +5398,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L762"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -21703,4 +21852,401 @@
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="70"/>
+    <col min="2" max="6" width="4.28515625" style="72" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="72" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="70" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" style="70" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="70"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="74" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="74" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="74" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="74" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="74" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="74" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="73" t="s">
+        <v>1308</v>
+      </c>
+      <c r="I7" s="73"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="I8" s="70" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="I9" s="70" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="74" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="74" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="74" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="73" t="s">
+        <v>1316</v>
+      </c>
+      <c r="I12" s="73"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="I13" s="70" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C14" s="71" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="I14" s="70" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C15" s="71" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="I15" s="70" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="I16" s="70" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="I18" s="70" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>1324</v>
+      </c>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="I19" s="70" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="I20" s="70" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C21" s="71" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="I21" s="70" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="I22" s="70" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="74" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="73" t="s">
+        <v>1305</v>
+      </c>
+      <c r="I23" s="73"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="I25" s="70" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D26" s="71" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="I26" s="70" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D27" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E27" s="71" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pertanggal 21 Maret 2022 11:00
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4107,9 +4107,6 @@
     <t>Menyembunyikan Data Gudang</t>
   </si>
   <si>
-    <t>transaction.show.supplyChain.setWarehouse</t>
-  </si>
-  <si>
     <t>transaction.read.dataRecord.supplyChain.getWarehouseInboundOrder</t>
   </si>
   <si>
@@ -4522,6 +4519,9 @@
   </si>
   <si>
     <t>Memunculkan Data Gudang</t>
+  </si>
+  <si>
+    <t>transaction.unhide.supplyChain.setWarehouse</t>
   </si>
 </sst>
 </file>
@@ -5058,6 +5058,10 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5085,12 +5089,8 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5405,10 +5405,10 @@
   <dimension ref="A1:L762"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C545" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C680" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C558" sqref="C558"/>
+      <selection pane="bottomRight" activeCell="F684" sqref="F684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5442,29 +5442,29 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="65" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="35"/>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="70" t="s">
         <v>596</v>
       </c>
-      <c r="F2" s="69"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="35"/>
-      <c r="H2" s="65" t="s">
+      <c r="H2" s="67" t="s">
         <v>334</v>
       </c>
-      <c r="I2" s="66"/>
-      <c r="J2" s="67"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="69"/>
       <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:11" s="34" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="64"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="36"/>
       <c r="E3" s="42" t="s">
         <v>335</v>
@@ -5815,10 +5815,10 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="35"/>
       <c r="B20" s="7" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>1221</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>1222</v>
       </c>
       <c r="D20" s="35"/>
       <c r="E20" s="29">
@@ -6153,10 +6153,10 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
       <c r="B38" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>1227</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>1228</v>
       </c>
       <c r="D38" s="35"/>
       <c r="E38" s="29">
@@ -6237,10 +6237,10 @@
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="35"/>
       <c r="B42" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>1229</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>1230</v>
       </c>
       <c r="D42" s="35"/>
       <c r="E42" s="29">
@@ -6258,10 +6258,10 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>1231</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>1232</v>
       </c>
       <c r="D43" s="35"/>
       <c r="E43" s="29">
@@ -6313,10 +6313,10 @@
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="35"/>
       <c r="B46" s="7" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>1287</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>1288</v>
       </c>
       <c r="D46" s="35"/>
       <c r="E46" s="29">
@@ -6795,10 +6795,10 @@
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
       <c r="B72" s="7" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>1253</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>1254</v>
       </c>
       <c r="D72" s="35"/>
       <c r="E72" s="29">
@@ -9370,10 +9370,10 @@
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="35"/>
       <c r="B199" s="7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C199" s="4" t="s">
         <v>1237</v>
-      </c>
-      <c r="C199" s="4" t="s">
-        <v>1238</v>
       </c>
       <c r="D199" s="35"/>
       <c r="E199" s="29">
@@ -9391,10 +9391,10 @@
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="35"/>
       <c r="B200" s="7" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C200" s="4" t="s">
         <v>1239</v>
-      </c>
-      <c r="C200" s="4" t="s">
-        <v>1240</v>
       </c>
       <c r="D200" s="35"/>
       <c r="E200" s="29">
@@ -9635,10 +9635,10 @@
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="35"/>
       <c r="B212" s="7" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C212" s="4" t="s">
         <v>1257</v>
-      </c>
-      <c r="C212" s="4" t="s">
-        <v>1258</v>
       </c>
       <c r="D212" s="35"/>
       <c r="E212" s="29">
@@ -9656,10 +9656,10 @@
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="35"/>
       <c r="B213" s="7" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C213" s="4" t="s">
         <v>1255</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>1256</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="29">
@@ -9677,10 +9677,10 @@
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="35"/>
       <c r="B214" s="7" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C214" s="4" t="s">
         <v>1265</v>
-      </c>
-      <c r="C214" s="4" t="s">
-        <v>1266</v>
       </c>
       <c r="D214" s="35"/>
       <c r="E214" s="29">
@@ -12288,10 +12288,10 @@
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="35"/>
       <c r="B327" s="7" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C327" s="4" t="s">
         <v>1241</v>
-      </c>
-      <c r="C327" s="4" t="s">
-        <v>1242</v>
       </c>
       <c r="D327" s="35"/>
       <c r="E327" s="29">
@@ -12313,10 +12313,10 @@
     <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="35"/>
       <c r="B328" s="7" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C328" s="4" t="s">
         <v>1243</v>
-      </c>
-      <c r="C328" s="4" t="s">
-        <v>1244</v>
       </c>
       <c r="D328" s="35"/>
       <c r="E328" s="29">
@@ -12488,10 +12488,10 @@
     <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="35"/>
       <c r="B335" s="7" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C335" s="4" t="s">
         <v>1213</v>
-      </c>
-      <c r="C335" s="4" t="s">
-        <v>1214</v>
       </c>
       <c r="D335" s="35"/>
       <c r="E335" s="29">
@@ -12513,10 +12513,10 @@
     <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="35"/>
       <c r="B336" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C336" s="4" t="s">
         <v>1217</v>
-      </c>
-      <c r="C336" s="4" t="s">
-        <v>1218</v>
       </c>
       <c r="D336" s="35"/>
       <c r="E336" s="29">
@@ -12538,10 +12538,10 @@
     <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="35"/>
       <c r="B337" s="7" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C337" s="4" t="s">
         <v>1215</v>
-      </c>
-      <c r="C337" s="4" t="s">
-        <v>1216</v>
       </c>
       <c r="D337" s="35"/>
       <c r="E337" s="29">
@@ -12563,10 +12563,10 @@
     <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="35"/>
       <c r="B338" s="7" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C338" s="4" t="s">
         <v>1219</v>
-      </c>
-      <c r="C338" s="4" t="s">
-        <v>1220</v>
       </c>
       <c r="D338" s="35"/>
       <c r="E338" s="29">
@@ -12626,10 +12626,10 @@
     <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="35"/>
       <c r="B341" s="7" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C341" s="4" t="s">
         <v>1267</v>
-      </c>
-      <c r="C341" s="4" t="s">
-        <v>1268</v>
       </c>
       <c r="D341" s="35"/>
       <c r="E341" s="29">
@@ -12651,10 +12651,10 @@
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="35"/>
       <c r="B342" s="7" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="D342" s="35"/>
       <c r="E342" s="29">
@@ -12676,10 +12676,10 @@
     <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="35"/>
       <c r="B343" s="7" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C343" s="4" t="s">
         <v>1270</v>
-      </c>
-      <c r="C343" s="4" t="s">
-        <v>1271</v>
       </c>
       <c r="D343" s="35"/>
       <c r="E343" s="29">
@@ -13926,10 +13926,10 @@
     <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="35"/>
       <c r="B401" s="7" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C401" s="4" t="s">
         <v>1223</v>
-      </c>
-      <c r="C401" s="4" t="s">
-        <v>1224</v>
       </c>
       <c r="D401" s="35"/>
       <c r="E401" s="29">
@@ -14915,10 +14915,10 @@
     <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" s="35"/>
       <c r="B446" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C446" s="4" t="s">
         <v>1225</v>
-      </c>
-      <c r="C446" s="4" t="s">
-        <v>1226</v>
       </c>
       <c r="D446" s="35"/>
       <c r="E446" s="29">
@@ -14999,10 +14999,10 @@
     <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="35"/>
       <c r="B450" s="7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C450" s="4" t="s">
         <v>1233</v>
-      </c>
-      <c r="C450" s="4" t="s">
-        <v>1234</v>
       </c>
       <c r="D450" s="35"/>
       <c r="E450" s="29">
@@ -15020,10 +15020,10 @@
     <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" s="35"/>
       <c r="B451" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C451" s="4" t="s">
         <v>1235</v>
-      </c>
-      <c r="C451" s="4" t="s">
-        <v>1236</v>
       </c>
       <c r="D451" s="35"/>
       <c r="E451" s="29">
@@ -15075,10 +15075,10 @@
     <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" s="35"/>
       <c r="B454" s="7" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C454" s="4" t="s">
         <v>1285</v>
-      </c>
-      <c r="C454" s="4" t="s">
-        <v>1286</v>
       </c>
       <c r="D454" s="35"/>
       <c r="E454" s="29">
@@ -16899,10 +16899,10 @@
     <row r="538" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A538" s="35"/>
       <c r="B538" s="13" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C538" s="4" t="s">
         <v>1249</v>
-      </c>
-      <c r="C538" s="4" t="s">
-        <v>1250</v>
       </c>
       <c r="D538" s="35"/>
       <c r="E538" s="29">
@@ -16927,10 +16927,10 @@
     <row r="539" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A539" s="35"/>
       <c r="B539" s="13" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C539" s="4" t="s">
         <v>1251</v>
-      </c>
-      <c r="C539" s="4" t="s">
-        <v>1252</v>
       </c>
       <c r="D539" s="35"/>
       <c r="E539" s="29">
@@ -17123,10 +17123,10 @@
     <row r="546" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A546" s="35"/>
       <c r="B546" s="13" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C546" s="14" t="s">
         <v>1197</v>
-      </c>
-      <c r="C546" s="14" t="s">
-        <v>1198</v>
       </c>
       <c r="D546" s="35"/>
       <c r="E546" s="29">
@@ -17151,10 +17151,10 @@
     <row r="547" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A547" s="35"/>
       <c r="B547" s="13" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C547" s="14" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D547" s="35"/>
       <c r="E547" s="29">
@@ -17179,10 +17179,10 @@
     <row r="548" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A548" s="35"/>
       <c r="B548" s="13" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C548" s="14" t="s">
         <v>1199</v>
-      </c>
-      <c r="C548" s="14" t="s">
-        <v>1200</v>
       </c>
       <c r="D548" s="35"/>
       <c r="E548" s="29">
@@ -17207,10 +17207,10 @@
     <row r="549" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A549" s="35"/>
       <c r="B549" s="13" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C549" s="14" t="s">
         <v>1202</v>
-      </c>
-      <c r="C549" s="14" t="s">
-        <v>1203</v>
       </c>
       <c r="D549" s="35"/>
       <c r="E549" s="29">
@@ -17276,10 +17276,10 @@
     <row r="552" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A552" s="35"/>
       <c r="B552" s="13" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C552" s="4" t="s">
         <v>1279</v>
-      </c>
-      <c r="C552" s="4" t="s">
-        <v>1280</v>
       </c>
       <c r="D552" s="35"/>
       <c r="E552" s="29">
@@ -17304,10 +17304,10 @@
     <row r="553" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A553" s="35"/>
       <c r="B553" s="13" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C553" s="4" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="D553" s="35"/>
       <c r="E553" s="29">
@@ -17332,10 +17332,10 @@
     <row r="554" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A554" s="35"/>
       <c r="B554" s="13" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C554" s="4" t="s">
         <v>1282</v>
-      </c>
-      <c r="C554" s="4" t="s">
-        <v>1283</v>
       </c>
       <c r="D554" s="35"/>
       <c r="E554" s="29">
@@ -17386,65 +17386,69 @@
     <row r="557" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A557" s="35"/>
       <c r="B557" s="7" t="s">
-        <v>1196</v>
+        <v>1032</v>
       </c>
       <c r="C557" s="4" t="s">
-        <v>1334</v>
+        <v>1033</v>
       </c>
       <c r="D557" s="35"/>
       <c r="E557" s="29">
-        <v>44628</v>
+        <v>44572</v>
       </c>
       <c r="F557" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G557" s="35"/>
       <c r="H557" s="29"/>
-      <c r="I557" s="19">
-        <v>1</v>
-      </c>
-      <c r="J557" s="20">
-        <v>0</v>
-      </c>
+      <c r="I557" s="19"/>
+      <c r="J557" s="20"/>
       <c r="K557" s="35"/>
     </row>
-    <row r="558" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A558" s="35"/>
-      <c r="B558" s="7"/>
-      <c r="C558" s="4"/>
+      <c r="B558" s="11"/>
+      <c r="C558" s="12"/>
       <c r="D558" s="35"/>
-      <c r="E558" s="29"/>
-      <c r="F558" s="53"/>
+      <c r="E558" s="32"/>
+      <c r="F558" s="55"/>
       <c r="G558" s="35"/>
-      <c r="H558" s="29"/>
-      <c r="I558" s="19"/>
-      <c r="J558" s="20"/>
+      <c r="H558" s="32"/>
+      <c r="I558" s="23"/>
+      <c r="J558" s="24"/>
       <c r="K558" s="35"/>
     </row>
-    <row r="559" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A559" s="35"/>
-      <c r="B559" s="9"/>
-      <c r="C559" s="10"/>
+      <c r="B559" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C559" s="4" t="s">
+        <v>401</v>
+      </c>
       <c r="D559" s="35"/>
-      <c r="E559" s="30"/>
-      <c r="F559" s="54"/>
+      <c r="E559" s="29">
+        <v>44257</v>
+      </c>
+      <c r="F559" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G559" s="35"/>
-      <c r="H559" s="30"/>
-      <c r="I559" s="21"/>
-      <c r="J559" s="22"/>
+      <c r="H559" s="29"/>
+      <c r="I559" s="19"/>
+      <c r="J559" s="20"/>
       <c r="K559" s="35"/>
     </row>
     <row r="560" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A560" s="35"/>
       <c r="B560" s="7" t="s">
-        <v>1032</v>
+        <v>396</v>
       </c>
       <c r="C560" s="4" t="s">
-        <v>1033</v>
+        <v>397</v>
       </c>
       <c r="D560" s="35"/>
       <c r="E560" s="29">
-        <v>44572</v>
+        <v>44257</v>
       </c>
       <c r="F560" s="53" t="s">
         <v>597</v>
@@ -17455,106 +17459,114 @@
       <c r="J560" s="20"/>
       <c r="K560" s="35"/>
     </row>
-    <row r="561" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A561" s="35"/>
-      <c r="B561" s="11"/>
-      <c r="C561" s="12"/>
+      <c r="B561" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C561" s="4" t="s">
+        <v>399</v>
+      </c>
       <c r="D561" s="35"/>
-      <c r="E561" s="32"/>
-      <c r="F561" s="55"/>
+      <c r="E561" s="29">
+        <v>44257</v>
+      </c>
+      <c r="F561" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G561" s="35"/>
-      <c r="H561" s="32"/>
-      <c r="I561" s="23"/>
-      <c r="J561" s="24"/>
+      <c r="H561" s="29"/>
+      <c r="I561" s="19"/>
+      <c r="J561" s="20"/>
       <c r="K561" s="35"/>
     </row>
-    <row r="562" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A562" s="35"/>
-      <c r="B562" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="C562" s="4" t="s">
-        <v>401</v>
-      </c>
+      <c r="B562" s="11"/>
+      <c r="C562" s="12"/>
       <c r="D562" s="35"/>
-      <c r="E562" s="29">
-        <v>44257</v>
-      </c>
-      <c r="F562" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E562" s="32"/>
+      <c r="F562" s="55"/>
       <c r="G562" s="35"/>
-      <c r="H562" s="29"/>
-      <c r="I562" s="19"/>
-      <c r="J562" s="20"/>
+      <c r="H562" s="32"/>
+      <c r="I562" s="23"/>
+      <c r="J562" s="24"/>
       <c r="K562" s="35"/>
     </row>
     <row r="563" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A563" s="35"/>
       <c r="B563" s="7" t="s">
-        <v>396</v>
+        <v>614</v>
       </c>
       <c r="C563" s="4" t="s">
-        <v>397</v>
+        <v>615</v>
       </c>
       <c r="D563" s="35"/>
       <c r="E563" s="29">
-        <v>44257</v>
+        <v>44319</v>
       </c>
       <c r="F563" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G563" s="35"/>
       <c r="H563" s="29"/>
-      <c r="I563" s="19"/>
-      <c r="J563" s="20"/>
+      <c r="I563" s="19">
+        <v>1</v>
+      </c>
+      <c r="J563" s="20">
+        <v>0</v>
+      </c>
       <c r="K563" s="35"/>
     </row>
-    <row r="564" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A564" s="35"/>
-      <c r="B564" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="C564" s="4" t="s">
-        <v>399</v>
-      </c>
+      <c r="B564" s="11"/>
+      <c r="C564" s="12"/>
       <c r="D564" s="35"/>
-      <c r="E564" s="29">
-        <v>44257</v>
-      </c>
-      <c r="F564" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E564" s="32"/>
+      <c r="F564" s="55"/>
       <c r="G564" s="35"/>
-      <c r="H564" s="29"/>
-      <c r="I564" s="19"/>
-      <c r="J564" s="20"/>
+      <c r="H564" s="32"/>
+      <c r="I564" s="23"/>
+      <c r="J564" s="24"/>
       <c r="K564" s="35"/>
     </row>
-    <row r="565" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A565" s="35"/>
-      <c r="B565" s="11"/>
-      <c r="C565" s="12"/>
+      <c r="B565" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C565" s="4" t="s">
+        <v>255</v>
+      </c>
       <c r="D565" s="35"/>
-      <c r="E565" s="32"/>
-      <c r="F565" s="55"/>
+      <c r="E565" s="29">
+        <v>44151</v>
+      </c>
+      <c r="F565" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G565" s="35"/>
-      <c r="H565" s="32"/>
-      <c r="I565" s="23"/>
-      <c r="J565" s="24"/>
+      <c r="H565" s="29"/>
+      <c r="I565" s="19">
+        <v>1</v>
+      </c>
+      <c r="J565" s="20">
+        <v>0</v>
+      </c>
       <c r="K565" s="35"/>
     </row>
     <row r="566" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A566" s="35"/>
       <c r="B566" s="7" t="s">
-        <v>614</v>
+        <v>368</v>
       </c>
       <c r="C566" s="4" t="s">
-        <v>615</v>
+        <v>369</v>
       </c>
       <c r="D566" s="35"/>
       <c r="E566" s="29">
-        <v>44319</v>
+        <v>44245</v>
       </c>
       <c r="F566" s="53" t="s">
         <v>597</v>
@@ -17569,30 +17581,42 @@
       </c>
       <c r="K566" s="35"/>
     </row>
-    <row r="567" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A567" s="35"/>
-      <c r="B567" s="11"/>
-      <c r="C567" s="12"/>
+      <c r="B567" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C567" s="4" t="s">
+        <v>371</v>
+      </c>
       <c r="D567" s="35"/>
-      <c r="E567" s="32"/>
-      <c r="F567" s="55"/>
+      <c r="E567" s="29">
+        <v>44231</v>
+      </c>
+      <c r="F567" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G567" s="35"/>
-      <c r="H567" s="32"/>
-      <c r="I567" s="23"/>
-      <c r="J567" s="24"/>
+      <c r="H567" s="29"/>
+      <c r="I567" s="19">
+        <v>1</v>
+      </c>
+      <c r="J567" s="20">
+        <v>0</v>
+      </c>
       <c r="K567" s="35"/>
     </row>
     <row r="568" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A568" s="35"/>
       <c r="B568" s="7" t="s">
-        <v>254</v>
+        <v>355</v>
       </c>
       <c r="C568" s="4" t="s">
-        <v>255</v>
+        <v>356</v>
       </c>
       <c r="D568" s="35"/>
       <c r="E568" s="29">
-        <v>44151</v>
+        <v>44230</v>
       </c>
       <c r="F568" s="53" t="s">
         <v>597</v>
@@ -17609,128 +17633,116 @@
     </row>
     <row r="569" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A569" s="35"/>
-      <c r="B569" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="C569" s="4" t="s">
-        <v>369</v>
+      <c r="B569" s="44" t="s">
+        <v>404</v>
+      </c>
+      <c r="C569" s="45" t="s">
+        <v>405</v>
       </c>
       <c r="D569" s="35"/>
       <c r="E569" s="29">
-        <v>44245</v>
+        <v>44264</v>
       </c>
       <c r="F569" s="53" t="s">
         <v>597</v>
       </c>
-      <c r="G569" s="35"/>
-      <c r="H569" s="29"/>
-      <c r="I569" s="19">
-        <v>1</v>
-      </c>
-      <c r="J569" s="20">
+      <c r="G569" s="46"/>
+      <c r="H569" s="47"/>
+      <c r="I569" s="48">
+        <v>1</v>
+      </c>
+      <c r="J569" s="49">
         <v>0</v>
       </c>
       <c r="K569" s="35"/>
     </row>
-    <row r="570" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A570" s="35"/>
-      <c r="B570" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="C570" s="4" t="s">
-        <v>371</v>
-      </c>
+      <c r="B570" s="11"/>
+      <c r="C570" s="12"/>
       <c r="D570" s="35"/>
-      <c r="E570" s="29">
-        <v>44231</v>
-      </c>
-      <c r="F570" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E570" s="32"/>
+      <c r="F570" s="55"/>
       <c r="G570" s="35"/>
-      <c r="H570" s="29"/>
-      <c r="I570" s="19">
-        <v>1</v>
-      </c>
-      <c r="J570" s="20">
-        <v>0</v>
-      </c>
+      <c r="H570" s="32"/>
+      <c r="I570" s="23"/>
+      <c r="J570" s="24"/>
       <c r="K570" s="35"/>
     </row>
     <row r="571" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A571" s="35"/>
       <c r="B571" s="7" t="s">
-        <v>355</v>
+        <v>406</v>
       </c>
       <c r="C571" s="4" t="s">
-        <v>356</v>
+        <v>407</v>
       </c>
       <c r="D571" s="35"/>
       <c r="E571" s="29">
-        <v>44230</v>
+        <v>44271</v>
       </c>
       <c r="F571" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G571" s="35"/>
       <c r="H571" s="29"/>
-      <c r="I571" s="19">
-        <v>1</v>
-      </c>
-      <c r="J571" s="20">
-        <v>0</v>
-      </c>
+      <c r="I571" s="19"/>
+      <c r="J571" s="20"/>
       <c r="K571" s="35"/>
     </row>
     <row r="572" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A572" s="35"/>
-      <c r="B572" s="44" t="s">
-        <v>404</v>
-      </c>
-      <c r="C572" s="45" t="s">
-        <v>405</v>
+      <c r="B572" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C572" s="4" t="s">
+        <v>413</v>
       </c>
       <c r="D572" s="35"/>
       <c r="E572" s="29">
-        <v>44264</v>
+        <v>44278</v>
       </c>
       <c r="F572" s="53" t="s">
         <v>597</v>
       </c>
-      <c r="G572" s="46"/>
-      <c r="H572" s="47"/>
-      <c r="I572" s="48">
-        <v>1</v>
-      </c>
-      <c r="J572" s="49">
-        <v>0</v>
-      </c>
+      <c r="G572" s="35"/>
+      <c r="H572" s="29"/>
+      <c r="I572" s="19"/>
+      <c r="J572" s="20"/>
       <c r="K572" s="35"/>
     </row>
-    <row r="573" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A573" s="35"/>
-      <c r="B573" s="11"/>
-      <c r="C573" s="12"/>
+      <c r="B573" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C573" s="4" t="s">
+        <v>409</v>
+      </c>
       <c r="D573" s="35"/>
-      <c r="E573" s="32"/>
-      <c r="F573" s="55"/>
+      <c r="E573" s="29">
+        <v>44271</v>
+      </c>
+      <c r="F573" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G573" s="35"/>
-      <c r="H573" s="32"/>
-      <c r="I573" s="23"/>
-      <c r="J573" s="24"/>
+      <c r="H573" s="29"/>
+      <c r="I573" s="19"/>
+      <c r="J573" s="20"/>
       <c r="K573" s="35"/>
     </row>
     <row r="574" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A574" s="35"/>
       <c r="B574" s="7" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="C574" s="4" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D574" s="35"/>
       <c r="E574" s="29">
-        <v>44271</v>
+        <v>44272</v>
       </c>
       <c r="F574" s="53" t="s">
         <v>597</v>
@@ -17741,59 +17753,55 @@
       <c r="J574" s="20"/>
       <c r="K574" s="35"/>
     </row>
-    <row r="575" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A575" s="35"/>
-      <c r="B575" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="C575" s="4" t="s">
-        <v>413</v>
-      </c>
+      <c r="B575" s="11"/>
+      <c r="C575" s="12"/>
       <c r="D575" s="35"/>
-      <c r="E575" s="29">
-        <v>44278</v>
-      </c>
-      <c r="F575" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E575" s="32"/>
+      <c r="F575" s="55"/>
       <c r="G575" s="35"/>
-      <c r="H575" s="29"/>
-      <c r="I575" s="19"/>
-      <c r="J575" s="20"/>
+      <c r="H575" s="32"/>
+      <c r="I575" s="23"/>
+      <c r="J575" s="24"/>
       <c r="K575" s="35"/>
     </row>
     <row r="576" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A576" s="35"/>
       <c r="B576" s="7" t="s">
-        <v>408</v>
+        <v>64</v>
       </c>
       <c r="C576" s="4" t="s">
-        <v>409</v>
+        <v>65</v>
       </c>
       <c r="D576" s="35"/>
       <c r="E576" s="29">
-        <v>44271</v>
+        <v>44151</v>
       </c>
       <c r="F576" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G576" s="35"/>
       <c r="H576" s="29"/>
-      <c r="I576" s="19"/>
-      <c r="J576" s="20"/>
+      <c r="I576" s="19">
+        <v>1</v>
+      </c>
+      <c r="J576" s="20">
+        <v>0</v>
+      </c>
       <c r="K576" s="35"/>
     </row>
     <row r="577" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A577" s="35"/>
       <c r="B577" s="7" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C577" s="4" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="D577" s="35"/>
       <c r="E577" s="29">
-        <v>44272</v>
+        <v>44258</v>
       </c>
       <c r="F577" s="53" t="s">
         <v>597</v>
@@ -17819,96 +17827,112 @@
     </row>
     <row r="579" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A579" s="35"/>
-      <c r="B579" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C579" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="B579" s="7"/>
+      <c r="C579" s="4"/>
       <c r="D579" s="35"/>
-      <c r="E579" s="29">
-        <v>44151</v>
-      </c>
-      <c r="F579" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E579" s="29"/>
+      <c r="F579" s="53"/>
       <c r="G579" s="35"/>
       <c r="H579" s="29"/>
-      <c r="I579" s="19">
-        <v>1</v>
-      </c>
-      <c r="J579" s="20">
-        <v>0</v>
-      </c>
+      <c r="I579" s="19"/>
+      <c r="J579" s="20"/>
       <c r="K579" s="35"/>
     </row>
-    <row r="580" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A580" s="35"/>
-      <c r="B580" s="7" t="s">
-        <v>402</v>
-      </c>
-      <c r="C580" s="4" t="s">
-        <v>403</v>
-      </c>
+      <c r="B580" s="9"/>
+      <c r="C580" s="10"/>
       <c r="D580" s="35"/>
-      <c r="E580" s="29">
-        <v>44258</v>
-      </c>
-      <c r="F580" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E580" s="30"/>
+      <c r="F580" s="54"/>
       <c r="G580" s="35"/>
-      <c r="H580" s="29"/>
-      <c r="I580" s="19"/>
-      <c r="J580" s="20"/>
+      <c r="H580" s="30"/>
+      <c r="I580" s="21"/>
+      <c r="J580" s="22"/>
       <c r="K580" s="35"/>
     </row>
-    <row r="581" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A581" s="35"/>
-      <c r="B581" s="11"/>
-      <c r="C581" s="12"/>
+      <c r="B581" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="C581" s="4" t="s">
+        <v>665</v>
+      </c>
       <c r="D581" s="35"/>
-      <c r="E581" s="32"/>
-      <c r="F581" s="55"/>
+      <c r="E581" s="29">
+        <v>44382</v>
+      </c>
+      <c r="F581" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G581" s="35"/>
-      <c r="H581" s="32"/>
-      <c r="I581" s="23"/>
-      <c r="J581" s="24"/>
+      <c r="H581" s="29"/>
+      <c r="I581" s="19">
+        <v>1</v>
+      </c>
+      <c r="J581" s="20">
+        <v>0</v>
+      </c>
       <c r="K581" s="35"/>
     </row>
     <row r="582" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A582" s="35"/>
-      <c r="B582" s="7"/>
-      <c r="C582" s="4"/>
+      <c r="B582" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="C582" s="4" t="s">
+        <v>666</v>
+      </c>
       <c r="D582" s="35"/>
-      <c r="E582" s="29"/>
-      <c r="F582" s="53"/>
+      <c r="E582" s="29">
+        <v>44382</v>
+      </c>
+      <c r="F582" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G582" s="35"/>
       <c r="H582" s="29"/>
-      <c r="I582" s="19"/>
-      <c r="J582" s="20"/>
+      <c r="I582" s="19">
+        <v>1</v>
+      </c>
+      <c r="J582" s="20">
+        <v>0</v>
+      </c>
       <c r="K582" s="35"/>
     </row>
-    <row r="583" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A583" s="35"/>
-      <c r="B583" s="9"/>
-      <c r="C583" s="10"/>
+      <c r="B583" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="C583" s="4" t="s">
+        <v>667</v>
+      </c>
       <c r="D583" s="35"/>
-      <c r="E583" s="30"/>
-      <c r="F583" s="54"/>
+      <c r="E583" s="29">
+        <v>44382</v>
+      </c>
+      <c r="F583" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G583" s="35"/>
-      <c r="H583" s="30"/>
-      <c r="I583" s="21"/>
-      <c r="J583" s="22"/>
+      <c r="H583" s="29"/>
+      <c r="I583" s="19">
+        <v>1</v>
+      </c>
+      <c r="J583" s="20">
+        <v>0</v>
+      </c>
       <c r="K583" s="35"/>
     </row>
     <row r="584" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A584" s="35"/>
       <c r="B584" s="7" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="C584" s="4" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="D584" s="35"/>
       <c r="E584" s="29">
@@ -17930,10 +17954,10 @@
     <row r="585" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A585" s="35"/>
       <c r="B585" s="7" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="C585" s="4" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="D585" s="35"/>
       <c r="E585" s="29">
@@ -17952,101 +17976,89 @@
       </c>
       <c r="K585" s="35"/>
     </row>
-    <row r="586" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A586" s="35"/>
-      <c r="B586" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="C586" s="4" t="s">
-        <v>667</v>
-      </c>
+      <c r="B586" s="11"/>
+      <c r="C586" s="12"/>
       <c r="D586" s="35"/>
-      <c r="E586" s="29">
-        <v>44382</v>
-      </c>
-      <c r="F586" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E586" s="32"/>
+      <c r="F586" s="55"/>
       <c r="G586" s="35"/>
-      <c r="H586" s="29"/>
-      <c r="I586" s="19">
-        <v>1</v>
-      </c>
-      <c r="J586" s="20">
-        <v>0</v>
-      </c>
+      <c r="H586" s="32"/>
+      <c r="I586" s="23"/>
+      <c r="J586" s="24"/>
       <c r="K586" s="35"/>
     </row>
     <row r="587" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A587" s="35"/>
       <c r="B587" s="7" t="s">
-        <v>731</v>
+        <v>616</v>
       </c>
       <c r="C587" s="4" t="s">
-        <v>668</v>
+        <v>617</v>
       </c>
       <c r="D587" s="35"/>
       <c r="E587" s="29">
-        <v>44382</v>
+        <v>44379</v>
       </c>
       <c r="F587" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G587" s="35"/>
       <c r="H587" s="29"/>
-      <c r="I587" s="19">
-        <v>1</v>
-      </c>
-      <c r="J587" s="20">
-        <v>0</v>
-      </c>
+      <c r="I587" s="19"/>
+      <c r="J587" s="20"/>
       <c r="K587" s="35"/>
     </row>
     <row r="588" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A588" s="35"/>
       <c r="B588" s="7" t="s">
-        <v>732</v>
+        <v>514</v>
       </c>
       <c r="C588" s="4" t="s">
-        <v>669</v>
+        <v>436</v>
       </c>
       <c r="D588" s="35"/>
       <c r="E588" s="29">
-        <v>44382</v>
+        <v>44362</v>
       </c>
       <c r="F588" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G588" s="35"/>
       <c r="H588" s="29"/>
-      <c r="I588" s="19">
-        <v>1</v>
-      </c>
-      <c r="J588" s="20">
-        <v>0</v>
-      </c>
+      <c r="I588" s="19"/>
+      <c r="J588" s="20"/>
       <c r="K588" s="35"/>
     </row>
-    <row r="589" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A589" s="35"/>
-      <c r="B589" s="11"/>
-      <c r="C589" s="12"/>
+      <c r="B589" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="C589" s="4" t="s">
+        <v>619</v>
+      </c>
       <c r="D589" s="35"/>
-      <c r="E589" s="32"/>
-      <c r="F589" s="55"/>
+      <c r="E589" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F589" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G589" s="35"/>
-      <c r="H589" s="32"/>
-      <c r="I589" s="23"/>
-      <c r="J589" s="24"/>
+      <c r="H589" s="29"/>
+      <c r="I589" s="19"/>
+      <c r="J589" s="20"/>
       <c r="K589" s="35"/>
     </row>
     <row r="590" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A590" s="35"/>
       <c r="B590" s="7" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="C590" s="4" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="D590" s="35"/>
       <c r="E590" s="29">
@@ -18064,10 +18076,10 @@
     <row r="591" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A591" s="35"/>
       <c r="B591" s="7" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C591" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="D591" s="35"/>
       <c r="E591" s="29">
@@ -18085,14 +18097,14 @@
     <row r="592" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A592" s="35"/>
       <c r="B592" s="7" t="s">
-        <v>618</v>
+        <v>516</v>
       </c>
       <c r="C592" s="4" t="s">
-        <v>619</v>
+        <v>441</v>
       </c>
       <c r="D592" s="35"/>
       <c r="E592" s="29">
-        <v>44379</v>
+        <v>44362</v>
       </c>
       <c r="F592" s="53" t="s">
         <v>597</v>
@@ -18103,59 +18115,55 @@
       <c r="J592" s="20"/>
       <c r="K592" s="35"/>
     </row>
-    <row r="593" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A593" s="35"/>
-      <c r="B593" s="7" t="s">
-        <v>620</v>
-      </c>
-      <c r="C593" s="4" t="s">
-        <v>621</v>
-      </c>
+      <c r="B593" s="11"/>
+      <c r="C593" s="12"/>
       <c r="D593" s="35"/>
-      <c r="E593" s="29">
-        <v>44379</v>
-      </c>
-      <c r="F593" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E593" s="32"/>
+      <c r="F593" s="55"/>
       <c r="G593" s="35"/>
-      <c r="H593" s="29"/>
-      <c r="I593" s="19"/>
-      <c r="J593" s="20"/>
+      <c r="H593" s="32"/>
+      <c r="I593" s="23"/>
+      <c r="J593" s="24"/>
       <c r="K593" s="35"/>
     </row>
     <row r="594" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A594" s="35"/>
       <c r="B594" s="7" t="s">
-        <v>515</v>
+        <v>622</v>
       </c>
       <c r="C594" s="4" t="s">
-        <v>429</v>
+        <v>625</v>
       </c>
       <c r="D594" s="35"/>
       <c r="E594" s="29">
-        <v>44362</v>
+        <v>44379</v>
       </c>
       <c r="F594" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G594" s="35"/>
       <c r="H594" s="29"/>
-      <c r="I594" s="19"/>
-      <c r="J594" s="20"/>
+      <c r="I594" s="19">
+        <v>1</v>
+      </c>
+      <c r="J594" s="20">
+        <v>0</v>
+      </c>
       <c r="K594" s="35"/>
     </row>
     <row r="595" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A595" s="35"/>
       <c r="B595" s="7" t="s">
-        <v>516</v>
+        <v>623</v>
       </c>
       <c r="C595" s="4" t="s">
-        <v>441</v>
+        <v>626</v>
       </c>
       <c r="D595" s="35"/>
       <c r="E595" s="29">
-        <v>44362</v>
+        <v>44379</v>
       </c>
       <c r="F595" s="53" t="s">
         <v>597</v>
@@ -18166,51 +18174,47 @@
       <c r="J595" s="20"/>
       <c r="K595" s="35"/>
     </row>
-    <row r="596" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A596" s="35"/>
-      <c r="B596" s="11"/>
-      <c r="C596" s="12"/>
+      <c r="B596" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="C596" s="4" t="s">
+        <v>627</v>
+      </c>
       <c r="D596" s="35"/>
-      <c r="E596" s="32"/>
-      <c r="F596" s="55"/>
+      <c r="E596" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F596" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G596" s="35"/>
-      <c r="H596" s="32"/>
-      <c r="I596" s="23"/>
-      <c r="J596" s="24"/>
+      <c r="H596" s="29"/>
+      <c r="I596" s="19"/>
+      <c r="J596" s="20"/>
       <c r="K596" s="35"/>
     </row>
-    <row r="597" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A597" s="35"/>
-      <c r="B597" s="7" t="s">
-        <v>622</v>
-      </c>
-      <c r="C597" s="4" t="s">
-        <v>625</v>
-      </c>
+      <c r="B597" s="11"/>
+      <c r="C597" s="12"/>
       <c r="D597" s="35"/>
-      <c r="E597" s="29">
-        <v>44379</v>
-      </c>
-      <c r="F597" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E597" s="32"/>
+      <c r="F597" s="55"/>
       <c r="G597" s="35"/>
-      <c r="H597" s="29"/>
-      <c r="I597" s="19">
-        <v>1</v>
-      </c>
-      <c r="J597" s="20">
-        <v>0</v>
-      </c>
+      <c r="H597" s="32"/>
+      <c r="I597" s="23"/>
+      <c r="J597" s="24"/>
       <c r="K597" s="35"/>
     </row>
     <row r="598" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A598" s="35"/>
       <c r="B598" s="7" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="C598" s="4" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="D598" s="35"/>
       <c r="E598" s="29">
@@ -18221,17 +18225,21 @@
       </c>
       <c r="G598" s="35"/>
       <c r="H598" s="29"/>
-      <c r="I598" s="19"/>
-      <c r="J598" s="20"/>
+      <c r="I598" s="19">
+        <v>1</v>
+      </c>
+      <c r="J598" s="20">
+        <v>0</v>
+      </c>
       <c r="K598" s="35"/>
     </row>
     <row r="599" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A599" s="35"/>
       <c r="B599" s="7" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="C599" s="4" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="D599" s="35"/>
       <c r="E599" s="29">
@@ -18242,80 +18250,84 @@
       </c>
       <c r="G599" s="35"/>
       <c r="H599" s="29"/>
-      <c r="I599" s="19"/>
-      <c r="J599" s="20"/>
+      <c r="I599" s="19">
+        <v>1</v>
+      </c>
+      <c r="J599" s="20">
+        <v>0</v>
+      </c>
       <c r="K599" s="35"/>
     </row>
-    <row r="600" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A600" s="35"/>
-      <c r="B600" s="11"/>
-      <c r="C600" s="12"/>
+      <c r="B600" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="C600" s="4" t="s">
+        <v>838</v>
+      </c>
       <c r="D600" s="35"/>
-      <c r="E600" s="32"/>
-      <c r="F600" s="55"/>
+      <c r="E600" s="29">
+        <v>44406</v>
+      </c>
+      <c r="F600" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G600" s="35"/>
-      <c r="H600" s="32"/>
-      <c r="I600" s="23"/>
-      <c r="J600" s="24"/>
+      <c r="H600" s="29"/>
+      <c r="I600" s="19"/>
+      <c r="J600" s="20"/>
       <c r="K600" s="35"/>
     </row>
     <row r="601" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A601" s="35"/>
       <c r="B601" s="7" t="s">
-        <v>628</v>
+        <v>835</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>630</v>
+        <v>839</v>
       </c>
       <c r="D601" s="35"/>
       <c r="E601" s="29">
-        <v>44379</v>
+        <v>44406</v>
       </c>
       <c r="F601" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G601" s="35"/>
       <c r="H601" s="29"/>
-      <c r="I601" s="19">
-        <v>1</v>
-      </c>
-      <c r="J601" s="20">
-        <v>0</v>
-      </c>
+      <c r="I601" s="19"/>
+      <c r="J601" s="20"/>
       <c r="K601" s="35"/>
     </row>
     <row r="602" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A602" s="35"/>
       <c r="B602" s="7" t="s">
-        <v>629</v>
+        <v>836</v>
       </c>
       <c r="C602" s="4" t="s">
-        <v>631</v>
+        <v>840</v>
       </c>
       <c r="D602" s="35"/>
       <c r="E602" s="29">
-        <v>44379</v>
+        <v>44406</v>
       </c>
       <c r="F602" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G602" s="35"/>
       <c r="H602" s="29"/>
-      <c r="I602" s="19">
-        <v>1</v>
-      </c>
-      <c r="J602" s="20">
-        <v>0</v>
-      </c>
+      <c r="I602" s="19"/>
+      <c r="J602" s="20"/>
       <c r="K602" s="35"/>
     </row>
     <row r="603" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A603" s="35"/>
       <c r="B603" s="7" t="s">
-        <v>834</v>
+        <v>837</v>
       </c>
       <c r="C603" s="4" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="D603" s="35"/>
       <c r="E603" s="29">
@@ -18330,67 +18342,67 @@
       <c r="J603" s="20"/>
       <c r="K603" s="35"/>
     </row>
-    <row r="604" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A604" s="35"/>
-      <c r="B604" s="7" t="s">
-        <v>835</v>
-      </c>
-      <c r="C604" s="4" t="s">
-        <v>839</v>
-      </c>
+      <c r="B604" s="11"/>
+      <c r="C604" s="12"/>
       <c r="D604" s="35"/>
-      <c r="E604" s="29">
-        <v>44406</v>
-      </c>
-      <c r="F604" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E604" s="32"/>
+      <c r="F604" s="55"/>
       <c r="G604" s="35"/>
-      <c r="H604" s="29"/>
-      <c r="I604" s="19"/>
-      <c r="J604" s="20"/>
+      <c r="H604" s="32"/>
+      <c r="I604" s="23"/>
+      <c r="J604" s="24"/>
       <c r="K604" s="35"/>
     </row>
     <row r="605" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A605" s="35"/>
       <c r="B605" s="7" t="s">
-        <v>836</v>
+        <v>632</v>
       </c>
       <c r="C605" s="4" t="s">
-        <v>840</v>
+        <v>634</v>
       </c>
       <c r="D605" s="35"/>
       <c r="E605" s="29">
-        <v>44406</v>
+        <v>44379</v>
       </c>
       <c r="F605" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G605" s="35"/>
       <c r="H605" s="29"/>
-      <c r="I605" s="19"/>
-      <c r="J605" s="20"/>
+      <c r="I605" s="19">
+        <v>1</v>
+      </c>
+      <c r="J605" s="20">
+        <v>0</v>
+      </c>
       <c r="K605" s="35"/>
     </row>
     <row r="606" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A606" s="35"/>
       <c r="B606" s="7" t="s">
-        <v>837</v>
+        <v>633</v>
       </c>
       <c r="C606" s="4" t="s">
-        <v>841</v>
+        <v>635</v>
       </c>
       <c r="D606" s="35"/>
       <c r="E606" s="29">
-        <v>44406</v>
+        <v>44379</v>
       </c>
       <c r="F606" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G606" s="35"/>
       <c r="H606" s="29"/>
-      <c r="I606" s="19"/>
-      <c r="J606" s="20"/>
+      <c r="I606" s="19">
+        <v>1</v>
+      </c>
+      <c r="J606" s="20">
+        <v>0</v>
+      </c>
       <c r="K606" s="35"/>
     </row>
     <row r="607" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18409,10 +18421,10 @@
     <row r="608" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A608" s="35"/>
       <c r="B608" s="7" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="C608" s="4" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="D608" s="35"/>
       <c r="E608" s="29">
@@ -18431,55 +18443,55 @@
       </c>
       <c r="K608" s="35"/>
     </row>
-    <row r="609" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A609" s="35"/>
-      <c r="B609" s="7" t="s">
-        <v>633</v>
-      </c>
-      <c r="C609" s="4" t="s">
-        <v>635</v>
-      </c>
+      <c r="B609" s="11"/>
+      <c r="C609" s="12"/>
       <c r="D609" s="35"/>
-      <c r="E609" s="29">
-        <v>44379</v>
-      </c>
-      <c r="F609" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E609" s="32"/>
+      <c r="F609" s="55"/>
       <c r="G609" s="35"/>
-      <c r="H609" s="29"/>
-      <c r="I609" s="19">
-        <v>1</v>
-      </c>
-      <c r="J609" s="20">
-        <v>0</v>
-      </c>
+      <c r="H609" s="32"/>
+      <c r="I609" s="23"/>
+      <c r="J609" s="24"/>
       <c r="K609" s="35"/>
     </row>
-    <row r="610" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A610" s="35"/>
-      <c r="B610" s="11"/>
-      <c r="C610" s="12"/>
+      <c r="B610" s="7" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C610" s="4" t="s">
+        <v>1026</v>
+      </c>
       <c r="D610" s="35"/>
-      <c r="E610" s="32"/>
-      <c r="F610" s="55"/>
+      <c r="E610" s="29">
+        <v>44572</v>
+      </c>
+      <c r="F610" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G610" s="35"/>
-      <c r="H610" s="32"/>
-      <c r="I610" s="23"/>
-      <c r="J610" s="24"/>
+      <c r="H610" s="29"/>
+      <c r="I610" s="19">
+        <v>1</v>
+      </c>
+      <c r="J610" s="20">
+        <v>0</v>
+      </c>
       <c r="K610" s="35"/>
     </row>
     <row r="611" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A611" s="35"/>
       <c r="B611" s="7" t="s">
-        <v>636</v>
+        <v>1021</v>
       </c>
       <c r="C611" s="4" t="s">
-        <v>637</v>
+        <v>1027</v>
       </c>
       <c r="D611" s="35"/>
       <c r="E611" s="29">
-        <v>44379</v>
+        <v>44572</v>
       </c>
       <c r="F611" s="53" t="s">
         <v>597</v>
@@ -18494,30 +18506,42 @@
       </c>
       <c r="K611" s="35"/>
     </row>
-    <row r="612" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A612" s="35"/>
-      <c r="B612" s="11"/>
-      <c r="C612" s="12"/>
+      <c r="B612" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="C612" s="4" t="s">
+        <v>639</v>
+      </c>
       <c r="D612" s="35"/>
-      <c r="E612" s="32"/>
-      <c r="F612" s="55"/>
+      <c r="E612" s="29">
+        <v>44379</v>
+      </c>
+      <c r="F612" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G612" s="35"/>
-      <c r="H612" s="32"/>
-      <c r="I612" s="23"/>
-      <c r="J612" s="24"/>
+      <c r="H612" s="29"/>
+      <c r="I612" s="19">
+        <v>1</v>
+      </c>
+      <c r="J612" s="20">
+        <v>0</v>
+      </c>
       <c r="K612" s="35"/>
     </row>
     <row r="613" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A613" s="35"/>
       <c r="B613" s="7" t="s">
-        <v>1020</v>
+        <v>952</v>
       </c>
       <c r="C613" s="4" t="s">
-        <v>1026</v>
+        <v>953</v>
       </c>
       <c r="D613" s="35"/>
       <c r="E613" s="29">
-        <v>44572</v>
+        <v>44491</v>
       </c>
       <c r="F613" s="53" t="s">
         <v>597</v>
@@ -18535,14 +18559,14 @@
     <row r="614" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A614" s="35"/>
       <c r="B614" s="7" t="s">
-        <v>1021</v>
+        <v>954</v>
       </c>
       <c r="C614" s="4" t="s">
-        <v>1027</v>
+        <v>955</v>
       </c>
       <c r="D614" s="35"/>
       <c r="E614" s="29">
-        <v>44572</v>
+        <v>44491</v>
       </c>
       <c r="F614" s="53" t="s">
         <v>597</v>
@@ -18557,147 +18581,147 @@
       </c>
       <c r="K614" s="35"/>
     </row>
-    <row r="615" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A615" s="35"/>
-      <c r="B615" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="C615" s="4" t="s">
-        <v>639</v>
-      </c>
+      <c r="B615" s="11"/>
+      <c r="C615" s="12"/>
       <c r="D615" s="35"/>
-      <c r="E615" s="29">
-        <v>44379</v>
-      </c>
-      <c r="F615" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E615" s="32"/>
+      <c r="F615" s="55"/>
       <c r="G615" s="35"/>
-      <c r="H615" s="29"/>
-      <c r="I615" s="19">
-        <v>1</v>
-      </c>
-      <c r="J615" s="20">
-        <v>0</v>
-      </c>
+      <c r="H615" s="32"/>
+      <c r="I615" s="23"/>
+      <c r="J615" s="24"/>
       <c r="K615" s="35"/>
     </row>
     <row r="616" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A616" s="35"/>
       <c r="B616" s="7" t="s">
-        <v>952</v>
+        <v>980</v>
       </c>
       <c r="C616" s="4" t="s">
-        <v>953</v>
+        <v>982</v>
       </c>
       <c r="D616" s="35"/>
       <c r="E616" s="29">
-        <v>44491</v>
+        <v>44526</v>
       </c>
       <c r="F616" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G616" s="35"/>
       <c r="H616" s="29"/>
-      <c r="I616" s="19">
-        <v>1</v>
-      </c>
-      <c r="J616" s="20">
-        <v>0</v>
-      </c>
+      <c r="I616" s="19"/>
+      <c r="J616" s="20"/>
       <c r="K616" s="35"/>
     </row>
     <row r="617" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A617" s="35"/>
       <c r="B617" s="7" t="s">
-        <v>954</v>
+        <v>981</v>
       </c>
       <c r="C617" s="4" t="s">
-        <v>955</v>
+        <v>983</v>
       </c>
       <c r="D617" s="35"/>
       <c r="E617" s="29">
-        <v>44491</v>
+        <v>44526</v>
       </c>
       <c r="F617" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G617" s="35"/>
       <c r="H617" s="29"/>
-      <c r="I617" s="19">
-        <v>1</v>
-      </c>
-      <c r="J617" s="20">
-        <v>0</v>
-      </c>
+      <c r="I617" s="19"/>
+      <c r="J617" s="20"/>
       <c r="K617" s="35"/>
     </row>
-    <row r="618" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A618" s="35"/>
-      <c r="B618" s="11"/>
-      <c r="C618" s="12"/>
+      <c r="B618" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C618" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D618" s="35"/>
-      <c r="E618" s="32"/>
-      <c r="F618" s="55"/>
+      <c r="E618" s="29">
+        <v>44148</v>
+      </c>
+      <c r="F618" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G618" s="35"/>
-      <c r="H618" s="32"/>
-      <c r="I618" s="23"/>
-      <c r="J618" s="24"/>
+      <c r="H618" s="29"/>
+      <c r="I618" s="19">
+        <v>1</v>
+      </c>
+      <c r="J618" s="20">
+        <v>0</v>
+      </c>
       <c r="K618" s="35"/>
     </row>
     <row r="619" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A619" s="35"/>
       <c r="B619" s="7" t="s">
-        <v>980</v>
+        <v>913</v>
       </c>
       <c r="C619" s="4" t="s">
-        <v>982</v>
+        <v>914</v>
       </c>
       <c r="D619" s="35"/>
       <c r="E619" s="29">
-        <v>44526</v>
+        <v>44420</v>
       </c>
       <c r="F619" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G619" s="35"/>
       <c r="H619" s="29"/>
-      <c r="I619" s="19"/>
-      <c r="J619" s="20"/>
+      <c r="I619" s="19">
+        <v>1</v>
+      </c>
+      <c r="J619" s="20">
+        <v>0</v>
+      </c>
       <c r="K619" s="35"/>
     </row>
     <row r="620" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A620" s="35"/>
       <c r="B620" s="7" t="s">
-        <v>981</v>
+        <v>125</v>
       </c>
       <c r="C620" s="4" t="s">
-        <v>983</v>
+        <v>107</v>
       </c>
       <c r="D620" s="35"/>
       <c r="E620" s="29">
-        <v>44526</v>
+        <v>44172</v>
       </c>
       <c r="F620" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G620" s="35"/>
       <c r="H620" s="29"/>
-      <c r="I620" s="19"/>
-      <c r="J620" s="20"/>
+      <c r="I620" s="19">
+        <v>1</v>
+      </c>
+      <c r="J620" s="20">
+        <v>0</v>
+      </c>
       <c r="K620" s="35"/>
     </row>
     <row r="621" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A621" s="35"/>
       <c r="B621" s="7" t="s">
-        <v>14</v>
+        <v>260</v>
       </c>
       <c r="C621" s="4" t="s">
-        <v>55</v>
+        <v>261</v>
       </c>
       <c r="D621" s="35"/>
       <c r="E621" s="29">
-        <v>44148</v>
+        <v>44172</v>
       </c>
       <c r="F621" s="53" t="s">
         <v>597</v>
@@ -18715,14 +18739,14 @@
     <row r="622" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A622" s="35"/>
       <c r="B622" s="7" t="s">
-        <v>913</v>
+        <v>126</v>
       </c>
       <c r="C622" s="4" t="s">
-        <v>914</v>
+        <v>108</v>
       </c>
       <c r="D622" s="35"/>
       <c r="E622" s="29">
-        <v>44420</v>
+        <v>44172</v>
       </c>
       <c r="F622" s="53" t="s">
         <v>597</v>
@@ -18740,10 +18764,10 @@
     <row r="623" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A623" s="35"/>
       <c r="B623" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C623" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D623" s="35"/>
       <c r="E623" s="29">
@@ -18765,14 +18789,14 @@
     <row r="624" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A624" s="35"/>
       <c r="B624" s="7" t="s">
-        <v>260</v>
+        <v>128</v>
       </c>
       <c r="C624" s="4" t="s">
-        <v>261</v>
+        <v>110</v>
       </c>
       <c r="D624" s="35"/>
       <c r="E624" s="29">
-        <v>44172</v>
+        <v>44376</v>
       </c>
       <c r="F624" s="53" t="s">
         <v>597</v>
@@ -18790,14 +18814,14 @@
     <row r="625" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A625" s="35"/>
       <c r="B625" s="7" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C625" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D625" s="35"/>
       <c r="E625" s="29">
-        <v>44172</v>
+        <v>44379</v>
       </c>
       <c r="F625" s="53" t="s">
         <v>597</v>
@@ -18815,39 +18839,35 @@
     <row r="626" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A626" s="35"/>
       <c r="B626" s="7" t="s">
-        <v>127</v>
+        <v>867</v>
       </c>
       <c r="C626" s="4" t="s">
-        <v>109</v>
+        <v>868</v>
       </c>
       <c r="D626" s="35"/>
       <c r="E626" s="29">
-        <v>44172</v>
+        <v>44407</v>
       </c>
       <c r="F626" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G626" s="35"/>
       <c r="H626" s="29"/>
-      <c r="I626" s="19">
-        <v>1</v>
-      </c>
-      <c r="J626" s="20">
-        <v>0</v>
-      </c>
+      <c r="I626" s="19"/>
+      <c r="J626" s="20"/>
       <c r="K626" s="35"/>
     </row>
     <row r="627" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A627" s="35"/>
       <c r="B627" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C627" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D627" s="35"/>
       <c r="E627" s="29">
-        <v>44376</v>
+        <v>44379</v>
       </c>
       <c r="F627" s="53" t="s">
         <v>597</v>
@@ -18865,10 +18885,10 @@
     <row r="628" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A628" s="35"/>
       <c r="B628" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C628" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D628" s="35"/>
       <c r="E628" s="29">
@@ -18890,56 +18910,56 @@
     <row r="629" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A629" s="35"/>
       <c r="B629" s="7" t="s">
-        <v>867</v>
+        <v>899</v>
       </c>
       <c r="C629" s="4" t="s">
-        <v>868</v>
+        <v>901</v>
       </c>
       <c r="D629" s="35"/>
       <c r="E629" s="29">
-        <v>44407</v>
+        <v>44411</v>
       </c>
       <c r="F629" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G629" s="35"/>
       <c r="H629" s="29"/>
-      <c r="I629" s="19"/>
-      <c r="J629" s="20"/>
+      <c r="I629" s="19">
+        <v>1</v>
+      </c>
+      <c r="J629" s="20">
+        <v>0</v>
+      </c>
       <c r="K629" s="35"/>
     </row>
     <row r="630" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A630" s="35"/>
       <c r="B630" s="7" t="s">
-        <v>130</v>
+        <v>900</v>
       </c>
       <c r="C630" s="4" t="s">
-        <v>112</v>
+        <v>902</v>
       </c>
       <c r="D630" s="35"/>
       <c r="E630" s="29">
-        <v>44379</v>
+        <v>44411</v>
       </c>
       <c r="F630" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G630" s="35"/>
       <c r="H630" s="29"/>
-      <c r="I630" s="19">
-        <v>1</v>
-      </c>
-      <c r="J630" s="20">
-        <v>0</v>
-      </c>
+      <c r="I630" s="19"/>
+      <c r="J630" s="20"/>
       <c r="K630" s="35"/>
     </row>
     <row r="631" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A631" s="35"/>
       <c r="B631" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C631" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D631" s="35"/>
       <c r="E631" s="29">
@@ -18961,14 +18981,14 @@
     <row r="632" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A632" s="35"/>
       <c r="B632" s="7" t="s">
-        <v>899</v>
+        <v>133</v>
       </c>
       <c r="C632" s="4" t="s">
-        <v>901</v>
+        <v>115</v>
       </c>
       <c r="D632" s="35"/>
       <c r="E632" s="29">
-        <v>44411</v>
+        <v>44379</v>
       </c>
       <c r="F632" s="53" t="s">
         <v>597</v>
@@ -18986,31 +19006,35 @@
     <row r="633" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A633" s="35"/>
       <c r="B633" s="7" t="s">
-        <v>900</v>
+        <v>134</v>
       </c>
       <c r="C633" s="4" t="s">
-        <v>902</v>
+        <v>116</v>
       </c>
       <c r="D633" s="35"/>
       <c r="E633" s="29">
-        <v>44411</v>
+        <v>44379</v>
       </c>
       <c r="F633" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G633" s="35"/>
       <c r="H633" s="29"/>
-      <c r="I633" s="19"/>
-      <c r="J633" s="20"/>
+      <c r="I633" s="19">
+        <v>1</v>
+      </c>
+      <c r="J633" s="20">
+        <v>0</v>
+      </c>
       <c r="K633" s="35"/>
     </row>
     <row r="634" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A634" s="35"/>
       <c r="B634" s="7" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C634" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D634" s="35"/>
       <c r="E634" s="29">
@@ -19032,10 +19056,10 @@
     <row r="635" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A635" s="35"/>
       <c r="B635" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C635" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D635" s="35"/>
       <c r="E635" s="29">
@@ -19057,10 +19081,10 @@
     <row r="636" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A636" s="35"/>
       <c r="B636" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C636" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D636" s="35"/>
       <c r="E636" s="29">
@@ -19082,10 +19106,10 @@
     <row r="637" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A637" s="35"/>
       <c r="B637" s="7" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C637" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D637" s="35"/>
       <c r="E637" s="29">
@@ -19107,10 +19131,10 @@
     <row r="638" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A638" s="35"/>
       <c r="B638" s="7" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C638" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D638" s="35"/>
       <c r="E638" s="29">
@@ -19132,14 +19156,14 @@
     <row r="639" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A639" s="35"/>
       <c r="B639" s="7" t="s">
-        <v>137</v>
+        <v>815</v>
       </c>
       <c r="C639" s="4" t="s">
-        <v>119</v>
+        <v>816</v>
       </c>
       <c r="D639" s="35"/>
       <c r="E639" s="29">
-        <v>44379</v>
+        <v>44406</v>
       </c>
       <c r="F639" s="53" t="s">
         <v>597</v>
@@ -19157,10 +19181,10 @@
     <row r="640" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A640" s="35"/>
       <c r="B640" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C640" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D640" s="35"/>
       <c r="E640" s="29">
@@ -19182,10 +19206,10 @@
     <row r="641" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A641" s="35"/>
       <c r="B641" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C641" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D641" s="35"/>
       <c r="E641" s="29">
@@ -19207,14 +19231,14 @@
     <row r="642" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A642" s="35"/>
       <c r="B642" s="7" t="s">
-        <v>815</v>
+        <v>142</v>
       </c>
       <c r="C642" s="4" t="s">
-        <v>816</v>
+        <v>124</v>
       </c>
       <c r="D642" s="35"/>
       <c r="E642" s="29">
-        <v>44406</v>
+        <v>44379</v>
       </c>
       <c r="F642" s="53" t="s">
         <v>597</v>
@@ -19232,10 +19256,10 @@
     <row r="643" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A643" s="35"/>
       <c r="B643" s="7" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C643" s="4" t="s">
-        <v>122</v>
+        <v>593</v>
       </c>
       <c r="D643" s="35"/>
       <c r="E643" s="29">
@@ -19257,10 +19281,10 @@
     <row r="644" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A644" s="35"/>
       <c r="B644" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C644" s="4" t="s">
-        <v>123</v>
+        <v>640</v>
       </c>
       <c r="D644" s="35"/>
       <c r="E644" s="29">
@@ -19282,10 +19306,10 @@
     <row r="645" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A645" s="35"/>
       <c r="B645" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C645" s="4" t="s">
-        <v>124</v>
+        <v>641</v>
       </c>
       <c r="D645" s="35"/>
       <c r="E645" s="29">
@@ -19307,10 +19331,10 @@
     <row r="646" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A646" s="35"/>
       <c r="B646" s="7" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C646" s="4" t="s">
-        <v>593</v>
+        <v>642</v>
       </c>
       <c r="D646" s="35"/>
       <c r="E646" s="29">
@@ -19332,14 +19356,14 @@
     <row r="647" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A647" s="35"/>
       <c r="B647" s="7" t="s">
-        <v>144</v>
+        <v>1126</v>
       </c>
       <c r="C647" s="4" t="s">
-        <v>640</v>
+        <v>1127</v>
       </c>
       <c r="D647" s="35"/>
       <c r="E647" s="29">
-        <v>44379</v>
+        <v>44624</v>
       </c>
       <c r="F647" s="53" t="s">
         <v>597</v>
@@ -19357,14 +19381,14 @@
     <row r="648" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A648" s="35"/>
       <c r="B648" s="7" t="s">
-        <v>145</v>
+        <v>1128</v>
       </c>
       <c r="C648" s="4" t="s">
-        <v>641</v>
+        <v>1129</v>
       </c>
       <c r="D648" s="35"/>
       <c r="E648" s="29">
-        <v>44379</v>
+        <v>44624</v>
       </c>
       <c r="F648" s="53" t="s">
         <v>597</v>
@@ -19382,10 +19406,10 @@
     <row r="649" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A649" s="35"/>
       <c r="B649" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C649" s="4" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D649" s="35"/>
       <c r="E649" s="29">
@@ -19407,14 +19431,14 @@
     <row r="650" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A650" s="35"/>
       <c r="B650" s="7" t="s">
-        <v>1126</v>
+        <v>148</v>
       </c>
       <c r="C650" s="4" t="s">
-        <v>1127</v>
+        <v>644</v>
       </c>
       <c r="D650" s="35"/>
       <c r="E650" s="29">
-        <v>44624</v>
+        <v>44379</v>
       </c>
       <c r="F650" s="53" t="s">
         <v>597</v>
@@ -19432,14 +19456,14 @@
     <row r="651" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A651" s="35"/>
       <c r="B651" s="7" t="s">
-        <v>1128</v>
+        <v>149</v>
       </c>
       <c r="C651" s="4" t="s">
-        <v>1129</v>
+        <v>645</v>
       </c>
       <c r="D651" s="35"/>
       <c r="E651" s="29">
-        <v>44624</v>
+        <v>44379</v>
       </c>
       <c r="F651" s="53" t="s">
         <v>597</v>
@@ -19457,10 +19481,10 @@
     <row r="652" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A652" s="35"/>
       <c r="B652" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C652" s="4" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="D652" s="35"/>
       <c r="E652" s="29">
@@ -19482,35 +19506,31 @@
     <row r="653" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A653" s="35"/>
       <c r="B653" s="7" t="s">
-        <v>148</v>
+        <v>855</v>
       </c>
       <c r="C653" s="4" t="s">
-        <v>644</v>
+        <v>856</v>
       </c>
       <c r="D653" s="35"/>
       <c r="E653" s="29">
-        <v>44379</v>
+        <v>44407</v>
       </c>
       <c r="F653" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G653" s="35"/>
       <c r="H653" s="29"/>
-      <c r="I653" s="19">
-        <v>1</v>
-      </c>
-      <c r="J653" s="20">
-        <v>0</v>
-      </c>
+      <c r="I653" s="19"/>
+      <c r="J653" s="20"/>
       <c r="K653" s="35"/>
     </row>
     <row r="654" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A654" s="35"/>
       <c r="B654" s="7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C654" s="4" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D654" s="35"/>
       <c r="E654" s="29">
@@ -19532,10 +19552,10 @@
     <row r="655" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A655" s="35"/>
       <c r="B655" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C655" s="4" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="D655" s="35"/>
       <c r="E655" s="29">
@@ -19557,31 +19577,35 @@
     <row r="656" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A656" s="35"/>
       <c r="B656" s="7" t="s">
-        <v>855</v>
+        <v>153</v>
       </c>
       <c r="C656" s="4" t="s">
-        <v>856</v>
+        <v>649</v>
       </c>
       <c r="D656" s="35"/>
       <c r="E656" s="29">
-        <v>44407</v>
+        <v>44379</v>
       </c>
       <c r="F656" s="53" t="s">
         <v>597</v>
       </c>
       <c r="G656" s="35"/>
       <c r="H656" s="29"/>
-      <c r="I656" s="19"/>
-      <c r="J656" s="20"/>
+      <c r="I656" s="19">
+        <v>1</v>
+      </c>
+      <c r="J656" s="20">
+        <v>0</v>
+      </c>
       <c r="K656" s="35"/>
     </row>
     <row r="657" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A657" s="35"/>
       <c r="B657" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C657" s="4" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="D657" s="35"/>
       <c r="E657" s="29">
@@ -19603,10 +19627,10 @@
     <row r="658" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A658" s="35"/>
       <c r="B658" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C658" s="4" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="D658" s="35"/>
       <c r="E658" s="29">
@@ -19628,10 +19652,10 @@
     <row r="659" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A659" s="35"/>
       <c r="B659" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C659" s="4" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="D659" s="35"/>
       <c r="E659" s="29">
@@ -19650,42 +19674,30 @@
       </c>
       <c r="K659" s="35"/>
     </row>
-    <row r="660" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A660" s="35"/>
-      <c r="B660" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C660" s="4" t="s">
-        <v>650</v>
-      </c>
+      <c r="B660" s="11"/>
+      <c r="C660" s="12"/>
       <c r="D660" s="35"/>
-      <c r="E660" s="29">
-        <v>44379</v>
-      </c>
-      <c r="F660" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E660" s="32"/>
+      <c r="F660" s="55"/>
       <c r="G660" s="35"/>
-      <c r="H660" s="29"/>
-      <c r="I660" s="19">
-        <v>1</v>
-      </c>
-      <c r="J660" s="20">
-        <v>0</v>
-      </c>
+      <c r="H660" s="32"/>
+      <c r="I660" s="23"/>
+      <c r="J660" s="24"/>
       <c r="K660" s="35"/>
     </row>
     <row r="661" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A661" s="35"/>
       <c r="B661" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C661" s="4" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="D661" s="35"/>
       <c r="E661" s="29">
-        <v>44379</v>
+        <v>44382</v>
       </c>
       <c r="F661" s="53" t="s">
         <v>597</v>
@@ -19703,14 +19715,14 @@
     <row r="662" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A662" s="35"/>
       <c r="B662" s="7" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="C662" s="4" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D662" s="35"/>
       <c r="E662" s="29">
-        <v>44379</v>
+        <v>44382</v>
       </c>
       <c r="F662" s="53" t="s">
         <v>597</v>
@@ -19725,55 +19737,55 @@
       </c>
       <c r="K662" s="35"/>
     </row>
-    <row r="663" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A663" s="35"/>
-      <c r="B663" s="11"/>
-      <c r="C663" s="12"/>
+      <c r="B663" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="C663" s="4" t="s">
+        <v>725</v>
+      </c>
       <c r="D663" s="35"/>
-      <c r="E663" s="32"/>
-      <c r="F663" s="55"/>
+      <c r="E663" s="29">
+        <v>44384</v>
+      </c>
+      <c r="F663" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G663" s="35"/>
-      <c r="H663" s="32"/>
-      <c r="I663" s="23"/>
-      <c r="J663" s="24"/>
+      <c r="H663" s="29"/>
+      <c r="I663" s="19">
+        <v>1</v>
+      </c>
+      <c r="J663" s="20">
+        <v>0</v>
+      </c>
       <c r="K663" s="35"/>
     </row>
-    <row r="664" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A664" s="35"/>
-      <c r="B664" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C664" s="4" t="s">
-        <v>653</v>
-      </c>
+      <c r="B664" s="11"/>
+      <c r="C664" s="12"/>
       <c r="D664" s="35"/>
-      <c r="E664" s="29">
-        <v>44382</v>
-      </c>
-      <c r="F664" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E664" s="32"/>
+      <c r="F664" s="55"/>
       <c r="G664" s="35"/>
-      <c r="H664" s="29"/>
-      <c r="I664" s="19">
-        <v>1</v>
-      </c>
-      <c r="J664" s="20">
-        <v>0</v>
-      </c>
+      <c r="H664" s="32"/>
+      <c r="I664" s="23"/>
+      <c r="J664" s="24"/>
       <c r="K664" s="35"/>
     </row>
     <row r="665" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A665" s="35"/>
       <c r="B665" s="7" t="s">
-        <v>177</v>
+        <v>1244</v>
       </c>
       <c r="C665" s="4" t="s">
-        <v>654</v>
+        <v>1245</v>
       </c>
       <c r="D665" s="35"/>
       <c r="E665" s="29">
-        <v>44382</v>
+        <v>44628</v>
       </c>
       <c r="F665" s="53" t="s">
         <v>597</v>
@@ -19791,14 +19803,14 @@
     <row r="666" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A666" s="35"/>
       <c r="B666" s="7" t="s">
-        <v>724</v>
+        <v>1246</v>
       </c>
       <c r="C666" s="4" t="s">
-        <v>725</v>
+        <v>1247</v>
       </c>
       <c r="D666" s="35"/>
       <c r="E666" s="29">
-        <v>44384</v>
+        <v>44628</v>
       </c>
       <c r="F666" s="53" t="s">
         <v>597</v>
@@ -19813,30 +19825,42 @@
       </c>
       <c r="K666" s="35"/>
     </row>
-    <row r="667" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A667" s="35"/>
-      <c r="B667" s="11"/>
-      <c r="C667" s="12"/>
+      <c r="B667" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="C667" s="4" t="s">
+        <v>660</v>
+      </c>
       <c r="D667" s="35"/>
-      <c r="E667" s="32"/>
-      <c r="F667" s="55"/>
+      <c r="E667" s="29">
+        <v>44382</v>
+      </c>
+      <c r="F667" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G667" s="35"/>
-      <c r="H667" s="32"/>
-      <c r="I667" s="23"/>
-      <c r="J667" s="24"/>
+      <c r="H667" s="29"/>
+      <c r="I667" s="19">
+        <v>1</v>
+      </c>
+      <c r="J667" s="20">
+        <v>0</v>
+      </c>
       <c r="K667" s="35"/>
     </row>
     <row r="668" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A668" s="35"/>
       <c r="B668" s="7" t="s">
-        <v>1245</v>
+        <v>656</v>
       </c>
       <c r="C668" s="4" t="s">
-        <v>1246</v>
+        <v>661</v>
       </c>
       <c r="D668" s="35"/>
       <c r="E668" s="29">
-        <v>44628</v>
+        <v>44382</v>
       </c>
       <c r="F668" s="53" t="s">
         <v>597</v>
@@ -19854,14 +19878,14 @@
     <row r="669" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A669" s="35"/>
       <c r="B669" s="7" t="s">
-        <v>1247</v>
+        <v>657</v>
       </c>
       <c r="C669" s="4" t="s">
-        <v>1248</v>
+        <v>662</v>
       </c>
       <c r="D669" s="35"/>
       <c r="E669" s="29">
-        <v>44628</v>
+        <v>44382</v>
       </c>
       <c r="F669" s="53" t="s">
         <v>597</v>
@@ -19879,10 +19903,10 @@
     <row r="670" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A670" s="35"/>
       <c r="B670" s="7" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="C670" s="4" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="D670" s="35"/>
       <c r="E670" s="29">
@@ -19904,10 +19928,10 @@
     <row r="671" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A671" s="35"/>
       <c r="B671" s="7" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C671" s="4" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="D671" s="35"/>
       <c r="E671" s="29">
@@ -19929,14 +19953,14 @@
     <row r="672" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A672" s="35"/>
       <c r="B672" s="7" t="s">
-        <v>657</v>
+        <v>1078</v>
       </c>
       <c r="C672" s="4" t="s">
-        <v>662</v>
+        <v>1079</v>
       </c>
       <c r="D672" s="35"/>
       <c r="E672" s="29">
-        <v>44382</v>
+        <v>44621</v>
       </c>
       <c r="F672" s="53" t="s">
         <v>597</v>
@@ -19954,14 +19978,14 @@
     <row r="673" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A673" s="35"/>
       <c r="B673" s="7" t="s">
-        <v>658</v>
+        <v>1204</v>
       </c>
       <c r="C673" s="4" t="s">
-        <v>663</v>
+        <v>1205</v>
       </c>
       <c r="D673" s="35"/>
       <c r="E673" s="29">
-        <v>44382</v>
+        <v>44628</v>
       </c>
       <c r="F673" s="53" t="s">
         <v>597</v>
@@ -19979,14 +20003,14 @@
     <row r="674" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A674" s="35"/>
       <c r="B674" s="7" t="s">
-        <v>659</v>
+        <v>1208</v>
       </c>
       <c r="C674" s="4" t="s">
-        <v>664</v>
+        <v>1210</v>
       </c>
       <c r="D674" s="35"/>
       <c r="E674" s="29">
-        <v>44382</v>
+        <v>44628</v>
       </c>
       <c r="F674" s="53" t="s">
         <v>597</v>
@@ -20004,14 +20028,14 @@
     <row r="675" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A675" s="35"/>
       <c r="B675" s="7" t="s">
-        <v>1078</v>
+        <v>1206</v>
       </c>
       <c r="C675" s="4" t="s">
-        <v>1079</v>
+        <v>1207</v>
       </c>
       <c r="D675" s="35"/>
       <c r="E675" s="29">
-        <v>44621</v>
+        <v>44628</v>
       </c>
       <c r="F675" s="53" t="s">
         <v>597</v>
@@ -20029,10 +20053,10 @@
     <row r="676" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A676" s="35"/>
       <c r="B676" s="7" t="s">
-        <v>1205</v>
+        <v>1209</v>
       </c>
       <c r="C676" s="4" t="s">
-        <v>1206</v>
+        <v>1211</v>
       </c>
       <c r="D676" s="35"/>
       <c r="E676" s="29">
@@ -20054,14 +20078,14 @@
     <row r="677" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A677" s="35"/>
       <c r="B677" s="7" t="s">
-        <v>1209</v>
+        <v>1080</v>
       </c>
       <c r="C677" s="4" t="s">
-        <v>1211</v>
+        <v>1081</v>
       </c>
       <c r="D677" s="35"/>
       <c r="E677" s="29">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="F677" s="53" t="s">
         <v>597</v>
@@ -20076,42 +20100,30 @@
       </c>
       <c r="K677" s="35"/>
     </row>
-    <row r="678" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A678" s="35"/>
-      <c r="B678" s="7" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C678" s="4" t="s">
-        <v>1208</v>
-      </c>
+      <c r="B678" s="11"/>
+      <c r="C678" s="12"/>
       <c r="D678" s="35"/>
-      <c r="E678" s="29">
-        <v>44628</v>
-      </c>
-      <c r="F678" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E678" s="32"/>
+      <c r="F678" s="55"/>
       <c r="G678" s="35"/>
-      <c r="H678" s="29"/>
-      <c r="I678" s="19">
-        <v>1</v>
-      </c>
-      <c r="J678" s="20">
-        <v>0</v>
-      </c>
+      <c r="H678" s="32"/>
+      <c r="I678" s="23"/>
+      <c r="J678" s="24"/>
       <c r="K678" s="35"/>
     </row>
     <row r="679" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A679" s="35"/>
       <c r="B679" s="7" t="s">
-        <v>1210</v>
+        <v>1272</v>
       </c>
       <c r="C679" s="4" t="s">
-        <v>1212</v>
+        <v>1275</v>
       </c>
       <c r="D679" s="35"/>
       <c r="E679" s="29">
-        <v>44628</v>
+        <v>44635</v>
       </c>
       <c r="F679" s="53" t="s">
         <v>597</v>
@@ -20129,14 +20141,14 @@
     <row r="680" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A680" s="35"/>
       <c r="B680" s="7" t="s">
-        <v>1080</v>
+        <v>1273</v>
       </c>
       <c r="C680" s="4" t="s">
-        <v>1081</v>
+        <v>1276</v>
       </c>
       <c r="D680" s="35"/>
       <c r="E680" s="29">
-        <v>44621</v>
+        <v>44635</v>
       </c>
       <c r="F680" s="53" t="s">
         <v>597</v>
@@ -20151,80 +20163,68 @@
       </c>
       <c r="K680" s="35"/>
     </row>
-    <row r="681" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A681" s="35"/>
-      <c r="B681" s="11"/>
-      <c r="C681" s="12"/>
+      <c r="B681" s="7" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C681" s="4" t="s">
+        <v>1277</v>
+      </c>
       <c r="D681" s="35"/>
-      <c r="E681" s="32"/>
-      <c r="F681" s="55"/>
+      <c r="E681" s="29">
+        <v>44636</v>
+      </c>
+      <c r="F681" s="53" t="s">
+        <v>597</v>
+      </c>
       <c r="G681" s="35"/>
-      <c r="H681" s="32"/>
-      <c r="I681" s="23"/>
-      <c r="J681" s="24"/>
+      <c r="H681" s="29"/>
+      <c r="I681" s="19">
+        <v>1</v>
+      </c>
+      <c r="J681" s="20">
+        <v>0</v>
+      </c>
       <c r="K681" s="35"/>
     </row>
     <row r="682" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A682" s="35"/>
-      <c r="B682" s="7" t="s">
-        <v>1273</v>
-      </c>
-      <c r="C682" s="4" t="s">
-        <v>1276</v>
-      </c>
+      <c r="B682" s="7"/>
+      <c r="C682" s="4"/>
       <c r="D682" s="35"/>
-      <c r="E682" s="29">
-        <v>44635</v>
-      </c>
-      <c r="F682" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E682" s="29"/>
+      <c r="F682" s="53"/>
       <c r="G682" s="35"/>
       <c r="H682" s="29"/>
-      <c r="I682" s="19">
-        <v>1</v>
-      </c>
-      <c r="J682" s="20">
-        <v>0</v>
-      </c>
+      <c r="I682" s="19"/>
+      <c r="J682" s="20"/>
       <c r="K682" s="35"/>
     </row>
-    <row r="683" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A683" s="35"/>
-      <c r="B683" s="7" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C683" s="4" t="s">
-        <v>1277</v>
-      </c>
+      <c r="B683" s="9"/>
+      <c r="C683" s="10"/>
       <c r="D683" s="35"/>
-      <c r="E683" s="29">
-        <v>44635</v>
-      </c>
-      <c r="F683" s="53" t="s">
-        <v>597</v>
-      </c>
+      <c r="E683" s="30"/>
+      <c r="F683" s="54"/>
       <c r="G683" s="35"/>
-      <c r="H683" s="29"/>
-      <c r="I683" s="19">
-        <v>1</v>
-      </c>
-      <c r="J683" s="20">
-        <v>0</v>
-      </c>
+      <c r="H683" s="30"/>
+      <c r="I683" s="21"/>
+      <c r="J683" s="22"/>
       <c r="K683" s="35"/>
     </row>
     <row r="684" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A684" s="35"/>
       <c r="B684" s="7" t="s">
-        <v>1275</v>
+        <v>1334</v>
       </c>
       <c r="C684" s="4" t="s">
-        <v>1278</v>
+        <v>1333</v>
       </c>
       <c r="D684" s="35"/>
       <c r="E684" s="29">
-        <v>44636</v>
+        <v>44628</v>
       </c>
       <c r="F684" s="53" t="s">
         <v>597</v>
@@ -21741,10 +21741,10 @@
     <row r="756" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A756" s="35"/>
       <c r="B756" s="7" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C756" s="4" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="D756" s="35"/>
       <c r="E756" s="29">
@@ -21762,10 +21762,10 @@
     <row r="757" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A757" s="35"/>
       <c r="B757" s="7" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C757" s="4" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="D757" s="35"/>
       <c r="E757" s="29">
@@ -21783,10 +21783,10 @@
     <row r="758" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A758" s="35"/>
       <c r="B758" s="7" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C758" s="4" t="s">
         <v>1263</v>
-      </c>
-      <c r="C758" s="4" t="s">
-        <v>1264</v>
       </c>
       <c r="D758" s="35"/>
       <c r="E758" s="29">
@@ -21854,7 +21854,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F4:F6 F9 F49:F51 F62:F63 F65 F67:F69 F123:F129 F132:F137 F217:F221 F223:F227 F237:F239 F251 F323:F325 F442:F444 F468:F469 F562:F564 F566 F568:F572 F574:F577 F579:F580 F590:F595 F597:F599 F608:F609 F248:F249 F611 F664:F666 F584:F588 F694:F696 F190:F193 F740:F743 F529:F532 F457:F459 F195:F197 F745:F747 F120 F97 F56:F59 F391 F54 F139:F146 F383:F384 F349:F351 F241:F246 F601:F606 F471:F476 F93 F34:F36 F75:F76 F403:F404 F22:F23 F253:F272 F461:F466 F229:F235 F687:F692 F437:F440 F560 F478:F481 F613:F617 F406:F409 F78 F81:F89 F99:F118 F379:F381 F749:F754 F148:F188 F698:F738 F619:F662 F483:F527 F274:F321 F353:F377 F411:F435 F25:F32 F346 F557 F539:F550 F680 E677:F679 F401 F12:F20 F393:F399 F38:F44 F446:F452 F199:F210 F327:F339 F668:F676 F534:F538 F72 F212:F214 F756:F758 F341:F343 F682:F684 F552:F554 F454 F46" numberStoredAsText="1"/>
+    <ignoredError sqref="F4:F6 F9 F49:F51 F62:F63 F65 F67:F69 F123:F129 F132:F137 F217:F221 F223:F227 F237:F239 F251 F323:F325 F442:F444 F468:F469 F559:F561 F563 F565:F569 F571:F574 F576:F577 F587:F592 F594:F596 F605:F606 F248:F249 F608 F661:F663 F581:F585 F694:F696 F190:F193 F740:F743 F529:F532 F457:F459 F195:F197 F745:F747 F120 F97 F56:F59 F391 F54 F139:F146 F383:F384 F349:F351 F241:F246 F598:F603 F471:F476 F93 F34:F36 F75:F76 F403:F404 F22:F23 F253:F272 F461:F466 F229:F235 F687:F692 F437:F440 F557 F478:F481 F610:F614 F406:F409 F78 F81:F89 F99:F118 F379:F381 F749:F754 F148:F188 F698:F738 F616:F659 F483:F527 F274:F321 F353:F377 F411:F435 F25:F32 F346 F539:F550 F677 E674:F676 F401 F12:F20 F393:F399 F38:F44 F446:F452 F199:F210 F327:F339 F665:F673 F534:F538 F72 F212:F214 F756:F758 F341:F343 F679:F681 F552:F554 F454 F46 F684" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -21870,17 +21870,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="70"/>
-    <col min="2" max="6" width="4.28515625" style="72" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="72" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="70" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" style="70" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="70"/>
+    <col min="1" max="1" width="9.140625" style="61"/>
+    <col min="2" max="6" width="4.28515625" style="62" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="62" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="61" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" style="61" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="61"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="74" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C2" s="74"/>
       <c r="D2" s="74"/>
@@ -21890,7 +21890,7 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="74" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C3" s="74"/>
       <c r="D3" s="74"/>
@@ -21900,7 +21900,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="74" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C4" s="74"/>
       <c r="D4" s="74"/>
@@ -21910,7 +21910,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="74" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="74"/>
@@ -21920,7 +21920,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="74" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C6" s="74"/>
       <c r="D6" s="74"/>
@@ -21930,7 +21930,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="74" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C7" s="74"/>
       <c r="D7" s="74"/>
@@ -21938,43 +21938,43 @@
       <c r="F7" s="74"/>
       <c r="G7" s="74"/>
       <c r="H7" s="73" t="s">
+        <v>1306</v>
+      </c>
+      <c r="I7" s="73"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="I8" s="61" t="s">
         <v>1307</v>
       </c>
-      <c r="I7" s="73"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C8" s="71" t="s">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C9" s="72" t="s">
         <v>1305</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="I8" s="70" t="s">
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="I9" s="61" t="s">
         <v>1308</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>1306</v>
-      </c>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="I9" s="70" t="s">
-        <v>1309</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="74" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C10" s="74"/>
       <c r="D10" s="74"/>
@@ -21984,7 +21984,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="74" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C11" s="74"/>
       <c r="D11" s="74"/>
@@ -21994,7 +21994,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="74" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C12" s="74"/>
       <c r="D12" s="74"/>
@@ -22002,173 +22002,173 @@
       <c r="F12" s="74"/>
       <c r="G12" s="74"/>
       <c r="H12" s="73" t="s">
+        <v>1314</v>
+      </c>
+      <c r="I12" s="73"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C13" s="72" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="I13" s="61" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="I14" s="61" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C15" s="72" t="s">
         <v>1315</v>
       </c>
-      <c r="I12" s="73"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C13" s="71" t="s">
-        <v>1300</v>
-      </c>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="I13" s="70" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>1312</v>
-      </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="I14" s="70" t="s">
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="I15" s="61" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="I16" s="61" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D18" s="72" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="I18" s="61" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D19" s="72" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="I19" s="61" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C20" s="72" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="I20" s="61" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C21" s="72" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="I21" s="61" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C22" s="72" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="I22" s="61" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C23" s="72" t="s">
         <v>1330</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="I15" s="70" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>1317</v>
-      </c>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="I16" s="70" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>1321</v>
-      </c>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C18" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D18" s="71" t="s">
-        <v>1322</v>
-      </c>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="I18" s="70" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C19" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D19" s="71" t="s">
-        <v>1323</v>
-      </c>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="I19" s="70" t="s">
-        <v>1324</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C20" s="71" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="I20" s="70" t="s">
-        <v>1333</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C21" s="71" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="I21" s="70" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>1314</v>
-      </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="I22" s="70" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C23" s="71" t="s">
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="I23" s="61" t="s">
         <v>1331</v>
-      </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="I23" s="70" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="74" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="C24" s="74"/>
       <c r="D24" s="74"/>
@@ -22176,97 +22176,97 @@
       <c r="F24" s="74"/>
       <c r="G24" s="74"/>
       <c r="H24" s="73" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="I24" s="73"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="C25" s="71" t="s">
-        <v>1303</v>
-      </c>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
+      <c r="B25" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C26" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D26" s="71" t="s">
+      <c r="C26" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D26" s="72" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="I26" s="61" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D27" s="72" t="s">
         <v>1301</v>
       </c>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="I26" s="70" t="s">
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="I27" s="61" t="s">
         <v>1310</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C27" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D27" s="71" t="s">
-        <v>1302</v>
-      </c>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="I27" s="70" t="s">
-        <v>1311</v>
-      </c>
-    </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D28" s="72" t="s">
-        <v>1299</v>
-      </c>
-      <c r="E28" s="71" t="s">
-        <v>1313</v>
-      </c>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
+      <c r="D28" s="62" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E28" s="72" t="s">
+        <v>1312</v>
+      </c>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B24:G24"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 08 April 2022 14:44
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -5113,13 +5113,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5432,7 +5432,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C377" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C387" sqref="C387"/>
+      <selection pane="bottomRight" activeCell="C390" sqref="C390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -21987,80 +21987,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="74" t="s">
         <v>1286</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="74" t="s">
         <v>1287</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="74" t="s">
         <v>1288</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="74" t="s">
         <v>1289</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="74" t="s">
         <v>1290</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="74" t="s">
         <v>1291</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="74" t="s">
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="73" t="s">
         <v>1304</v>
       </c>
-      <c r="I7" s="74"/>
+      <c r="I7" s="73"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="72" t="s">
         <v>1302</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
       <c r="I8" s="61" t="s">
         <v>1305</v>
       </c>
@@ -22069,62 +22069,62 @@
       <c r="B9" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="72" t="s">
         <v>1303</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
       <c r="I9" s="61" t="s">
         <v>1306</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="74" t="s">
         <v>1292</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>1293</v>
       </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>1294</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="74" t="s">
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="73" t="s">
         <v>1312</v>
       </c>
-      <c r="I12" s="74"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="72" t="s">
         <v>1297</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
       <c r="I13" s="61" t="s">
         <v>1326</v>
       </c>
@@ -22133,13 +22133,13 @@
       <c r="B14" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="72" t="s">
         <v>1309</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
       <c r="I14" s="61" t="s">
         <v>1327</v>
       </c>
@@ -22148,13 +22148,13 @@
       <c r="B15" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="72" t="s">
         <v>1313</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
       <c r="I15" s="61" t="s">
         <v>1325</v>
       </c>
@@ -22163,13 +22163,13 @@
       <c r="B16" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="72" t="s">
         <v>1314</v>
       </c>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
       <c r="I16" s="61" t="s">
         <v>1315</v>
       </c>
@@ -22178,24 +22178,24 @@
       <c r="B17" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="72" t="s">
         <v>1318</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="72" t="s">
         <v>1319</v>
       </c>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
       <c r="I18" s="61" t="s">
         <v>1324</v>
       </c>
@@ -22204,12 +22204,12 @@
       <c r="C19" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="72" t="s">
         <v>1320</v>
       </c>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
       <c r="I19" s="61" t="s">
         <v>1321</v>
       </c>
@@ -22218,13 +22218,13 @@
       <c r="B20" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="72" t="s">
         <v>1322</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
       <c r="I20" s="61" t="s">
         <v>1330</v>
       </c>
@@ -22233,13 +22233,13 @@
       <c r="B21" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="72" t="s">
         <v>1316</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
       <c r="I21" s="61" t="s">
         <v>1317</v>
       </c>
@@ -22248,13 +22248,13 @@
       <c r="B22" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="72" t="s">
         <v>1311</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
       <c r="I22" s="61" t="s">
         <v>1323</v>
       </c>
@@ -22263,53 +22263,53 @@
       <c r="B23" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="72" t="s">
         <v>1328</v>
       </c>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
       <c r="I23" s="61" t="s">
         <v>1329</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="74" t="s">
         <v>1295</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="74" t="s">
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="73" t="s">
         <v>1301</v>
       </c>
-      <c r="I24" s="74"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="72" t="s">
         <v>1300</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="72" t="s">
         <v>1298</v>
       </c>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
       <c r="I26" s="61" t="s">
         <v>1307</v>
       </c>
@@ -22318,12 +22318,12 @@
       <c r="C27" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="D27" s="73" t="s">
+      <c r="D27" s="72" t="s">
         <v>1299</v>
       </c>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
       <c r="I27" s="61" t="s">
         <v>1308</v>
       </c>
@@ -22332,24 +22332,28 @@
       <c r="D28" s="62" t="s">
         <v>1296</v>
       </c>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="72" t="s">
         <v>1310</v>
       </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -22365,16 +22369,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 25 Mei 2022 19:23
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -5651,10 +5651,10 @@
   <dimension ref="A1:L806"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C430" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C148" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B440" sqref="B440"/>
+      <selection pane="bottomRight" activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Pertanggal 15 Juni 2022 11:51
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -5841,10 +5841,10 @@
   <dimension ref="A1:L846"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C421" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C436" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E430" sqref="E430"/>
+      <selection pane="bottomRight" activeCell="C439" sqref="C439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Pertanggal 17 Juni 2022 17:01
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4815,15 +4815,9 @@
     <t>Mendapatkan Daftar Perincian Uang Muka (Advance)</t>
   </si>
   <si>
-    <t>transaction.read.dataList.humanResource.getWorkerCurrentJobsPosition</t>
-  </si>
-  <si>
     <t>Mendapatkan Daftar Posisi Jabatan Pekerja saat Ini</t>
   </si>
   <si>
-    <t>dataPickList.humanResource.getWorkerCurrentJobsPosition</t>
-  </si>
-  <si>
     <t>Mendapatkan Data Picklist Posisi Jabatan Pekerja saat ini</t>
   </si>
   <si>
@@ -5023,6 +5017,12 @@
   </si>
   <si>
     <t>Mendapatkan Data Entitas Jenis Institusi</t>
+  </si>
+  <si>
+    <t>transaction.read.dataList.humanResource.getWorkerJobsPositionCurrent</t>
+  </si>
+  <si>
+    <t>dataPickList.humanResource.getWorkerJobsPositionCurrent</t>
   </si>
 </sst>
 </file>
@@ -5590,13 +5590,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5906,10 +5906,10 @@
   <dimension ref="A1:L859"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C436" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E448" sqref="E448"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6426,10 +6426,10 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
       <c r="B26" s="7" t="s">
-        <v>1434</v>
+        <v>1501</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D26" s="35"/>
       <c r="E26" s="29">
@@ -6502,10 +6502,10 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
       <c r="B30" s="7" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D30" s="35"/>
       <c r="E30" s="29">
@@ -6523,10 +6523,10 @@
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D31" s="35"/>
       <c r="E31" s="29">
@@ -6544,10 +6544,10 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="7" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="D32" s="35"/>
       <c r="E32" s="29">
@@ -6565,10 +6565,10 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
       <c r="B33" s="7" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D33" s="35"/>
       <c r="E33" s="29">
@@ -6586,10 +6586,10 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="35"/>
       <c r="B34" s="7" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="D34" s="35"/>
       <c r="E34" s="29">
@@ -14964,10 +14964,10 @@
     <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="35"/>
       <c r="B426" s="7" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C426" s="4" t="s">
         <v>1470</v>
-      </c>
-      <c r="C426" s="4" t="s">
-        <v>1472</v>
       </c>
       <c r="D426" s="35"/>
       <c r="E426" s="29">
@@ -14985,10 +14985,10 @@
     <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="35"/>
       <c r="B427" s="7" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C427" s="4" t="s">
         <v>1471</v>
-      </c>
-      <c r="C427" s="4" t="s">
-        <v>1473</v>
       </c>
       <c r="D427" s="35"/>
       <c r="E427" s="29">
@@ -15019,10 +15019,10 @@
     <row r="429" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A429" s="35"/>
       <c r="B429" s="7" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="D429" s="35"/>
       <c r="E429" s="29">
@@ -15053,10 +15053,10 @@
     <row r="431" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A431" s="35"/>
       <c r="B431" s="7" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="D431" s="35"/>
       <c r="E431" s="29">
@@ -15074,10 +15074,10 @@
     <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" s="35"/>
       <c r="B432" s="7" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="D432" s="35"/>
       <c r="E432" s="29">
@@ -15108,10 +15108,10 @@
     <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="35"/>
       <c r="B434" s="7" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="C434" s="4" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="D434" s="35"/>
       <c r="E434" s="29">
@@ -15142,10 +15142,10 @@
     <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" s="35"/>
       <c r="B436" s="7" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="C436" s="4" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="D436" s="35"/>
       <c r="E436" s="29">
@@ -15163,10 +15163,10 @@
     <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" s="35"/>
       <c r="B437" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="C437" s="4" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="D437" s="35"/>
       <c r="E437" s="29">
@@ -15184,10 +15184,10 @@
     <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" s="35"/>
       <c r="B438" s="7" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C438" s="4" t="s">
         <v>1454</v>
-      </c>
-      <c r="C438" s="4" t="s">
-        <v>1456</v>
       </c>
       <c r="D438" s="35"/>
       <c r="E438" s="29">
@@ -15205,10 +15205,10 @@
     <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" s="35"/>
       <c r="B439" s="7" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="C439" s="4" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="D439" s="35"/>
       <c r="E439" s="29">
@@ -15226,10 +15226,10 @@
     <row r="440" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A440" s="35"/>
       <c r="B440" s="7" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C440" s="4" t="s">
         <v>1455</v>
-      </c>
-      <c r="C440" s="4" t="s">
-        <v>1457</v>
       </c>
       <c r="D440" s="35"/>
       <c r="E440" s="29">
@@ -15247,10 +15247,10 @@
     <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" s="35"/>
       <c r="B441" s="7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="C441" s="4" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="D441" s="35"/>
       <c r="E441" s="29">
@@ -15268,10 +15268,10 @@
     <row r="442" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A442" s="35"/>
       <c r="B442" s="7" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="C442" s="4" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="D442" s="35"/>
       <c r="E442" s="29">
@@ -15289,10 +15289,10 @@
     <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" s="35"/>
       <c r="B443" s="7" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="C443" s="4" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="D443" s="35"/>
       <c r="E443" s="29">
@@ -15310,10 +15310,10 @@
     <row r="444" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A444" s="35"/>
       <c r="B444" s="7" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="C444" s="4" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="D444" s="35"/>
       <c r="E444" s="29">
@@ -15331,10 +15331,10 @@
     <row r="445" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A445" s="35"/>
       <c r="B445" s="7" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="C445" s="4" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="D445" s="35"/>
       <c r="E445" s="29">
@@ -15352,10 +15352,10 @@
     <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" s="35"/>
       <c r="B446" s="7" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="C446" s="4" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="D446" s="35"/>
       <c r="E446" s="29">
@@ -15373,10 +15373,10 @@
     <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" s="35"/>
       <c r="B447" s="7" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="C447" s="4" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="D447" s="35"/>
       <c r="E447" s="29">
@@ -15394,10 +15394,10 @@
     <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" s="35"/>
       <c r="B448" s="7" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="C448" s="4" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="D448" s="35"/>
       <c r="E448" s="29">
@@ -15415,10 +15415,10 @@
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A449" s="35"/>
       <c r="B449" s="7" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="C449" s="4" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="D449" s="35"/>
       <c r="E449" s="29">
@@ -15436,10 +15436,10 @@
     <row r="450" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A450" s="35"/>
       <c r="B450" s="7" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="D450" s="35"/>
       <c r="E450" s="29">
@@ -15457,10 +15457,10 @@
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A451" s="35"/>
       <c r="B451" s="7" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="C451" s="4" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="D451" s="35"/>
       <c r="E451" s="29">
@@ -15491,10 +15491,10 @@
     <row r="453" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A453" s="35"/>
       <c r="B453" s="13" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="C453" s="4" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="D453" s="35"/>
       <c r="E453" s="29">
@@ -15519,10 +15519,10 @@
     <row r="454" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A454" s="35"/>
       <c r="B454" s="13" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="C454" s="4" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="D454" s="35"/>
       <c r="E454" s="29">
@@ -15560,10 +15560,10 @@
     <row r="456" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A456" s="35"/>
       <c r="B456" s="13" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="C456" s="4" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="D456" s="35"/>
       <c r="E456" s="29">
@@ -15588,10 +15588,10 @@
     <row r="457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A457" s="35"/>
       <c r="B457" s="13" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="C457" s="4" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="D457" s="35"/>
       <c r="E457" s="29">
@@ -15616,10 +15616,10 @@
     <row r="458" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A458" s="35"/>
       <c r="B458" s="13" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="C458" s="4" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="D458" s="35"/>
       <c r="E458" s="29">
@@ -15644,10 +15644,10 @@
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A459" s="35"/>
       <c r="B459" s="13" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="C459" s="4" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="D459" s="35"/>
       <c r="E459" s="29">
@@ -16217,10 +16217,10 @@
     <row r="489" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A489" s="35"/>
       <c r="B489" s="7" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C489" s="4" t="s">
         <v>1432</v>
-      </c>
-      <c r="C489" s="4" t="s">
-        <v>1433</v>
       </c>
       <c r="D489" s="35"/>
       <c r="E489" s="29">
@@ -24406,80 +24406,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="74" t="s">
         <v>1281</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="74" t="s">
         <v>1282</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="74" t="s">
         <v>1283</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="74" t="s">
         <v>1284</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="74" t="s">
         <v>1285</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="74" t="s">
         <v>1286</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="74" t="s">
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="I7" s="74"/>
+      <c r="I7" s="73"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="72" t="s">
         <v>1297</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
       <c r="I8" s="61" t="s">
         <v>1300</v>
       </c>
@@ -24488,62 +24488,62 @@
       <c r="B9" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="72" t="s">
         <v>1298</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
       <c r="I9" s="61" t="s">
         <v>1301</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="74" t="s">
         <v>1287</v>
       </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="72"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>1288</v>
       </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="74" t="s">
         <v>1289</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="74" t="s">
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="73" t="s">
         <v>1307</v>
       </c>
-      <c r="I12" s="74"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="72" t="s">
         <v>1292</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
       <c r="I13" s="61" t="s">
         <v>1321</v>
       </c>
@@ -24552,13 +24552,13 @@
       <c r="B14" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="72" t="s">
         <v>1304</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
       <c r="I14" s="61" t="s">
         <v>1322</v>
       </c>
@@ -24567,13 +24567,13 @@
       <c r="B15" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="72" t="s">
         <v>1308</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
       <c r="I15" s="61" t="s">
         <v>1320</v>
       </c>
@@ -24582,13 +24582,13 @@
       <c r="B16" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="72" t="s">
         <v>1309</v>
       </c>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
       <c r="I16" s="61" t="s">
         <v>1310</v>
       </c>
@@ -24597,24 +24597,24 @@
       <c r="B17" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="72" t="s">
         <v>1313</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="72" t="s">
         <v>1314</v>
       </c>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
       <c r="I18" s="61" t="s">
         <v>1319</v>
       </c>
@@ -24623,12 +24623,12 @@
       <c r="C19" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="72" t="s">
         <v>1315</v>
       </c>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
       <c r="I19" s="61" t="s">
         <v>1316</v>
       </c>
@@ -24637,13 +24637,13 @@
       <c r="B20" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="72" t="s">
         <v>1317</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
       <c r="I20" s="61" t="s">
         <v>1325</v>
       </c>
@@ -24652,13 +24652,13 @@
       <c r="B21" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="72" t="s">
         <v>1311</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
       <c r="I21" s="61" t="s">
         <v>1312</v>
       </c>
@@ -24667,13 +24667,13 @@
       <c r="B22" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="72" t="s">
         <v>1306</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
       <c r="I22" s="61" t="s">
         <v>1318</v>
       </c>
@@ -24682,53 +24682,53 @@
       <c r="B23" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="72" t="s">
         <v>1323</v>
       </c>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
       <c r="I23" s="61" t="s">
         <v>1324</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="74" t="s">
         <v>1290</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="74" t="s">
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="73" t="s">
         <v>1296</v>
       </c>
-      <c r="I24" s="74"/>
+      <c r="I24" s="73"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="72" t="s">
         <v>1295</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="72" t="s">
         <v>1293</v>
       </c>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
       <c r="I26" s="61" t="s">
         <v>1302</v>
       </c>
@@ -24737,12 +24737,12 @@
       <c r="C27" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="D27" s="73" t="s">
+      <c r="D27" s="72" t="s">
         <v>1294</v>
       </c>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
       <c r="I27" s="61" t="s">
         <v>1303</v>
       </c>
@@ -24751,24 +24751,28 @@
       <c r="D28" s="62" t="s">
         <v>1291</v>
       </c>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="72" t="s">
         <v>1305</v>
       </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -24784,16 +24788,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 28 Juli 2022 14:06 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -5238,99 +5238,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Mengeset Upload File Tunggal untuk </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Staging Area</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> berdasarkan ID </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Staging File</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mengeset Pemindahan </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Local Storage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>ke</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> CloudStorage</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">berdasarkan ID </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Staging File</t>
-    </r>
-  </si>
-  <si>
-    <t>fileHandling.upload.stagingArea.localStorage.setFiles</t>
-  </si>
-  <si>
-    <t>fileHandling.upload.stagingArea.cloudStorage.setFiles</t>
-  </si>
-  <si>
     <t>fileHandling.upload.stagingArea.cloudStorage.getFilesList</t>
   </si>
   <si>
@@ -5418,6 +5325,99 @@
         <family val="2"/>
       </rPr>
       <t>Cloud Storage</t>
+    </r>
+  </si>
+  <si>
+    <t>fileHandling.upload.stagingArea.localStorage.setFileThenCopyToCloudStorage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mengeset Upload File Tunggal untuk </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Staging Area</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ke </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Local Storage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> lalu mennyalinnya ke </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cloud Storage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> berdasarkan ID </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Staging File</t>
+    </r>
+  </si>
+  <si>
+    <t>fileHandling.upload.stagingArea.localStorage.deleteDirectory</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Menghapus Direktori di </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Local Storage</t>
     </r>
   </si>
 </sst>
@@ -6305,7 +6305,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomRight" activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7636,10 +7636,10 @@
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
       <c r="B68" s="7" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
       <c r="D68" s="35"/>
       <c r="E68" s="29">
@@ -7657,10 +7657,10 @@
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="35"/>
       <c r="B69" s="7" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="D69" s="35"/>
       <c r="E69" s="29">
@@ -7678,10 +7678,10 @@
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="35"/>
       <c r="B70" s="7" t="s">
-        <v>1609</v>
+        <v>1616</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>1607</v>
+        <v>1617</v>
       </c>
       <c r="D70" s="35"/>
       <c r="E70" s="29">
@@ -7699,10 +7699,10 @@
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="35"/>
       <c r="B71" s="7" t="s">
-        <v>1612</v>
+        <v>1608</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="D71" s="35"/>
       <c r="E71" s="29">
@@ -7720,10 +7720,10 @@
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="35"/>
       <c r="B72" s="7" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>1614</v>
+        <v>1610</v>
       </c>
       <c r="D72" s="35"/>
       <c r="E72" s="29">
@@ -7738,13 +7738,13 @@
       <c r="J72" s="20"/>
       <c r="K72" s="35"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A73" s="35"/>
       <c r="B73" s="7" t="s">
-        <v>1608</v>
+        <v>1614</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>1606</v>
+        <v>1615</v>
       </c>
       <c r="D73" s="35"/>
       <c r="E73" s="29">

</xml_diff>

<commit_message>
Update Pertanggal 15 September 2022 10:39 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -6374,13 +6374,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -6690,10 +6690,10 @@
   <dimension ref="A1:L953"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C484" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C514" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C490" sqref="C490"/>
+      <selection pane="bottomRight" activeCell="E526" sqref="E526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -17825,7 +17825,7 @@
       </c>
       <c r="D525" s="35"/>
       <c r="E525" s="29">
-        <v>44728</v>
+        <v>44819</v>
       </c>
       <c r="F525" s="53" t="s">
         <v>596</v>
@@ -27233,80 +27233,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="72" t="s">
         <v>1269</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="72" t="s">
         <v>1270</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="72" t="s">
         <v>1271</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="72" t="s">
         <v>1272</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="72" t="s">
         <v>1273</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="72" t="s">
         <v>1274</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="73" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="74" t="s">
         <v>1287</v>
       </c>
-      <c r="I7" s="73"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>1285</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
       <c r="I8" s="61" t="s">
         <v>1288</v>
       </c>
@@ -27315,62 +27315,62 @@
       <c r="B9" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="73" t="s">
         <v>1286</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="I9" s="61" t="s">
         <v>1289</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="72" t="s">
         <v>1275</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>1276</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="72" t="s">
         <v>1277</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="73" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="74" t="s">
         <v>1295</v>
       </c>
-      <c r="I12" s="73"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="73" t="s">
         <v>1280</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
       <c r="I13" s="61" t="s">
         <v>1309</v>
       </c>
@@ -27379,13 +27379,13 @@
       <c r="B14" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="73" t="s">
         <v>1292</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="61" t="s">
         <v>1310</v>
       </c>
@@ -27394,13 +27394,13 @@
       <c r="B15" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="73" t="s">
         <v>1296</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="I15" s="61" t="s">
         <v>1308</v>
       </c>
@@ -27409,13 +27409,13 @@
       <c r="B16" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="73" t="s">
         <v>1297</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
       <c r="I16" s="61" t="s">
         <v>1298</v>
       </c>
@@ -27424,24 +27424,24 @@
       <c r="B17" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="73" t="s">
         <v>1301</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="73" t="s">
         <v>1302</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
       <c r="I18" s="61" t="s">
         <v>1307</v>
       </c>
@@ -27450,12 +27450,12 @@
       <c r="C19" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="73" t="s">
         <v>1303</v>
       </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
       <c r="I19" s="61" t="s">
         <v>1304</v>
       </c>
@@ -27464,13 +27464,13 @@
       <c r="B20" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="73" t="s">
         <v>1305</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="I20" s="61" t="s">
         <v>1313</v>
       </c>
@@ -27479,13 +27479,13 @@
       <c r="B21" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
       <c r="I21" s="61" t="s">
         <v>1300</v>
       </c>
@@ -27494,13 +27494,13 @@
       <c r="B22" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="73" t="s">
         <v>1294</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
       <c r="I22" s="61" t="s">
         <v>1306</v>
       </c>
@@ -27509,53 +27509,53 @@
       <c r="B23" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="73" t="s">
         <v>1311</v>
       </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="I23" s="61" t="s">
         <v>1312</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="73" t="s">
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="74" t="s">
         <v>1284</v>
       </c>
-      <c r="I24" s="73"/>
+      <c r="I24" s="74"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="73" t="s">
         <v>1283</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="73" t="s">
         <v>1281</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
       <c r="I26" s="61" t="s">
         <v>1290</v>
       </c>
@@ -27564,12 +27564,12 @@
       <c r="C27" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="73" t="s">
         <v>1282</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="I27" s="61" t="s">
         <v>1291</v>
       </c>
@@ -27578,28 +27578,24 @@
       <c r="D28" s="62" t="s">
         <v>1279</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="73" t="s">
         <v>1293</v>
       </c>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -27615,12 +27611,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 30 September 2022 18:24 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -5950,9 +5950,6 @@
     <t>Mendapatkan Data Entitas Versi Material Produk Rakitan atau Material Produk Komponen</t>
   </si>
   <si>
-    <t>Mendapatkan Data Entitas Orang atau Cabang Institusi</t>
-  </si>
-  <si>
     <t>transaction.update.finance.setInvoiceSupplierAdditionalCost</t>
   </si>
   <si>
@@ -6092,6 +6089,22 @@
   </si>
   <si>
     <t>Mendapatkan Data Entitas Perincian Perintah Pembayaran</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mendapatkan Data Entitas Entity : 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="5"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">     - Orang atau 
+     - Cabang Institusi</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6981,10 +6994,10 @@
   <dimension ref="A1:L1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C486" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C522" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C495" sqref="C495"/>
+      <selection pane="bottomRight" activeCell="C523" sqref="C523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -10606,10 +10619,10 @@
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="35"/>
       <c r="B189" s="7" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C189" s="14" t="s">
         <v>1728</v>
-      </c>
-      <c r="C189" s="14" t="s">
-        <v>1729</v>
       </c>
       <c r="D189" s="35"/>
       <c r="E189" s="29">
@@ -10686,10 +10699,10 @@
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="35"/>
       <c r="B193" s="7" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D193" s="35"/>
       <c r="E193" s="29">
@@ -10707,10 +10720,10 @@
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="35"/>
       <c r="B194" s="7" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D194" s="35"/>
       <c r="E194" s="29">
@@ -10728,10 +10741,10 @@
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="35"/>
       <c r="B195" s="7" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D195" s="35"/>
       <c r="E195" s="29">
@@ -17374,10 +17387,10 @@
     <row r="493" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A493" s="35"/>
       <c r="B493" s="7" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C493" s="4" t="s">
         <v>1742</v>
-      </c>
-      <c r="C493" s="4" t="s">
-        <v>1743</v>
       </c>
       <c r="D493" s="35"/>
       <c r="E493" s="29">
@@ -17395,10 +17408,10 @@
     <row r="494" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A494" s="35"/>
       <c r="B494" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C494" s="4" t="s">
         <v>1749</v>
-      </c>
-      <c r="C494" s="4" t="s">
-        <v>1750</v>
       </c>
       <c r="D494" s="35"/>
       <c r="E494" s="29">
@@ -17416,10 +17429,10 @@
     <row r="495" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A495" s="35"/>
       <c r="B495" s="7" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C495" s="4" t="s">
         <v>1751</v>
-      </c>
-      <c r="C495" s="4" t="s">
-        <v>1752</v>
       </c>
       <c r="D495" s="35"/>
       <c r="E495" s="29">
@@ -17437,10 +17450,10 @@
     <row r="496" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A496" s="35"/>
       <c r="B496" s="7" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D496" s="35"/>
       <c r="E496" s="29">
@@ -17458,10 +17471,10 @@
     <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497" s="35"/>
       <c r="B497" s="7" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="C497" s="4" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D497" s="35"/>
       <c r="E497" s="29">
@@ -17479,10 +17492,10 @@
     <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498" s="35"/>
       <c r="B498" s="7" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D498" s="35"/>
       <c r="E498" s="29">
@@ -17500,10 +17513,10 @@
     <row r="499" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A499" s="35"/>
       <c r="B499" s="7" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D499" s="35"/>
       <c r="E499" s="29">
@@ -17521,10 +17534,10 @@
     <row r="500" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A500" s="35"/>
       <c r="B500" s="7" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D500" s="35"/>
       <c r="E500" s="29">
@@ -17974,7 +17987,7 @@
         <v>1507</v>
       </c>
       <c r="C522" s="4" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D522" s="35"/>
       <c r="E522" s="29">
@@ -18115,13 +18128,13 @@
       <c r="J528" s="20"/>
       <c r="K528" s="35"/>
     </row>
-    <row r="529" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A529" s="35"/>
       <c r="B529" s="7" t="s">
         <v>1699</v>
       </c>
       <c r="C529" s="4" t="s">
-        <v>1719</v>
+        <v>1752</v>
       </c>
       <c r="D529" s="35"/>
       <c r="E529" s="29">
@@ -26928,10 +26941,10 @@
     <row r="927" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A927" s="35"/>
       <c r="B927" s="7" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C927" s="14" t="s">
         <v>1720</v>
-      </c>
-      <c r="C927" s="14" t="s">
-        <v>1721</v>
       </c>
       <c r="D927" s="35"/>
       <c r="E927" s="29">
@@ -26970,10 +26983,10 @@
     <row r="929" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A929" s="35"/>
       <c r="B929" s="7" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C929" s="14" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D929" s="35"/>
       <c r="E929" s="29">
@@ -26991,10 +27004,10 @@
     <row r="930" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A930" s="35"/>
       <c r="B930" s="7" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="C930" s="14" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D930" s="35"/>
       <c r="E930" s="29">
@@ -27012,10 +27025,10 @@
     <row r="931" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A931" s="35"/>
       <c r="B931" s="7" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="C931" s="14" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="D931" s="35"/>
       <c r="E931" s="29">

</xml_diff>

<commit_message>
Update Pertanggal 7 Oktober 2022 10:29 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -6022,12 +6022,6 @@
     <t>Mendapatkan Data Entitas Pendanaan Pembayaran</t>
   </si>
   <si>
-    <t>transaction.read.dataEntities.finance.getUnderlying</t>
-  </si>
-  <si>
-    <t>transaction.read.dataEntities.finance.getUnderlyingDetail</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Mendapatkan Data Entitas Dokumen : 
 </t>
@@ -6183,6 +6177,12 @@
   </si>
   <si>
     <t>Menginstruksikan Server Database : Vacuum dan Analyze Ulang seluruh Tabel yang ada</t>
+  </si>
+  <si>
+    <t>transaction.read.dataEntities.finance.getUnderlyingPaymentDetail</t>
+  </si>
+  <si>
+    <t>transaction.read.dataEntities.finance.getUnderlyingPaymentInstructionDetail</t>
   </si>
 </sst>
 </file>
@@ -6756,13 +6756,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -7072,10 +7072,10 @@
   <dimension ref="A1:L1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C502" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F99" sqref="F99"/>
+      <selection pane="bottomRight" activeCell="B512" sqref="B512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8968,10 +8968,10 @@
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="35"/>
       <c r="B98" s="7" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="D98" s="35"/>
       <c r="E98" s="29">
@@ -10710,10 +10710,10 @@
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="35"/>
       <c r="B190" s="7" t="s">
+        <v>1759</v>
+      </c>
+      <c r="C190" s="14" t="s">
         <v>1761</v>
-      </c>
-      <c r="C190" s="14" t="s">
-        <v>1763</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="29">
@@ -10731,10 +10731,10 @@
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="35"/>
       <c r="B191" s="7" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C191" s="14" t="s">
         <v>1762</v>
-      </c>
-      <c r="C191" s="14" t="s">
-        <v>1764</v>
       </c>
       <c r="D191" s="35"/>
       <c r="E191" s="29">
@@ -10929,10 +10929,10 @@
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="35"/>
       <c r="B201" s="7" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="C201" s="14" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="D201" s="35"/>
       <c r="E201" s="29">
@@ -16007,10 +16007,10 @@
     <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="35"/>
       <c r="B427" s="7" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="D427" s="35"/>
       <c r="E427" s="29">
@@ -17082,10 +17082,10 @@
     <row r="474" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A474" s="35"/>
       <c r="B474" s="7" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="D474" s="35"/>
       <c r="E474" s="29">
@@ -17512,10 +17512,10 @@
     <row r="496" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A496" s="35"/>
       <c r="B496" s="7" t="s">
+        <v>1767</v>
+      </c>
+      <c r="C496" s="4" t="s">
         <v>1769</v>
-      </c>
-      <c r="C496" s="4" t="s">
-        <v>1771</v>
       </c>
       <c r="D496" s="35"/>
       <c r="E496" s="29">
@@ -17533,10 +17533,10 @@
     <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497" s="35"/>
       <c r="B497" s="7" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C497" s="4" t="s">
         <v>1770</v>
-      </c>
-      <c r="C497" s="4" t="s">
-        <v>1772</v>
       </c>
       <c r="D497" s="35"/>
       <c r="E497" s="29">
@@ -17680,10 +17680,10 @@
     <row r="504" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A504" s="35"/>
       <c r="B504" s="7" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="C504" s="4" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="D504" s="35"/>
       <c r="E504" s="29">
@@ -17701,10 +17701,10 @@
     <row r="505" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A505" s="35"/>
       <c r="B505" s="7" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="C505" s="4" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="D505" s="35"/>
       <c r="E505" s="29">
@@ -17722,10 +17722,10 @@
     <row r="506" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A506" s="35"/>
       <c r="B506" s="7" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
       <c r="C506" s="4" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="D506" s="35"/>
       <c r="E506" s="29">
@@ -17806,10 +17806,10 @@
     <row r="510" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A510" s="35"/>
       <c r="B510" s="7" t="s">
+        <v>1777</v>
+      </c>
+      <c r="C510" s="4" t="s">
         <v>1743</v>
-      </c>
-      <c r="C510" s="4" t="s">
-        <v>1745</v>
       </c>
       <c r="D510" s="35"/>
       <c r="E510" s="29">
@@ -17827,10 +17827,10 @@
     <row r="511" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A511" s="35"/>
       <c r="B511" s="7" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C511" s="4" t="s">
         <v>1744</v>
-      </c>
-      <c r="C511" s="4" t="s">
-        <v>1746</v>
       </c>
       <c r="D511" s="35"/>
       <c r="E511" s="29">
@@ -17929,10 +17929,10 @@
     <row r="517" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A517" s="35"/>
       <c r="B517" s="7" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="C517" s="4" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="D517" s="35"/>
       <c r="E517" s="29">
@@ -18301,7 +18301,7 @@
         <v>1507</v>
       </c>
       <c r="C534" s="4" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="D534" s="35"/>
       <c r="E534" s="29">
@@ -18448,7 +18448,7 @@
         <v>1699</v>
       </c>
       <c r="C541" s="4" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="D541" s="35"/>
       <c r="E541" s="29">
@@ -27234,10 +27234,10 @@
     <row r="938" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A938" s="35"/>
       <c r="B938" s="7" t="s">
+        <v>1763</v>
+      </c>
+      <c r="C938" s="14" t="s">
         <v>1765</v>
-      </c>
-      <c r="C938" s="14" t="s">
-        <v>1767</v>
       </c>
       <c r="D938" s="35"/>
       <c r="E938" s="29">
@@ -27255,10 +27255,10 @@
     <row r="939" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A939" s="35"/>
       <c r="B939" s="7" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C939" s="14" t="s">
         <v>1766</v>
-      </c>
-      <c r="C939" s="14" t="s">
-        <v>1768</v>
       </c>
       <c r="D939" s="35"/>
       <c r="E939" s="29">
@@ -27415,10 +27415,10 @@
     <row r="947" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A947" s="35"/>
       <c r="B947" s="7" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="C947" s="14" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="D947" s="35"/>
       <c r="E947" s="29">
@@ -28916,80 +28916,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="72" t="s">
         <v>1267</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="72" t="s">
         <v>1268</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="72" t="s">
         <v>1269</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="72" t="s">
         <v>1270</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="72" t="s">
         <v>1271</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="72" t="s">
         <v>1272</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="73" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="74" t="s">
         <v>1285</v>
       </c>
-      <c r="I7" s="73"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>1283</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
       <c r="I8" s="61" t="s">
         <v>1286</v>
       </c>
@@ -28998,62 +28998,62 @@
       <c r="B9" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="73" t="s">
         <v>1284</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="I9" s="61" t="s">
         <v>1287</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="72" t="s">
         <v>1273</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>1274</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="72" t="s">
         <v>1275</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="73" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="74" t="s">
         <v>1293</v>
       </c>
-      <c r="I12" s="73"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="73" t="s">
         <v>1278</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
       <c r="I13" s="61" t="s">
         <v>1307</v>
       </c>
@@ -29062,13 +29062,13 @@
       <c r="B14" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="73" t="s">
         <v>1290</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="61" t="s">
         <v>1308</v>
       </c>
@@ -29077,13 +29077,13 @@
       <c r="B15" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="73" t="s">
         <v>1294</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="I15" s="61" t="s">
         <v>1306</v>
       </c>
@@ -29092,13 +29092,13 @@
       <c r="B16" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="73" t="s">
         <v>1295</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
       <c r="I16" s="61" t="s">
         <v>1296</v>
       </c>
@@ -29107,24 +29107,24 @@
       <c r="B17" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="73" t="s">
         <v>1300</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
       <c r="I18" s="61" t="s">
         <v>1305</v>
       </c>
@@ -29133,12 +29133,12 @@
       <c r="C19" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="73" t="s">
         <v>1301</v>
       </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
       <c r="I19" s="61" t="s">
         <v>1302</v>
       </c>
@@ -29147,13 +29147,13 @@
       <c r="B20" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="73" t="s">
         <v>1303</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="I20" s="61" t="s">
         <v>1311</v>
       </c>
@@ -29162,13 +29162,13 @@
       <c r="B21" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="73" t="s">
         <v>1297</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
       <c r="I21" s="61" t="s">
         <v>1298</v>
       </c>
@@ -29177,13 +29177,13 @@
       <c r="B22" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="73" t="s">
         <v>1292</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
       <c r="I22" s="61" t="s">
         <v>1304</v>
       </c>
@@ -29192,53 +29192,53 @@
       <c r="B23" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="73" t="s">
         <v>1309</v>
       </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="I23" s="61" t="s">
         <v>1310</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="72" t="s">
         <v>1276</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="73" t="s">
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="74" t="s">
         <v>1282</v>
       </c>
-      <c r="I24" s="73"/>
+      <c r="I24" s="74"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="73" t="s">
         <v>1281</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="73" t="s">
         <v>1279</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
       <c r="I26" s="61" t="s">
         <v>1288</v>
       </c>
@@ -29247,12 +29247,12 @@
       <c r="C27" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="73" t="s">
         <v>1280</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="I27" s="61" t="s">
         <v>1289</v>
       </c>
@@ -29261,28 +29261,24 @@
       <c r="D28" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="73" t="s">
         <v>1291</v>
       </c>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -29298,12 +29294,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 12 Oktober 2022 11:22 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -6864,13 +6864,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -29386,80 +29386,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="72" t="s">
         <v>1267</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="72" t="s">
         <v>1268</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="72" t="s">
         <v>1269</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="72" t="s">
         <v>1270</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="72" t="s">
         <v>1271</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="72" t="s">
         <v>1272</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="73" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="74" t="s">
         <v>1285</v>
       </c>
-      <c r="I7" s="73"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="73" t="s">
         <v>1283</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
       <c r="I8" s="61" t="s">
         <v>1286</v>
       </c>
@@ -29468,62 +29468,62 @@
       <c r="B9" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="73" t="s">
         <v>1284</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="I9" s="61" t="s">
         <v>1287</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="72" t="s">
         <v>1273</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>1274</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="72" t="s">
         <v>1275</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="73" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="74" t="s">
         <v>1293</v>
       </c>
-      <c r="I12" s="73"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="73" t="s">
         <v>1278</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
       <c r="I13" s="61" t="s">
         <v>1307</v>
       </c>
@@ -29532,13 +29532,13 @@
       <c r="B14" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="73" t="s">
         <v>1290</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="61" t="s">
         <v>1308</v>
       </c>
@@ -29547,13 +29547,13 @@
       <c r="B15" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="73" t="s">
         <v>1294</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="I15" s="61" t="s">
         <v>1306</v>
       </c>
@@ -29562,13 +29562,13 @@
       <c r="B16" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="73" t="s">
         <v>1295</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
       <c r="I16" s="61" t="s">
         <v>1296</v>
       </c>
@@ -29577,24 +29577,24 @@
       <c r="B17" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="73" t="s">
         <v>1300</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
       <c r="I18" s="61" t="s">
         <v>1305</v>
       </c>
@@ -29603,12 +29603,12 @@
       <c r="C19" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="73" t="s">
         <v>1301</v>
       </c>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
       <c r="I19" s="61" t="s">
         <v>1302</v>
       </c>
@@ -29617,13 +29617,13 @@
       <c r="B20" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="73" t="s">
         <v>1303</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="I20" s="61" t="s">
         <v>1311</v>
       </c>
@@ -29632,13 +29632,13 @@
       <c r="B21" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="73" t="s">
         <v>1297</v>
       </c>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
       <c r="I21" s="61" t="s">
         <v>1298</v>
       </c>
@@ -29647,13 +29647,13 @@
       <c r="B22" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C22" s="72" t="s">
+      <c r="C22" s="73" t="s">
         <v>1292</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
       <c r="I22" s="61" t="s">
         <v>1304</v>
       </c>
@@ -29662,53 +29662,53 @@
       <c r="B23" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="73" t="s">
         <v>1309</v>
       </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="I23" s="61" t="s">
         <v>1310</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="72" t="s">
         <v>1276</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="73" t="s">
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="74" t="s">
         <v>1282</v>
       </c>
-      <c r="I24" s="73"/>
+      <c r="I24" s="74"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="C25" s="72" t="s">
+      <c r="C25" s="73" t="s">
         <v>1281</v>
       </c>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D26" s="72" t="s">
+      <c r="D26" s="73" t="s">
         <v>1279</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
       <c r="I26" s="61" t="s">
         <v>1288</v>
       </c>
@@ -29717,12 +29717,12 @@
       <c r="C27" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="D27" s="72" t="s">
+      <c r="D27" s="73" t="s">
         <v>1280</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="I27" s="61" t="s">
         <v>1289</v>
       </c>
@@ -29731,28 +29731,24 @@
       <c r="D28" s="62" t="s">
         <v>1277</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E28" s="73" t="s">
         <v>1291</v>
       </c>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -29768,12 +29764,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 1 November 2022 11:45 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -8048,13 +8048,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -31665,80 +31665,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="75" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="75" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="75" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="75" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="75" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="75" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="75" t="s">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="75"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="73" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
       <c r="I8" s="61" t="s">
         <v>1276</v>
       </c>
@@ -31747,62 +31747,62 @@
       <c r="B9" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="I9" s="61" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="75" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="75" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="75" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="75" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="74" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="75"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="73" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
       <c r="I13" s="61" t="s">
         <v>1297</v>
       </c>
@@ -31811,13 +31811,13 @@
       <c r="B14" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="73" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="61" t="s">
         <v>1298</v>
       </c>
@@ -31826,13 +31826,13 @@
       <c r="B15" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="I15" s="61" t="s">
         <v>1296</v>
       </c>
@@ -31841,13 +31841,13 @@
       <c r="B16" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
       <c r="I16" s="61" t="s">
         <v>1286</v>
       </c>
@@ -31856,24 +31856,24 @@
       <c r="B17" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="73" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="73" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
       <c r="I18" s="61" t="s">
         <v>1295</v>
       </c>
@@ -31882,12 +31882,12 @@
       <c r="C19" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="74" t="s">
+      <c r="D19" s="73" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
       <c r="I19" s="61" t="s">
         <v>1292</v>
       </c>
@@ -31896,13 +31896,13 @@
       <c r="B20" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="73" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="I20" s="61" t="s">
         <v>1301</v>
       </c>
@@ -31911,13 +31911,13 @@
       <c r="B21" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="73" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
       <c r="I21" s="61" t="s">
         <v>1288</v>
       </c>
@@ -31926,13 +31926,13 @@
       <c r="B22" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="73" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
       <c r="I22" s="61" t="s">
         <v>1294</v>
       </c>
@@ -31941,53 +31941,53 @@
       <c r="B23" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="I23" s="61" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="75" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="75" t="s">
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="74" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="75"/>
+      <c r="I24" s="74"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="73" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="73" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
       <c r="I26" s="61" t="s">
         <v>1278</v>
       </c>
@@ -31996,12 +31996,12 @@
       <c r="C27" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="73" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="I27" s="61" t="s">
         <v>1279</v>
       </c>
@@ -32010,24 +32010,28 @@
       <c r="D28" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="73" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -32043,16 +32047,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 27 Januari 2023 11:17 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -7978,16 +7978,16 @@
     <t>Mendapatkan Data Picklist App Object - Work Flow Path</t>
   </si>
   <si>
-    <t>dataPickList.sysConfig.getBusinessDocumentWorkFlowPath</t>
-  </si>
-  <si>
-    <t>Mendapatkan Data Picklist Work Flow Path Dokumen Bisnis</t>
-  </si>
-  <si>
-    <t>transaction.read.dataList.sysConfig.getBusinessDocumentWorkFlowPath</t>
-  </si>
-  <si>
-    <t>Mendapatkan Daftar Work Flow Path Dokumen Bisnis</t>
+    <t>transaction.read.dataList.sysConfig.getBusinessDocumentTypeWorkFlowPath</t>
+  </si>
+  <si>
+    <t>dataPickList.sysConfig.getBusinessDocumentTypeWorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Picklist Work Flow Path untuk Jenis Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Work Flow Path untuk Jenis Dokumen Bisnis</t>
   </si>
 </sst>
 </file>
@@ -8591,13 +8591,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -8912,10 +8912,10 @@
   <dimension ref="A1:L1176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C695" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C694" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B703" sqref="B703"/>
+      <selection pane="bottomRight" activeCell="C704" sqref="C704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9389,10 +9389,10 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="7" t="s">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="29">
@@ -23532,7 +23532,7 @@
     <row r="703" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A703" s="35"/>
       <c r="B703" s="7" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="C703" s="4" t="s">
         <v>2011</v>
@@ -33745,80 +33745,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="75" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="75" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="75" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="75" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="75" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="75" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="75" t="s">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="75"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="73" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
       <c r="I8" s="61" t="s">
         <v>1276</v>
       </c>
@@ -33827,62 +33827,62 @@
       <c r="B9" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="I9" s="61" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="75" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="75" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="75" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="75" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="74" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="75"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="73" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
       <c r="I13" s="61" t="s">
         <v>1297</v>
       </c>
@@ -33891,13 +33891,13 @@
       <c r="B14" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="73" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="61" t="s">
         <v>1298</v>
       </c>
@@ -33906,13 +33906,13 @@
       <c r="B15" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="I15" s="61" t="s">
         <v>1296</v>
       </c>
@@ -33921,13 +33921,13 @@
       <c r="B16" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
       <c r="I16" s="61" t="s">
         <v>1286</v>
       </c>
@@ -33936,24 +33936,24 @@
       <c r="B17" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="73" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="73" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
       <c r="I18" s="61" t="s">
         <v>1295</v>
       </c>
@@ -33962,12 +33962,12 @@
       <c r="C19" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="74" t="s">
+      <c r="D19" s="73" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
       <c r="I19" s="61" t="s">
         <v>1292</v>
       </c>
@@ -33976,13 +33976,13 @@
       <c r="B20" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="73" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="I20" s="61" t="s">
         <v>1301</v>
       </c>
@@ -33991,13 +33991,13 @@
       <c r="B21" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="73" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
       <c r="I21" s="61" t="s">
         <v>1288</v>
       </c>
@@ -34006,13 +34006,13 @@
       <c r="B22" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="73" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
       <c r="I22" s="61" t="s">
         <v>1294</v>
       </c>
@@ -34021,53 +34021,53 @@
       <c r="B23" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="I23" s="61" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="75" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="75" t="s">
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="74" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="75"/>
+      <c r="I24" s="74"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="73" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="73" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
       <c r="I26" s="61" t="s">
         <v>1278</v>
       </c>
@@ -34076,12 +34076,12 @@
       <c r="C27" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="73" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="I27" s="61" t="s">
         <v>1279</v>
       </c>
@@ -34090,24 +34090,28 @@
       <c r="D28" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="73" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -34123,16 +34127,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 14 Februari 2023 11:07 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3069" uniqueCount="2029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="2036">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8039,6 +8039,119 @@
   </si>
   <si>
     <t>Mendapatkan Data Entitas Log Riwayat Jalur Work Flow Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.getApprovementHistoryList</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.getCurrentAndNextStage</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.general.getBusinessDocumentTypeWorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Tahapan Saat Ini dan Tahapan Selanjutnya pada WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Riwayat Persetujuan WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>Mendapatkan Jalur WorkFlow untuk Jenis Dokumen Bisnis</t>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>SER</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>CTION.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>OCUMENT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>ORK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>LOW</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -8642,13 +8755,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -8960,13 +9073,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1186"/>
+  <dimension ref="A1:L1193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C680" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C1180" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C697" sqref="C697"/>
+      <selection pane="bottomRight" activeCell="B1183" sqref="B1183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -33969,48 +34082,165 @@
       <c r="J1182" s="20"/>
       <c r="K1182" s="35"/>
     </row>
-    <row r="1183" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1183" s="35"/>
-      <c r="B1183" s="8"/>
-      <c r="C1183" s="6"/>
+      <c r="B1183" s="7"/>
+      <c r="C1183" s="4"/>
       <c r="D1183" s="35"/>
-      <c r="E1183" s="33"/>
-      <c r="F1183" s="56"/>
+      <c r="E1183" s="29"/>
+      <c r="F1183" s="53"/>
       <c r="G1183" s="35"/>
-      <c r="H1183" s="33"/>
-      <c r="I1183" s="25"/>
-      <c r="J1183" s="26"/>
+      <c r="H1183" s="29"/>
+      <c r="I1183" s="19"/>
+      <c r="J1183" s="20"/>
       <c r="K1183" s="35"/>
     </row>
     <row r="1184" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1184" s="35"/>
-      <c r="B1184" s="38"/>
-      <c r="C1184" s="39"/>
+      <c r="B1184" s="9"/>
+      <c r="C1184" s="10"/>
       <c r="D1184" s="35"/>
-      <c r="E1184" s="40"/>
-      <c r="F1184" s="50"/>
+      <c r="E1184" s="30"/>
+      <c r="F1184" s="54"/>
       <c r="G1184" s="35"/>
-      <c r="H1184" s="40"/>
-      <c r="I1184" s="41"/>
-      <c r="J1184" s="41"/>
+      <c r="H1184" s="30"/>
+      <c r="I1184" s="21"/>
+      <c r="J1184" s="22"/>
       <c r="K1184" s="35"/>
     </row>
-    <row r="1186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1185" s="35"/>
+      <c r="B1185" s="63" t="s">
+        <v>2035</v>
+      </c>
+      <c r="C1185" s="10"/>
+      <c r="D1185" s="35"/>
+      <c r="E1185" s="30"/>
+      <c r="F1185" s="54"/>
+      <c r="G1185" s="35"/>
+      <c r="H1185" s="30"/>
+      <c r="I1185" s="21"/>
+      <c r="J1185" s="22"/>
+      <c r="K1185" s="35"/>
+    </row>
+    <row r="1186" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1186" s="35"/>
-      <c r="B1186" s="7" t="s">
+      <c r="B1186" s="9"/>
+      <c r="C1186" s="10"/>
+      <c r="D1186" s="35"/>
+      <c r="E1186" s="30"/>
+      <c r="F1186" s="54"/>
+      <c r="G1186" s="35"/>
+      <c r="H1186" s="30"/>
+      <c r="I1186" s="21"/>
+      <c r="J1186" s="22"/>
+      <c r="K1186" s="35"/>
+    </row>
+    <row r="1187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1187" s="35"/>
+      <c r="B1187" s="7" t="s">
+        <v>2029</v>
+      </c>
+      <c r="C1187" s="4" t="s">
+        <v>2033</v>
+      </c>
+      <c r="D1187" s="35"/>
+      <c r="E1187" s="29">
+        <v>44971</v>
+      </c>
+      <c r="F1187" s="53" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1187" s="35"/>
+      <c r="H1187" s="29"/>
+      <c r="I1187" s="19"/>
+      <c r="J1187" s="20"/>
+      <c r="K1187" s="35"/>
+    </row>
+    <row r="1188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1188" s="35"/>
+      <c r="B1188" s="7" t="s">
+        <v>2030</v>
+      </c>
+      <c r="C1188" s="4" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D1188" s="35"/>
+      <c r="E1188" s="29">
+        <v>44971</v>
+      </c>
+      <c r="F1188" s="53" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1188" s="35"/>
+      <c r="H1188" s="29"/>
+      <c r="I1188" s="19"/>
+      <c r="J1188" s="20"/>
+      <c r="K1188" s="35"/>
+    </row>
+    <row r="1189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1189" s="35"/>
+      <c r="B1189" s="7" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C1189" s="4" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D1189" s="35"/>
+      <c r="E1189" s="29">
+        <v>44971</v>
+      </c>
+      <c r="F1189" s="53" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1189" s="35"/>
+      <c r="H1189" s="29"/>
+      <c r="I1189" s="19"/>
+      <c r="J1189" s="20"/>
+      <c r="K1189" s="35"/>
+    </row>
+    <row r="1190" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1190" s="35"/>
+      <c r="B1190" s="8"/>
+      <c r="C1190" s="6"/>
+      <c r="D1190" s="35"/>
+      <c r="E1190" s="33"/>
+      <c r="F1190" s="56"/>
+      <c r="G1190" s="35"/>
+      <c r="H1190" s="33"/>
+      <c r="I1190" s="25"/>
+      <c r="J1190" s="26"/>
+      <c r="K1190" s="35"/>
+    </row>
+    <row r="1191" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1191" s="35"/>
+      <c r="B1191" s="38"/>
+      <c r="C1191" s="39"/>
+      <c r="D1191" s="35"/>
+      <c r="E1191" s="40"/>
+      <c r="F1191" s="50"/>
+      <c r="G1191" s="35"/>
+      <c r="H1191" s="40"/>
+      <c r="I1191" s="41"/>
+      <c r="J1191" s="41"/>
+      <c r="K1191" s="35"/>
+    </row>
+    <row r="1193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1193" s="35"/>
+      <c r="B1193" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="C1186" s="4" t="s">
+      <c r="C1193" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="D1186" s="35"/>
-      <c r="E1186" s="29"/>
-      <c r="F1186" s="53"/>
-      <c r="G1186" s="35"/>
-      <c r="H1186" s="29"/>
-      <c r="I1186" s="19"/>
-      <c r="J1186" s="20"/>
-      <c r="K1186" s="35"/>
+      <c r="D1193" s="35"/>
+      <c r="E1193" s="29"/>
+      <c r="F1193" s="53"/>
+      <c r="G1193" s="35"/>
+      <c r="H1193" s="29"/>
+      <c r="I1193" s="19"/>
+      <c r="J1193" s="20"/>
+      <c r="K1193" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -34047,80 +34277,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="73" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="73" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="73" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="74" t="s">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="75" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="74"/>
+      <c r="I7" s="75"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="74" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
       <c r="I8" s="61" t="s">
         <v>1276</v>
       </c>
@@ -34129,62 +34359,62 @@
       <c r="B9" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="74" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
       <c r="I9" s="61" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="73" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="73" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="73" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="74" t="s">
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="75" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="74"/>
+      <c r="I12" s="75"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="74" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
       <c r="I13" s="61" t="s">
         <v>1297</v>
       </c>
@@ -34193,13 +34423,13 @@
       <c r="B14" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="74" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
       <c r="I14" s="61" t="s">
         <v>1298</v>
       </c>
@@ -34208,13 +34438,13 @@
       <c r="B15" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="74" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
       <c r="I15" s="61" t="s">
         <v>1296</v>
       </c>
@@ -34223,13 +34453,13 @@
       <c r="B16" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="74" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
       <c r="I16" s="61" t="s">
         <v>1286</v>
       </c>
@@ -34238,24 +34468,24 @@
       <c r="B17" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="74" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="74" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
       <c r="I18" s="61" t="s">
         <v>1295</v>
       </c>
@@ -34264,12 +34494,12 @@
       <c r="C19" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="74" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
       <c r="I19" s="61" t="s">
         <v>1292</v>
       </c>
@@ -34278,13 +34508,13 @@
       <c r="B20" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="74" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
       <c r="I20" s="61" t="s">
         <v>1301</v>
       </c>
@@ -34293,13 +34523,13 @@
       <c r="B21" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="74" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
       <c r="I21" s="61" t="s">
         <v>1288</v>
       </c>
@@ -34308,13 +34538,13 @@
       <c r="B22" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="74" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
       <c r="I22" s="61" t="s">
         <v>1294</v>
       </c>
@@ -34323,53 +34553,53 @@
       <c r="B23" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="74" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
       <c r="I23" s="61" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="73" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="74" t="s">
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="75" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="74"/>
+      <c r="I24" s="75"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="74" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="74" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
       <c r="I26" s="61" t="s">
         <v>1278</v>
       </c>
@@ -34378,12 +34608,12 @@
       <c r="C27" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="73" t="s">
+      <c r="D27" s="74" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
       <c r="I27" s="61" t="s">
         <v>1279</v>
       </c>
@@ -34392,28 +34622,24 @@
       <c r="D28" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="74" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -34429,12 +34655,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 14 Februari 2023 11:56 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="2036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3082" uniqueCount="2038">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8152,6 +8152,12 @@
       </rPr>
       <t>LOW</t>
     </r>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.general.getBusinessDocumentTypeWorkFlowPathBySubmitterEntityID</t>
+  </si>
+  <si>
+    <t>Mendapatkan Jalur WorkFlow untuk Jenis Dokumen Bisnis berdasarkan ID Entitas Submitter</t>
   </si>
 </sst>
 </file>
@@ -9073,13 +9079,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1193"/>
+  <dimension ref="A1:L1194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C1180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C1176" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B1183" sqref="B1183"/>
+      <selection pane="bottomRight" activeCell="E1190" sqref="E1190:F1190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -34199,48 +34205,69 @@
       <c r="J1189" s="20"/>
       <c r="K1189" s="35"/>
     </row>
-    <row r="1190" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1190" s="35"/>
-      <c r="B1190" s="8"/>
-      <c r="C1190" s="6"/>
+      <c r="B1190" s="7" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C1190" s="4" t="s">
+        <v>2037</v>
+      </c>
       <c r="D1190" s="35"/>
-      <c r="E1190" s="33"/>
-      <c r="F1190" s="56"/>
+      <c r="E1190" s="29">
+        <v>44971</v>
+      </c>
+      <c r="F1190" s="53" t="s">
+        <v>592</v>
+      </c>
       <c r="G1190" s="35"/>
-      <c r="H1190" s="33"/>
-      <c r="I1190" s="25"/>
-      <c r="J1190" s="26"/>
+      <c r="H1190" s="29"/>
+      <c r="I1190" s="19"/>
+      <c r="J1190" s="20"/>
       <c r="K1190" s="35"/>
     </row>
-    <row r="1191" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1191" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1191" s="35"/>
-      <c r="B1191" s="38"/>
-      <c r="C1191" s="39"/>
+      <c r="B1191" s="8"/>
+      <c r="C1191" s="6"/>
       <c r="D1191" s="35"/>
-      <c r="E1191" s="40"/>
-      <c r="F1191" s="50"/>
+      <c r="E1191" s="33"/>
+      <c r="F1191" s="56"/>
       <c r="G1191" s="35"/>
-      <c r="H1191" s="40"/>
-      <c r="I1191" s="41"/>
-      <c r="J1191" s="41"/>
+      <c r="H1191" s="33"/>
+      <c r="I1191" s="25"/>
+      <c r="J1191" s="26"/>
       <c r="K1191" s="35"/>
     </row>
-    <row r="1193" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1193" s="35"/>
-      <c r="B1193" s="7" t="s">
+    <row r="1192" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1192" s="35"/>
+      <c r="B1192" s="38"/>
+      <c r="C1192" s="39"/>
+      <c r="D1192" s="35"/>
+      <c r="E1192" s="40"/>
+      <c r="F1192" s="50"/>
+      <c r="G1192" s="35"/>
+      <c r="H1192" s="40"/>
+      <c r="I1192" s="41"/>
+      <c r="J1192" s="41"/>
+      <c r="K1192" s="35"/>
+    </row>
+    <row r="1194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1194" s="35"/>
+      <c r="B1194" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="C1193" s="4" t="s">
+      <c r="C1194" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="D1193" s="35"/>
-      <c r="E1193" s="29"/>
-      <c r="F1193" s="53"/>
-      <c r="G1193" s="35"/>
-      <c r="H1193" s="29"/>
-      <c r="I1193" s="19"/>
-      <c r="J1193" s="20"/>
-      <c r="K1193" s="35"/>
+      <c r="D1194" s="35"/>
+      <c r="E1194" s="29"/>
+      <c r="F1194" s="53"/>
+      <c r="G1194" s="35"/>
+      <c r="H1194" s="29"/>
+      <c r="I1194" s="19"/>
+      <c r="J1194" s="20"/>
+      <c r="K1194" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Update Pertanggal 15 Februari 2023 12:19 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3082" uniqueCount="2038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="2042">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8158,6 +8158,18 @@
   </si>
   <si>
     <t>Mendapatkan Jalur WorkFlow untuk Jenis Dokumen Bisnis berdasarkan ID Entitas Submitter</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.general.getWorkFlowVersionByWorkFlowPathID</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.setApproverAction</t>
+  </si>
+  <si>
+    <t>Menyimpan Approver Action pada Work Flow Dokumen</t>
+  </si>
+  <si>
+    <t>Mendapatkan Versi WorkFlow berdasarkan ID Jalur WorkFlow</t>
   </si>
 </sst>
 </file>
@@ -8761,13 +8773,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9079,13 +9091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1194"/>
+  <dimension ref="A1:L1196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C1176" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1190" sqref="E1190:F1190"/>
+      <selection pane="bottomRight" activeCell="C1193" sqref="C1193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -34187,10 +34199,10 @@
     <row r="1189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1189" s="35"/>
       <c r="B1189" s="7" t="s">
-        <v>2031</v>
+        <v>2039</v>
       </c>
       <c r="C1189" s="4" t="s">
-        <v>2034</v>
+        <v>2040</v>
       </c>
       <c r="D1189" s="35"/>
       <c r="E1189" s="29">
@@ -34208,10 +34220,10 @@
     <row r="1190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1190" s="35"/>
       <c r="B1190" s="7" t="s">
-        <v>2036</v>
+        <v>2031</v>
       </c>
       <c r="C1190" s="4" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="D1190" s="35"/>
       <c r="E1190" s="29">
@@ -34226,48 +34238,90 @@
       <c r="J1190" s="20"/>
       <c r="K1190" s="35"/>
     </row>
-    <row r="1191" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1191" s="35"/>
-      <c r="B1191" s="8"/>
-      <c r="C1191" s="6"/>
+      <c r="B1191" s="7" t="s">
+        <v>2036</v>
+      </c>
+      <c r="C1191" s="4" t="s">
+        <v>2037</v>
+      </c>
       <c r="D1191" s="35"/>
-      <c r="E1191" s="33"/>
-      <c r="F1191" s="56"/>
+      <c r="E1191" s="29">
+        <v>44971</v>
+      </c>
+      <c r="F1191" s="53" t="s">
+        <v>592</v>
+      </c>
       <c r="G1191" s="35"/>
-      <c r="H1191" s="33"/>
-      <c r="I1191" s="25"/>
-      <c r="J1191" s="26"/>
+      <c r="H1191" s="29"/>
+      <c r="I1191" s="19"/>
+      <c r="J1191" s="20"/>
       <c r="K1191" s="35"/>
     </row>
-    <row r="1192" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1192" s="35"/>
-      <c r="B1192" s="38"/>
-      <c r="C1192" s="39"/>
+      <c r="B1192" s="7" t="s">
+        <v>2038</v>
+      </c>
+      <c r="C1192" s="4" t="s">
+        <v>2041</v>
+      </c>
       <c r="D1192" s="35"/>
-      <c r="E1192" s="40"/>
-      <c r="F1192" s="50"/>
+      <c r="E1192" s="29">
+        <v>44972</v>
+      </c>
+      <c r="F1192" s="53" t="s">
+        <v>592</v>
+      </c>
       <c r="G1192" s="35"/>
-      <c r="H1192" s="40"/>
-      <c r="I1192" s="41"/>
-      <c r="J1192" s="41"/>
+      <c r="H1192" s="29"/>
+      <c r="I1192" s="19"/>
+      <c r="J1192" s="20"/>
       <c r="K1192" s="35"/>
     </row>
-    <row r="1194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1193" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1193" s="35"/>
+      <c r="B1193" s="8"/>
+      <c r="C1193" s="6"/>
+      <c r="D1193" s="35"/>
+      <c r="E1193" s="33"/>
+      <c r="F1193" s="56"/>
+      <c r="G1193" s="35"/>
+      <c r="H1193" s="33"/>
+      <c r="I1193" s="25"/>
+      <c r="J1193" s="26"/>
+      <c r="K1193" s="35"/>
+    </row>
+    <row r="1194" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="35"/>
-      <c r="B1194" s="7" t="s">
+      <c r="B1194" s="38"/>
+      <c r="C1194" s="39"/>
+      <c r="D1194" s="35"/>
+      <c r="E1194" s="40"/>
+      <c r="F1194" s="50"/>
+      <c r="G1194" s="35"/>
+      <c r="H1194" s="40"/>
+      <c r="I1194" s="41"/>
+      <c r="J1194" s="41"/>
+      <c r="K1194" s="35"/>
+    </row>
+    <row r="1196" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1196" s="35"/>
+      <c r="B1196" s="7" t="s">
         <v>364</v>
       </c>
-      <c r="C1194" s="4" t="s">
+      <c r="C1196" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="D1194" s="35"/>
-      <c r="E1194" s="29"/>
-      <c r="F1194" s="53"/>
-      <c r="G1194" s="35"/>
-      <c r="H1194" s="29"/>
-      <c r="I1194" s="19"/>
-      <c r="J1194" s="20"/>
-      <c r="K1194" s="35"/>
+      <c r="D1196" s="35"/>
+      <c r="E1196" s="29"/>
+      <c r="F1196" s="53"/>
+      <c r="G1196" s="35"/>
+      <c r="H1196" s="29"/>
+      <c r="I1196" s="19"/>
+      <c r="J1196" s="20"/>
+      <c r="K1196" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -34304,80 +34358,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="75" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="75" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="75" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="75" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="75" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="75" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="75" t="s">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="75"/>
+      <c r="I7" s="74"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="73" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
       <c r="I8" s="61" t="s">
         <v>1276</v>
       </c>
@@ -34386,62 +34440,62 @@
       <c r="B9" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
       <c r="I9" s="61" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="75" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="75" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="75" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="75" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="74" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="75"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="73" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
       <c r="I13" s="61" t="s">
         <v>1297</v>
       </c>
@@ -34450,13 +34504,13 @@
       <c r="B14" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="73" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="61" t="s">
         <v>1298</v>
       </c>
@@ -34465,13 +34519,13 @@
       <c r="B15" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="74" t="s">
+      <c r="C15" s="73" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
       <c r="I15" s="61" t="s">
         <v>1296</v>
       </c>
@@ -34480,13 +34534,13 @@
       <c r="B16" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="73" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
       <c r="I16" s="61" t="s">
         <v>1286</v>
       </c>
@@ -34495,24 +34549,24 @@
       <c r="B17" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="74" t="s">
+      <c r="C17" s="73" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="73" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
       <c r="I18" s="61" t="s">
         <v>1295</v>
       </c>
@@ -34521,12 +34575,12 @@
       <c r="C19" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="74" t="s">
+      <c r="D19" s="73" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
       <c r="I19" s="61" t="s">
         <v>1292</v>
       </c>
@@ -34535,13 +34589,13 @@
       <c r="B20" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="73" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
       <c r="I20" s="61" t="s">
         <v>1301</v>
       </c>
@@ -34550,13 +34604,13 @@
       <c r="B21" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="73" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
       <c r="I21" s="61" t="s">
         <v>1288</v>
       </c>
@@ -34565,13 +34619,13 @@
       <c r="B22" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="73" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
       <c r="I22" s="61" t="s">
         <v>1294</v>
       </c>
@@ -34580,53 +34634,53 @@
       <c r="B23" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="73" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
       <c r="I23" s="61" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="75" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="75" t="s">
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="74" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="75"/>
+      <c r="I24" s="74"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="73" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="73" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
       <c r="I26" s="61" t="s">
         <v>1278</v>
       </c>
@@ -34635,12 +34689,12 @@
       <c r="C27" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="73" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="I27" s="61" t="s">
         <v>1279</v>
       </c>
@@ -34649,24 +34703,28 @@
       <c r="D28" s="62" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="74" t="s">
+      <c r="E28" s="73" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -34682,16 +34740,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 3 Maret 2023 11:14 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4096" uniqueCount="2057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4104" uniqueCount="2061">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8215,6 +8215,18 @@
   </si>
   <si>
     <t>Mendapatkan Data Entitas Pemetaan Jenis Dokumen Bisnis pada Work Flow</t>
+  </si>
+  <si>
+    <t>transaction.create.sysConfig.setWorkFlowPathSequenceRemapping</t>
+  </si>
+  <si>
+    <t>Menyimpan Data Baru Pemetaan Ulang Urutan Jalur WorkFlow</t>
+  </si>
+  <si>
+    <t>transaction.update.sysConfig.setWorkFlowPathSequenceRemapping</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Pemetaan Ulang Urutan Jalur WorkFlow</t>
   </si>
 </sst>
 </file>
@@ -8882,22 +8894,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8932,6 +8938,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -9251,13 +9263,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1205"/>
+  <dimension ref="A1:M1206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D689" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D1169" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F699" sqref="F699"/>
+      <selection pane="bottomRight" activeCell="E1186" sqref="E1186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9293,31 +9305,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="75" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="81"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="75" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="78"/>
-      <c r="K2" s="79"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="76"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9339,8 +9351,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9353,10 +9365,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="71" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="70"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9369,8 +9381,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9487,8 +9499,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9501,10 +9513,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="71" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9517,8 +9529,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9599,8 +9611,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9613,10 +9625,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="71" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="70"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9629,8 +9641,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="72"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9705,8 +9717,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9735,8 +9747,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11313,8 +11325,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="71"/>
-      <c r="C95" s="72"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="70"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11327,10 +11339,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="69" t="s">
+      <c r="B96" s="71" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="70"/>
+      <c r="C96" s="72"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11343,8 +11355,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="71"/>
-      <c r="C97" s="72"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="70"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11503,8 +11515,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="71"/>
-      <c r="C104" s="72"/>
+      <c r="B104" s="69"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11517,10 +11529,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="69" t="s">
+      <c r="B105" s="71" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="70"/>
+      <c r="C105" s="72"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11533,8 +11545,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="71"/>
-      <c r="C106" s="72"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="70"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12039,8 +12051,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="71"/>
-      <c r="C130" s="72"/>
+      <c r="B130" s="69"/>
+      <c r="C130" s="70"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12053,10 +12065,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="69" t="s">
+      <c r="B131" s="71" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="70"/>
+      <c r="C131" s="72"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12069,8 +12081,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="71"/>
-      <c r="C132" s="72"/>
+      <c r="B132" s="69"/>
+      <c r="C132" s="70"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12181,8 +12193,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="71"/>
-      <c r="C137" s="72"/>
+      <c r="B137" s="69"/>
+      <c r="C137" s="70"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12195,10 +12207,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="69" t="s">
+      <c r="B138" s="71" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="70"/>
+      <c r="C138" s="72"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12211,8 +12223,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="71"/>
-      <c r="C139" s="72"/>
+      <c r="B139" s="69"/>
+      <c r="C139" s="70"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12373,8 +12385,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="71"/>
-      <c r="C147" s="72"/>
+      <c r="B147" s="69"/>
+      <c r="C147" s="70"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12387,10 +12399,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="69" t="s">
+      <c r="B148" s="71" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="70"/>
+      <c r="C148" s="72"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12403,8 +12415,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="71"/>
-      <c r="C149" s="72"/>
+      <c r="B149" s="69"/>
+      <c r="C149" s="70"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12565,8 +12577,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="71"/>
-      <c r="C157" s="72"/>
+      <c r="B157" s="69"/>
+      <c r="C157" s="70"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12679,8 +12691,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="71"/>
-      <c r="C163" s="72"/>
+      <c r="B163" s="69"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12693,10 +12705,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="69" t="s">
+      <c r="B164" s="71" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="70"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12709,8 +12721,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="71"/>
-      <c r="C165" s="72"/>
+      <c r="B165" s="69"/>
+      <c r="C165" s="70"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -12967,8 +12979,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="71"/>
-      <c r="C177" s="72"/>
+      <c r="B177" s="69"/>
+      <c r="C177" s="70"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -12981,10 +12993,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="69" t="s">
+      <c r="B178" s="71" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="70"/>
+      <c r="C178" s="72"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -12997,8 +13009,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="71"/>
-      <c r="C179" s="72"/>
+      <c r="B179" s="69"/>
+      <c r="C179" s="70"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13063,8 +13075,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="71"/>
-      <c r="C183" s="72"/>
+      <c r="B183" s="69"/>
+      <c r="C183" s="70"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13077,10 +13089,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="69" t="s">
+      <c r="B184" s="71" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="70"/>
+      <c r="C184" s="72"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13093,8 +13105,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="71"/>
-      <c r="C185" s="72"/>
+      <c r="B185" s="69"/>
+      <c r="C185" s="70"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13679,8 +13691,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="71"/>
-      <c r="C211" s="72"/>
+      <c r="B211" s="69"/>
+      <c r="C211" s="70"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13693,10 +13705,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="69" t="s">
+      <c r="B212" s="71" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="70"/>
+      <c r="C212" s="72"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13709,8 +13721,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="71"/>
-      <c r="C213" s="72"/>
+      <c r="B213" s="69"/>
+      <c r="C213" s="70"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13905,8 +13917,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="71"/>
-      <c r="C222" s="72"/>
+      <c r="B222" s="69"/>
+      <c r="C222" s="70"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13919,10 +13931,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="69" t="s">
+      <c r="B223" s="71" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="70"/>
+      <c r="C223" s="72"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -13935,8 +13947,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="71"/>
-      <c r="C224" s="72"/>
+      <c r="B224" s="69"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16659,18 +16671,28 @@
       <c r="K337" s="14"/>
       <c r="L337" s="29"/>
     </row>
-    <row r="338" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338" s="29"/>
-      <c r="B338" s="59"/>
-      <c r="C338" s="64"/>
-      <c r="D338" s="7"/>
+      <c r="B338" s="56" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C338" s="54" t="s">
+        <v>2057</v>
+      </c>
+      <c r="D338" s="3" t="s">
+        <v>2058</v>
+      </c>
       <c r="E338" s="29"/>
-      <c r="F338" s="26"/>
-      <c r="G338" s="46"/>
+      <c r="F338" s="23">
+        <v>44988</v>
+      </c>
+      <c r="G338" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H338" s="29"/>
-      <c r="I338" s="26"/>
-      <c r="J338" s="17"/>
-      <c r="K338" s="18"/>
+      <c r="I338" s="23"/>
+      <c r="J338" s="13"/>
+      <c r="K338" s="14"/>
       <c r="L338" s="29"/>
     </row>
     <row r="339" spans="1:12" x14ac:dyDescent="0.25">
@@ -16761,8 +16783,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="71"/>
-      <c r="C343" s="72"/>
+      <c r="B343" s="69"/>
+      <c r="C343" s="70"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16775,10 +16797,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="69" t="s">
+      <c r="B344" s="71" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="70"/>
+      <c r="C344" s="72"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16791,8 +16813,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="71"/>
-      <c r="C345" s="72"/>
+      <c r="B345" s="69"/>
+      <c r="C345" s="70"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20417,8 +20439,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="71"/>
-      <c r="C484" s="72"/>
+      <c r="B484" s="69"/>
+      <c r="C484" s="70"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20473,8 +20495,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="71"/>
-      <c r="C487" s="72"/>
+      <c r="B487" s="69"/>
+      <c r="C487" s="70"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20487,10 +20509,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="69" t="s">
+      <c r="B488" s="71" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="70"/>
+      <c r="C488" s="72"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20503,8 +20525,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="71"/>
-      <c r="C489" s="72"/>
+      <c r="B489" s="69"/>
+      <c r="C489" s="70"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22103,8 +22125,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="71"/>
-      <c r="C553" s="72"/>
+      <c r="B553" s="69"/>
+      <c r="C553" s="70"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22117,10 +22139,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="69" t="s">
+      <c r="B554" s="71" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="70"/>
+      <c r="C554" s="72"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22133,8 +22155,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="71"/>
-      <c r="C555" s="72"/>
+      <c r="B555" s="69"/>
+      <c r="C555" s="70"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -25885,8 +25907,8 @@
     </row>
     <row r="708" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A708" s="29"/>
-      <c r="B708" s="71"/>
-      <c r="C708" s="72"/>
+      <c r="B708" s="69"/>
+      <c r="C708" s="70"/>
       <c r="D708" s="6"/>
       <c r="E708" s="29"/>
       <c r="F708" s="24"/>
@@ -25899,10 +25921,10 @@
     </row>
     <row r="709" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A709" s="29"/>
-      <c r="B709" s="69" t="s">
+      <c r="B709" s="71" t="s">
         <v>1853</v>
       </c>
-      <c r="C709" s="70"/>
+      <c r="C709" s="72"/>
       <c r="D709" s="6"/>
       <c r="E709" s="29"/>
       <c r="F709" s="24"/>
@@ -25915,8 +25937,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="71"/>
-      <c r="C710" s="72"/>
+      <c r="B710" s="69"/>
+      <c r="C710" s="70"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -28373,8 +28395,8 @@
     </row>
     <row r="813" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A813" s="29"/>
-      <c r="B813" s="71"/>
-      <c r="C813" s="72"/>
+      <c r="B813" s="69"/>
+      <c r="C813" s="70"/>
       <c r="D813" s="6"/>
       <c r="E813" s="29"/>
       <c r="F813" s="24"/>
@@ -28387,10 +28409,10 @@
     </row>
     <row r="814" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A814" s="29"/>
-      <c r="B814" s="69" t="s">
+      <c r="B814" s="71" t="s">
         <v>1854</v>
       </c>
-      <c r="C814" s="70"/>
+      <c r="C814" s="72"/>
       <c r="D814" s="6"/>
       <c r="E814" s="29"/>
       <c r="F814" s="24"/>
@@ -28403,8 +28425,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="71"/>
-      <c r="C815" s="72"/>
+      <c r="B815" s="69"/>
+      <c r="C815" s="70"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -31318,8 +31340,8 @@
     </row>
     <row r="929" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A929" s="29"/>
-      <c r="B929" s="71"/>
-      <c r="C929" s="72"/>
+      <c r="B929" s="69"/>
+      <c r="C929" s="70"/>
       <c r="D929" s="6"/>
       <c r="E929" s="29"/>
       <c r="F929" s="24"/>
@@ -31332,10 +31354,10 @@
     </row>
     <row r="930" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A930" s="29"/>
-      <c r="B930" s="69" t="s">
+      <c r="B930" s="71" t="s">
         <v>1952</v>
       </c>
-      <c r="C930" s="70"/>
+      <c r="C930" s="72"/>
       <c r="D930" s="6"/>
       <c r="E930" s="29"/>
       <c r="F930" s="24"/>
@@ -31348,8 +31370,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="71"/>
-      <c r="C931" s="72"/>
+      <c r="B931" s="69"/>
+      <c r="C931" s="70"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31483,8 +31505,8 @@
     </row>
     <row r="937" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A937" s="29"/>
-      <c r="B937" s="71"/>
-      <c r="C937" s="72"/>
+      <c r="B937" s="69"/>
+      <c r="C937" s="70"/>
       <c r="D937" s="6"/>
       <c r="E937" s="29"/>
       <c r="F937" s="24"/>
@@ -31497,10 +31519,10 @@
     </row>
     <row r="938" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A938" s="29"/>
-      <c r="B938" s="69" t="s">
+      <c r="B938" s="71" t="s">
         <v>1855</v>
       </c>
-      <c r="C938" s="70"/>
+      <c r="C938" s="72"/>
       <c r="D938" s="6"/>
       <c r="E938" s="29"/>
       <c r="F938" s="24"/>
@@ -31513,8 +31535,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="71"/>
-      <c r="C939" s="72"/>
+      <c r="B939" s="69"/>
+      <c r="C939" s="70"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -32037,8 +32059,8 @@
     </row>
     <row r="963" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A963" s="29"/>
-      <c r="B963" s="71"/>
-      <c r="C963" s="72"/>
+      <c r="B963" s="69"/>
+      <c r="C963" s="70"/>
       <c r="D963" s="6"/>
       <c r="E963" s="29"/>
       <c r="F963" s="24"/>
@@ -32051,10 +32073,10 @@
     </row>
     <row r="964" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A964" s="29"/>
-      <c r="B964" s="69" t="s">
+      <c r="B964" s="71" t="s">
         <v>1856</v>
       </c>
-      <c r="C964" s="70"/>
+      <c r="C964" s="72"/>
       <c r="D964" s="6"/>
       <c r="E964" s="29"/>
       <c r="F964" s="24"/>
@@ -32067,8 +32089,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="71"/>
-      <c r="C965" s="72"/>
+      <c r="B965" s="69"/>
+      <c r="C965" s="70"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -34977,8 +34999,8 @@
     </row>
     <row r="1078" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1078" s="29"/>
-      <c r="B1078" s="71"/>
-      <c r="C1078" s="72"/>
+      <c r="B1078" s="69"/>
+      <c r="C1078" s="70"/>
       <c r="D1078" s="6"/>
       <c r="E1078" s="29"/>
       <c r="F1078" s="24"/>
@@ -34991,10 +35013,10 @@
     </row>
     <row r="1079" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1079" s="29"/>
-      <c r="B1079" s="69" t="s">
+      <c r="B1079" s="71" t="s">
         <v>1857</v>
       </c>
-      <c r="C1079" s="70"/>
+      <c r="C1079" s="72"/>
       <c r="D1079" s="6"/>
       <c r="E1079" s="29"/>
       <c r="F1079" s="24"/>
@@ -35007,8 +35029,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="71"/>
-      <c r="C1080" s="72"/>
+      <c r="B1080" s="69"/>
+      <c r="C1080" s="70"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35063,8 +35085,8 @@
     </row>
     <row r="1083" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1083" s="29"/>
-      <c r="B1083" s="71"/>
-      <c r="C1083" s="72"/>
+      <c r="B1083" s="69"/>
+      <c r="C1083" s="70"/>
       <c r="D1083" s="6"/>
       <c r="E1083" s="29"/>
       <c r="F1083" s="24"/>
@@ -35077,10 +35099,10 @@
     </row>
     <row r="1084" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1084" s="29"/>
-      <c r="B1084" s="69" t="s">
+      <c r="B1084" s="71" t="s">
         <v>1858</v>
       </c>
-      <c r="C1084" s="70"/>
+      <c r="C1084" s="72"/>
       <c r="D1084" s="6"/>
       <c r="E1084" s="29"/>
       <c r="F1084" s="24"/>
@@ -35093,8 +35115,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="71"/>
-      <c r="C1085" s="72"/>
+      <c r="B1085" s="69"/>
+      <c r="C1085" s="70"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -37457,42 +37479,42 @@
       <c r="K1185" s="14"/>
       <c r="L1185" s="29"/>
     </row>
-    <row r="1186" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1186" s="29"/>
-      <c r="B1186" s="59"/>
-      <c r="C1186" s="64"/>
-      <c r="D1186" s="7"/>
+      <c r="B1186" s="56" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C1186" s="54" t="s">
+        <v>2059</v>
+      </c>
+      <c r="D1186" s="3" t="s">
+        <v>2060</v>
+      </c>
       <c r="E1186" s="29"/>
-      <c r="F1186" s="26"/>
-      <c r="G1186" s="46"/>
+      <c r="F1186" s="23">
+        <v>44988</v>
+      </c>
+      <c r="G1186" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1186" s="29"/>
-      <c r="I1186" s="26"/>
-      <c r="J1186" s="17"/>
-      <c r="K1186" s="18"/>
+      <c r="I1186" s="23"/>
+      <c r="J1186" s="13"/>
+      <c r="K1186" s="14"/>
       <c r="L1186" s="29"/>
     </row>
-    <row r="1187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1187" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1187" s="29"/>
-      <c r="B1187" s="56" t="s">
-        <v>2049</v>
-      </c>
-      <c r="C1187" s="54" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D1187" s="3" t="s">
-        <v>1229</v>
-      </c>
+      <c r="B1187" s="59"/>
+      <c r="C1187" s="64"/>
+      <c r="D1187" s="7"/>
       <c r="E1187" s="29"/>
-      <c r="F1187" s="23">
-        <v>44635</v>
-      </c>
-      <c r="G1187" s="44" t="s">
-        <v>592</v>
-      </c>
+      <c r="F1187" s="26"/>
+      <c r="G1187" s="46"/>
       <c r="H1187" s="29"/>
-      <c r="I1187" s="23"/>
-      <c r="J1187" s="13"/>
-      <c r="K1187" s="14"/>
+      <c r="I1187" s="26"/>
+      <c r="J1187" s="17"/>
+      <c r="K1187" s="18"/>
       <c r="L1187" s="29"/>
     </row>
     <row r="1188" spans="1:12" x14ac:dyDescent="0.25">
@@ -37501,10 +37523,10 @@
         <v>2049</v>
       </c>
       <c r="C1188" s="54" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="D1188" s="3" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="E1188" s="29"/>
       <c r="F1188" s="23">
@@ -37525,14 +37547,14 @@
         <v>2049</v>
       </c>
       <c r="C1189" s="54" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="D1189" s="3" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="E1189" s="29"/>
       <c r="F1189" s="23">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="G1189" s="44" t="s">
         <v>592</v>
@@ -37545,37 +37567,45 @@
     </row>
     <row r="1190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1190" s="29"/>
-      <c r="B1190" s="57"/>
-      <c r="C1190" s="54"/>
-      <c r="D1190" s="3"/>
+      <c r="B1190" s="56" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C1190" s="54" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D1190" s="3" t="s">
+        <v>1232</v>
+      </c>
       <c r="E1190" s="29"/>
-      <c r="F1190" s="23"/>
-      <c r="G1190" s="44"/>
+      <c r="F1190" s="23">
+        <v>44636</v>
+      </c>
+      <c r="G1190" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1190" s="29"/>
       <c r="I1190" s="23"/>
       <c r="J1190" s="13"/>
       <c r="K1190" s="14"/>
       <c r="L1190" s="29"/>
     </row>
-    <row r="1191" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1191" s="29"/>
-      <c r="B1191" s="71"/>
-      <c r="C1191" s="72"/>
-      <c r="D1191" s="6"/>
+      <c r="B1191" s="57"/>
+      <c r="C1191" s="54"/>
+      <c r="D1191" s="3"/>
       <c r="E1191" s="29"/>
-      <c r="F1191" s="24"/>
-      <c r="G1191" s="45"/>
+      <c r="F1191" s="23"/>
+      <c r="G1191" s="44"/>
       <c r="H1191" s="29"/>
-      <c r="I1191" s="24"/>
-      <c r="J1191" s="15"/>
-      <c r="K1191" s="16"/>
+      <c r="I1191" s="23"/>
+      <c r="J1191" s="13"/>
+      <c r="K1191" s="14"/>
       <c r="L1191" s="29"/>
     </row>
-    <row r="1192" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1192" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1192" s="29"/>
-      <c r="B1192" s="69" t="s">
-        <v>2035</v>
-      </c>
+      <c r="B1192" s="69"/>
       <c r="C1192" s="70"/>
       <c r="D1192" s="6"/>
       <c r="E1192" s="29"/>
@@ -37587,9 +37617,11 @@
       <c r="K1192" s="16"/>
       <c r="L1192" s="29"/>
     </row>
-    <row r="1193" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1193" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1193" s="29"/>
-      <c r="B1193" s="71"/>
+      <c r="B1193" s="71" t="s">
+        <v>2035</v>
+      </c>
       <c r="C1193" s="72"/>
       <c r="D1193" s="6"/>
       <c r="E1193" s="29"/>
@@ -37601,28 +37633,18 @@
       <c r="K1193" s="16"/>
       <c r="L1193" s="29"/>
     </row>
-    <row r="1194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="56" t="s">
-        <v>2049</v>
-      </c>
-      <c r="C1194" s="54" t="s">
-        <v>2029</v>
-      </c>
-      <c r="D1194" s="3" t="s">
-        <v>2033</v>
-      </c>
+      <c r="B1194" s="69"/>
+      <c r="C1194" s="70"/>
+      <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
-      <c r="F1194" s="23">
-        <v>44971</v>
-      </c>
-      <c r="G1194" s="44" t="s">
-        <v>592</v>
-      </c>
+      <c r="F1194" s="24"/>
+      <c r="G1194" s="45"/>
       <c r="H1194" s="29"/>
-      <c r="I1194" s="23"/>
-      <c r="J1194" s="13"/>
-      <c r="K1194" s="14"/>
+      <c r="I1194" s="24"/>
+      <c r="J1194" s="15"/>
+      <c r="K1194" s="16"/>
       <c r="L1194" s="29"/>
     </row>
     <row r="1195" spans="1:12" x14ac:dyDescent="0.25">
@@ -37631,10 +37653,10 @@
         <v>2049</v>
       </c>
       <c r="C1195" s="54" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D1195" s="3" t="s">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="E1195" s="29"/>
       <c r="F1195" s="23">
@@ -37655,10 +37677,10 @@
         <v>2049</v>
       </c>
       <c r="C1196" s="54" t="s">
-        <v>2039</v>
+        <v>2030</v>
       </c>
       <c r="D1196" s="3" t="s">
-        <v>2040</v>
+        <v>2032</v>
       </c>
       <c r="E1196" s="29"/>
       <c r="F1196" s="23">
@@ -37679,17 +37701,17 @@
         <v>2049</v>
       </c>
       <c r="C1197" s="54" t="s">
-        <v>2031</v>
+        <v>2039</v>
       </c>
       <c r="D1197" s="3" t="s">
-        <v>2034</v>
+        <v>2040</v>
       </c>
       <c r="E1197" s="29"/>
       <c r="F1197" s="23">
-        <v>44987</v>
+        <v>44971</v>
       </c>
       <c r="G1197" s="44" t="s">
-        <v>2048</v>
+        <v>592</v>
       </c>
       <c r="H1197" s="29"/>
       <c r="I1197" s="23"/>
@@ -37697,23 +37719,23 @@
       <c r="K1197" s="14"/>
       <c r="L1197" s="29"/>
     </row>
-    <row r="1198" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1198" s="29"/>
       <c r="B1198" s="56" t="s">
         <v>2049</v>
       </c>
       <c r="C1198" s="54" t="s">
-        <v>2046</v>
+        <v>2031</v>
       </c>
       <c r="D1198" s="3" t="s">
-        <v>2047</v>
+        <v>2034</v>
       </c>
       <c r="E1198" s="29"/>
       <c r="F1198" s="23">
         <v>44987</v>
       </c>
       <c r="G1198" s="44" t="s">
-        <v>592</v>
+        <v>2048</v>
       </c>
       <c r="H1198" s="29"/>
       <c r="I1198" s="23"/>
@@ -37721,23 +37743,23 @@
       <c r="K1198" s="14"/>
       <c r="L1198" s="29"/>
     </row>
-    <row r="1199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1199" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1199" s="29"/>
       <c r="B1199" s="56" t="s">
         <v>2049</v>
       </c>
       <c r="C1199" s="54" t="s">
-        <v>2036</v>
+        <v>2046</v>
       </c>
       <c r="D1199" s="3" t="s">
-        <v>2037</v>
+        <v>2047</v>
       </c>
       <c r="E1199" s="29"/>
       <c r="F1199" s="23">
         <v>44987</v>
       </c>
       <c r="G1199" s="44" t="s">
-        <v>2048</v>
+        <v>592</v>
       </c>
       <c r="H1199" s="29"/>
       <c r="I1199" s="23"/>
@@ -37745,93 +37767,117 @@
       <c r="K1199" s="14"/>
       <c r="L1199" s="29"/>
     </row>
-    <row r="1200" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1200" s="29"/>
       <c r="B1200" s="56" t="s">
         <v>2049</v>
       </c>
       <c r="C1200" s="54" t="s">
-        <v>2050</v>
-      </c>
-      <c r="D1200" s="3"/>
+        <v>2036</v>
+      </c>
+      <c r="D1200" s="3" t="s">
+        <v>2037</v>
+      </c>
       <c r="E1200" s="29"/>
-      <c r="F1200" s="23"/>
-      <c r="G1200" s="44"/>
+      <c r="F1200" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1200" s="44" t="s">
+        <v>2048</v>
+      </c>
       <c r="H1200" s="29"/>
       <c r="I1200" s="23"/>
       <c r="J1200" s="13"/>
       <c r="K1200" s="14"/>
       <c r="L1200" s="29"/>
     </row>
-    <row r="1201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1201" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1201" s="29"/>
       <c r="B1201" s="56" t="s">
         <v>2049</v>
       </c>
       <c r="C1201" s="54" t="s">
-        <v>2038</v>
-      </c>
-      <c r="D1201" s="3" t="s">
-        <v>2041</v>
-      </c>
+        <v>2050</v>
+      </c>
+      <c r="D1201" s="3"/>
       <c r="E1201" s="29"/>
-      <c r="F1201" s="23">
-        <v>44972</v>
-      </c>
-      <c r="G1201" s="44" t="s">
-        <v>592</v>
-      </c>
+      <c r="F1201" s="23"/>
+      <c r="G1201" s="44"/>
       <c r="H1201" s="29"/>
       <c r="I1201" s="23"/>
       <c r="J1201" s="13"/>
       <c r="K1201" s="14"/>
       <c r="L1201" s="29"/>
     </row>
-    <row r="1202" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1202" s="29"/>
-      <c r="B1202" s="60"/>
-      <c r="C1202" s="67"/>
-      <c r="D1202" s="5"/>
+      <c r="B1202" s="56" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C1202" s="54" t="s">
+        <v>2038</v>
+      </c>
+      <c r="D1202" s="3" t="s">
+        <v>2041</v>
+      </c>
       <c r="E1202" s="29"/>
-      <c r="F1202" s="27"/>
-      <c r="G1202" s="47"/>
+      <c r="F1202" s="23">
+        <v>44972</v>
+      </c>
+      <c r="G1202" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1202" s="29"/>
-      <c r="I1202" s="27"/>
-      <c r="J1202" s="19"/>
-      <c r="K1202" s="20"/>
+      <c r="I1202" s="23"/>
+      <c r="J1202" s="13"/>
+      <c r="K1202" s="14"/>
       <c r="L1202" s="29"/>
     </row>
-    <row r="1203" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1203" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1203" s="29"/>
-      <c r="B1203" s="55"/>
-      <c r="C1203" s="62"/>
-      <c r="D1203" s="32"/>
+      <c r="B1203" s="60"/>
+      <c r="C1203" s="67"/>
+      <c r="D1203" s="5"/>
       <c r="E1203" s="29"/>
-      <c r="F1203" s="33"/>
-      <c r="G1203" s="41"/>
+      <c r="F1203" s="27"/>
+      <c r="G1203" s="47"/>
       <c r="H1203" s="29"/>
-      <c r="I1203" s="33"/>
-      <c r="J1203" s="34"/>
-      <c r="K1203" s="34"/>
+      <c r="I1203" s="27"/>
+      <c r="J1203" s="19"/>
+      <c r="K1203" s="20"/>
       <c r="L1203" s="29"/>
     </row>
-    <row r="1205" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1205" s="29"/>
-      <c r="B1205" s="55"/>
-      <c r="C1205" s="54" t="s">
+    <row r="1204" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1204" s="29"/>
+      <c r="B1204" s="55"/>
+      <c r="C1204" s="62"/>
+      <c r="D1204" s="32"/>
+      <c r="E1204" s="29"/>
+      <c r="F1204" s="33"/>
+      <c r="G1204" s="41"/>
+      <c r="H1204" s="29"/>
+      <c r="I1204" s="33"/>
+      <c r="J1204" s="34"/>
+      <c r="K1204" s="34"/>
+      <c r="L1204" s="29"/>
+    </row>
+    <row r="1206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1206" s="29"/>
+      <c r="B1206" s="55"/>
+      <c r="C1206" s="54" t="s">
         <v>364</v>
       </c>
-      <c r="D1205" s="3" t="s">
+      <c r="D1206" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E1205" s="29"/>
-      <c r="F1205" s="23"/>
-      <c r="G1205" s="44"/>
-      <c r="H1205" s="29"/>
-      <c r="I1205" s="23"/>
-      <c r="J1205" s="13"/>
-      <c r="K1205" s="14"/>
-      <c r="L1205" s="29"/>
+      <c r="E1206" s="29"/>
+      <c r="F1206" s="23"/>
+      <c r="G1206" s="44"/>
+      <c r="H1206" s="29"/>
+      <c r="I1206" s="23"/>
+      <c r="J1206" s="13"/>
+      <c r="K1206" s="14"/>
+      <c r="L1206" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -37845,11 +37891,25 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B132:C132"/>
     <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B139:C139"/>
     <mergeCell ref="B147:C147"/>
     <mergeCell ref="B149:C149"/>
     <mergeCell ref="B148:C148"/>
     <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
     <mergeCell ref="B157:C157"/>
     <mergeCell ref="B163:C163"/>
     <mergeCell ref="B165:C165"/>
@@ -37857,11 +37917,6 @@
     <mergeCell ref="B179:C179"/>
     <mergeCell ref="B178:C178"/>
     <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
     <mergeCell ref="B489:C489"/>
     <mergeCell ref="B553:C553"/>
     <mergeCell ref="B555:C555"/>
@@ -37875,9 +37930,9 @@
     <mergeCell ref="B1078:C1078"/>
     <mergeCell ref="B1080:C1080"/>
     <mergeCell ref="B964:C964"/>
-    <mergeCell ref="B1191:C1191"/>
+    <mergeCell ref="B1192:C1192"/>
+    <mergeCell ref="B1194:C1194"/>
     <mergeCell ref="B1193:C1193"/>
-    <mergeCell ref="B1192:C1192"/>
     <mergeCell ref="B1084:C1084"/>
     <mergeCell ref="B1079:C1079"/>
     <mergeCell ref="B938:C938"/>
@@ -37890,6 +37945,10 @@
     <mergeCell ref="B929:C929"/>
     <mergeCell ref="B931:C931"/>
     <mergeCell ref="B937:C937"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B488:C488"/>
     <mergeCell ref="B344:C344"/>
     <mergeCell ref="B223:C223"/>
@@ -37900,26 +37959,13 @@
     <mergeCell ref="B345:C345"/>
     <mergeCell ref="B484:C484"/>
     <mergeCell ref="B487:C487"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B185:C185"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G14 G102 G133:G134 G136 G143:G145 G214:G220 G225:G230 G346:G350 G352:G356 G366:G368 G384 G458:G460 G796:G798 G827:G828 G942:G944 G946 G948:G952 G954:G957 G959:G960 G972:G977 G979:G981 G990:G991 G377:G378 G997 G1052:G1054 G966:G970 G1093:G1095 G312:G315 G1166:G1169 G900:G903 G816:G818 G317:G319 G1171:G1173 G209 G186 G128 G108 G232:G239 G490:G492 G370:G375 G983:G988 G830:G835 G180 G79:G81 G158:G159 G56 G406 G820:G825 G358:G364 G1086:G1091 G791:G794 G940 G851 G1004 G161 G166:G174 G188:G207 G298:G308 G1152:G1162 G1009:G1050 G856:G898 G411:G456 G76:G77 G485 G1070 F1067:G1069 G29:G37 G463:G476 G339:G341 G1187:G1189 G480:G482 G1074:G1076 G925:G927 G811 G93 G1081 G150:G153 G1057:G1066 G909:G923 G544:G551 G532:G535 G806:G809 G847:G849 G386:G404 G999:G1002 G905:G907 G49 G60 G784:G787 G155 G584:G585 G853:G854 G621:G622 G1006:G1007 G1119:G1120 G505:G506 G408:G409 G265:G266 G650:G652 G637:G643 G647:G648 G624:G627 G70:G72 G88:G91 G322:G334 G800:G803 G1176:G1182 G538:G542 G680:G682 G665 G573 G618:G619 G605:G607 G750:G753 G83:G86 G759:G760 G58 G755:G757 G570 G703:G708 G719:G732 G655:G663 G283:G296 G1137:G1150 G768:G775 G68 G734:G740 G513:G524 G508:G511 G1122:G1135 G268:G281 G762:G766 G526:G530 G747 G777:G782 G98:G99 G686:G691" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G14 G102 G133:G134 G136 G143:G145 G214:G220 G225:G230 G346:G350 G352:G356 G366:G368 G384 G458:G460 G796:G798 G827:G828 G942:G944 G946 G948:G952 G954:G957 G959:G960 G972:G977 G979:G981 G990:G991 G377:G378 G997 G1052:G1054 G966:G970 G1093:G1095 G312:G315 G1166:G1169 G900:G903 G816:G818 G317:G319 G1171:G1173 G209 G186 G128 G108 G232:G239 G490:G492 G370:G375 G983:G988 G830:G835 G180 G79:G81 G158:G159 G56 G406 G820:G825 G358:G364 G1086:G1091 G791:G794 G940 G851 G1004 G161 G166:G174 G188:G207 G298:G308 G1152:G1162 G1009:G1050 G856:G898 G411:G456 G76:G77 G485 G1070 F1067:G1069 G29:G37 G463:G476 G339:G341 G1188:G1190 G480:G482 G1074:G1076 G925:G927 G811 G93 G1081 G150:G153 G1057:G1066 G909:G923 G544:G551 G532:G535 G806:G809 G847:G849 G386:G404 G999:G1002 G905:G907 G49 G60 G784:G787 G155 G584:G585 G853:G854 G621:G622 G1006:G1007 G1119:G1120 G505:G506 G408:G409 G265:G266 G650:G652 G637:G643 G647:G648 G624:G627 G70:G72 G88:G91 G322:G334 G800:G803 G1176:G1182 G538:G542 G680:G682 G665 G573 G618:G619 G605:G607 G750:G753 G83:G86 G759:G760 G58 G755:G757 G570 G703:G708 G719:G732 G655:G663 G283:G296 G1137:G1150 G768:G775 G68 G734:G740 G513:G524 G508:G511 G1122:G1135 G268:G281 G762:G766 G526:G530 G747 G777:G782 G98:G99 G686:G691" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Pertanggal 3 Maret 2023 14:47 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -8894,24 +8894,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -8945,13 +8927,31 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9266,10 +9266,10 @@
   <dimension ref="A1:M1206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D1169" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D692" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1186" sqref="E1186"/>
+      <selection pane="bottomRight" activeCell="F699" sqref="F699"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9305,31 +9305,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="73" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="84" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="72" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="73"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="75" t="s">
+      <c r="I2" s="69" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="76"/>
-      <c r="K2" s="77"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="74"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9351,8 +9351,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9365,10 +9365,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="80" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9381,8 +9381,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9499,8 +9499,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9513,10 +9513,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="80" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="72"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9529,8 +9529,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9611,8 +9611,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9625,10 +9625,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="80" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="72"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9641,8 +9641,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="83"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9717,8 +9717,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9747,8 +9747,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11325,8 +11325,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="69"/>
-      <c r="C95" s="70"/>
+      <c r="B95" s="82"/>
+      <c r="C95" s="83"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11339,10 +11339,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="71" t="s">
+      <c r="B96" s="80" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="72"/>
+      <c r="C96" s="81"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11355,8 +11355,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="69"/>
-      <c r="C97" s="70"/>
+      <c r="B97" s="82"/>
+      <c r="C97" s="83"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11515,8 +11515,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="82"/>
+      <c r="C104" s="83"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11529,10 +11529,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="71" t="s">
+      <c r="B105" s="80" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="72"/>
+      <c r="C105" s="81"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11545,8 +11545,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="69"/>
-      <c r="C106" s="70"/>
+      <c r="B106" s="82"/>
+      <c r="C106" s="83"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12051,8 +12051,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="69"/>
-      <c r="C130" s="70"/>
+      <c r="B130" s="82"/>
+      <c r="C130" s="83"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12065,10 +12065,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="71" t="s">
+      <c r="B131" s="80" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="72"/>
+      <c r="C131" s="81"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12081,8 +12081,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="69"/>
-      <c r="C132" s="70"/>
+      <c r="B132" s="82"/>
+      <c r="C132" s="83"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12193,8 +12193,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="82"/>
+      <c r="C137" s="83"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12207,10 +12207,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="71" t="s">
+      <c r="B138" s="80" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="72"/>
+      <c r="C138" s="81"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12223,8 +12223,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="69"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="82"/>
+      <c r="C139" s="83"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12385,8 +12385,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="69"/>
-      <c r="C147" s="70"/>
+      <c r="B147" s="82"/>
+      <c r="C147" s="83"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12399,10 +12399,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="71" t="s">
+      <c r="B148" s="80" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="72"/>
+      <c r="C148" s="81"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12415,8 +12415,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="69"/>
-      <c r="C149" s="70"/>
+      <c r="B149" s="82"/>
+      <c r="C149" s="83"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12577,8 +12577,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="69"/>
-      <c r="C157" s="70"/>
+      <c r="B157" s="82"/>
+      <c r="C157" s="83"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12691,8 +12691,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="69"/>
-      <c r="C163" s="70"/>
+      <c r="B163" s="82"/>
+      <c r="C163" s="83"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12705,10 +12705,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="71" t="s">
+      <c r="B164" s="80" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="72"/>
+      <c r="C164" s="81"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12721,8 +12721,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="69"/>
-      <c r="C165" s="70"/>
+      <c r="B165" s="82"/>
+      <c r="C165" s="83"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -12979,8 +12979,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="69"/>
-      <c r="C177" s="70"/>
+      <c r="B177" s="82"/>
+      <c r="C177" s="83"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -12993,10 +12993,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="71" t="s">
+      <c r="B178" s="80" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="72"/>
+      <c r="C178" s="81"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -13009,8 +13009,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="69"/>
-      <c r="C179" s="70"/>
+      <c r="B179" s="82"/>
+      <c r="C179" s="83"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13075,8 +13075,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="69"/>
-      <c r="C183" s="70"/>
+      <c r="B183" s="82"/>
+      <c r="C183" s="83"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13089,10 +13089,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="71" t="s">
+      <c r="B184" s="80" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="72"/>
+      <c r="C184" s="81"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13105,8 +13105,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="69"/>
-      <c r="C185" s="70"/>
+      <c r="B185" s="82"/>
+      <c r="C185" s="83"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13691,8 +13691,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="69"/>
-      <c r="C211" s="70"/>
+      <c r="B211" s="82"/>
+      <c r="C211" s="83"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13705,10 +13705,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="71" t="s">
+      <c r="B212" s="80" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="72"/>
+      <c r="C212" s="81"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13721,8 +13721,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="69"/>
-      <c r="C213" s="70"/>
+      <c r="B213" s="82"/>
+      <c r="C213" s="83"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13917,8 +13917,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="69"/>
-      <c r="C222" s="70"/>
+      <c r="B222" s="82"/>
+      <c r="C222" s="83"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13931,10 +13931,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="71" t="s">
+      <c r="B223" s="80" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="72"/>
+      <c r="C223" s="81"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -13947,8 +13947,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="69"/>
-      <c r="C224" s="70"/>
+      <c r="B224" s="82"/>
+      <c r="C224" s="83"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16783,8 +16783,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="69"/>
-      <c r="C343" s="70"/>
+      <c r="B343" s="82"/>
+      <c r="C343" s="83"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16797,10 +16797,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="71" t="s">
+      <c r="B344" s="80" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="72"/>
+      <c r="C344" s="81"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16813,8 +16813,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="69"/>
-      <c r="C345" s="70"/>
+      <c r="B345" s="82"/>
+      <c r="C345" s="83"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20439,8 +20439,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="69"/>
-      <c r="C484" s="70"/>
+      <c r="B484" s="82"/>
+      <c r="C484" s="83"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20495,8 +20495,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="69"/>
-      <c r="C487" s="70"/>
+      <c r="B487" s="82"/>
+      <c r="C487" s="83"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20509,10 +20509,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="71" t="s">
+      <c r="B488" s="80" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="72"/>
+      <c r="C488" s="81"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20525,8 +20525,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="69"/>
-      <c r="C489" s="70"/>
+      <c r="B489" s="82"/>
+      <c r="C489" s="83"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22125,8 +22125,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="69"/>
-      <c r="C553" s="70"/>
+      <c r="B553" s="82"/>
+      <c r="C553" s="83"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22139,10 +22139,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="71" t="s">
+      <c r="B554" s="80" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="72"/>
+      <c r="C554" s="81"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22155,8 +22155,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="69"/>
-      <c r="C555" s="70"/>
+      <c r="B555" s="82"/>
+      <c r="C555" s="83"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -25663,7 +25663,7 @@
       </c>
       <c r="E698" s="29"/>
       <c r="F698" s="23">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="G698" s="44" t="s">
         <v>592</v>
@@ -25907,8 +25907,8 @@
     </row>
     <row r="708" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A708" s="29"/>
-      <c r="B708" s="69"/>
-      <c r="C708" s="70"/>
+      <c r="B708" s="82"/>
+      <c r="C708" s="83"/>
       <c r="D708" s="6"/>
       <c r="E708" s="29"/>
       <c r="F708" s="24"/>
@@ -25921,10 +25921,10 @@
     </row>
     <row r="709" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A709" s="29"/>
-      <c r="B709" s="71" t="s">
+      <c r="B709" s="80" t="s">
         <v>1853</v>
       </c>
-      <c r="C709" s="72"/>
+      <c r="C709" s="81"/>
       <c r="D709" s="6"/>
       <c r="E709" s="29"/>
       <c r="F709" s="24"/>
@@ -25937,8 +25937,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="69"/>
-      <c r="C710" s="70"/>
+      <c r="B710" s="82"/>
+      <c r="C710" s="83"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -28395,8 +28395,8 @@
     </row>
     <row r="813" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A813" s="29"/>
-      <c r="B813" s="69"/>
-      <c r="C813" s="70"/>
+      <c r="B813" s="82"/>
+      <c r="C813" s="83"/>
       <c r="D813" s="6"/>
       <c r="E813" s="29"/>
       <c r="F813" s="24"/>
@@ -28409,10 +28409,10 @@
     </row>
     <row r="814" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A814" s="29"/>
-      <c r="B814" s="71" t="s">
+      <c r="B814" s="80" t="s">
         <v>1854</v>
       </c>
-      <c r="C814" s="72"/>
+      <c r="C814" s="81"/>
       <c r="D814" s="6"/>
       <c r="E814" s="29"/>
       <c r="F814" s="24"/>
@@ -28425,8 +28425,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="69"/>
-      <c r="C815" s="70"/>
+      <c r="B815" s="82"/>
+      <c r="C815" s="83"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -31340,8 +31340,8 @@
     </row>
     <row r="929" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A929" s="29"/>
-      <c r="B929" s="69"/>
-      <c r="C929" s="70"/>
+      <c r="B929" s="82"/>
+      <c r="C929" s="83"/>
       <c r="D929" s="6"/>
       <c r="E929" s="29"/>
       <c r="F929" s="24"/>
@@ -31354,10 +31354,10 @@
     </row>
     <row r="930" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A930" s="29"/>
-      <c r="B930" s="71" t="s">
+      <c r="B930" s="80" t="s">
         <v>1952</v>
       </c>
-      <c r="C930" s="72"/>
+      <c r="C930" s="81"/>
       <c r="D930" s="6"/>
       <c r="E930" s="29"/>
       <c r="F930" s="24"/>
@@ -31370,8 +31370,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="69"/>
-      <c r="C931" s="70"/>
+      <c r="B931" s="82"/>
+      <c r="C931" s="83"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31505,8 +31505,8 @@
     </row>
     <row r="937" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A937" s="29"/>
-      <c r="B937" s="69"/>
-      <c r="C937" s="70"/>
+      <c r="B937" s="82"/>
+      <c r="C937" s="83"/>
       <c r="D937" s="6"/>
       <c r="E937" s="29"/>
       <c r="F937" s="24"/>
@@ -31519,10 +31519,10 @@
     </row>
     <row r="938" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A938" s="29"/>
-      <c r="B938" s="71" t="s">
+      <c r="B938" s="80" t="s">
         <v>1855</v>
       </c>
-      <c r="C938" s="72"/>
+      <c r="C938" s="81"/>
       <c r="D938" s="6"/>
       <c r="E938" s="29"/>
       <c r="F938" s="24"/>
@@ -31535,8 +31535,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="69"/>
-      <c r="C939" s="70"/>
+      <c r="B939" s="82"/>
+      <c r="C939" s="83"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -32059,8 +32059,8 @@
     </row>
     <row r="963" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A963" s="29"/>
-      <c r="B963" s="69"/>
-      <c r="C963" s="70"/>
+      <c r="B963" s="82"/>
+      <c r="C963" s="83"/>
       <c r="D963" s="6"/>
       <c r="E963" s="29"/>
       <c r="F963" s="24"/>
@@ -32073,10 +32073,10 @@
     </row>
     <row r="964" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A964" s="29"/>
-      <c r="B964" s="71" t="s">
+      <c r="B964" s="80" t="s">
         <v>1856</v>
       </c>
-      <c r="C964" s="72"/>
+      <c r="C964" s="81"/>
       <c r="D964" s="6"/>
       <c r="E964" s="29"/>
       <c r="F964" s="24"/>
@@ -32089,8 +32089,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="69"/>
-      <c r="C965" s="70"/>
+      <c r="B965" s="82"/>
+      <c r="C965" s="83"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -34999,8 +34999,8 @@
     </row>
     <row r="1078" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1078" s="29"/>
-      <c r="B1078" s="69"/>
-      <c r="C1078" s="70"/>
+      <c r="B1078" s="82"/>
+      <c r="C1078" s="83"/>
       <c r="D1078" s="6"/>
       <c r="E1078" s="29"/>
       <c r="F1078" s="24"/>
@@ -35013,10 +35013,10 @@
     </row>
     <row r="1079" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1079" s="29"/>
-      <c r="B1079" s="71" t="s">
+      <c r="B1079" s="80" t="s">
         <v>1857</v>
       </c>
-      <c r="C1079" s="72"/>
+      <c r="C1079" s="81"/>
       <c r="D1079" s="6"/>
       <c r="E1079" s="29"/>
       <c r="F1079" s="24"/>
@@ -35029,8 +35029,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="69"/>
-      <c r="C1080" s="70"/>
+      <c r="B1080" s="82"/>
+      <c r="C1080" s="83"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35085,8 +35085,8 @@
     </row>
     <row r="1083" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1083" s="29"/>
-      <c r="B1083" s="69"/>
-      <c r="C1083" s="70"/>
+      <c r="B1083" s="82"/>
+      <c r="C1083" s="83"/>
       <c r="D1083" s="6"/>
       <c r="E1083" s="29"/>
       <c r="F1083" s="24"/>
@@ -35099,10 +35099,10 @@
     </row>
     <row r="1084" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1084" s="29"/>
-      <c r="B1084" s="71" t="s">
+      <c r="B1084" s="80" t="s">
         <v>1858</v>
       </c>
-      <c r="C1084" s="72"/>
+      <c r="C1084" s="81"/>
       <c r="D1084" s="6"/>
       <c r="E1084" s="29"/>
       <c r="F1084" s="24"/>
@@ -35115,8 +35115,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="69"/>
-      <c r="C1085" s="70"/>
+      <c r="B1085" s="82"/>
+      <c r="C1085" s="83"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -37605,8 +37605,8 @@
     </row>
     <row r="1192" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1192" s="29"/>
-      <c r="B1192" s="69"/>
-      <c r="C1192" s="70"/>
+      <c r="B1192" s="82"/>
+      <c r="C1192" s="83"/>
       <c r="D1192" s="6"/>
       <c r="E1192" s="29"/>
       <c r="F1192" s="24"/>
@@ -37619,10 +37619,10 @@
     </row>
     <row r="1193" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1193" s="29"/>
-      <c r="B1193" s="71" t="s">
+      <c r="B1193" s="80" t="s">
         <v>2035</v>
       </c>
-      <c r="C1193" s="72"/>
+      <c r="C1193" s="81"/>
       <c r="D1193" s="6"/>
       <c r="E1193" s="29"/>
       <c r="F1193" s="24"/>
@@ -37635,8 +37635,8 @@
     </row>
     <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="69"/>
-      <c r="C1194" s="70"/>
+      <c r="B1194" s="82"/>
+      <c r="C1194" s="83"/>
       <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
       <c r="F1194" s="24"/>
@@ -37881,11 +37881,65 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B488:C488"/>
+    <mergeCell ref="B344:C344"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B343:C343"/>
+    <mergeCell ref="B345:C345"/>
+    <mergeCell ref="B484:C484"/>
+    <mergeCell ref="B487:C487"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B938:C938"/>
+    <mergeCell ref="B930:C930"/>
+    <mergeCell ref="B814:C814"/>
+    <mergeCell ref="B709:C709"/>
+    <mergeCell ref="B554:C554"/>
+    <mergeCell ref="B815:C815"/>
+    <mergeCell ref="B813:C813"/>
+    <mergeCell ref="B929:C929"/>
+    <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B937:C937"/>
+    <mergeCell ref="B1192:C1192"/>
+    <mergeCell ref="B1194:C1194"/>
+    <mergeCell ref="B1193:C1193"/>
+    <mergeCell ref="B1084:C1084"/>
+    <mergeCell ref="B1079:C1079"/>
+    <mergeCell ref="B939:C939"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B963:C963"/>
+    <mergeCell ref="B1083:C1083"/>
+    <mergeCell ref="B1085:C1085"/>
+    <mergeCell ref="B1078:C1078"/>
+    <mergeCell ref="B1080:C1080"/>
+    <mergeCell ref="B964:C964"/>
+    <mergeCell ref="B489:C489"/>
+    <mergeCell ref="B553:C553"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B708:C708"/>
+    <mergeCell ref="B710:C710"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B138:C138"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D2:D3"/>
@@ -37902,65 +37956,11 @@
     <mergeCell ref="B106:C106"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B489:C489"/>
-    <mergeCell ref="B553:C553"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B708:C708"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B963:C963"/>
-    <mergeCell ref="B1083:C1083"/>
-    <mergeCell ref="B1085:C1085"/>
-    <mergeCell ref="B1078:C1078"/>
-    <mergeCell ref="B1080:C1080"/>
-    <mergeCell ref="B964:C964"/>
-    <mergeCell ref="B1192:C1192"/>
-    <mergeCell ref="B1194:C1194"/>
-    <mergeCell ref="B1193:C1193"/>
-    <mergeCell ref="B1084:C1084"/>
-    <mergeCell ref="B1079:C1079"/>
-    <mergeCell ref="B938:C938"/>
-    <mergeCell ref="B930:C930"/>
-    <mergeCell ref="B814:C814"/>
-    <mergeCell ref="B709:C709"/>
-    <mergeCell ref="B554:C554"/>
-    <mergeCell ref="B815:C815"/>
-    <mergeCell ref="B813:C813"/>
-    <mergeCell ref="B929:C929"/>
-    <mergeCell ref="B931:C931"/>
-    <mergeCell ref="B937:C937"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B488:C488"/>
-    <mergeCell ref="B344:C344"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B343:C343"/>
-    <mergeCell ref="B345:C345"/>
-    <mergeCell ref="B484:C484"/>
-    <mergeCell ref="B487:C487"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -37990,80 +37990,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="88" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="88" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="88" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="88" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="87" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="88"/>
+      <c r="I7" s="87"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="86" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38072,62 +38072,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="86" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="88" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="88" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="88" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="88" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="87" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="88"/>
+      <c r="I12" s="87"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="86" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38136,13 +38136,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="86" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38151,13 +38151,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="86" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38166,13 +38166,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="86" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38181,24 +38181,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="86" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="86" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38207,12 +38207,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="86" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38221,13 +38221,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="86" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38236,13 +38236,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="86" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38251,13 +38251,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="86" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38266,53 +38266,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="86" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="88" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="88" t="s">
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="87" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="88"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="86" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="86" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38321,12 +38321,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38335,24 +38335,28 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="87" t="s">
+      <c r="E28" s="86" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38368,16 +38372,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 7 Maret 2023 14:43 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4114" uniqueCount="2066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4134" uniqueCount="2076">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8244,6 +8244,36 @@
   <si>
     <t>userAction.documentWorkFlow.general.
 getBusinessDocumentTypeWorkFlowPathBySubmitterEntityID</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.setUserApprovalAcceptation</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.setUserApprovalPermanentRejection</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.setUserApprovalRejection</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.setUserResubmission</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.setUserSubmission</t>
+  </si>
+  <si>
+    <t>Menyimpan Aksi Submit dari User pada WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>Menyimpan Aksi Resubmit dari User pada WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>Menyimpan Aksi Penerimaan Persetujuan dari User pada WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>Menyimpan Aksi Penolakan Permanen Persetujuan dari User pada WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>Menyimpan Aksi Penolakan Persetujuan dari User pada WorkFlow Dokumen</t>
   </si>
 </sst>
 </file>
@@ -8911,6 +8941,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -8944,31 +8992,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9280,13 +9310,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1208"/>
+  <dimension ref="A1:M1214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D1193" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D1203" sqref="D1203"/>
+      <selection pane="bottomRight" activeCell="C1208" sqref="C1208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9322,31 +9352,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="84" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="73"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="75" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="71"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9368,8 +9398,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9382,10 +9412,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="71" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="81"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9398,8 +9428,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9516,8 +9546,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9530,10 +9560,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="71" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="81"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9546,8 +9576,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9628,8 +9658,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9642,10 +9672,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="71" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="81"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9658,8 +9688,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9734,8 +9764,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9764,8 +9794,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11342,8 +11372,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="82"/>
-      <c r="C95" s="83"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="70"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11356,10 +11386,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="80" t="s">
+      <c r="B96" s="71" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="81"/>
+      <c r="C96" s="72"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11372,8 +11402,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="82"/>
-      <c r="C97" s="83"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="70"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11532,8 +11562,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="82"/>
-      <c r="C104" s="83"/>
+      <c r="B104" s="69"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11546,10 +11576,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="80" t="s">
+      <c r="B105" s="71" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="81"/>
+      <c r="C105" s="72"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11562,8 +11592,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="82"/>
-      <c r="C106" s="83"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="70"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12068,8 +12098,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="82"/>
-      <c r="C130" s="83"/>
+      <c r="B130" s="69"/>
+      <c r="C130" s="70"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12082,10 +12112,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="80" t="s">
+      <c r="B131" s="71" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="81"/>
+      <c r="C131" s="72"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12098,8 +12128,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="82"/>
-      <c r="C132" s="83"/>
+      <c r="B132" s="69"/>
+      <c r="C132" s="70"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12210,8 +12240,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="82"/>
-      <c r="C137" s="83"/>
+      <c r="B137" s="69"/>
+      <c r="C137" s="70"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12224,10 +12254,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="80" t="s">
+      <c r="B138" s="71" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="81"/>
+      <c r="C138" s="72"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12240,8 +12270,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="82"/>
-      <c r="C139" s="83"/>
+      <c r="B139" s="69"/>
+      <c r="C139" s="70"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12402,8 +12432,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="82"/>
-      <c r="C147" s="83"/>
+      <c r="B147" s="69"/>
+      <c r="C147" s="70"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12416,10 +12446,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="80" t="s">
+      <c r="B148" s="71" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="81"/>
+      <c r="C148" s="72"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12432,8 +12462,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="82"/>
-      <c r="C149" s="83"/>
+      <c r="B149" s="69"/>
+      <c r="C149" s="70"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12594,8 +12624,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="82"/>
-      <c r="C157" s="83"/>
+      <c r="B157" s="69"/>
+      <c r="C157" s="70"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12708,8 +12738,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="82"/>
-      <c r="C163" s="83"/>
+      <c r="B163" s="69"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12722,10 +12752,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="80" t="s">
+      <c r="B164" s="71" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="81"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12738,8 +12768,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="82"/>
-      <c r="C165" s="83"/>
+      <c r="B165" s="69"/>
+      <c r="C165" s="70"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -12996,8 +13026,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="82"/>
-      <c r="C177" s="83"/>
+      <c r="B177" s="69"/>
+      <c r="C177" s="70"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -13010,10 +13040,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="80" t="s">
+      <c r="B178" s="71" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="81"/>
+      <c r="C178" s="72"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -13026,8 +13056,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="82"/>
-      <c r="C179" s="83"/>
+      <c r="B179" s="69"/>
+      <c r="C179" s="70"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13092,8 +13122,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="82"/>
-      <c r="C183" s="83"/>
+      <c r="B183" s="69"/>
+      <c r="C183" s="70"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13106,10 +13136,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="80" t="s">
+      <c r="B184" s="71" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="81"/>
+      <c r="C184" s="72"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13122,8 +13152,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="82"/>
-      <c r="C185" s="83"/>
+      <c r="B185" s="69"/>
+      <c r="C185" s="70"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13708,8 +13738,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="82"/>
-      <c r="C211" s="83"/>
+      <c r="B211" s="69"/>
+      <c r="C211" s="70"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13722,10 +13752,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="80" t="s">
+      <c r="B212" s="71" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="81"/>
+      <c r="C212" s="72"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13738,8 +13768,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="82"/>
-      <c r="C213" s="83"/>
+      <c r="B213" s="69"/>
+      <c r="C213" s="70"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13934,8 +13964,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="82"/>
-      <c r="C222" s="83"/>
+      <c r="B222" s="69"/>
+      <c r="C222" s="70"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13948,10 +13978,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="80" t="s">
+      <c r="B223" s="71" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="81"/>
+      <c r="C223" s="72"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -13964,8 +13994,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="82"/>
-      <c r="C224" s="83"/>
+      <c r="B224" s="69"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16800,8 +16830,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="82"/>
-      <c r="C343" s="83"/>
+      <c r="B343" s="69"/>
+      <c r="C343" s="70"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16814,10 +16844,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="80" t="s">
+      <c r="B344" s="71" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="81"/>
+      <c r="C344" s="72"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16830,8 +16860,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="82"/>
-      <c r="C345" s="83"/>
+      <c r="B345" s="69"/>
+      <c r="C345" s="70"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20456,8 +20486,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="82"/>
-      <c r="C484" s="83"/>
+      <c r="B484" s="69"/>
+      <c r="C484" s="70"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20512,8 +20542,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="82"/>
-      <c r="C487" s="83"/>
+      <c r="B487" s="69"/>
+      <c r="C487" s="70"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20526,10 +20556,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="80" t="s">
+      <c r="B488" s="71" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="81"/>
+      <c r="C488" s="72"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20542,8 +20572,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="82"/>
-      <c r="C489" s="83"/>
+      <c r="B489" s="69"/>
+      <c r="C489" s="70"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22142,8 +22172,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="82"/>
-      <c r="C553" s="83"/>
+      <c r="B553" s="69"/>
+      <c r="C553" s="70"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22156,10 +22186,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="80" t="s">
+      <c r="B554" s="71" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="81"/>
+      <c r="C554" s="72"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22172,8 +22202,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="82"/>
-      <c r="C555" s="83"/>
+      <c r="B555" s="69"/>
+      <c r="C555" s="70"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -25972,8 +26002,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="82"/>
-      <c r="C710" s="83"/>
+      <c r="B710" s="69"/>
+      <c r="C710" s="70"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -25986,10 +26016,10 @@
     </row>
     <row r="711" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A711" s="29"/>
-      <c r="B711" s="80" t="s">
+      <c r="B711" s="71" t="s">
         <v>1853</v>
       </c>
-      <c r="C711" s="81"/>
+      <c r="C711" s="72"/>
       <c r="D711" s="6"/>
       <c r="E711" s="29"/>
       <c r="F711" s="24"/>
@@ -26002,8 +26032,8 @@
     </row>
     <row r="712" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712" s="29"/>
-      <c r="B712" s="82"/>
-      <c r="C712" s="83"/>
+      <c r="B712" s="69"/>
+      <c r="C712" s="70"/>
       <c r="D712" s="6"/>
       <c r="E712" s="29"/>
       <c r="F712" s="24"/>
@@ -28460,8 +28490,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="82"/>
-      <c r="C815" s="83"/>
+      <c r="B815" s="69"/>
+      <c r="C815" s="70"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -28474,10 +28504,10 @@
     </row>
     <row r="816" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A816" s="29"/>
-      <c r="B816" s="80" t="s">
+      <c r="B816" s="71" t="s">
         <v>1854</v>
       </c>
-      <c r="C816" s="81"/>
+      <c r="C816" s="72"/>
       <c r="D816" s="6"/>
       <c r="E816" s="29"/>
       <c r="F816" s="24"/>
@@ -28490,8 +28520,8 @@
     </row>
     <row r="817" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817" s="29"/>
-      <c r="B817" s="82"/>
-      <c r="C817" s="83"/>
+      <c r="B817" s="69"/>
+      <c r="C817" s="70"/>
       <c r="D817" s="6"/>
       <c r="E817" s="29"/>
       <c r="F817" s="24"/>
@@ -31405,8 +31435,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="82"/>
-      <c r="C931" s="83"/>
+      <c r="B931" s="69"/>
+      <c r="C931" s="70"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31419,10 +31449,10 @@
     </row>
     <row r="932" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A932" s="29"/>
-      <c r="B932" s="80" t="s">
+      <c r="B932" s="71" t="s">
         <v>1952</v>
       </c>
-      <c r="C932" s="81"/>
+      <c r="C932" s="72"/>
       <c r="D932" s="6"/>
       <c r="E932" s="29"/>
       <c r="F932" s="24"/>
@@ -31435,8 +31465,8 @@
     </row>
     <row r="933" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933" s="29"/>
-      <c r="B933" s="82"/>
-      <c r="C933" s="83"/>
+      <c r="B933" s="69"/>
+      <c r="C933" s="70"/>
       <c r="D933" s="6"/>
       <c r="E933" s="29"/>
       <c r="F933" s="24"/>
@@ -31570,8 +31600,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="82"/>
-      <c r="C939" s="83"/>
+      <c r="B939" s="69"/>
+      <c r="C939" s="70"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -31584,10 +31614,10 @@
     </row>
     <row r="940" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A940" s="29"/>
-      <c r="B940" s="80" t="s">
+      <c r="B940" s="71" t="s">
         <v>1855</v>
       </c>
-      <c r="C940" s="81"/>
+      <c r="C940" s="72"/>
       <c r="D940" s="6"/>
       <c r="E940" s="29"/>
       <c r="F940" s="24"/>
@@ -31600,8 +31630,8 @@
     </row>
     <row r="941" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941" s="29"/>
-      <c r="B941" s="82"/>
-      <c r="C941" s="83"/>
+      <c r="B941" s="69"/>
+      <c r="C941" s="70"/>
       <c r="D941" s="6"/>
       <c r="E941" s="29"/>
       <c r="F941" s="24"/>
@@ -32124,8 +32154,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="82"/>
-      <c r="C965" s="83"/>
+      <c r="B965" s="69"/>
+      <c r="C965" s="70"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -32138,10 +32168,10 @@
     </row>
     <row r="966" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A966" s="29"/>
-      <c r="B966" s="80" t="s">
+      <c r="B966" s="71" t="s">
         <v>1856</v>
       </c>
-      <c r="C966" s="81"/>
+      <c r="C966" s="72"/>
       <c r="D966" s="6"/>
       <c r="E966" s="29"/>
       <c r="F966" s="24"/>
@@ -32154,8 +32184,8 @@
     </row>
     <row r="967" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967" s="29"/>
-      <c r="B967" s="82"/>
-      <c r="C967" s="83"/>
+      <c r="B967" s="69"/>
+      <c r="C967" s="70"/>
       <c r="D967" s="6"/>
       <c r="E967" s="29"/>
       <c r="F967" s="24"/>
@@ -35064,8 +35094,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="82"/>
-      <c r="C1080" s="83"/>
+      <c r="B1080" s="69"/>
+      <c r="C1080" s="70"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35078,10 +35108,10 @@
     </row>
     <row r="1081" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1081" s="29"/>
-      <c r="B1081" s="80" t="s">
+      <c r="B1081" s="71" t="s">
         <v>1857</v>
       </c>
-      <c r="C1081" s="81"/>
+      <c r="C1081" s="72"/>
       <c r="D1081" s="6"/>
       <c r="E1081" s="29"/>
       <c r="F1081" s="24"/>
@@ -35094,8 +35124,8 @@
     </row>
     <row r="1082" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="29"/>
-      <c r="B1082" s="82"/>
-      <c r="C1082" s="83"/>
+      <c r="B1082" s="69"/>
+      <c r="C1082" s="70"/>
       <c r="D1082" s="6"/>
       <c r="E1082" s="29"/>
       <c r="F1082" s="24"/>
@@ -35150,8 +35180,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="82"/>
-      <c r="C1085" s="83"/>
+      <c r="B1085" s="69"/>
+      <c r="C1085" s="70"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -35164,10 +35194,10 @@
     </row>
     <row r="1086" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1086" s="29"/>
-      <c r="B1086" s="80" t="s">
+      <c r="B1086" s="71" t="s">
         <v>1858</v>
       </c>
-      <c r="C1086" s="81"/>
+      <c r="C1086" s="72"/>
       <c r="D1086" s="6"/>
       <c r="E1086" s="29"/>
       <c r="F1086" s="24"/>
@@ -35180,8 +35210,8 @@
     </row>
     <row r="1087" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1087" s="29"/>
-      <c r="B1087" s="82"/>
-      <c r="C1087" s="83"/>
+      <c r="B1087" s="69"/>
+      <c r="C1087" s="70"/>
       <c r="D1087" s="6"/>
       <c r="E1087" s="29"/>
       <c r="F1087" s="24"/>
@@ -37670,8 +37700,8 @@
     </row>
     <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="82"/>
-      <c r="C1194" s="83"/>
+      <c r="B1194" s="69"/>
+      <c r="C1194" s="70"/>
       <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
       <c r="F1194" s="24"/>
@@ -37684,10 +37714,10 @@
     </row>
     <row r="1195" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1195" s="29"/>
-      <c r="B1195" s="80" t="s">
+      <c r="B1195" s="71" t="s">
         <v>2035</v>
       </c>
-      <c r="C1195" s="81"/>
+      <c r="C1195" s="72"/>
       <c r="D1195" s="6"/>
       <c r="E1195" s="29"/>
       <c r="F1195" s="24"/>
@@ -37700,8 +37730,8 @@
     </row>
     <row r="1196" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1196" s="29"/>
-      <c r="B1196" s="82"/>
-      <c r="C1196" s="83"/>
+      <c r="B1196" s="69"/>
+      <c r="C1196" s="70"/>
       <c r="D1196" s="6"/>
       <c r="E1196" s="29"/>
       <c r="F1196" s="24"/>
@@ -37790,17 +37820,17 @@
         <v>2047</v>
       </c>
       <c r="C1200" s="54" t="s">
-        <v>2031</v>
+        <v>2066</v>
       </c>
       <c r="D1200" s="3" t="s">
-        <v>2034</v>
+        <v>2073</v>
       </c>
       <c r="E1200" s="29"/>
       <c r="F1200" s="23">
-        <v>44987</v>
+        <v>44992</v>
       </c>
       <c r="G1200" s="44" t="s">
-        <v>2046</v>
+        <v>592</v>
       </c>
       <c r="H1200" s="29"/>
       <c r="I1200" s="23"/>
@@ -37808,20 +37838,20 @@
       <c r="K1200" s="14"/>
       <c r="L1200" s="29"/>
     </row>
-    <row r="1201" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1201" s="29"/>
       <c r="B1201" s="56" t="s">
         <v>2047</v>
       </c>
       <c r="C1201" s="54" t="s">
-        <v>2064</v>
+        <v>2067</v>
       </c>
       <c r="D1201" s="3" t="s">
-        <v>2045</v>
+        <v>2074</v>
       </c>
       <c r="E1201" s="29"/>
       <c r="F1201" s="23">
-        <v>44987</v>
+        <v>44992</v>
       </c>
       <c r="G1201" s="44" t="s">
         <v>592</v>
@@ -37832,23 +37862,23 @@
       <c r="K1201" s="14"/>
       <c r="L1201" s="29"/>
     </row>
-    <row r="1202" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1202" s="29"/>
       <c r="B1202" s="56" t="s">
         <v>2047</v>
       </c>
       <c r="C1202" s="54" t="s">
-        <v>2065</v>
+        <v>2068</v>
       </c>
       <c r="D1202" s="3" t="s">
-        <v>2036</v>
+        <v>2075</v>
       </c>
       <c r="E1202" s="29"/>
       <c r="F1202" s="23">
-        <v>44987</v>
+        <v>44992</v>
       </c>
       <c r="G1202" s="44" t="s">
-        <v>2046</v>
+        <v>592</v>
       </c>
       <c r="H1202" s="29"/>
       <c r="I1202" s="23"/>
@@ -37856,20 +37886,20 @@
       <c r="K1202" s="14"/>
       <c r="L1202" s="29"/>
     </row>
-    <row r="1203" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1203" s="29"/>
       <c r="B1203" s="56" t="s">
         <v>2047</v>
       </c>
       <c r="C1203" s="54" t="s">
-        <v>2048</v>
+        <v>2069</v>
       </c>
       <c r="D1203" s="3" t="s">
-        <v>2063</v>
+        <v>2071</v>
       </c>
       <c r="E1203" s="29"/>
       <c r="F1203" s="23">
-        <v>44987</v>
+        <v>44992</v>
       </c>
       <c r="G1203" s="44" t="s">
         <v>592</v>
@@ -37886,14 +37916,14 @@
         <v>2047</v>
       </c>
       <c r="C1204" s="54" t="s">
-        <v>2037</v>
+        <v>2070</v>
       </c>
       <c r="D1204" s="3" t="s">
-        <v>2040</v>
+        <v>2072</v>
       </c>
       <c r="E1204" s="29"/>
       <c r="F1204" s="23">
-        <v>44972</v>
+        <v>44992</v>
       </c>
       <c r="G1204" s="44" t="s">
         <v>592</v>
@@ -37904,54 +37934,252 @@
       <c r="K1204" s="14"/>
       <c r="L1204" s="29"/>
     </row>
-    <row r="1205" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1205" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1205" s="29"/>
-      <c r="B1205" s="60"/>
-      <c r="C1205" s="67"/>
-      <c r="D1205" s="5"/>
+      <c r="B1205" s="59"/>
+      <c r="C1205" s="64"/>
+      <c r="D1205" s="7"/>
       <c r="E1205" s="29"/>
-      <c r="F1205" s="27"/>
-      <c r="G1205" s="47"/>
+      <c r="F1205" s="26"/>
+      <c r="G1205" s="46"/>
       <c r="H1205" s="29"/>
-      <c r="I1205" s="27"/>
-      <c r="J1205" s="19"/>
-      <c r="K1205" s="20"/>
+      <c r="I1205" s="26"/>
+      <c r="J1205" s="17"/>
+      <c r="K1205" s="18"/>
       <c r="L1205" s="29"/>
     </row>
-    <row r="1206" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1206" s="29"/>
-      <c r="B1206" s="55"/>
-      <c r="C1206" s="62"/>
-      <c r="D1206" s="32"/>
+      <c r="B1206" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1206" s="54" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D1206" s="3" t="s">
+        <v>2034</v>
+      </c>
       <c r="E1206" s="29"/>
-      <c r="F1206" s="33"/>
-      <c r="G1206" s="41"/>
+      <c r="F1206" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1206" s="44" t="s">
+        <v>2046</v>
+      </c>
       <c r="H1206" s="29"/>
-      <c r="I1206" s="33"/>
-      <c r="J1206" s="34"/>
-      <c r="K1206" s="34"/>
+      <c r="I1206" s="23"/>
+      <c r="J1206" s="13"/>
+      <c r="K1206" s="14"/>
       <c r="L1206" s="29"/>
     </row>
-    <row r="1208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1207" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1207" s="29"/>
+      <c r="B1207" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1207" s="54" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D1207" s="3" t="s">
+        <v>2045</v>
+      </c>
+      <c r="E1207" s="29"/>
+      <c r="F1207" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1207" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="H1207" s="29"/>
+      <c r="I1207" s="23"/>
+      <c r="J1207" s="13"/>
+      <c r="K1207" s="14"/>
+      <c r="L1207" s="29"/>
+    </row>
+    <row r="1208" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1208" s="29"/>
-      <c r="B1208" s="55"/>
+      <c r="B1208" s="56" t="s">
+        <v>2047</v>
+      </c>
       <c r="C1208" s="54" t="s">
-        <v>364</v>
+        <v>2065</v>
       </c>
       <c r="D1208" s="3" t="s">
-        <v>365</v>
+        <v>2036</v>
       </c>
       <c r="E1208" s="29"/>
-      <c r="F1208" s="23"/>
-      <c r="G1208" s="44"/>
+      <c r="F1208" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1208" s="44" t="s">
+        <v>2046</v>
+      </c>
       <c r="H1208" s="29"/>
       <c r="I1208" s="23"/>
       <c r="J1208" s="13"/>
       <c r="K1208" s="14"/>
       <c r="L1208" s="29"/>
     </row>
+    <row r="1209" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1209" s="29"/>
+      <c r="B1209" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1209" s="54" t="s">
+        <v>2048</v>
+      </c>
+      <c r="D1209" s="3" t="s">
+        <v>2063</v>
+      </c>
+      <c r="E1209" s="29"/>
+      <c r="F1209" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1209" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="H1209" s="29"/>
+      <c r="I1209" s="23"/>
+      <c r="J1209" s="13"/>
+      <c r="K1209" s="14"/>
+      <c r="L1209" s="29"/>
+    </row>
+    <row r="1210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1210" s="29"/>
+      <c r="B1210" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1210" s="54" t="s">
+        <v>2037</v>
+      </c>
+      <c r="D1210" s="3" t="s">
+        <v>2040</v>
+      </c>
+      <c r="E1210" s="29"/>
+      <c r="F1210" s="23">
+        <v>44972</v>
+      </c>
+      <c r="G1210" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="H1210" s="29"/>
+      <c r="I1210" s="23"/>
+      <c r="J1210" s="13"/>
+      <c r="K1210" s="14"/>
+      <c r="L1210" s="29"/>
+    </row>
+    <row r="1211" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1211" s="29"/>
+      <c r="B1211" s="60"/>
+      <c r="C1211" s="67"/>
+      <c r="D1211" s="5"/>
+      <c r="E1211" s="29"/>
+      <c r="F1211" s="27"/>
+      <c r="G1211" s="47"/>
+      <c r="H1211" s="29"/>
+      <c r="I1211" s="27"/>
+      <c r="J1211" s="19"/>
+      <c r="K1211" s="20"/>
+      <c r="L1211" s="29"/>
+    </row>
+    <row r="1212" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1212" s="29"/>
+      <c r="B1212" s="55"/>
+      <c r="C1212" s="62"/>
+      <c r="D1212" s="32"/>
+      <c r="E1212" s="29"/>
+      <c r="F1212" s="33"/>
+      <c r="G1212" s="41"/>
+      <c r="H1212" s="29"/>
+      <c r="I1212" s="33"/>
+      <c r="J1212" s="34"/>
+      <c r="K1212" s="34"/>
+      <c r="L1212" s="29"/>
+    </row>
+    <row r="1214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1214" s="29"/>
+      <c r="B1214" s="55"/>
+      <c r="C1214" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1214" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1214" s="29"/>
+      <c r="F1214" s="23"/>
+      <c r="G1214" s="44"/>
+      <c r="H1214" s="29"/>
+      <c r="I1214" s="23"/>
+      <c r="J1214" s="13"/>
+      <c r="K1214" s="14"/>
+      <c r="L1214" s="29"/>
+    </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B489:C489"/>
+    <mergeCell ref="B553:C553"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B710:C710"/>
+    <mergeCell ref="B712:C712"/>
+    <mergeCell ref="B941:C941"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B1085:C1085"/>
+    <mergeCell ref="B1087:C1087"/>
+    <mergeCell ref="B1080:C1080"/>
+    <mergeCell ref="B1082:C1082"/>
+    <mergeCell ref="B966:C966"/>
+    <mergeCell ref="B1194:C1194"/>
+    <mergeCell ref="B1196:C1196"/>
+    <mergeCell ref="B1195:C1195"/>
+    <mergeCell ref="B1086:C1086"/>
+    <mergeCell ref="B1081:C1081"/>
+    <mergeCell ref="B940:C940"/>
+    <mergeCell ref="B932:C932"/>
+    <mergeCell ref="B816:C816"/>
+    <mergeCell ref="B711:C711"/>
+    <mergeCell ref="B554:C554"/>
+    <mergeCell ref="B817:C817"/>
+    <mergeCell ref="B815:C815"/>
+    <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B933:C933"/>
+    <mergeCell ref="B939:C939"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B23:C23"/>
@@ -37968,75 +38196,11 @@
     <mergeCell ref="B487:C487"/>
     <mergeCell ref="B183:C183"/>
     <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B940:C940"/>
-    <mergeCell ref="B932:C932"/>
-    <mergeCell ref="B816:C816"/>
-    <mergeCell ref="B711:C711"/>
-    <mergeCell ref="B554:C554"/>
-    <mergeCell ref="B817:C817"/>
-    <mergeCell ref="B815:C815"/>
-    <mergeCell ref="B931:C931"/>
-    <mergeCell ref="B933:C933"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B1194:C1194"/>
-    <mergeCell ref="B1196:C1196"/>
-    <mergeCell ref="B1195:C1195"/>
-    <mergeCell ref="B1086:C1086"/>
-    <mergeCell ref="B1081:C1081"/>
-    <mergeCell ref="B941:C941"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B1085:C1085"/>
-    <mergeCell ref="B1087:C1087"/>
-    <mergeCell ref="B1080:C1080"/>
-    <mergeCell ref="B1082:C1082"/>
-    <mergeCell ref="B966:C966"/>
-    <mergeCell ref="B489:C489"/>
-    <mergeCell ref="B553:C553"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B712:C712"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G14 G102 G133:G134 G136 G143:G145 G214:G220 G225:G230 G346:G350 G352:G356 G366:G368 G384 G458:G460 G798:G800 G829:G830 G944:G946 G948 G950:G954 G956:G959 G961:G962 G974:G979 G981:G983 G992:G993 G377:G378 G999 G1054:G1056 G968:G972 G1095:G1097 G312:G315 G1168:G1171 G902:G905 G818:G820 G317:G319 G1173:G1175 G209 G186 G128 G108 G232:G239 G490:G492 G370:G375 G985:G990 G832:G837 G180 G79:G81 G158:G159 G56 G406 G822:G827 G358:G364 G1088:G1093 G793:G796 G942 G853 G1006 G161 G166:G174 G188:G207 G298:G308 G1154:G1164 G1011:G1052 G858:G900 G411:G456 G76:G77 G485 G1072 F1069:G1071 G29:G37 G463:G476 G339:G341 G1190:G1192 G480:G482 G1076:G1078 G927:G929 G813 G93 G1083 G150:G153 G1059:G1068 G911:G925 G544:G551 G532:G535 G808:G811 G849:G851 G386:G404 G1001:G1004 G907:G909 G49 G60 G786:G789 G155 G584:G585 G855:G856 G621:G622 G1008:G1009 G1121:G1122 G505:G506 G408:G409 G265:G266 G650:G652 G637:G643 G647:G648 G624:G627 G70:G72 G88:G91 G322:G334 G802:G805 G1178:G1184 G538:G542 G680:G682 G665 G573 G618:G619 G605:G607 G752:G755 G83:G86 G761:G762 G58 G757:G759 G570 G705:G710 G721:G734 G655:G663 G283:G296 G1139:G1152 G770:G777 G68 G736:G742 G513:G524 G508:G511 G1124:G1137 G268:G281 G764:G768 G526:G530 G749 G779:G784 G98:G99 G686:G691" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G14 G102 G133:G134 G136 G143:G145 G214:G220 G225:G230 G346:G350 G352:G356 G366:G368 G384 G458:G460 G798:G800 G829:G830 G944:G946 G948 G950:G954 G956:G959 G961:G962 G974:G979 G981:G983 G992:G993 G377:G378 G999 G1054:G1056 G968:G972 G1095:G1097 G312:G315 G1168:G1171 G902:G905 G818:G820 G317:G319 G1173:G1175 G209 G186 G128 G108 G232:G239 G490:G492 G370:G375 G985:G990 G832:G837 G180 G79:G81 G158:G159 G56 G406 G822:G827 G358:G364 G1088:G1093 G793:G796 G942 G853 G1006 G161 G166:G174 G188:G207 G298:G308 G1154:G1164 G1011:G1052 G858:G900 G411:G456 G76:G77 G485 G1072 F1069:G1071 G29:G37 G463:G476 G339:G341 G1190:G1192 G480:G482 G1076:G1078 G927:G929 G813 G93 G1083 G150:G153 G1059:G1068 G911:G925 G544:G551 G532:G535 G808:G811 G849:G851 G386:G404 G1001:G1004 G907:G909 G49 G60 G786:G789 G155 G584:G585 G855:G856 G621:G622 G1008:G1009 G1121:G1122 G505:G506 G408:G409 G265:G266 G650:G652 G637:G643 G647:G648 G624:G627 G70:G72 G88:G91 G322:G334 G802:G805 G1178:G1184 G538:G542 G680:G682 G665 G573 G618:G619 G605:G607 G752:G755 G83:G86 G761:G762 G58 G757:G759 G570 G705:G710 G721:G734 G655:G663 G283:G296 G1139:G1152 G770:G777 G68 G736:G742 G513:G524 G508:G511 G1124:G1137 G268:G281 G764:G768 G526:G530 G749 G779:G784 G98:G99 G686:G691 G1197:G1210" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -38061,80 +38225,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38143,62 +38307,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38207,13 +38371,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38222,13 +38386,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38237,13 +38401,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38252,24 +38416,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38278,12 +38442,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38292,13 +38456,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38307,13 +38471,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38322,13 +38486,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38337,53 +38501,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38392,12 +38556,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38406,28 +38570,24 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38443,12 +38603,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 9 Maret 2023 08:44 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -8941,24 +8941,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -8992,13 +8974,31 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9352,31 +9352,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="73" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="84" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="72" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="73"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="75" t="s">
+      <c r="I2" s="69" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="76"/>
-      <c r="K2" s="77"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="74"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9398,8 +9398,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9412,10 +9412,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="80" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9428,8 +9428,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9546,8 +9546,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9560,10 +9560,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="80" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="72"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9576,8 +9576,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9658,8 +9658,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9672,10 +9672,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="80" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="72"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9688,8 +9688,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="83"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9764,8 +9764,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9794,8 +9794,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11372,8 +11372,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="69"/>
-      <c r="C95" s="70"/>
+      <c r="B95" s="82"/>
+      <c r="C95" s="83"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11386,10 +11386,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="71" t="s">
+      <c r="B96" s="80" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="72"/>
+      <c r="C96" s="81"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11402,8 +11402,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="69"/>
-      <c r="C97" s="70"/>
+      <c r="B97" s="82"/>
+      <c r="C97" s="83"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11562,8 +11562,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="82"/>
+      <c r="C104" s="83"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11576,10 +11576,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="71" t="s">
+      <c r="B105" s="80" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="72"/>
+      <c r="C105" s="81"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11592,8 +11592,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="69"/>
-      <c r="C106" s="70"/>
+      <c r="B106" s="82"/>
+      <c r="C106" s="83"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12098,8 +12098,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="69"/>
-      <c r="C130" s="70"/>
+      <c r="B130" s="82"/>
+      <c r="C130" s="83"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12112,10 +12112,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="71" t="s">
+      <c r="B131" s="80" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="72"/>
+      <c r="C131" s="81"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12128,8 +12128,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="69"/>
-      <c r="C132" s="70"/>
+      <c r="B132" s="82"/>
+      <c r="C132" s="83"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12240,8 +12240,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="82"/>
+      <c r="C137" s="83"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12254,10 +12254,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="71" t="s">
+      <c r="B138" s="80" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="72"/>
+      <c r="C138" s="81"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12270,8 +12270,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="69"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="82"/>
+      <c r="C139" s="83"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12432,8 +12432,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="69"/>
-      <c r="C147" s="70"/>
+      <c r="B147" s="82"/>
+      <c r="C147" s="83"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12446,10 +12446,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="71" t="s">
+      <c r="B148" s="80" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="72"/>
+      <c r="C148" s="81"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12462,8 +12462,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="69"/>
-      <c r="C149" s="70"/>
+      <c r="B149" s="82"/>
+      <c r="C149" s="83"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12624,8 +12624,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="69"/>
-      <c r="C157" s="70"/>
+      <c r="B157" s="82"/>
+      <c r="C157" s="83"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12738,8 +12738,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="69"/>
-      <c r="C163" s="70"/>
+      <c r="B163" s="82"/>
+      <c r="C163" s="83"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12752,10 +12752,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="71" t="s">
+      <c r="B164" s="80" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="72"/>
+      <c r="C164" s="81"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12768,8 +12768,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="69"/>
-      <c r="C165" s="70"/>
+      <c r="B165" s="82"/>
+      <c r="C165" s="83"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -13026,8 +13026,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="69"/>
-      <c r="C177" s="70"/>
+      <c r="B177" s="82"/>
+      <c r="C177" s="83"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -13040,10 +13040,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="71" t="s">
+      <c r="B178" s="80" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="72"/>
+      <c r="C178" s="81"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -13056,8 +13056,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="69"/>
-      <c r="C179" s="70"/>
+      <c r="B179" s="82"/>
+      <c r="C179" s="83"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13122,8 +13122,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="69"/>
-      <c r="C183" s="70"/>
+      <c r="B183" s="82"/>
+      <c r="C183" s="83"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13136,10 +13136,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="71" t="s">
+      <c r="B184" s="80" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="72"/>
+      <c r="C184" s="81"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13152,8 +13152,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="69"/>
-      <c r="C185" s="70"/>
+      <c r="B185" s="82"/>
+      <c r="C185" s="83"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13738,8 +13738,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="69"/>
-      <c r="C211" s="70"/>
+      <c r="B211" s="82"/>
+      <c r="C211" s="83"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13752,10 +13752,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="71" t="s">
+      <c r="B212" s="80" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="72"/>
+      <c r="C212" s="81"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13768,8 +13768,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="69"/>
-      <c r="C213" s="70"/>
+      <c r="B213" s="82"/>
+      <c r="C213" s="83"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13964,8 +13964,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="69"/>
-      <c r="C222" s="70"/>
+      <c r="B222" s="82"/>
+      <c r="C222" s="83"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13978,10 +13978,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="71" t="s">
+      <c r="B223" s="80" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="72"/>
+      <c r="C223" s="81"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -13994,8 +13994,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="69"/>
-      <c r="C224" s="70"/>
+      <c r="B224" s="82"/>
+      <c r="C224" s="83"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16830,8 +16830,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="69"/>
-      <c r="C343" s="70"/>
+      <c r="B343" s="82"/>
+      <c r="C343" s="83"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16844,10 +16844,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="71" t="s">
+      <c r="B344" s="80" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="72"/>
+      <c r="C344" s="81"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16860,8 +16860,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="69"/>
-      <c r="C345" s="70"/>
+      <c r="B345" s="82"/>
+      <c r="C345" s="83"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20486,8 +20486,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="69"/>
-      <c r="C484" s="70"/>
+      <c r="B484" s="82"/>
+      <c r="C484" s="83"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20542,8 +20542,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="69"/>
-      <c r="C487" s="70"/>
+      <c r="B487" s="82"/>
+      <c r="C487" s="83"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20556,10 +20556,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="71" t="s">
+      <c r="B488" s="80" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="72"/>
+      <c r="C488" s="81"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20572,8 +20572,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="69"/>
-      <c r="C489" s="70"/>
+      <c r="B489" s="82"/>
+      <c r="C489" s="83"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22172,8 +22172,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="69"/>
-      <c r="C553" s="70"/>
+      <c r="B553" s="82"/>
+      <c r="C553" s="83"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22186,10 +22186,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="71" t="s">
+      <c r="B554" s="80" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="72"/>
+      <c r="C554" s="81"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22202,8 +22202,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="69"/>
-      <c r="C555" s="70"/>
+      <c r="B555" s="82"/>
+      <c r="C555" s="83"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -26002,8 +26002,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="69"/>
-      <c r="C710" s="70"/>
+      <c r="B710" s="82"/>
+      <c r="C710" s="83"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -26016,10 +26016,10 @@
     </row>
     <row r="711" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A711" s="29"/>
-      <c r="B711" s="71" t="s">
+      <c r="B711" s="80" t="s">
         <v>1853</v>
       </c>
-      <c r="C711" s="72"/>
+      <c r="C711" s="81"/>
       <c r="D711" s="6"/>
       <c r="E711" s="29"/>
       <c r="F711" s="24"/>
@@ -26032,8 +26032,8 @@
     </row>
     <row r="712" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712" s="29"/>
-      <c r="B712" s="69"/>
-      <c r="C712" s="70"/>
+      <c r="B712" s="82"/>
+      <c r="C712" s="83"/>
       <c r="D712" s="6"/>
       <c r="E712" s="29"/>
       <c r="F712" s="24"/>
@@ -28490,8 +28490,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="69"/>
-      <c r="C815" s="70"/>
+      <c r="B815" s="82"/>
+      <c r="C815" s="83"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -28504,10 +28504,10 @@
     </row>
     <row r="816" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A816" s="29"/>
-      <c r="B816" s="71" t="s">
+      <c r="B816" s="80" t="s">
         <v>1854</v>
       </c>
-      <c r="C816" s="72"/>
+      <c r="C816" s="81"/>
       <c r="D816" s="6"/>
       <c r="E816" s="29"/>
       <c r="F816" s="24"/>
@@ -28520,8 +28520,8 @@
     </row>
     <row r="817" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817" s="29"/>
-      <c r="B817" s="69"/>
-      <c r="C817" s="70"/>
+      <c r="B817" s="82"/>
+      <c r="C817" s="83"/>
       <c r="D817" s="6"/>
       <c r="E817" s="29"/>
       <c r="F817" s="24"/>
@@ -31435,8 +31435,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="69"/>
-      <c r="C931" s="70"/>
+      <c r="B931" s="82"/>
+      <c r="C931" s="83"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31449,10 +31449,10 @@
     </row>
     <row r="932" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A932" s="29"/>
-      <c r="B932" s="71" t="s">
+      <c r="B932" s="80" t="s">
         <v>1952</v>
       </c>
-      <c r="C932" s="72"/>
+      <c r="C932" s="81"/>
       <c r="D932" s="6"/>
       <c r="E932" s="29"/>
       <c r="F932" s="24"/>
@@ -31465,8 +31465,8 @@
     </row>
     <row r="933" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933" s="29"/>
-      <c r="B933" s="69"/>
-      <c r="C933" s="70"/>
+      <c r="B933" s="82"/>
+      <c r="C933" s="83"/>
       <c r="D933" s="6"/>
       <c r="E933" s="29"/>
       <c r="F933" s="24"/>
@@ -31600,8 +31600,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="69"/>
-      <c r="C939" s="70"/>
+      <c r="B939" s="82"/>
+      <c r="C939" s="83"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -31614,10 +31614,10 @@
     </row>
     <row r="940" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A940" s="29"/>
-      <c r="B940" s="71" t="s">
+      <c r="B940" s="80" t="s">
         <v>1855</v>
       </c>
-      <c r="C940" s="72"/>
+      <c r="C940" s="81"/>
       <c r="D940" s="6"/>
       <c r="E940" s="29"/>
       <c r="F940" s="24"/>
@@ -31630,8 +31630,8 @@
     </row>
     <row r="941" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941" s="29"/>
-      <c r="B941" s="69"/>
-      <c r="C941" s="70"/>
+      <c r="B941" s="82"/>
+      <c r="C941" s="83"/>
       <c r="D941" s="6"/>
       <c r="E941" s="29"/>
       <c r="F941" s="24"/>
@@ -32154,8 +32154,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="69"/>
-      <c r="C965" s="70"/>
+      <c r="B965" s="82"/>
+      <c r="C965" s="83"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -32168,10 +32168,10 @@
     </row>
     <row r="966" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A966" s="29"/>
-      <c r="B966" s="71" t="s">
+      <c r="B966" s="80" t="s">
         <v>1856</v>
       </c>
-      <c r="C966" s="72"/>
+      <c r="C966" s="81"/>
       <c r="D966" s="6"/>
       <c r="E966" s="29"/>
       <c r="F966" s="24"/>
@@ -32184,8 +32184,8 @@
     </row>
     <row r="967" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967" s="29"/>
-      <c r="B967" s="69"/>
-      <c r="C967" s="70"/>
+      <c r="B967" s="82"/>
+      <c r="C967" s="83"/>
       <c r="D967" s="6"/>
       <c r="E967" s="29"/>
       <c r="F967" s="24"/>
@@ -35094,8 +35094,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="69"/>
-      <c r="C1080" s="70"/>
+      <c r="B1080" s="82"/>
+      <c r="C1080" s="83"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35108,10 +35108,10 @@
     </row>
     <row r="1081" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1081" s="29"/>
-      <c r="B1081" s="71" t="s">
+      <c r="B1081" s="80" t="s">
         <v>1857</v>
       </c>
-      <c r="C1081" s="72"/>
+      <c r="C1081" s="81"/>
       <c r="D1081" s="6"/>
       <c r="E1081" s="29"/>
       <c r="F1081" s="24"/>
@@ -35124,8 +35124,8 @@
     </row>
     <row r="1082" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="29"/>
-      <c r="B1082" s="69"/>
-      <c r="C1082" s="70"/>
+      <c r="B1082" s="82"/>
+      <c r="C1082" s="83"/>
       <c r="D1082" s="6"/>
       <c r="E1082" s="29"/>
       <c r="F1082" s="24"/>
@@ -35180,8 +35180,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="69"/>
-      <c r="C1085" s="70"/>
+      <c r="B1085" s="82"/>
+      <c r="C1085" s="83"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -35194,10 +35194,10 @@
     </row>
     <row r="1086" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1086" s="29"/>
-      <c r="B1086" s="71" t="s">
+      <c r="B1086" s="80" t="s">
         <v>1858</v>
       </c>
-      <c r="C1086" s="72"/>
+      <c r="C1086" s="81"/>
       <c r="D1086" s="6"/>
       <c r="E1086" s="29"/>
       <c r="F1086" s="24"/>
@@ -35210,8 +35210,8 @@
     </row>
     <row r="1087" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1087" s="29"/>
-      <c r="B1087" s="69"/>
-      <c r="C1087" s="70"/>
+      <c r="B1087" s="82"/>
+      <c r="C1087" s="83"/>
       <c r="D1087" s="6"/>
       <c r="E1087" s="29"/>
       <c r="F1087" s="24"/>
@@ -37700,8 +37700,8 @@
     </row>
     <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="69"/>
-      <c r="C1194" s="70"/>
+      <c r="B1194" s="82"/>
+      <c r="C1194" s="83"/>
       <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
       <c r="F1194" s="24"/>
@@ -37714,10 +37714,10 @@
     </row>
     <row r="1195" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1195" s="29"/>
-      <c r="B1195" s="71" t="s">
+      <c r="B1195" s="80" t="s">
         <v>2035</v>
       </c>
-      <c r="C1195" s="72"/>
+      <c r="C1195" s="81"/>
       <c r="D1195" s="6"/>
       <c r="E1195" s="29"/>
       <c r="F1195" s="24"/>
@@ -37730,8 +37730,8 @@
     </row>
     <row r="1196" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1196" s="29"/>
-      <c r="B1196" s="69"/>
-      <c r="C1196" s="70"/>
+      <c r="B1196" s="82"/>
+      <c r="C1196" s="83"/>
       <c r="D1196" s="6"/>
       <c r="E1196" s="29"/>
       <c r="F1196" s="24"/>
@@ -38116,11 +38116,65 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B488:C488"/>
+    <mergeCell ref="B344:C344"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B343:C343"/>
+    <mergeCell ref="B345:C345"/>
+    <mergeCell ref="B484:C484"/>
+    <mergeCell ref="B487:C487"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B940:C940"/>
+    <mergeCell ref="B932:C932"/>
+    <mergeCell ref="B816:C816"/>
+    <mergeCell ref="B711:C711"/>
+    <mergeCell ref="B554:C554"/>
+    <mergeCell ref="B817:C817"/>
+    <mergeCell ref="B815:C815"/>
+    <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B933:C933"/>
+    <mergeCell ref="B939:C939"/>
+    <mergeCell ref="B1194:C1194"/>
+    <mergeCell ref="B1196:C1196"/>
+    <mergeCell ref="B1195:C1195"/>
+    <mergeCell ref="B1086:C1086"/>
+    <mergeCell ref="B1081:C1081"/>
+    <mergeCell ref="B941:C941"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B1085:C1085"/>
+    <mergeCell ref="B1087:C1087"/>
+    <mergeCell ref="B1080:C1080"/>
+    <mergeCell ref="B1082:C1082"/>
+    <mergeCell ref="B966:C966"/>
+    <mergeCell ref="B489:C489"/>
+    <mergeCell ref="B553:C553"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B710:C710"/>
+    <mergeCell ref="B712:C712"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B138:C138"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D2:D3"/>
@@ -38137,65 +38191,11 @@
     <mergeCell ref="B106:C106"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B489:C489"/>
-    <mergeCell ref="B553:C553"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B712:C712"/>
-    <mergeCell ref="B941:C941"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B1085:C1085"/>
-    <mergeCell ref="B1087:C1087"/>
-    <mergeCell ref="B1080:C1080"/>
-    <mergeCell ref="B1082:C1082"/>
-    <mergeCell ref="B966:C966"/>
-    <mergeCell ref="B1194:C1194"/>
-    <mergeCell ref="B1196:C1196"/>
-    <mergeCell ref="B1195:C1195"/>
-    <mergeCell ref="B1086:C1086"/>
-    <mergeCell ref="B1081:C1081"/>
-    <mergeCell ref="B940:C940"/>
-    <mergeCell ref="B932:C932"/>
-    <mergeCell ref="B816:C816"/>
-    <mergeCell ref="B711:C711"/>
-    <mergeCell ref="B554:C554"/>
-    <mergeCell ref="B817:C817"/>
-    <mergeCell ref="B815:C815"/>
-    <mergeCell ref="B931:C931"/>
-    <mergeCell ref="B933:C933"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B488:C488"/>
-    <mergeCell ref="B344:C344"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B343:C343"/>
-    <mergeCell ref="B345:C345"/>
-    <mergeCell ref="B484:C484"/>
-    <mergeCell ref="B487:C487"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38225,80 +38225,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="88" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="88" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="88" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="88" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="87" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="88"/>
+      <c r="I7" s="87"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="86" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38307,62 +38307,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="86" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="88" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="88" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="88" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="88" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="87" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="88"/>
+      <c r="I12" s="87"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="86" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38371,13 +38371,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="86" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38386,13 +38386,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="86" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38401,13 +38401,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="86" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38416,24 +38416,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="86" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="86" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38442,12 +38442,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="86" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38456,13 +38456,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="86" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38471,13 +38471,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="86" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38486,13 +38486,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="86" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38501,53 +38501,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="86" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="88" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="88" t="s">
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="87" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="88"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="86" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="86" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38556,12 +38556,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38570,24 +38570,28 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="87" t="s">
+      <c r="E28" s="86" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38603,16 +38607,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 16 Maret 2023 18:30 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4134" uniqueCount="2076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="2078">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8274,6 +8274,12 @@
   </si>
   <si>
     <t>Menyimpan Aksi Penolakan Persetujuan dari User pada WorkFlow Dokumen</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.approvalStage.isBusinessDocumentFinalApproved</t>
+  </si>
+  <si>
+    <t>Mengecek Status Final Approve pada Dokumen Bisnis</t>
   </si>
 </sst>
 </file>
@@ -8941,6 +8947,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -8974,31 +8998,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9310,13 +9316,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1214"/>
+  <dimension ref="A1:M1215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D1193" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="E1190" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C1208" sqref="C1208"/>
+      <selection pane="bottomRight" activeCell="I1199" sqref="I1199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9352,31 +9358,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="84" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="73"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="75" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="71"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9398,8 +9404,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9412,10 +9418,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="71" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="81"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9428,8 +9434,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9546,8 +9552,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9560,10 +9566,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="71" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="81"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9576,8 +9582,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9658,8 +9664,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9672,10 +9678,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="71" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="81"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9688,8 +9694,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9764,8 +9770,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9794,8 +9800,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11372,8 +11378,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="82"/>
-      <c r="C95" s="83"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="70"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11386,10 +11392,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="80" t="s">
+      <c r="B96" s="71" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="81"/>
+      <c r="C96" s="72"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11402,8 +11408,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="82"/>
-      <c r="C97" s="83"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="70"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11562,8 +11568,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="82"/>
-      <c r="C104" s="83"/>
+      <c r="B104" s="69"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11576,10 +11582,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="80" t="s">
+      <c r="B105" s="71" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="81"/>
+      <c r="C105" s="72"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11592,8 +11598,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="82"/>
-      <c r="C106" s="83"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="70"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12098,8 +12104,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="82"/>
-      <c r="C130" s="83"/>
+      <c r="B130" s="69"/>
+      <c r="C130" s="70"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12112,10 +12118,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="80" t="s">
+      <c r="B131" s="71" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="81"/>
+      <c r="C131" s="72"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12128,8 +12134,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="82"/>
-      <c r="C132" s="83"/>
+      <c r="B132" s="69"/>
+      <c r="C132" s="70"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12240,8 +12246,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="82"/>
-      <c r="C137" s="83"/>
+      <c r="B137" s="69"/>
+      <c r="C137" s="70"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12254,10 +12260,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="80" t="s">
+      <c r="B138" s="71" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="81"/>
+      <c r="C138" s="72"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12270,8 +12276,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="82"/>
-      <c r="C139" s="83"/>
+      <c r="B139" s="69"/>
+      <c r="C139" s="70"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12432,8 +12438,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="82"/>
-      <c r="C147" s="83"/>
+      <c r="B147" s="69"/>
+      <c r="C147" s="70"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12446,10 +12452,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="80" t="s">
+      <c r="B148" s="71" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="81"/>
+      <c r="C148" s="72"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12462,8 +12468,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="82"/>
-      <c r="C149" s="83"/>
+      <c r="B149" s="69"/>
+      <c r="C149" s="70"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12624,8 +12630,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="82"/>
-      <c r="C157" s="83"/>
+      <c r="B157" s="69"/>
+      <c r="C157" s="70"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12738,8 +12744,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="82"/>
-      <c r="C163" s="83"/>
+      <c r="B163" s="69"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12752,10 +12758,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="80" t="s">
+      <c r="B164" s="71" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="81"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12768,8 +12774,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="82"/>
-      <c r="C165" s="83"/>
+      <c r="B165" s="69"/>
+      <c r="C165" s="70"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -13026,8 +13032,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="82"/>
-      <c r="C177" s="83"/>
+      <c r="B177" s="69"/>
+      <c r="C177" s="70"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -13040,10 +13046,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="80" t="s">
+      <c r="B178" s="71" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="81"/>
+      <c r="C178" s="72"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -13056,8 +13062,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="82"/>
-      <c r="C179" s="83"/>
+      <c r="B179" s="69"/>
+      <c r="C179" s="70"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13122,8 +13128,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="82"/>
-      <c r="C183" s="83"/>
+      <c r="B183" s="69"/>
+      <c r="C183" s="70"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13136,10 +13142,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="80" t="s">
+      <c r="B184" s="71" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="81"/>
+      <c r="C184" s="72"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13152,8 +13158,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="82"/>
-      <c r="C185" s="83"/>
+      <c r="B185" s="69"/>
+      <c r="C185" s="70"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13738,8 +13744,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="82"/>
-      <c r="C211" s="83"/>
+      <c r="B211" s="69"/>
+      <c r="C211" s="70"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13752,10 +13758,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="80" t="s">
+      <c r="B212" s="71" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="81"/>
+      <c r="C212" s="72"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13768,8 +13774,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="82"/>
-      <c r="C213" s="83"/>
+      <c r="B213" s="69"/>
+      <c r="C213" s="70"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13964,8 +13970,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="82"/>
-      <c r="C222" s="83"/>
+      <c r="B222" s="69"/>
+      <c r="C222" s="70"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13978,10 +13984,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="80" t="s">
+      <c r="B223" s="71" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="81"/>
+      <c r="C223" s="72"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -13994,8 +14000,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="82"/>
-      <c r="C224" s="83"/>
+      <c r="B224" s="69"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16830,8 +16836,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="82"/>
-      <c r="C343" s="83"/>
+      <c r="B343" s="69"/>
+      <c r="C343" s="70"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16844,10 +16850,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="80" t="s">
+      <c r="B344" s="71" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="81"/>
+      <c r="C344" s="72"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16860,8 +16866,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="82"/>
-      <c r="C345" s="83"/>
+      <c r="B345" s="69"/>
+      <c r="C345" s="70"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20486,8 +20492,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="82"/>
-      <c r="C484" s="83"/>
+      <c r="B484" s="69"/>
+      <c r="C484" s="70"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20542,8 +20548,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="82"/>
-      <c r="C487" s="83"/>
+      <c r="B487" s="69"/>
+      <c r="C487" s="70"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20556,10 +20562,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="80" t="s">
+      <c r="B488" s="71" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="81"/>
+      <c r="C488" s="72"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20572,8 +20578,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="82"/>
-      <c r="C489" s="83"/>
+      <c r="B489" s="69"/>
+      <c r="C489" s="70"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22172,8 +22178,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="82"/>
-      <c r="C553" s="83"/>
+      <c r="B553" s="69"/>
+      <c r="C553" s="70"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22186,10 +22192,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="80" t="s">
+      <c r="B554" s="71" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="81"/>
+      <c r="C554" s="72"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22202,8 +22208,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="82"/>
-      <c r="C555" s="83"/>
+      <c r="B555" s="69"/>
+      <c r="C555" s="70"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -26002,8 +26008,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="82"/>
-      <c r="C710" s="83"/>
+      <c r="B710" s="69"/>
+      <c r="C710" s="70"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -26016,10 +26022,10 @@
     </row>
     <row r="711" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A711" s="29"/>
-      <c r="B711" s="80" t="s">
+      <c r="B711" s="71" t="s">
         <v>1853</v>
       </c>
-      <c r="C711" s="81"/>
+      <c r="C711" s="72"/>
       <c r="D711" s="6"/>
       <c r="E711" s="29"/>
       <c r="F711" s="24"/>
@@ -26032,8 +26038,8 @@
     </row>
     <row r="712" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712" s="29"/>
-      <c r="B712" s="82"/>
-      <c r="C712" s="83"/>
+      <c r="B712" s="69"/>
+      <c r="C712" s="70"/>
       <c r="D712" s="6"/>
       <c r="E712" s="29"/>
       <c r="F712" s="24"/>
@@ -28490,8 +28496,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="82"/>
-      <c r="C815" s="83"/>
+      <c r="B815" s="69"/>
+      <c r="C815" s="70"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -28504,10 +28510,10 @@
     </row>
     <row r="816" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A816" s="29"/>
-      <c r="B816" s="80" t="s">
+      <c r="B816" s="71" t="s">
         <v>1854</v>
       </c>
-      <c r="C816" s="81"/>
+      <c r="C816" s="72"/>
       <c r="D816" s="6"/>
       <c r="E816" s="29"/>
       <c r="F816" s="24"/>
@@ -28520,8 +28526,8 @@
     </row>
     <row r="817" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817" s="29"/>
-      <c r="B817" s="82"/>
-      <c r="C817" s="83"/>
+      <c r="B817" s="69"/>
+      <c r="C817" s="70"/>
       <c r="D817" s="6"/>
       <c r="E817" s="29"/>
       <c r="F817" s="24"/>
@@ -31435,8 +31441,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="82"/>
-      <c r="C931" s="83"/>
+      <c r="B931" s="69"/>
+      <c r="C931" s="70"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31449,10 +31455,10 @@
     </row>
     <row r="932" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A932" s="29"/>
-      <c r="B932" s="80" t="s">
+      <c r="B932" s="71" t="s">
         <v>1952</v>
       </c>
-      <c r="C932" s="81"/>
+      <c r="C932" s="72"/>
       <c r="D932" s="6"/>
       <c r="E932" s="29"/>
       <c r="F932" s="24"/>
@@ -31465,8 +31471,8 @@
     </row>
     <row r="933" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933" s="29"/>
-      <c r="B933" s="82"/>
-      <c r="C933" s="83"/>
+      <c r="B933" s="69"/>
+      <c r="C933" s="70"/>
       <c r="D933" s="6"/>
       <c r="E933" s="29"/>
       <c r="F933" s="24"/>
@@ -31600,8 +31606,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="82"/>
-      <c r="C939" s="83"/>
+      <c r="B939" s="69"/>
+      <c r="C939" s="70"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -31614,10 +31620,10 @@
     </row>
     <row r="940" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A940" s="29"/>
-      <c r="B940" s="80" t="s">
+      <c r="B940" s="71" t="s">
         <v>1855</v>
       </c>
-      <c r="C940" s="81"/>
+      <c r="C940" s="72"/>
       <c r="D940" s="6"/>
       <c r="E940" s="29"/>
       <c r="F940" s="24"/>
@@ -31630,8 +31636,8 @@
     </row>
     <row r="941" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941" s="29"/>
-      <c r="B941" s="82"/>
-      <c r="C941" s="83"/>
+      <c r="B941" s="69"/>
+      <c r="C941" s="70"/>
       <c r="D941" s="6"/>
       <c r="E941" s="29"/>
       <c r="F941" s="24"/>
@@ -32154,8 +32160,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="82"/>
-      <c r="C965" s="83"/>
+      <c r="B965" s="69"/>
+      <c r="C965" s="70"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -32168,10 +32174,10 @@
     </row>
     <row r="966" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A966" s="29"/>
-      <c r="B966" s="80" t="s">
+      <c r="B966" s="71" t="s">
         <v>1856</v>
       </c>
-      <c r="C966" s="81"/>
+      <c r="C966" s="72"/>
       <c r="D966" s="6"/>
       <c r="E966" s="29"/>
       <c r="F966" s="24"/>
@@ -32184,8 +32190,8 @@
     </row>
     <row r="967" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967" s="29"/>
-      <c r="B967" s="82"/>
-      <c r="C967" s="83"/>
+      <c r="B967" s="69"/>
+      <c r="C967" s="70"/>
       <c r="D967" s="6"/>
       <c r="E967" s="29"/>
       <c r="F967" s="24"/>
@@ -35094,8 +35100,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="82"/>
-      <c r="C1080" s="83"/>
+      <c r="B1080" s="69"/>
+      <c r="C1080" s="70"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35108,10 +35114,10 @@
     </row>
     <row r="1081" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1081" s="29"/>
-      <c r="B1081" s="80" t="s">
+      <c r="B1081" s="71" t="s">
         <v>1857</v>
       </c>
-      <c r="C1081" s="81"/>
+      <c r="C1081" s="72"/>
       <c r="D1081" s="6"/>
       <c r="E1081" s="29"/>
       <c r="F1081" s="24"/>
@@ -35124,8 +35130,8 @@
     </row>
     <row r="1082" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="29"/>
-      <c r="B1082" s="82"/>
-      <c r="C1082" s="83"/>
+      <c r="B1082" s="69"/>
+      <c r="C1082" s="70"/>
       <c r="D1082" s="6"/>
       <c r="E1082" s="29"/>
       <c r="F1082" s="24"/>
@@ -35180,8 +35186,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="82"/>
-      <c r="C1085" s="83"/>
+      <c r="B1085" s="69"/>
+      <c r="C1085" s="70"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -35194,10 +35200,10 @@
     </row>
     <row r="1086" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1086" s="29"/>
-      <c r="B1086" s="80" t="s">
+      <c r="B1086" s="71" t="s">
         <v>1858</v>
       </c>
-      <c r="C1086" s="81"/>
+      <c r="C1086" s="72"/>
       <c r="D1086" s="6"/>
       <c r="E1086" s="29"/>
       <c r="F1086" s="24"/>
@@ -35210,8 +35216,8 @@
     </row>
     <row r="1087" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1087" s="29"/>
-      <c r="B1087" s="82"/>
-      <c r="C1087" s="83"/>
+      <c r="B1087" s="69"/>
+      <c r="C1087" s="70"/>
       <c r="D1087" s="6"/>
       <c r="E1087" s="29"/>
       <c r="F1087" s="24"/>
@@ -37700,8 +37706,8 @@
     </row>
     <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="82"/>
-      <c r="C1194" s="83"/>
+      <c r="B1194" s="69"/>
+      <c r="C1194" s="70"/>
       <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
       <c r="F1194" s="24"/>
@@ -37714,10 +37720,10 @@
     </row>
     <row r="1195" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1195" s="29"/>
-      <c r="B1195" s="80" t="s">
+      <c r="B1195" s="71" t="s">
         <v>2035</v>
       </c>
-      <c r="C1195" s="81"/>
+      <c r="C1195" s="72"/>
       <c r="D1195" s="6"/>
       <c r="E1195" s="29"/>
       <c r="F1195" s="24"/>
@@ -37730,8 +37736,8 @@
     </row>
     <row r="1196" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1196" s="29"/>
-      <c r="B1196" s="82"/>
-      <c r="C1196" s="83"/>
+      <c r="B1196" s="69"/>
+      <c r="C1196" s="70"/>
       <c r="D1196" s="6"/>
       <c r="E1196" s="29"/>
       <c r="F1196" s="24"/>
@@ -37796,14 +37802,14 @@
         <v>2047</v>
       </c>
       <c r="C1199" s="54" t="s">
-        <v>2038</v>
+        <v>2076</v>
       </c>
       <c r="D1199" s="3" t="s">
-        <v>2039</v>
+        <v>2077</v>
       </c>
       <c r="E1199" s="29"/>
       <c r="F1199" s="23">
-        <v>44971</v>
+        <v>45001</v>
       </c>
       <c r="G1199" s="44" t="s">
         <v>592</v>
@@ -37820,14 +37826,14 @@
         <v>2047</v>
       </c>
       <c r="C1200" s="54" t="s">
-        <v>2066</v>
+        <v>2038</v>
       </c>
       <c r="D1200" s="3" t="s">
-        <v>2073</v>
+        <v>2039</v>
       </c>
       <c r="E1200" s="29"/>
       <c r="F1200" s="23">
-        <v>44992</v>
+        <v>44971</v>
       </c>
       <c r="G1200" s="44" t="s">
         <v>592</v>
@@ -37844,10 +37850,10 @@
         <v>2047</v>
       </c>
       <c r="C1201" s="54" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D1201" s="3" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="E1201" s="29"/>
       <c r="F1201" s="23">
@@ -37868,10 +37874,10 @@
         <v>2047</v>
       </c>
       <c r="C1202" s="54" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="D1202" s="3" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="E1202" s="29"/>
       <c r="F1202" s="23">
@@ -37892,10 +37898,10 @@
         <v>2047</v>
       </c>
       <c r="C1203" s="54" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D1203" s="3" t="s">
-        <v>2071</v>
+        <v>2075</v>
       </c>
       <c r="E1203" s="29"/>
       <c r="F1203" s="23">
@@ -37916,10 +37922,10 @@
         <v>2047</v>
       </c>
       <c r="C1204" s="54" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D1204" s="3" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="E1204" s="29"/>
       <c r="F1204" s="23">
@@ -37934,61 +37940,61 @@
       <c r="K1204" s="14"/>
       <c r="L1204" s="29"/>
     </row>
-    <row r="1205" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1205" s="29"/>
-      <c r="B1205" s="59"/>
-      <c r="C1205" s="64"/>
-      <c r="D1205" s="7"/>
+      <c r="B1205" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1205" s="54" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D1205" s="3" t="s">
+        <v>2072</v>
+      </c>
       <c r="E1205" s="29"/>
-      <c r="F1205" s="26"/>
-      <c r="G1205" s="46"/>
+      <c r="F1205" s="23">
+        <v>44992</v>
+      </c>
+      <c r="G1205" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1205" s="29"/>
-      <c r="I1205" s="26"/>
-      <c r="J1205" s="17"/>
-      <c r="K1205" s="18"/>
+      <c r="I1205" s="23"/>
+      <c r="J1205" s="13"/>
+      <c r="K1205" s="14"/>
       <c r="L1205" s="29"/>
     </row>
-    <row r="1206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1206" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1206" s="29"/>
-      <c r="B1206" s="56" t="s">
-        <v>2047</v>
-      </c>
-      <c r="C1206" s="54" t="s">
-        <v>2031</v>
-      </c>
-      <c r="D1206" s="3" t="s">
-        <v>2034</v>
-      </c>
+      <c r="B1206" s="59"/>
+      <c r="C1206" s="64"/>
+      <c r="D1206" s="7"/>
       <c r="E1206" s="29"/>
-      <c r="F1206" s="23">
-        <v>44987</v>
-      </c>
-      <c r="G1206" s="44" t="s">
-        <v>2046</v>
-      </c>
+      <c r="F1206" s="26"/>
+      <c r="G1206" s="46"/>
       <c r="H1206" s="29"/>
-      <c r="I1206" s="23"/>
-      <c r="J1206" s="13"/>
-      <c r="K1206" s="14"/>
+      <c r="I1206" s="26"/>
+      <c r="J1206" s="17"/>
+      <c r="K1206" s="18"/>
       <c r="L1206" s="29"/>
     </row>
-    <row r="1207" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1207" s="29"/>
       <c r="B1207" s="56" t="s">
         <v>2047</v>
       </c>
       <c r="C1207" s="54" t="s">
-        <v>2064</v>
+        <v>2031</v>
       </c>
       <c r="D1207" s="3" t="s">
-        <v>2045</v>
+        <v>2034</v>
       </c>
       <c r="E1207" s="29"/>
       <c r="F1207" s="23">
         <v>44987</v>
       </c>
       <c r="G1207" s="44" t="s">
-        <v>592</v>
+        <v>2046</v>
       </c>
       <c r="H1207" s="29"/>
       <c r="I1207" s="23"/>
@@ -38002,17 +38008,17 @@
         <v>2047</v>
       </c>
       <c r="C1208" s="54" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="D1208" s="3" t="s">
-        <v>2036</v>
+        <v>2045</v>
       </c>
       <c r="E1208" s="29"/>
       <c r="F1208" s="23">
         <v>44987</v>
       </c>
       <c r="G1208" s="44" t="s">
-        <v>2046</v>
+        <v>592</v>
       </c>
       <c r="H1208" s="29"/>
       <c r="I1208" s="23"/>
@@ -38026,17 +38032,17 @@
         <v>2047</v>
       </c>
       <c r="C1209" s="54" t="s">
-        <v>2048</v>
+        <v>2065</v>
       </c>
       <c r="D1209" s="3" t="s">
-        <v>2063</v>
+        <v>2036</v>
       </c>
       <c r="E1209" s="29"/>
       <c r="F1209" s="23">
         <v>44987</v>
       </c>
       <c r="G1209" s="44" t="s">
-        <v>592</v>
+        <v>2046</v>
       </c>
       <c r="H1209" s="29"/>
       <c r="I1209" s="23"/>
@@ -38044,20 +38050,20 @@
       <c r="K1209" s="14"/>
       <c r="L1209" s="29"/>
     </row>
-    <row r="1210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1210" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1210" s="29"/>
       <c r="B1210" s="56" t="s">
         <v>2047</v>
       </c>
       <c r="C1210" s="54" t="s">
-        <v>2037</v>
+        <v>2048</v>
       </c>
       <c r="D1210" s="3" t="s">
-        <v>2040</v>
+        <v>2063</v>
       </c>
       <c r="E1210" s="29"/>
       <c r="F1210" s="23">
-        <v>44972</v>
+        <v>44987</v>
       </c>
       <c r="G1210" s="44" t="s">
         <v>592</v>
@@ -38068,54 +38074,142 @@
       <c r="K1210" s="14"/>
       <c r="L1210" s="29"/>
     </row>
-    <row r="1211" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1211" s="29"/>
-      <c r="B1211" s="60"/>
-      <c r="C1211" s="67"/>
-      <c r="D1211" s="5"/>
+      <c r="B1211" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1211" s="54" t="s">
+        <v>2037</v>
+      </c>
+      <c r="D1211" s="3" t="s">
+        <v>2040</v>
+      </c>
       <c r="E1211" s="29"/>
-      <c r="F1211" s="27"/>
-      <c r="G1211" s="47"/>
+      <c r="F1211" s="23">
+        <v>44972</v>
+      </c>
+      <c r="G1211" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1211" s="29"/>
-      <c r="I1211" s="27"/>
-      <c r="J1211" s="19"/>
-      <c r="K1211" s="20"/>
+      <c r="I1211" s="23"/>
+      <c r="J1211" s="13"/>
+      <c r="K1211" s="14"/>
       <c r="L1211" s="29"/>
     </row>
-    <row r="1212" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1212" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1212" s="29"/>
-      <c r="B1212" s="55"/>
-      <c r="C1212" s="62"/>
-      <c r="D1212" s="32"/>
+      <c r="B1212" s="60"/>
+      <c r="C1212" s="67"/>
+      <c r="D1212" s="5"/>
       <c r="E1212" s="29"/>
-      <c r="F1212" s="33"/>
-      <c r="G1212" s="41"/>
+      <c r="F1212" s="27"/>
+      <c r="G1212" s="47"/>
       <c r="H1212" s="29"/>
-      <c r="I1212" s="33"/>
-      <c r="J1212" s="34"/>
-      <c r="K1212" s="34"/>
+      <c r="I1212" s="27"/>
+      <c r="J1212" s="19"/>
+      <c r="K1212" s="20"/>
       <c r="L1212" s="29"/>
     </row>
-    <row r="1214" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1214" s="29"/>
-      <c r="B1214" s="55"/>
-      <c r="C1214" s="54" t="s">
+    <row r="1213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1213" s="29"/>
+      <c r="B1213" s="55"/>
+      <c r="C1213" s="62"/>
+      <c r="D1213" s="32"/>
+      <c r="E1213" s="29"/>
+      <c r="F1213" s="33"/>
+      <c r="G1213" s="41"/>
+      <c r="H1213" s="29"/>
+      <c r="I1213" s="33"/>
+      <c r="J1213" s="34"/>
+      <c r="K1213" s="34"/>
+      <c r="L1213" s="29"/>
+    </row>
+    <row r="1215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1215" s="29"/>
+      <c r="B1215" s="55"/>
+      <c r="C1215" s="54" t="s">
         <v>364</v>
       </c>
-      <c r="D1214" s="3" t="s">
+      <c r="D1215" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E1214" s="29"/>
-      <c r="F1214" s="23"/>
-      <c r="G1214" s="44"/>
-      <c r="H1214" s="29"/>
-      <c r="I1214" s="23"/>
-      <c r="J1214" s="13"/>
-      <c r="K1214" s="14"/>
-      <c r="L1214" s="29"/>
+      <c r="E1215" s="29"/>
+      <c r="F1215" s="23"/>
+      <c r="G1215" s="44"/>
+      <c r="H1215" s="29"/>
+      <c r="I1215" s="23"/>
+      <c r="J1215" s="13"/>
+      <c r="K1215" s="14"/>
+      <c r="L1215" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B489:C489"/>
+    <mergeCell ref="B553:C553"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B710:C710"/>
+    <mergeCell ref="B712:C712"/>
+    <mergeCell ref="B941:C941"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B1085:C1085"/>
+    <mergeCell ref="B1087:C1087"/>
+    <mergeCell ref="B1080:C1080"/>
+    <mergeCell ref="B1082:C1082"/>
+    <mergeCell ref="B966:C966"/>
+    <mergeCell ref="B1194:C1194"/>
+    <mergeCell ref="B1196:C1196"/>
+    <mergeCell ref="B1195:C1195"/>
+    <mergeCell ref="B1086:C1086"/>
+    <mergeCell ref="B1081:C1081"/>
+    <mergeCell ref="B940:C940"/>
+    <mergeCell ref="B932:C932"/>
+    <mergeCell ref="B816:C816"/>
+    <mergeCell ref="B711:C711"/>
+    <mergeCell ref="B554:C554"/>
+    <mergeCell ref="B817:C817"/>
+    <mergeCell ref="B815:C815"/>
+    <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B933:C933"/>
+    <mergeCell ref="B939:C939"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B23:C23"/>
@@ -38132,75 +38226,11 @@
     <mergeCell ref="B487:C487"/>
     <mergeCell ref="B183:C183"/>
     <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B940:C940"/>
-    <mergeCell ref="B932:C932"/>
-    <mergeCell ref="B816:C816"/>
-    <mergeCell ref="B711:C711"/>
-    <mergeCell ref="B554:C554"/>
-    <mergeCell ref="B817:C817"/>
-    <mergeCell ref="B815:C815"/>
-    <mergeCell ref="B931:C931"/>
-    <mergeCell ref="B933:C933"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B1194:C1194"/>
-    <mergeCell ref="B1196:C1196"/>
-    <mergeCell ref="B1195:C1195"/>
-    <mergeCell ref="B1086:C1086"/>
-    <mergeCell ref="B1081:C1081"/>
-    <mergeCell ref="B941:C941"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B1085:C1085"/>
-    <mergeCell ref="B1087:C1087"/>
-    <mergeCell ref="B1080:C1080"/>
-    <mergeCell ref="B1082:C1082"/>
-    <mergeCell ref="B966:C966"/>
-    <mergeCell ref="B489:C489"/>
-    <mergeCell ref="B553:C553"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B712:C712"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G14 G102 G133:G134 G136 G143:G145 G214:G220 G225:G230 G346:G350 G352:G356 G366:G368 G384 G458:G460 G798:G800 G829:G830 G944:G946 G948 G950:G954 G956:G959 G961:G962 G974:G979 G981:G983 G992:G993 G377:G378 G999 G1054:G1056 G968:G972 G1095:G1097 G312:G315 G1168:G1171 G902:G905 G818:G820 G317:G319 G1173:G1175 G209 G186 G128 G108 G232:G239 G490:G492 G370:G375 G985:G990 G832:G837 G180 G79:G81 G158:G159 G56 G406 G822:G827 G358:G364 G1088:G1093 G793:G796 G942 G853 G1006 G161 G166:G174 G188:G207 G298:G308 G1154:G1164 G1011:G1052 G858:G900 G411:G456 G76:G77 G485 G1072 F1069:G1071 G29:G37 G463:G476 G339:G341 G1190:G1192 G480:G482 G1076:G1078 G927:G929 G813 G93 G1083 G150:G153 G1059:G1068 G911:G925 G544:G551 G532:G535 G808:G811 G849:G851 G386:G404 G1001:G1004 G907:G909 G49 G60 G786:G789 G155 G584:G585 G855:G856 G621:G622 G1008:G1009 G1121:G1122 G505:G506 G408:G409 G265:G266 G650:G652 G637:G643 G647:G648 G624:G627 G70:G72 G88:G91 G322:G334 G802:G805 G1178:G1184 G538:G542 G680:G682 G665 G573 G618:G619 G605:G607 G752:G755 G83:G86 G761:G762 G58 G757:G759 G570 G705:G710 G721:G734 G655:G663 G283:G296 G1139:G1152 G770:G777 G68 G736:G742 G513:G524 G508:G511 G1124:G1137 G268:G281 G764:G768 G526:G530 G749 G779:G784 G98:G99 G686:G691 G1197:G1210" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G14 G102 G133:G134 G136 G143:G145 G214:G220 G225:G230 G346:G350 G352:G356 G366:G368 G384 G458:G460 G798:G800 G829:G830 G944:G946 G948 G950:G954 G956:G959 G961:G962 G974:G979 G981:G983 G992:G993 G377:G378 G999 G1054:G1056 G968:G972 G1095:G1097 G312:G315 G1168:G1171 G902:G905 G818:G820 G317:G319 G1173:G1175 G209 G186 G128 G108 G232:G239 G490:G492 G370:G375 G985:G990 G832:G837 G180 G79:G81 G158:G159 G56 G406 G822:G827 G358:G364 G1088:G1093 G793:G796 G942 G853 G1006 G161 G166:G174 G188:G207 G298:G308 G1154:G1164 G1011:G1052 G858:G900 G411:G456 G76:G77 G485 G1072 F1069:G1071 G29:G37 G463:G476 G339:G341 G1190:G1192 G480:G482 G1076:G1078 G927:G929 G813 G93 G1083 G150:G153 G1059:G1068 G911:G925 G544:G551 G532:G535 G808:G811 G849:G851 G386:G404 G1001:G1004 G907:G909 G49 G60 G786:G789 G155 G584:G585 G855:G856 G621:G622 G1008:G1009 G1121:G1122 G505:G506 G408:G409 G265:G266 G650:G652 G637:G643 G647:G648 G624:G627 G70:G72 G88:G91 G322:G334 G802:G805 G1178:G1184 G538:G542 G680:G682 G665 G573 G618:G619 G605:G607 G752:G755 G83:G86 G761:G762 G58 G757:G759 G570 G705:G710 G721:G734 G655:G663 G283:G296 G1139:G1152 G770:G777 G68 G736:G742 G513:G524 G508:G511 G1124:G1137 G268:G281 G764:G768 G526:G530 G749 G779:G784 G98:G99 G686:G691 G1200:G1211 G1197:G1198" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -38225,80 +38255,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38307,62 +38337,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38371,13 +38401,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38386,13 +38416,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38401,13 +38431,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38416,24 +38446,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38442,12 +38472,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38456,13 +38486,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38471,13 +38501,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38486,13 +38516,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38501,53 +38531,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38556,12 +38586,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38570,28 +38600,24 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38607,12 +38633,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 17 Maret 2023 18:25 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="2078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="2082">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8280,6 +8280,18 @@
   </si>
   <si>
     <t>Mengecek Status Final Approve pada Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.remapping.manual.getWorkFlowPathSequenceSourceList</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.remapping.manual.getWorkFlowPathSequenceDestinationList</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Sumber untuk Pemetaan Ulang Manual Urutan Jalur WorkFlow</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Tujuan untuk Pemetaan Ulang Manual Urutan Jalur WorkFlow</t>
   </si>
 </sst>
 </file>
@@ -8947,24 +8959,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -8998,13 +8992,31 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9316,13 +9328,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1215"/>
+  <dimension ref="A1:M1218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="E1190" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="E1202" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I1199" sqref="I1199"/>
+      <selection pane="bottomRight" activeCell="I1214" sqref="I1214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9358,31 +9370,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="73" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="84" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="72" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="79"/>
+      <c r="G2" s="73"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="75" t="s">
+      <c r="I2" s="69" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="76"/>
-      <c r="K2" s="77"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="71"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="74"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9404,8 +9416,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9418,10 +9430,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="80" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="72"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9434,8 +9446,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9552,8 +9564,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9566,10 +9578,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="80" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="72"/>
+      <c r="C12" s="81"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9582,8 +9594,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9664,8 +9676,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9678,10 +9690,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="80" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="72"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9694,8 +9706,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="83"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9770,8 +9782,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9800,8 +9812,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11378,8 +11390,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="69"/>
-      <c r="C95" s="70"/>
+      <c r="B95" s="82"/>
+      <c r="C95" s="83"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11392,10 +11404,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="71" t="s">
+      <c r="B96" s="80" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="72"/>
+      <c r="C96" s="81"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11408,8 +11420,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="69"/>
-      <c r="C97" s="70"/>
+      <c r="B97" s="82"/>
+      <c r="C97" s="83"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11568,8 +11580,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="82"/>
+      <c r="C104" s="83"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11582,10 +11594,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="71" t="s">
+      <c r="B105" s="80" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="72"/>
+      <c r="C105" s="81"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11598,8 +11610,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="69"/>
-      <c r="C106" s="70"/>
+      <c r="B106" s="82"/>
+      <c r="C106" s="83"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12104,8 +12116,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="69"/>
-      <c r="C130" s="70"/>
+      <c r="B130" s="82"/>
+      <c r="C130" s="83"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12118,10 +12130,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="71" t="s">
+      <c r="B131" s="80" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="72"/>
+      <c r="C131" s="81"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12134,8 +12146,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="69"/>
-      <c r="C132" s="70"/>
+      <c r="B132" s="82"/>
+      <c r="C132" s="83"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12246,8 +12258,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="82"/>
+      <c r="C137" s="83"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12260,10 +12272,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="71" t="s">
+      <c r="B138" s="80" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="72"/>
+      <c r="C138" s="81"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12276,8 +12288,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="69"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="82"/>
+      <c r="C139" s="83"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12438,8 +12450,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="69"/>
-      <c r="C147" s="70"/>
+      <c r="B147" s="82"/>
+      <c r="C147" s="83"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12452,10 +12464,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="71" t="s">
+      <c r="B148" s="80" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="72"/>
+      <c r="C148" s="81"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12468,8 +12480,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="69"/>
-      <c r="C149" s="70"/>
+      <c r="B149" s="82"/>
+      <c r="C149" s="83"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12630,8 +12642,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="69"/>
-      <c r="C157" s="70"/>
+      <c r="B157" s="82"/>
+      <c r="C157" s="83"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12744,8 +12756,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="69"/>
-      <c r="C163" s="70"/>
+      <c r="B163" s="82"/>
+      <c r="C163" s="83"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12758,10 +12770,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="71" t="s">
+      <c r="B164" s="80" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="72"/>
+      <c r="C164" s="81"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12774,8 +12786,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="69"/>
-      <c r="C165" s="70"/>
+      <c r="B165" s="82"/>
+      <c r="C165" s="83"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -13032,8 +13044,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="69"/>
-      <c r="C177" s="70"/>
+      <c r="B177" s="82"/>
+      <c r="C177" s="83"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -13046,10 +13058,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="71" t="s">
+      <c r="B178" s="80" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="72"/>
+      <c r="C178" s="81"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -13062,8 +13074,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="69"/>
-      <c r="C179" s="70"/>
+      <c r="B179" s="82"/>
+      <c r="C179" s="83"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13128,8 +13140,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="69"/>
-      <c r="C183" s="70"/>
+      <c r="B183" s="82"/>
+      <c r="C183" s="83"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13142,10 +13154,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="71" t="s">
+      <c r="B184" s="80" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="72"/>
+      <c r="C184" s="81"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13158,8 +13170,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="69"/>
-      <c r="C185" s="70"/>
+      <c r="B185" s="82"/>
+      <c r="C185" s="83"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13744,8 +13756,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="69"/>
-      <c r="C211" s="70"/>
+      <c r="B211" s="82"/>
+      <c r="C211" s="83"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13758,10 +13770,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="71" t="s">
+      <c r="B212" s="80" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="72"/>
+      <c r="C212" s="81"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13774,8 +13786,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="69"/>
-      <c r="C213" s="70"/>
+      <c r="B213" s="82"/>
+      <c r="C213" s="83"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13970,8 +13982,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="69"/>
-      <c r="C222" s="70"/>
+      <c r="B222" s="82"/>
+      <c r="C222" s="83"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13984,10 +13996,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="71" t="s">
+      <c r="B223" s="80" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="72"/>
+      <c r="C223" s="81"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -14000,8 +14012,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="69"/>
-      <c r="C224" s="70"/>
+      <c r="B224" s="82"/>
+      <c r="C224" s="83"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16836,8 +16848,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="69"/>
-      <c r="C343" s="70"/>
+      <c r="B343" s="82"/>
+      <c r="C343" s="83"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16850,10 +16862,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="71" t="s">
+      <c r="B344" s="80" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="72"/>
+      <c r="C344" s="81"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16866,8 +16878,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="69"/>
-      <c r="C345" s="70"/>
+      <c r="B345" s="82"/>
+      <c r="C345" s="83"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20492,8 +20504,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="69"/>
-      <c r="C484" s="70"/>
+      <c r="B484" s="82"/>
+      <c r="C484" s="83"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20548,8 +20560,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="69"/>
-      <c r="C487" s="70"/>
+      <c r="B487" s="82"/>
+      <c r="C487" s="83"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20562,10 +20574,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="71" t="s">
+      <c r="B488" s="80" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="72"/>
+      <c r="C488" s="81"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20578,8 +20590,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="69"/>
-      <c r="C489" s="70"/>
+      <c r="B489" s="82"/>
+      <c r="C489" s="83"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22178,8 +22190,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="69"/>
-      <c r="C553" s="70"/>
+      <c r="B553" s="82"/>
+      <c r="C553" s="83"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22192,10 +22204,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="71" t="s">
+      <c r="B554" s="80" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="72"/>
+      <c r="C554" s="81"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22208,8 +22220,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="69"/>
-      <c r="C555" s="70"/>
+      <c r="B555" s="82"/>
+      <c r="C555" s="83"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -26008,8 +26020,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="69"/>
-      <c r="C710" s="70"/>
+      <c r="B710" s="82"/>
+      <c r="C710" s="83"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -26022,10 +26034,10 @@
     </row>
     <row r="711" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A711" s="29"/>
-      <c r="B711" s="71" t="s">
+      <c r="B711" s="80" t="s">
         <v>1853</v>
       </c>
-      <c r="C711" s="72"/>
+      <c r="C711" s="81"/>
       <c r="D711" s="6"/>
       <c r="E711" s="29"/>
       <c r="F711" s="24"/>
@@ -26038,8 +26050,8 @@
     </row>
     <row r="712" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712" s="29"/>
-      <c r="B712" s="69"/>
-      <c r="C712" s="70"/>
+      <c r="B712" s="82"/>
+      <c r="C712" s="83"/>
       <c r="D712" s="6"/>
       <c r="E712" s="29"/>
       <c r="F712" s="24"/>
@@ -28496,8 +28508,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="69"/>
-      <c r="C815" s="70"/>
+      <c r="B815" s="82"/>
+      <c r="C815" s="83"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -28510,10 +28522,10 @@
     </row>
     <row r="816" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A816" s="29"/>
-      <c r="B816" s="71" t="s">
+      <c r="B816" s="80" t="s">
         <v>1854</v>
       </c>
-      <c r="C816" s="72"/>
+      <c r="C816" s="81"/>
       <c r="D816" s="6"/>
       <c r="E816" s="29"/>
       <c r="F816" s="24"/>
@@ -28526,8 +28538,8 @@
     </row>
     <row r="817" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817" s="29"/>
-      <c r="B817" s="69"/>
-      <c r="C817" s="70"/>
+      <c r="B817" s="82"/>
+      <c r="C817" s="83"/>
       <c r="D817" s="6"/>
       <c r="E817" s="29"/>
       <c r="F817" s="24"/>
@@ -31441,8 +31453,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="69"/>
-      <c r="C931" s="70"/>
+      <c r="B931" s="82"/>
+      <c r="C931" s="83"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31455,10 +31467,10 @@
     </row>
     <row r="932" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A932" s="29"/>
-      <c r="B932" s="71" t="s">
+      <c r="B932" s="80" t="s">
         <v>1952</v>
       </c>
-      <c r="C932" s="72"/>
+      <c r="C932" s="81"/>
       <c r="D932" s="6"/>
       <c r="E932" s="29"/>
       <c r="F932" s="24"/>
@@ -31471,8 +31483,8 @@
     </row>
     <row r="933" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933" s="29"/>
-      <c r="B933" s="69"/>
-      <c r="C933" s="70"/>
+      <c r="B933" s="82"/>
+      <c r="C933" s="83"/>
       <c r="D933" s="6"/>
       <c r="E933" s="29"/>
       <c r="F933" s="24"/>
@@ -31606,8 +31618,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="69"/>
-      <c r="C939" s="70"/>
+      <c r="B939" s="82"/>
+      <c r="C939" s="83"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -31620,10 +31632,10 @@
     </row>
     <row r="940" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A940" s="29"/>
-      <c r="B940" s="71" t="s">
+      <c r="B940" s="80" t="s">
         <v>1855</v>
       </c>
-      <c r="C940" s="72"/>
+      <c r="C940" s="81"/>
       <c r="D940" s="6"/>
       <c r="E940" s="29"/>
       <c r="F940" s="24"/>
@@ -31636,8 +31648,8 @@
     </row>
     <row r="941" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941" s="29"/>
-      <c r="B941" s="69"/>
-      <c r="C941" s="70"/>
+      <c r="B941" s="82"/>
+      <c r="C941" s="83"/>
       <c r="D941" s="6"/>
       <c r="E941" s="29"/>
       <c r="F941" s="24"/>
@@ -32160,8 +32172,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="69"/>
-      <c r="C965" s="70"/>
+      <c r="B965" s="82"/>
+      <c r="C965" s="83"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -32174,10 +32186,10 @@
     </row>
     <row r="966" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A966" s="29"/>
-      <c r="B966" s="71" t="s">
+      <c r="B966" s="80" t="s">
         <v>1856</v>
       </c>
-      <c r="C966" s="72"/>
+      <c r="C966" s="81"/>
       <c r="D966" s="6"/>
       <c r="E966" s="29"/>
       <c r="F966" s="24"/>
@@ -32190,8 +32202,8 @@
     </row>
     <row r="967" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967" s="29"/>
-      <c r="B967" s="69"/>
-      <c r="C967" s="70"/>
+      <c r="B967" s="82"/>
+      <c r="C967" s="83"/>
       <c r="D967" s="6"/>
       <c r="E967" s="29"/>
       <c r="F967" s="24"/>
@@ -35100,8 +35112,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="69"/>
-      <c r="C1080" s="70"/>
+      <c r="B1080" s="82"/>
+      <c r="C1080" s="83"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35114,10 +35126,10 @@
     </row>
     <row r="1081" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1081" s="29"/>
-      <c r="B1081" s="71" t="s">
+      <c r="B1081" s="80" t="s">
         <v>1857</v>
       </c>
-      <c r="C1081" s="72"/>
+      <c r="C1081" s="81"/>
       <c r="D1081" s="6"/>
       <c r="E1081" s="29"/>
       <c r="F1081" s="24"/>
@@ -35130,8 +35142,8 @@
     </row>
     <row r="1082" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="29"/>
-      <c r="B1082" s="69"/>
-      <c r="C1082" s="70"/>
+      <c r="B1082" s="82"/>
+      <c r="C1082" s="83"/>
       <c r="D1082" s="6"/>
       <c r="E1082" s="29"/>
       <c r="F1082" s="24"/>
@@ -35186,8 +35198,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="69"/>
-      <c r="C1085" s="70"/>
+      <c r="B1085" s="82"/>
+      <c r="C1085" s="83"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -35200,10 +35212,10 @@
     </row>
     <row r="1086" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1086" s="29"/>
-      <c r="B1086" s="71" t="s">
+      <c r="B1086" s="80" t="s">
         <v>1858</v>
       </c>
-      <c r="C1086" s="72"/>
+      <c r="C1086" s="81"/>
       <c r="D1086" s="6"/>
       <c r="E1086" s="29"/>
       <c r="F1086" s="24"/>
@@ -35216,8 +35228,8 @@
     </row>
     <row r="1087" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1087" s="29"/>
-      <c r="B1087" s="69"/>
-      <c r="C1087" s="70"/>
+      <c r="B1087" s="82"/>
+      <c r="C1087" s="83"/>
       <c r="D1087" s="6"/>
       <c r="E1087" s="29"/>
       <c r="F1087" s="24"/>
@@ -37706,8 +37718,8 @@
     </row>
     <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="69"/>
-      <c r="C1194" s="70"/>
+      <c r="B1194" s="82"/>
+      <c r="C1194" s="83"/>
       <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
       <c r="F1194" s="24"/>
@@ -37720,10 +37732,10 @@
     </row>
     <row r="1195" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1195" s="29"/>
-      <c r="B1195" s="71" t="s">
+      <c r="B1195" s="80" t="s">
         <v>2035</v>
       </c>
-      <c r="C1195" s="72"/>
+      <c r="C1195" s="81"/>
       <c r="D1195" s="6"/>
       <c r="E1195" s="29"/>
       <c r="F1195" s="24"/>
@@ -37736,8 +37748,8 @@
     </row>
     <row r="1196" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1196" s="29"/>
-      <c r="B1196" s="69"/>
-      <c r="C1196" s="70"/>
+      <c r="B1196" s="82"/>
+      <c r="C1196" s="83"/>
       <c r="D1196" s="6"/>
       <c r="E1196" s="29"/>
       <c r="F1196" s="24"/>
@@ -38098,59 +38110,175 @@
       <c r="K1211" s="14"/>
       <c r="L1211" s="29"/>
     </row>
-    <row r="1212" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1212" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1212" s="29"/>
-      <c r="B1212" s="60"/>
-      <c r="C1212" s="67"/>
-      <c r="D1212" s="5"/>
+      <c r="B1212" s="59"/>
+      <c r="C1212" s="64"/>
+      <c r="D1212" s="7"/>
       <c r="E1212" s="29"/>
-      <c r="F1212" s="27"/>
-      <c r="G1212" s="47"/>
+      <c r="F1212" s="26"/>
+      <c r="G1212" s="46"/>
       <c r="H1212" s="29"/>
-      <c r="I1212" s="27"/>
-      <c r="J1212" s="19"/>
-      <c r="K1212" s="20"/>
+      <c r="I1212" s="26"/>
+      <c r="J1212" s="17"/>
+      <c r="K1212" s="18"/>
       <c r="L1212" s="29"/>
     </row>
-    <row r="1213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1213" s="29"/>
-      <c r="B1213" s="55"/>
-      <c r="C1213" s="62"/>
-      <c r="D1213" s="32"/>
+      <c r="B1213" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1213" s="54" t="s">
+        <v>2079</v>
+      </c>
+      <c r="D1213" s="3" t="s">
+        <v>2081</v>
+      </c>
       <c r="E1213" s="29"/>
-      <c r="F1213" s="33"/>
-      <c r="G1213" s="41"/>
+      <c r="F1213" s="23">
+        <v>45002</v>
+      </c>
+      <c r="G1213" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1213" s="29"/>
-      <c r="I1213" s="33"/>
-      <c r="J1213" s="34"/>
-      <c r="K1213" s="34"/>
+      <c r="I1213" s="23"/>
+      <c r="J1213" s="13"/>
+      <c r="K1213" s="14"/>
       <c r="L1213" s="29"/>
     </row>
-    <row r="1215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1214" s="29"/>
+      <c r="B1214" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1214" s="54" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D1214" s="3" t="s">
+        <v>2080</v>
+      </c>
+      <c r="E1214" s="29"/>
+      <c r="F1214" s="23">
+        <v>45002</v>
+      </c>
+      <c r="G1214" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="H1214" s="29"/>
+      <c r="I1214" s="23"/>
+      <c r="J1214" s="13"/>
+      <c r="K1214" s="14"/>
+      <c r="L1214" s="29"/>
+    </row>
+    <row r="1215" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1215" s="29"/>
-      <c r="B1215" s="55"/>
-      <c r="C1215" s="54" t="s">
+      <c r="B1215" s="60"/>
+      <c r="C1215" s="67"/>
+      <c r="D1215" s="5"/>
+      <c r="E1215" s="29"/>
+      <c r="F1215" s="27"/>
+      <c r="G1215" s="47"/>
+      <c r="H1215" s="29"/>
+      <c r="I1215" s="27"/>
+      <c r="J1215" s="19"/>
+      <c r="K1215" s="20"/>
+      <c r="L1215" s="29"/>
+    </row>
+    <row r="1216" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1216" s="29"/>
+      <c r="B1216" s="55"/>
+      <c r="C1216" s="62"/>
+      <c r="D1216" s="32"/>
+      <c r="E1216" s="29"/>
+      <c r="F1216" s="33"/>
+      <c r="G1216" s="41"/>
+      <c r="H1216" s="29"/>
+      <c r="I1216" s="33"/>
+      <c r="J1216" s="34"/>
+      <c r="K1216" s="34"/>
+      <c r="L1216" s="29"/>
+    </row>
+    <row r="1218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1218" s="29"/>
+      <c r="B1218" s="55"/>
+      <c r="C1218" s="54" t="s">
         <v>364</v>
       </c>
-      <c r="D1215" s="3" t="s">
+      <c r="D1218" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E1215" s="29"/>
-      <c r="F1215" s="23"/>
-      <c r="G1215" s="44"/>
-      <c r="H1215" s="29"/>
-      <c r="I1215" s="23"/>
-      <c r="J1215" s="13"/>
-      <c r="K1215" s="14"/>
-      <c r="L1215" s="29"/>
+      <c r="E1218" s="29"/>
+      <c r="F1218" s="23"/>
+      <c r="G1218" s="44"/>
+      <c r="H1218" s="29"/>
+      <c r="I1218" s="23"/>
+      <c r="J1218" s="13"/>
+      <c r="K1218" s="14"/>
+      <c r="L1218" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B488:C488"/>
+    <mergeCell ref="B344:C344"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B212:C212"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B343:C343"/>
+    <mergeCell ref="B345:C345"/>
+    <mergeCell ref="B484:C484"/>
+    <mergeCell ref="B487:C487"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B940:C940"/>
+    <mergeCell ref="B932:C932"/>
+    <mergeCell ref="B816:C816"/>
+    <mergeCell ref="B711:C711"/>
+    <mergeCell ref="B554:C554"/>
+    <mergeCell ref="B817:C817"/>
+    <mergeCell ref="B815:C815"/>
+    <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B933:C933"/>
+    <mergeCell ref="B939:C939"/>
+    <mergeCell ref="B1194:C1194"/>
+    <mergeCell ref="B1196:C1196"/>
+    <mergeCell ref="B1195:C1195"/>
+    <mergeCell ref="B1086:C1086"/>
+    <mergeCell ref="B1081:C1081"/>
+    <mergeCell ref="B941:C941"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B1085:C1085"/>
+    <mergeCell ref="B1087:C1087"/>
+    <mergeCell ref="B1080:C1080"/>
+    <mergeCell ref="B1082:C1082"/>
+    <mergeCell ref="B966:C966"/>
+    <mergeCell ref="B489:C489"/>
+    <mergeCell ref="B553:C553"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B710:C710"/>
+    <mergeCell ref="B712:C712"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B138:C138"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D2:D3"/>
@@ -38167,65 +38295,11 @@
     <mergeCell ref="B106:C106"/>
     <mergeCell ref="B130:C130"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B489:C489"/>
-    <mergeCell ref="B553:C553"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B712:C712"/>
-    <mergeCell ref="B941:C941"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B1085:C1085"/>
-    <mergeCell ref="B1087:C1087"/>
-    <mergeCell ref="B1080:C1080"/>
-    <mergeCell ref="B1082:C1082"/>
-    <mergeCell ref="B966:C966"/>
-    <mergeCell ref="B1194:C1194"/>
-    <mergeCell ref="B1196:C1196"/>
-    <mergeCell ref="B1195:C1195"/>
-    <mergeCell ref="B1086:C1086"/>
-    <mergeCell ref="B1081:C1081"/>
-    <mergeCell ref="B940:C940"/>
-    <mergeCell ref="B932:C932"/>
-    <mergeCell ref="B816:C816"/>
-    <mergeCell ref="B711:C711"/>
-    <mergeCell ref="B554:C554"/>
-    <mergeCell ref="B817:C817"/>
-    <mergeCell ref="B815:C815"/>
-    <mergeCell ref="B931:C931"/>
-    <mergeCell ref="B933:C933"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B488:C488"/>
-    <mergeCell ref="B344:C344"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B212:C212"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B343:C343"/>
-    <mergeCell ref="B345:C345"/>
-    <mergeCell ref="B484:C484"/>
-    <mergeCell ref="B487:C487"/>
-    <mergeCell ref="B183:C183"/>
-    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38255,80 +38329,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="88" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="88" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="88" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="88" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="87" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="88"/>
+      <c r="I7" s="87"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="86" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38337,62 +38411,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="86" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="88" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="88" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="88" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="88" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="87" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="88"/>
+      <c r="I12" s="87"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="86" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38401,13 +38475,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="86" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38416,13 +38490,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="86" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38431,13 +38505,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="86" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38446,24 +38520,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="86" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="86" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38472,12 +38546,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="86" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38486,13 +38560,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="86" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38501,13 +38575,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="86" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38516,13 +38590,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="86" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38531,53 +38605,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="86" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="88" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="88" t="s">
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="87" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="88"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="86" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="86" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38586,12 +38660,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38600,24 +38674,28 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="87" t="s">
+      <c r="E28" s="86" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38633,16 +38711,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 20 Maret 2023 11:39 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4146" uniqueCount="2082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="2084">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8292,6 +8292,12 @@
   </si>
   <si>
     <t>Mendapatkan Daftar Tujuan untuk Pemetaan Ulang Manual Urutan Jalur WorkFlow</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.remapping.manual.setWorkFlowPathSequenceRemapping</t>
+  </si>
+  <si>
+    <t>Menyimpan Pemetaan Urutan Jalur WorkFlow</t>
   </si>
 </sst>
 </file>
@@ -8959,6 +8965,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -8992,31 +9016,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9328,13 +9334,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1218"/>
+  <dimension ref="A1:M1219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="E1202" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D1202" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I1214" sqref="I1214"/>
+      <selection pane="bottomRight" activeCell="G1216" sqref="G1216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9370,31 +9376,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="84" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="73"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="75" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="71"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9416,8 +9422,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9430,10 +9436,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="71" t="s">
         <v>1852</v>
       </c>
-      <c r="C5" s="81"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9446,8 +9452,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9564,8 +9570,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9578,10 +9584,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="71" t="s">
         <v>1851</v>
       </c>
-      <c r="C12" s="81"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9594,8 +9600,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9676,8 +9682,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9690,10 +9696,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="71" t="s">
         <v>1850</v>
       </c>
-      <c r="C18" s="81"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9706,8 +9712,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9782,8 +9788,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9812,8 +9818,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11390,8 +11396,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="82"/>
-      <c r="C95" s="83"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="70"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11404,10 +11410,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="80" t="s">
+      <c r="B96" s="71" t="s">
         <v>1871</v>
       </c>
-      <c r="C96" s="81"/>
+      <c r="C96" s="72"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11420,8 +11426,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="82"/>
-      <c r="C97" s="83"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="70"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11580,8 +11586,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="82"/>
-      <c r="C104" s="83"/>
+      <c r="B104" s="69"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11594,10 +11600,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="80" t="s">
+      <c r="B105" s="71" t="s">
         <v>1870</v>
       </c>
-      <c r="C105" s="81"/>
+      <c r="C105" s="72"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11610,8 +11616,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="82"/>
-      <c r="C106" s="83"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="70"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12116,8 +12122,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="82"/>
-      <c r="C130" s="83"/>
+      <c r="B130" s="69"/>
+      <c r="C130" s="70"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12130,10 +12136,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="80" t="s">
+      <c r="B131" s="71" t="s">
         <v>1868</v>
       </c>
-      <c r="C131" s="81"/>
+      <c r="C131" s="72"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12146,8 +12152,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="82"/>
-      <c r="C132" s="83"/>
+      <c r="B132" s="69"/>
+      <c r="C132" s="70"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12258,8 +12264,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="82"/>
-      <c r="C137" s="83"/>
+      <c r="B137" s="69"/>
+      <c r="C137" s="70"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12272,10 +12278,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="80" t="s">
+      <c r="B138" s="71" t="s">
         <v>1869</v>
       </c>
-      <c r="C138" s="81"/>
+      <c r="C138" s="72"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12288,8 +12294,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="82"/>
-      <c r="C139" s="83"/>
+      <c r="B139" s="69"/>
+      <c r="C139" s="70"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12450,8 +12456,8 @@
     </row>
     <row r="147" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="29"/>
-      <c r="B147" s="82"/>
-      <c r="C147" s="83"/>
+      <c r="B147" s="69"/>
+      <c r="C147" s="70"/>
       <c r="D147" s="6"/>
       <c r="E147" s="29"/>
       <c r="F147" s="24"/>
@@ -12464,10 +12470,10 @@
     </row>
     <row r="148" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A148" s="29"/>
-      <c r="B148" s="80" t="s">
+      <c r="B148" s="71" t="s">
         <v>1867</v>
       </c>
-      <c r="C148" s="81"/>
+      <c r="C148" s="72"/>
       <c r="D148" s="6"/>
       <c r="E148" s="29"/>
       <c r="F148" s="24"/>
@@ -12480,8 +12486,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="82"/>
-      <c r="C149" s="83"/>
+      <c r="B149" s="69"/>
+      <c r="C149" s="70"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12642,8 +12648,8 @@
     </row>
     <row r="157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="29"/>
-      <c r="B157" s="82"/>
-      <c r="C157" s="83"/>
+      <c r="B157" s="69"/>
+      <c r="C157" s="70"/>
       <c r="D157" s="6"/>
       <c r="E157" s="29"/>
       <c r="F157" s="24"/>
@@ -12756,8 +12762,8 @@
     </row>
     <row r="163" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="82"/>
-      <c r="C163" s="83"/>
+      <c r="B163" s="69"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -12770,10 +12776,10 @@
     </row>
     <row r="164" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="80" t="s">
+      <c r="B164" s="71" t="s">
         <v>1866</v>
       </c>
-      <c r="C164" s="81"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -12786,8 +12792,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="82"/>
-      <c r="C165" s="83"/>
+      <c r="B165" s="69"/>
+      <c r="C165" s="70"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -13044,8 +13050,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="82"/>
-      <c r="C177" s="83"/>
+      <c r="B177" s="69"/>
+      <c r="C177" s="70"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -13058,10 +13064,10 @@
     </row>
     <row r="178" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A178" s="29"/>
-      <c r="B178" s="80" t="s">
+      <c r="B178" s="71" t="s">
         <v>1864</v>
       </c>
-      <c r="C178" s="81"/>
+      <c r="C178" s="72"/>
       <c r="D178" s="6"/>
       <c r="E178" s="29"/>
       <c r="F178" s="24"/>
@@ -13074,8 +13080,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="82"/>
-      <c r="C179" s="83"/>
+      <c r="B179" s="69"/>
+      <c r="C179" s="70"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13140,8 +13146,8 @@
     </row>
     <row r="183" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="29"/>
-      <c r="B183" s="82"/>
-      <c r="C183" s="83"/>
+      <c r="B183" s="69"/>
+      <c r="C183" s="70"/>
       <c r="D183" s="6"/>
       <c r="E183" s="29"/>
       <c r="F183" s="24"/>
@@ -13154,10 +13160,10 @@
     </row>
     <row r="184" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A184" s="29"/>
-      <c r="B184" s="80" t="s">
+      <c r="B184" s="71" t="s">
         <v>1865</v>
       </c>
-      <c r="C184" s="81"/>
+      <c r="C184" s="72"/>
       <c r="D184" s="6"/>
       <c r="E184" s="29"/>
       <c r="F184" s="24"/>
@@ -13170,8 +13176,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="82"/>
-      <c r="C185" s="83"/>
+      <c r="B185" s="69"/>
+      <c r="C185" s="70"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13756,8 +13762,8 @@
     </row>
     <row r="211" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="29"/>
-      <c r="B211" s="82"/>
-      <c r="C211" s="83"/>
+      <c r="B211" s="69"/>
+      <c r="C211" s="70"/>
       <c r="D211" s="6"/>
       <c r="E211" s="29"/>
       <c r="F211" s="24"/>
@@ -13770,10 +13776,10 @@
     </row>
     <row r="212" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="29"/>
-      <c r="B212" s="80" t="s">
+      <c r="B212" s="71" t="s">
         <v>1863</v>
       </c>
-      <c r="C212" s="81"/>
+      <c r="C212" s="72"/>
       <c r="D212" s="6"/>
       <c r="E212" s="29"/>
       <c r="F212" s="24"/>
@@ -13786,8 +13792,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="82"/>
-      <c r="C213" s="83"/>
+      <c r="B213" s="69"/>
+      <c r="C213" s="70"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13982,8 +13988,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="82"/>
-      <c r="C222" s="83"/>
+      <c r="B222" s="69"/>
+      <c r="C222" s="70"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -13996,10 +14002,10 @@
     </row>
     <row r="223" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="80" t="s">
+      <c r="B223" s="71" t="s">
         <v>1862</v>
       </c>
-      <c r="C223" s="81"/>
+      <c r="C223" s="72"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -14012,8 +14018,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="82"/>
-      <c r="C224" s="83"/>
+      <c r="B224" s="69"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -16848,8 +16854,8 @@
     </row>
     <row r="343" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="29"/>
-      <c r="B343" s="82"/>
-      <c r="C343" s="83"/>
+      <c r="B343" s="69"/>
+      <c r="C343" s="70"/>
       <c r="D343" s="6"/>
       <c r="E343" s="29"/>
       <c r="F343" s="24"/>
@@ -16862,10 +16868,10 @@
     </row>
     <row r="344" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A344" s="29"/>
-      <c r="B344" s="80" t="s">
+      <c r="B344" s="71" t="s">
         <v>1861</v>
       </c>
-      <c r="C344" s="81"/>
+      <c r="C344" s="72"/>
       <c r="D344" s="6"/>
       <c r="E344" s="29"/>
       <c r="F344" s="24"/>
@@ -16878,8 +16884,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="82"/>
-      <c r="C345" s="83"/>
+      <c r="B345" s="69"/>
+      <c r="C345" s="70"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -20504,8 +20510,8 @@
     </row>
     <row r="484" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A484" s="29"/>
-      <c r="B484" s="82"/>
-      <c r="C484" s="83"/>
+      <c r="B484" s="69"/>
+      <c r="C484" s="70"/>
       <c r="D484" s="6"/>
       <c r="E484" s="29"/>
       <c r="F484" s="24"/>
@@ -20560,8 +20566,8 @@
     </row>
     <row r="487" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A487" s="29"/>
-      <c r="B487" s="82"/>
-      <c r="C487" s="83"/>
+      <c r="B487" s="69"/>
+      <c r="C487" s="70"/>
       <c r="D487" s="6"/>
       <c r="E487" s="29"/>
       <c r="F487" s="24"/>
@@ -20574,10 +20580,10 @@
     </row>
     <row r="488" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A488" s="29"/>
-      <c r="B488" s="80" t="s">
+      <c r="B488" s="71" t="s">
         <v>1860</v>
       </c>
-      <c r="C488" s="81"/>
+      <c r="C488" s="72"/>
       <c r="D488" s="6"/>
       <c r="E488" s="29"/>
       <c r="F488" s="24"/>
@@ -20590,8 +20596,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="82"/>
-      <c r="C489" s="83"/>
+      <c r="B489" s="69"/>
+      <c r="C489" s="70"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -22190,8 +22196,8 @@
     </row>
     <row r="553" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="29"/>
-      <c r="B553" s="82"/>
-      <c r="C553" s="83"/>
+      <c r="B553" s="69"/>
+      <c r="C553" s="70"/>
       <c r="D553" s="6"/>
       <c r="E553" s="29"/>
       <c r="F553" s="24"/>
@@ -22204,10 +22210,10 @@
     </row>
     <row r="554" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A554" s="29"/>
-      <c r="B554" s="80" t="s">
+      <c r="B554" s="71" t="s">
         <v>1859</v>
       </c>
-      <c r="C554" s="81"/>
+      <c r="C554" s="72"/>
       <c r="D554" s="6"/>
       <c r="E554" s="29"/>
       <c r="F554" s="24"/>
@@ -22220,8 +22226,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="82"/>
-      <c r="C555" s="83"/>
+      <c r="B555" s="69"/>
+      <c r="C555" s="70"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -26020,8 +26026,8 @@
     </row>
     <row r="710" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710" s="29"/>
-      <c r="B710" s="82"/>
-      <c r="C710" s="83"/>
+      <c r="B710" s="69"/>
+      <c r="C710" s="70"/>
       <c r="D710" s="6"/>
       <c r="E710" s="29"/>
       <c r="F710" s="24"/>
@@ -26034,10 +26040,10 @@
     </row>
     <row r="711" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A711" s="29"/>
-      <c r="B711" s="80" t="s">
+      <c r="B711" s="71" t="s">
         <v>1853</v>
       </c>
-      <c r="C711" s="81"/>
+      <c r="C711" s="72"/>
       <c r="D711" s="6"/>
       <c r="E711" s="29"/>
       <c r="F711" s="24"/>
@@ -26050,8 +26056,8 @@
     </row>
     <row r="712" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712" s="29"/>
-      <c r="B712" s="82"/>
-      <c r="C712" s="83"/>
+      <c r="B712" s="69"/>
+      <c r="C712" s="70"/>
       <c r="D712" s="6"/>
       <c r="E712" s="29"/>
       <c r="F712" s="24"/>
@@ -28508,8 +28514,8 @@
     </row>
     <row r="815" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815" s="29"/>
-      <c r="B815" s="82"/>
-      <c r="C815" s="83"/>
+      <c r="B815" s="69"/>
+      <c r="C815" s="70"/>
       <c r="D815" s="6"/>
       <c r="E815" s="29"/>
       <c r="F815" s="24"/>
@@ -28522,10 +28528,10 @@
     </row>
     <row r="816" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A816" s="29"/>
-      <c r="B816" s="80" t="s">
+      <c r="B816" s="71" t="s">
         <v>1854</v>
       </c>
-      <c r="C816" s="81"/>
+      <c r="C816" s="72"/>
       <c r="D816" s="6"/>
       <c r="E816" s="29"/>
       <c r="F816" s="24"/>
@@ -28538,8 +28544,8 @@
     </row>
     <row r="817" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817" s="29"/>
-      <c r="B817" s="82"/>
-      <c r="C817" s="83"/>
+      <c r="B817" s="69"/>
+      <c r="C817" s="70"/>
       <c r="D817" s="6"/>
       <c r="E817" s="29"/>
       <c r="F817" s="24"/>
@@ -31453,8 +31459,8 @@
     </row>
     <row r="931" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931" s="29"/>
-      <c r="B931" s="82"/>
-      <c r="C931" s="83"/>
+      <c r="B931" s="69"/>
+      <c r="C931" s="70"/>
       <c r="D931" s="6"/>
       <c r="E931" s="29"/>
       <c r="F931" s="24"/>
@@ -31467,10 +31473,10 @@
     </row>
     <row r="932" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A932" s="29"/>
-      <c r="B932" s="80" t="s">
+      <c r="B932" s="71" t="s">
         <v>1952</v>
       </c>
-      <c r="C932" s="81"/>
+      <c r="C932" s="72"/>
       <c r="D932" s="6"/>
       <c r="E932" s="29"/>
       <c r="F932" s="24"/>
@@ -31483,8 +31489,8 @@
     </row>
     <row r="933" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933" s="29"/>
-      <c r="B933" s="82"/>
-      <c r="C933" s="83"/>
+      <c r="B933" s="69"/>
+      <c r="C933" s="70"/>
       <c r="D933" s="6"/>
       <c r="E933" s="29"/>
       <c r="F933" s="24"/>
@@ -31618,8 +31624,8 @@
     </row>
     <row r="939" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939" s="29"/>
-      <c r="B939" s="82"/>
-      <c r="C939" s="83"/>
+      <c r="B939" s="69"/>
+      <c r="C939" s="70"/>
       <c r="D939" s="6"/>
       <c r="E939" s="29"/>
       <c r="F939" s="24"/>
@@ -31632,10 +31638,10 @@
     </row>
     <row r="940" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A940" s="29"/>
-      <c r="B940" s="80" t="s">
+      <c r="B940" s="71" t="s">
         <v>1855</v>
       </c>
-      <c r="C940" s="81"/>
+      <c r="C940" s="72"/>
       <c r="D940" s="6"/>
       <c r="E940" s="29"/>
       <c r="F940" s="24"/>
@@ -31648,8 +31654,8 @@
     </row>
     <row r="941" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941" s="29"/>
-      <c r="B941" s="82"/>
-      <c r="C941" s="83"/>
+      <c r="B941" s="69"/>
+      <c r="C941" s="70"/>
       <c r="D941" s="6"/>
       <c r="E941" s="29"/>
       <c r="F941" s="24"/>
@@ -32172,8 +32178,8 @@
     </row>
     <row r="965" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965" s="29"/>
-      <c r="B965" s="82"/>
-      <c r="C965" s="83"/>
+      <c r="B965" s="69"/>
+      <c r="C965" s="70"/>
       <c r="D965" s="6"/>
       <c r="E965" s="29"/>
       <c r="F965" s="24"/>
@@ -32186,10 +32192,10 @@
     </row>
     <row r="966" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A966" s="29"/>
-      <c r="B966" s="80" t="s">
+      <c r="B966" s="71" t="s">
         <v>1856</v>
       </c>
-      <c r="C966" s="81"/>
+      <c r="C966" s="72"/>
       <c r="D966" s="6"/>
       <c r="E966" s="29"/>
       <c r="F966" s="24"/>
@@ -32202,8 +32208,8 @@
     </row>
     <row r="967" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967" s="29"/>
-      <c r="B967" s="82"/>
-      <c r="C967" s="83"/>
+      <c r="B967" s="69"/>
+      <c r="C967" s="70"/>
       <c r="D967" s="6"/>
       <c r="E967" s="29"/>
       <c r="F967" s="24"/>
@@ -35112,8 +35118,8 @@
     </row>
     <row r="1080" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1080" s="29"/>
-      <c r="B1080" s="82"/>
-      <c r="C1080" s="83"/>
+      <c r="B1080" s="69"/>
+      <c r="C1080" s="70"/>
       <c r="D1080" s="6"/>
       <c r="E1080" s="29"/>
       <c r="F1080" s="24"/>
@@ -35126,10 +35132,10 @@
     </row>
     <row r="1081" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1081" s="29"/>
-      <c r="B1081" s="80" t="s">
+      <c r="B1081" s="71" t="s">
         <v>1857</v>
       </c>
-      <c r="C1081" s="81"/>
+      <c r="C1081" s="72"/>
       <c r="D1081" s="6"/>
       <c r="E1081" s="29"/>
       <c r="F1081" s="24"/>
@@ -35142,8 +35148,8 @@
     </row>
     <row r="1082" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="29"/>
-      <c r="B1082" s="82"/>
-      <c r="C1082" s="83"/>
+      <c r="B1082" s="69"/>
+      <c r="C1082" s="70"/>
       <c r="D1082" s="6"/>
       <c r="E1082" s="29"/>
       <c r="F1082" s="24"/>
@@ -35198,8 +35204,8 @@
     </row>
     <row r="1085" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1085" s="29"/>
-      <c r="B1085" s="82"/>
-      <c r="C1085" s="83"/>
+      <c r="B1085" s="69"/>
+      <c r="C1085" s="70"/>
       <c r="D1085" s="6"/>
       <c r="E1085" s="29"/>
       <c r="F1085" s="24"/>
@@ -35212,10 +35218,10 @@
     </row>
     <row r="1086" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1086" s="29"/>
-      <c r="B1086" s="80" t="s">
+      <c r="B1086" s="71" t="s">
         <v>1858</v>
       </c>
-      <c r="C1086" s="81"/>
+      <c r="C1086" s="72"/>
       <c r="D1086" s="6"/>
       <c r="E1086" s="29"/>
       <c r="F1086" s="24"/>
@@ -35228,8 +35234,8 @@
     </row>
     <row r="1087" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1087" s="29"/>
-      <c r="B1087" s="82"/>
-      <c r="C1087" s="83"/>
+      <c r="B1087" s="69"/>
+      <c r="C1087" s="70"/>
       <c r="D1087" s="6"/>
       <c r="E1087" s="29"/>
       <c r="F1087" s="24"/>
@@ -37718,8 +37724,8 @@
     </row>
     <row r="1194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1194" s="29"/>
-      <c r="B1194" s="82"/>
-      <c r="C1194" s="83"/>
+      <c r="B1194" s="69"/>
+      <c r="C1194" s="70"/>
       <c r="D1194" s="6"/>
       <c r="E1194" s="29"/>
       <c r="F1194" s="24"/>
@@ -37732,10 +37738,10 @@
     </row>
     <row r="1195" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1195" s="29"/>
-      <c r="B1195" s="80" t="s">
+      <c r="B1195" s="71" t="s">
         <v>2035</v>
       </c>
-      <c r="C1195" s="81"/>
+      <c r="C1195" s="72"/>
       <c r="D1195" s="6"/>
       <c r="E1195" s="29"/>
       <c r="F1195" s="24"/>
@@ -37748,8 +37754,8 @@
     </row>
     <row r="1196" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1196" s="29"/>
-      <c r="B1196" s="82"/>
-      <c r="C1196" s="83"/>
+      <c r="B1196" s="69"/>
+      <c r="C1196" s="70"/>
       <c r="D1196" s="6"/>
       <c r="E1196" s="29"/>
       <c r="F1196" s="24"/>
@@ -38172,54 +38178,142 @@
       <c r="K1214" s="14"/>
       <c r="L1214" s="29"/>
     </row>
-    <row r="1215" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1215" s="29"/>
-      <c r="B1215" s="60"/>
-      <c r="C1215" s="67"/>
-      <c r="D1215" s="5"/>
+      <c r="B1215" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1215" s="54" t="s">
+        <v>2082</v>
+      </c>
+      <c r="D1215" s="3" t="s">
+        <v>2083</v>
+      </c>
       <c r="E1215" s="29"/>
-      <c r="F1215" s="27"/>
-      <c r="G1215" s="47"/>
+      <c r="F1215" s="23">
+        <v>45005</v>
+      </c>
+      <c r="G1215" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1215" s="29"/>
-      <c r="I1215" s="27"/>
-      <c r="J1215" s="19"/>
-      <c r="K1215" s="20"/>
+      <c r="I1215" s="23"/>
+      <c r="J1215" s="13"/>
+      <c r="K1215" s="14"/>
       <c r="L1215" s="29"/>
     </row>
-    <row r="1216" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1216" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1216" s="29"/>
-      <c r="B1216" s="55"/>
-      <c r="C1216" s="62"/>
-      <c r="D1216" s="32"/>
+      <c r="B1216" s="60"/>
+      <c r="C1216" s="67"/>
+      <c r="D1216" s="5"/>
       <c r="E1216" s="29"/>
-      <c r="F1216" s="33"/>
-      <c r="G1216" s="41"/>
+      <c r="F1216" s="27"/>
+      <c r="G1216" s="47"/>
       <c r="H1216" s="29"/>
-      <c r="I1216" s="33"/>
-      <c r="J1216" s="34"/>
-      <c r="K1216" s="34"/>
+      <c r="I1216" s="27"/>
+      <c r="J1216" s="19"/>
+      <c r="K1216" s="20"/>
       <c r="L1216" s="29"/>
     </row>
-    <row r="1218" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1218" s="29"/>
-      <c r="B1218" s="55"/>
-      <c r="C1218" s="54" t="s">
+    <row r="1217" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1217" s="29"/>
+      <c r="B1217" s="55"/>
+      <c r="C1217" s="62"/>
+      <c r="D1217" s="32"/>
+      <c r="E1217" s="29"/>
+      <c r="F1217" s="33"/>
+      <c r="G1217" s="41"/>
+      <c r="H1217" s="29"/>
+      <c r="I1217" s="33"/>
+      <c r="J1217" s="34"/>
+      <c r="K1217" s="34"/>
+      <c r="L1217" s="29"/>
+    </row>
+    <row r="1219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1219" s="29"/>
+      <c r="B1219" s="55"/>
+      <c r="C1219" s="54" t="s">
         <v>364</v>
       </c>
-      <c r="D1218" s="3" t="s">
+      <c r="D1219" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="E1218" s="29"/>
-      <c r="F1218" s="23"/>
-      <c r="G1218" s="44"/>
-      <c r="H1218" s="29"/>
-      <c r="I1218" s="23"/>
-      <c r="J1218" s="13"/>
-      <c r="K1218" s="14"/>
-      <c r="L1218" s="29"/>
+      <c r="E1219" s="29"/>
+      <c r="F1219" s="23"/>
+      <c r="G1219" s="44"/>
+      <c r="H1219" s="29"/>
+      <c r="I1219" s="23"/>
+      <c r="J1219" s="13"/>
+      <c r="K1219" s="14"/>
+      <c r="L1219" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B222:C222"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B489:C489"/>
+    <mergeCell ref="B553:C553"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B710:C710"/>
+    <mergeCell ref="B712:C712"/>
+    <mergeCell ref="B941:C941"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B965:C965"/>
+    <mergeCell ref="B1085:C1085"/>
+    <mergeCell ref="B1087:C1087"/>
+    <mergeCell ref="B1080:C1080"/>
+    <mergeCell ref="B1082:C1082"/>
+    <mergeCell ref="B966:C966"/>
+    <mergeCell ref="B1194:C1194"/>
+    <mergeCell ref="B1196:C1196"/>
+    <mergeCell ref="B1195:C1195"/>
+    <mergeCell ref="B1086:C1086"/>
+    <mergeCell ref="B1081:C1081"/>
+    <mergeCell ref="B940:C940"/>
+    <mergeCell ref="B932:C932"/>
+    <mergeCell ref="B816:C816"/>
+    <mergeCell ref="B711:C711"/>
+    <mergeCell ref="B554:C554"/>
+    <mergeCell ref="B817:C817"/>
+    <mergeCell ref="B815:C815"/>
+    <mergeCell ref="B931:C931"/>
+    <mergeCell ref="B933:C933"/>
+    <mergeCell ref="B939:C939"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B23:C23"/>
@@ -38236,70 +38330,6 @@
     <mergeCell ref="B487:C487"/>
     <mergeCell ref="B183:C183"/>
     <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B940:C940"/>
-    <mergeCell ref="B932:C932"/>
-    <mergeCell ref="B816:C816"/>
-    <mergeCell ref="B711:C711"/>
-    <mergeCell ref="B554:C554"/>
-    <mergeCell ref="B817:C817"/>
-    <mergeCell ref="B815:C815"/>
-    <mergeCell ref="B931:C931"/>
-    <mergeCell ref="B933:C933"/>
-    <mergeCell ref="B939:C939"/>
-    <mergeCell ref="B1194:C1194"/>
-    <mergeCell ref="B1196:C1196"/>
-    <mergeCell ref="B1195:C1195"/>
-    <mergeCell ref="B1086:C1086"/>
-    <mergeCell ref="B1081:C1081"/>
-    <mergeCell ref="B941:C941"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B965:C965"/>
-    <mergeCell ref="B1085:C1085"/>
-    <mergeCell ref="B1087:C1087"/>
-    <mergeCell ref="B1080:C1080"/>
-    <mergeCell ref="B1082:C1082"/>
-    <mergeCell ref="B966:C966"/>
-    <mergeCell ref="B489:C489"/>
-    <mergeCell ref="B553:C553"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B710:C710"/>
-    <mergeCell ref="B712:C712"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B222:C222"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38329,80 +38359,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38411,62 +38441,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38475,13 +38505,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38490,13 +38520,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38505,13 +38535,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38520,24 +38550,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38546,12 +38576,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38560,13 +38590,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38575,13 +38605,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38590,13 +38620,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38605,53 +38635,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38660,12 +38690,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38674,28 +38704,24 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38711,12 +38737,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 20 Maret 2023 16:57 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="2078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="2084">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8280,6 +8280,24 @@
   </si>
   <si>
     <t>Mengecek Status Final Approve pada Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.remapping.manual.getWorkFlowPathSequenceSourceList</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.remapping.manual.getWorkFlowPathSequenceDestinationList</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Sumber untuk Pemetaan Ulang Manual Urutan Jalur WorkFlow</t>
+  </si>
+  <si>
+    <t>Mendapatkan Daftar Tujuan untuk Pemetaan Ulang Manual Urutan Jalur WorkFlow</t>
+  </si>
+  <si>
+    <t>userAction.documentWorkFlow.remapping.manual.setWorkFlowPathSequenceRemapping</t>
+  </si>
+  <si>
+    <t>Menyimpan Pemetaan Urutan Jalur WorkFlow</t>
   </si>
 </sst>
 </file>
@@ -9316,13 +9334,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1215"/>
+  <dimension ref="A1:M1219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="E1190" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D1202" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I1199" sqref="I1199"/>
+      <selection pane="bottomRight" activeCell="G1216" sqref="G1216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -38098,51 +38116,137 @@
       <c r="K1211" s="14"/>
       <c r="L1211" s="29"/>
     </row>
-    <row r="1212" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1212" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1212" s="29"/>
-      <c r="B1212" s="60"/>
-      <c r="C1212" s="67"/>
-      <c r="D1212" s="5"/>
+      <c r="B1212" s="59"/>
+      <c r="C1212" s="64"/>
+      <c r="D1212" s="7"/>
       <c r="E1212" s="29"/>
-      <c r="F1212" s="27"/>
-      <c r="G1212" s="47"/>
+      <c r="F1212" s="26"/>
+      <c r="G1212" s="46"/>
       <c r="H1212" s="29"/>
-      <c r="I1212" s="27"/>
-      <c r="J1212" s="19"/>
-      <c r="K1212" s="20"/>
+      <c r="I1212" s="26"/>
+      <c r="J1212" s="17"/>
+      <c r="K1212" s="18"/>
       <c r="L1212" s="29"/>
     </row>
-    <row r="1213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1213" s="29"/>
-      <c r="B1213" s="55"/>
-      <c r="C1213" s="62"/>
-      <c r="D1213" s="32"/>
+      <c r="B1213" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1213" s="54" t="s">
+        <v>2079</v>
+      </c>
+      <c r="D1213" s="3" t="s">
+        <v>2081</v>
+      </c>
       <c r="E1213" s="29"/>
-      <c r="F1213" s="33"/>
-      <c r="G1213" s="41"/>
+      <c r="F1213" s="23">
+        <v>45002</v>
+      </c>
+      <c r="G1213" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1213" s="29"/>
-      <c r="I1213" s="33"/>
-      <c r="J1213" s="34"/>
-      <c r="K1213" s="34"/>
+      <c r="I1213" s="23"/>
+      <c r="J1213" s="13"/>
+      <c r="K1213" s="14"/>
       <c r="L1213" s="29"/>
+    </row>
+    <row r="1214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1214" s="29"/>
+      <c r="B1214" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="C1214" s="54" t="s">
+        <v>2078</v>
+      </c>
+      <c r="D1214" s="3" t="s">
+        <v>2080</v>
+      </c>
+      <c r="E1214" s="29"/>
+      <c r="F1214" s="23">
+        <v>45002</v>
+      </c>
+      <c r="G1214" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="H1214" s="29"/>
+      <c r="I1214" s="23"/>
+      <c r="J1214" s="13"/>
+      <c r="K1214" s="14"/>
+      <c r="L1214" s="29"/>
     </row>
     <row r="1215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1215" s="29"/>
-      <c r="B1215" s="55"/>
+      <c r="B1215" s="56" t="s">
+        <v>2047</v>
+      </c>
       <c r="C1215" s="54" t="s">
-        <v>364</v>
+        <v>2082</v>
       </c>
       <c r="D1215" s="3" t="s">
-        <v>365</v>
+        <v>2083</v>
       </c>
       <c r="E1215" s="29"/>
-      <c r="F1215" s="23"/>
-      <c r="G1215" s="44"/>
+      <c r="F1215" s="23">
+        <v>45005</v>
+      </c>
+      <c r="G1215" s="44" t="s">
+        <v>592</v>
+      </c>
       <c r="H1215" s="29"/>
       <c r="I1215" s="23"/>
       <c r="J1215" s="13"/>
       <c r="K1215" s="14"/>
       <c r="L1215" s="29"/>
+    </row>
+    <row r="1216" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1216" s="29"/>
+      <c r="B1216" s="60"/>
+      <c r="C1216" s="67"/>
+      <c r="D1216" s="5"/>
+      <c r="E1216" s="29"/>
+      <c r="F1216" s="27"/>
+      <c r="G1216" s="47"/>
+      <c r="H1216" s="29"/>
+      <c r="I1216" s="27"/>
+      <c r="J1216" s="19"/>
+      <c r="K1216" s="20"/>
+      <c r="L1216" s="29"/>
+    </row>
+    <row r="1217" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1217" s="29"/>
+      <c r="B1217" s="55"/>
+      <c r="C1217" s="62"/>
+      <c r="D1217" s="32"/>
+      <c r="E1217" s="29"/>
+      <c r="F1217" s="33"/>
+      <c r="G1217" s="41"/>
+      <c r="H1217" s="29"/>
+      <c r="I1217" s="33"/>
+      <c r="J1217" s="34"/>
+      <c r="K1217" s="34"/>
+      <c r="L1217" s="29"/>
+    </row>
+    <row r="1219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1219" s="29"/>
+      <c r="B1219" s="55"/>
+      <c r="C1219" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="D1219" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1219" s="29"/>
+      <c r="F1219" s="23"/>
+      <c r="G1219" s="44"/>
+      <c r="H1219" s="29"/>
+      <c r="I1219" s="23"/>
+      <c r="J1219" s="13"/>
+      <c r="K1219" s="14"/>
+      <c r="L1219" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="80">

</xml_diff>

<commit_message>
Update Pertanggal 13 April 2023 13:38 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -8977,6 +8977,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9010,31 +9028,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9388,31 +9388,31 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="84" t="s">
+      <c r="C2" s="81"/>
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="G2" s="73"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="29"/>
-      <c r="I2" s="69" t="s">
+      <c r="I2" s="75" t="s">
         <v>333</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="71"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="77"/>
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" s="28" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="85"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9434,8 +9434,8 @@
     </row>
     <row r="4" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="6"/>
       <c r="E4" s="29"/>
       <c r="F4" s="24"/>
@@ -9448,10 +9448,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="71" t="s">
         <v>1851</v>
       </c>
-      <c r="C5" s="81"/>
+      <c r="C5" s="72"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9464,8 +9464,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9582,8 +9582,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="83"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9596,10 +9596,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="71" t="s">
         <v>1850</v>
       </c>
-      <c r="C12" s="81"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9612,8 +9612,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="83"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9694,8 +9694,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="83"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9708,10 +9708,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="71" t="s">
         <v>1849</v>
       </c>
-      <c r="C18" s="81"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9724,8 +9724,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="83"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9800,8 +9800,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9830,8 +9830,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="70"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11408,8 +11408,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="82"/>
-      <c r="C95" s="83"/>
+      <c r="B95" s="69"/>
+      <c r="C95" s="70"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11422,10 +11422,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="80" t="s">
+      <c r="B96" s="71" t="s">
         <v>1870</v>
       </c>
-      <c r="C96" s="81"/>
+      <c r="C96" s="72"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11438,8 +11438,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="82"/>
-      <c r="C97" s="83"/>
+      <c r="B97" s="69"/>
+      <c r="C97" s="70"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11598,8 +11598,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="82"/>
-      <c r="C104" s="83"/>
+      <c r="B104" s="69"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11612,10 +11612,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="80" t="s">
+      <c r="B105" s="71" t="s">
         <v>1869</v>
       </c>
-      <c r="C105" s="81"/>
+      <c r="C105" s="72"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11628,8 +11628,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="82"/>
-      <c r="C106" s="83"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="70"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12134,8 +12134,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="82"/>
-      <c r="C130" s="83"/>
+      <c r="B130" s="69"/>
+      <c r="C130" s="70"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12148,10 +12148,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="80" t="s">
+      <c r="B131" s="71" t="s">
         <v>1867</v>
       </c>
-      <c r="C131" s="81"/>
+      <c r="C131" s="72"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12164,8 +12164,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="82"/>
-      <c r="C132" s="83"/>
+      <c r="B132" s="69"/>
+      <c r="C132" s="70"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12276,8 +12276,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="82"/>
-      <c r="C137" s="83"/>
+      <c r="B137" s="69"/>
+      <c r="C137" s="70"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12290,10 +12290,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="80" t="s">
+      <c r="B138" s="71" t="s">
         <v>1868</v>
       </c>
-      <c r="C138" s="81"/>
+      <c r="C138" s="72"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12306,8 +12306,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="82"/>
-      <c r="C139" s="83"/>
+      <c r="B139" s="69"/>
+      <c r="C139" s="70"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12516,8 +12516,8 @@
     </row>
     <row r="149" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="29"/>
-      <c r="B149" s="82"/>
-      <c r="C149" s="83"/>
+      <c r="B149" s="69"/>
+      <c r="C149" s="70"/>
       <c r="D149" s="6"/>
       <c r="E149" s="29"/>
       <c r="F149" s="24"/>
@@ -12530,10 +12530,10 @@
     </row>
     <row r="150" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
-      <c r="B150" s="80" t="s">
+      <c r="B150" s="71" t="s">
         <v>1866</v>
       </c>
-      <c r="C150" s="81"/>
+      <c r="C150" s="72"/>
       <c r="D150" s="6"/>
       <c r="E150" s="29"/>
       <c r="F150" s="24"/>
@@ -12546,8 +12546,8 @@
     </row>
     <row r="151" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
-      <c r="B151" s="82"/>
-      <c r="C151" s="83"/>
+      <c r="B151" s="69"/>
+      <c r="C151" s="70"/>
       <c r="D151" s="6"/>
       <c r="E151" s="29"/>
       <c r="F151" s="24"/>
@@ -12708,8 +12708,8 @@
     </row>
     <row r="159" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="29"/>
-      <c r="B159" s="82"/>
-      <c r="C159" s="83"/>
+      <c r="B159" s="69"/>
+      <c r="C159" s="70"/>
       <c r="D159" s="6"/>
       <c r="E159" s="29"/>
       <c r="F159" s="24"/>
@@ -12822,8 +12822,8 @@
     </row>
     <row r="165" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
-      <c r="B165" s="82"/>
-      <c r="C165" s="83"/>
+      <c r="B165" s="69"/>
+      <c r="C165" s="70"/>
       <c r="D165" s="6"/>
       <c r="E165" s="29"/>
       <c r="F165" s="24"/>
@@ -12836,10 +12836,10 @@
     </row>
     <row r="166" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A166" s="29"/>
-      <c r="B166" s="80" t="s">
+      <c r="B166" s="71" t="s">
         <v>1865</v>
       </c>
-      <c r="C166" s="81"/>
+      <c r="C166" s="72"/>
       <c r="D166" s="6"/>
       <c r="E166" s="29"/>
       <c r="F166" s="24"/>
@@ -12852,8 +12852,8 @@
     </row>
     <row r="167" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="29"/>
-      <c r="B167" s="82"/>
-      <c r="C167" s="83"/>
+      <c r="B167" s="69"/>
+      <c r="C167" s="70"/>
       <c r="D167" s="6"/>
       <c r="E167" s="29"/>
       <c r="F167" s="24"/>
@@ -13110,8 +13110,8 @@
     </row>
     <row r="179" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="29"/>
-      <c r="B179" s="82"/>
-      <c r="C179" s="83"/>
+      <c r="B179" s="69"/>
+      <c r="C179" s="70"/>
       <c r="D179" s="6"/>
       <c r="E179" s="29"/>
       <c r="F179" s="24"/>
@@ -13124,10 +13124,10 @@
     </row>
     <row r="180" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A180" s="29"/>
-      <c r="B180" s="80" t="s">
+      <c r="B180" s="71" t="s">
         <v>1863</v>
       </c>
-      <c r="C180" s="81"/>
+      <c r="C180" s="72"/>
       <c r="D180" s="6"/>
       <c r="E180" s="29"/>
       <c r="F180" s="24"/>
@@ -13140,8 +13140,8 @@
     </row>
     <row r="181" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="29"/>
-      <c r="B181" s="82"/>
-      <c r="C181" s="83"/>
+      <c r="B181" s="69"/>
+      <c r="C181" s="70"/>
       <c r="D181" s="6"/>
       <c r="E181" s="29"/>
       <c r="F181" s="24"/>
@@ -13206,8 +13206,8 @@
     </row>
     <row r="185" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="29"/>
-      <c r="B185" s="82"/>
-      <c r="C185" s="83"/>
+      <c r="B185" s="69"/>
+      <c r="C185" s="70"/>
       <c r="D185" s="6"/>
       <c r="E185" s="29"/>
       <c r="F185" s="24"/>
@@ -13220,10 +13220,10 @@
     </row>
     <row r="186" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A186" s="29"/>
-      <c r="B186" s="80" t="s">
+      <c r="B186" s="71" t="s">
         <v>1864</v>
       </c>
-      <c r="C186" s="81"/>
+      <c r="C186" s="72"/>
       <c r="D186" s="6"/>
       <c r="E186" s="29"/>
       <c r="F186" s="24"/>
@@ -13236,8 +13236,8 @@
     </row>
     <row r="187" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="29"/>
-      <c r="B187" s="82"/>
-      <c r="C187" s="83"/>
+      <c r="B187" s="69"/>
+      <c r="C187" s="70"/>
       <c r="D187" s="6"/>
       <c r="E187" s="29"/>
       <c r="F187" s="24"/>
@@ -13822,8 +13822,8 @@
     </row>
     <row r="213" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="29"/>
-      <c r="B213" s="82"/>
-      <c r="C213" s="83"/>
+      <c r="B213" s="69"/>
+      <c r="C213" s="70"/>
       <c r="D213" s="6"/>
       <c r="E213" s="29"/>
       <c r="F213" s="24"/>
@@ -13836,10 +13836,10 @@
     </row>
     <row r="214" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="29"/>
-      <c r="B214" s="80" t="s">
+      <c r="B214" s="71" t="s">
         <v>1862</v>
       </c>
-      <c r="C214" s="81"/>
+      <c r="C214" s="72"/>
       <c r="D214" s="6"/>
       <c r="E214" s="29"/>
       <c r="F214" s="24"/>
@@ -13852,8 +13852,8 @@
     </row>
     <row r="215" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="29"/>
-      <c r="B215" s="82"/>
-      <c r="C215" s="83"/>
+      <c r="B215" s="69"/>
+      <c r="C215" s="70"/>
       <c r="D215" s="6"/>
       <c r="E215" s="29"/>
       <c r="F215" s="24"/>
@@ -14048,8 +14048,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="82"/>
-      <c r="C224" s="83"/>
+      <c r="B224" s="69"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -14062,10 +14062,10 @@
     </row>
     <row r="225" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A225" s="29"/>
-      <c r="B225" s="80" t="s">
+      <c r="B225" s="71" t="s">
         <v>1861</v>
       </c>
-      <c r="C225" s="81"/>
+      <c r="C225" s="72"/>
       <c r="D225" s="6"/>
       <c r="E225" s="29"/>
       <c r="F225" s="24"/>
@@ -14078,8 +14078,8 @@
     </row>
     <row r="226" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="29"/>
-      <c r="B226" s="82"/>
-      <c r="C226" s="83"/>
+      <c r="B226" s="69"/>
+      <c r="C226" s="70"/>
       <c r="D226" s="6"/>
       <c r="E226" s="29"/>
       <c r="F226" s="24"/>
@@ -16914,8 +16914,8 @@
     </row>
     <row r="345" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="29"/>
-      <c r="B345" s="82"/>
-      <c r="C345" s="83"/>
+      <c r="B345" s="69"/>
+      <c r="C345" s="70"/>
       <c r="D345" s="6"/>
       <c r="E345" s="29"/>
       <c r="F345" s="24"/>
@@ -16928,10 +16928,10 @@
     </row>
     <row r="346" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A346" s="29"/>
-      <c r="B346" s="80" t="s">
+      <c r="B346" s="71" t="s">
         <v>1860</v>
       </c>
-      <c r="C346" s="81"/>
+      <c r="C346" s="72"/>
       <c r="D346" s="6"/>
       <c r="E346" s="29"/>
       <c r="F346" s="24"/>
@@ -16944,8 +16944,8 @@
     </row>
     <row r="347" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="29"/>
-      <c r="B347" s="82"/>
-      <c r="C347" s="83"/>
+      <c r="B347" s="69"/>
+      <c r="C347" s="70"/>
       <c r="D347" s="6"/>
       <c r="E347" s="29"/>
       <c r="F347" s="24"/>
@@ -20570,8 +20570,8 @@
     </row>
     <row r="486" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A486" s="29"/>
-      <c r="B486" s="82"/>
-      <c r="C486" s="83"/>
+      <c r="B486" s="69"/>
+      <c r="C486" s="70"/>
       <c r="D486" s="6"/>
       <c r="E486" s="29"/>
       <c r="F486" s="24"/>
@@ -20626,8 +20626,8 @@
     </row>
     <row r="489" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A489" s="29"/>
-      <c r="B489" s="82"/>
-      <c r="C489" s="83"/>
+      <c r="B489" s="69"/>
+      <c r="C489" s="70"/>
       <c r="D489" s="6"/>
       <c r="E489" s="29"/>
       <c r="F489" s="24"/>
@@ -20640,10 +20640,10 @@
     </row>
     <row r="490" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A490" s="29"/>
-      <c r="B490" s="80" t="s">
+      <c r="B490" s="71" t="s">
         <v>1859</v>
       </c>
-      <c r="C490" s="81"/>
+      <c r="C490" s="72"/>
       <c r="D490" s="6"/>
       <c r="E490" s="29"/>
       <c r="F490" s="24"/>
@@ -20656,8 +20656,8 @@
     </row>
     <row r="491" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A491" s="29"/>
-      <c r="B491" s="82"/>
-      <c r="C491" s="83"/>
+      <c r="B491" s="69"/>
+      <c r="C491" s="70"/>
       <c r="D491" s="6"/>
       <c r="E491" s="29"/>
       <c r="F491" s="24"/>
@@ -22256,8 +22256,8 @@
     </row>
     <row r="555" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555" s="29"/>
-      <c r="B555" s="82"/>
-      <c r="C555" s="83"/>
+      <c r="B555" s="69"/>
+      <c r="C555" s="70"/>
       <c r="D555" s="6"/>
       <c r="E555" s="29"/>
       <c r="F555" s="24"/>
@@ -22270,10 +22270,10 @@
     </row>
     <row r="556" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A556" s="29"/>
-      <c r="B556" s="80" t="s">
+      <c r="B556" s="71" t="s">
         <v>1858</v>
       </c>
-      <c r="C556" s="81"/>
+      <c r="C556" s="72"/>
       <c r="D556" s="6"/>
       <c r="E556" s="29"/>
       <c r="F556" s="24"/>
@@ -22286,8 +22286,8 @@
     </row>
     <row r="557" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A557" s="29"/>
-      <c r="B557" s="82"/>
-      <c r="C557" s="83"/>
+      <c r="B557" s="69"/>
+      <c r="C557" s="70"/>
       <c r="D557" s="6"/>
       <c r="E557" s="29"/>
       <c r="F557" s="24"/>
@@ -26086,8 +26086,8 @@
     </row>
     <row r="712" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712" s="29"/>
-      <c r="B712" s="82"/>
-      <c r="C712" s="83"/>
+      <c r="B712" s="69"/>
+      <c r="C712" s="70"/>
       <c r="D712" s="6"/>
       <c r="E712" s="29"/>
       <c r="F712" s="24"/>
@@ -26100,10 +26100,10 @@
     </row>
     <row r="713" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A713" s="29"/>
-      <c r="B713" s="80" t="s">
+      <c r="B713" s="71" t="s">
         <v>1852</v>
       </c>
-      <c r="C713" s="81"/>
+      <c r="C713" s="72"/>
       <c r="D713" s="6"/>
       <c r="E713" s="29"/>
       <c r="F713" s="24"/>
@@ -26116,8 +26116,8 @@
     </row>
     <row r="714" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A714" s="29"/>
-      <c r="B714" s="82"/>
-      <c r="C714" s="83"/>
+      <c r="B714" s="69"/>
+      <c r="C714" s="70"/>
       <c r="D714" s="6"/>
       <c r="E714" s="29"/>
       <c r="F714" s="24"/>
@@ -28574,8 +28574,8 @@
     </row>
     <row r="817" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817" s="29"/>
-      <c r="B817" s="82"/>
-      <c r="C817" s="83"/>
+      <c r="B817" s="69"/>
+      <c r="C817" s="70"/>
       <c r="D817" s="6"/>
       <c r="E817" s="29"/>
       <c r="F817" s="24"/>
@@ -28588,10 +28588,10 @@
     </row>
     <row r="818" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A818" s="29"/>
-      <c r="B818" s="80" t="s">
+      <c r="B818" s="71" t="s">
         <v>1853</v>
       </c>
-      <c r="C818" s="81"/>
+      <c r="C818" s="72"/>
       <c r="D818" s="6"/>
       <c r="E818" s="29"/>
       <c r="F818" s="24"/>
@@ -28604,8 +28604,8 @@
     </row>
     <row r="819" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A819" s="29"/>
-      <c r="B819" s="82"/>
-      <c r="C819" s="83"/>
+      <c r="B819" s="69"/>
+      <c r="C819" s="70"/>
       <c r="D819" s="6"/>
       <c r="E819" s="29"/>
       <c r="F819" s="24"/>
@@ -31519,8 +31519,8 @@
     </row>
     <row r="933" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933" s="29"/>
-      <c r="B933" s="82"/>
-      <c r="C933" s="83"/>
+      <c r="B933" s="69"/>
+      <c r="C933" s="70"/>
       <c r="D933" s="6"/>
       <c r="E933" s="29"/>
       <c r="F933" s="24"/>
@@ -31533,10 +31533,10 @@
     </row>
     <row r="934" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A934" s="29"/>
-      <c r="B934" s="80" t="s">
+      <c r="B934" s="71" t="s">
         <v>1951</v>
       </c>
-      <c r="C934" s="81"/>
+      <c r="C934" s="72"/>
       <c r="D934" s="6"/>
       <c r="E934" s="29"/>
       <c r="F934" s="24"/>
@@ -31549,8 +31549,8 @@
     </row>
     <row r="935" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A935" s="29"/>
-      <c r="B935" s="82"/>
-      <c r="C935" s="83"/>
+      <c r="B935" s="69"/>
+      <c r="C935" s="70"/>
       <c r="D935" s="6"/>
       <c r="E935" s="29"/>
       <c r="F935" s="24"/>
@@ -31684,8 +31684,8 @@
     </row>
     <row r="941" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941" s="29"/>
-      <c r="B941" s="82"/>
-      <c r="C941" s="83"/>
+      <c r="B941" s="69"/>
+      <c r="C941" s="70"/>
       <c r="D941" s="6"/>
       <c r="E941" s="29"/>
       <c r="F941" s="24"/>
@@ -31698,10 +31698,10 @@
     </row>
     <row r="942" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A942" s="29"/>
-      <c r="B942" s="80" t="s">
+      <c r="B942" s="71" t="s">
         <v>1854</v>
       </c>
-      <c r="C942" s="81"/>
+      <c r="C942" s="72"/>
       <c r="D942" s="6"/>
       <c r="E942" s="29"/>
       <c r="F942" s="24"/>
@@ -31714,8 +31714,8 @@
     </row>
     <row r="943" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A943" s="29"/>
-      <c r="B943" s="82"/>
-      <c r="C943" s="83"/>
+      <c r="B943" s="69"/>
+      <c r="C943" s="70"/>
       <c r="D943" s="6"/>
       <c r="E943" s="29"/>
       <c r="F943" s="24"/>
@@ -32238,8 +32238,8 @@
     </row>
     <row r="967" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967" s="29"/>
-      <c r="B967" s="82"/>
-      <c r="C967" s="83"/>
+      <c r="B967" s="69"/>
+      <c r="C967" s="70"/>
       <c r="D967" s="6"/>
       <c r="E967" s="29"/>
       <c r="F967" s="24"/>
@@ -32252,10 +32252,10 @@
     </row>
     <row r="968" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A968" s="29"/>
-      <c r="B968" s="80" t="s">
+      <c r="B968" s="71" t="s">
         <v>1855</v>
       </c>
-      <c r="C968" s="81"/>
+      <c r="C968" s="72"/>
       <c r="D968" s="6"/>
       <c r="E968" s="29"/>
       <c r="F968" s="24"/>
@@ -32268,8 +32268,8 @@
     </row>
     <row r="969" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A969" s="29"/>
-      <c r="B969" s="82"/>
-      <c r="C969" s="83"/>
+      <c r="B969" s="69"/>
+      <c r="C969" s="70"/>
       <c r="D969" s="6"/>
       <c r="E969" s="29"/>
       <c r="F969" s="24"/>
@@ -35178,8 +35178,8 @@
     </row>
     <row r="1082" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1082" s="29"/>
-      <c r="B1082" s="82"/>
-      <c r="C1082" s="83"/>
+      <c r="B1082" s="69"/>
+      <c r="C1082" s="70"/>
       <c r="D1082" s="6"/>
       <c r="E1082" s="29"/>
       <c r="F1082" s="24"/>
@@ -35192,10 +35192,10 @@
     </row>
     <row r="1083" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1083" s="29"/>
-      <c r="B1083" s="80" t="s">
+      <c r="B1083" s="71" t="s">
         <v>1856</v>
       </c>
-      <c r="C1083" s="81"/>
+      <c r="C1083" s="72"/>
       <c r="D1083" s="6"/>
       <c r="E1083" s="29"/>
       <c r="F1083" s="24"/>
@@ -35208,8 +35208,8 @@
     </row>
     <row r="1084" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1084" s="29"/>
-      <c r="B1084" s="82"/>
-      <c r="C1084" s="83"/>
+      <c r="B1084" s="69"/>
+      <c r="C1084" s="70"/>
       <c r="D1084" s="6"/>
       <c r="E1084" s="29"/>
       <c r="F1084" s="24"/>
@@ -35264,8 +35264,8 @@
     </row>
     <row r="1087" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1087" s="29"/>
-      <c r="B1087" s="82"/>
-      <c r="C1087" s="83"/>
+      <c r="B1087" s="69"/>
+      <c r="C1087" s="70"/>
       <c r="D1087" s="6"/>
       <c r="E1087" s="29"/>
       <c r="F1087" s="24"/>
@@ -35278,10 +35278,10 @@
     </row>
     <row r="1088" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1088" s="29"/>
-      <c r="B1088" s="80" t="s">
+      <c r="B1088" s="71" t="s">
         <v>1857</v>
       </c>
-      <c r="C1088" s="81"/>
+      <c r="C1088" s="72"/>
       <c r="D1088" s="6"/>
       <c r="E1088" s="29"/>
       <c r="F1088" s="24"/>
@@ -35294,8 +35294,8 @@
     </row>
     <row r="1089" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1089" s="29"/>
-      <c r="B1089" s="82"/>
-      <c r="C1089" s="83"/>
+      <c r="B1089" s="69"/>
+      <c r="C1089" s="70"/>
       <c r="D1089" s="6"/>
       <c r="E1089" s="29"/>
       <c r="F1089" s="24"/>
@@ -37784,8 +37784,8 @@
     </row>
     <row r="1196" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1196" s="29"/>
-      <c r="B1196" s="82"/>
-      <c r="C1196" s="83"/>
+      <c r="B1196" s="69"/>
+      <c r="C1196" s="70"/>
       <c r="D1196" s="6"/>
       <c r="E1196" s="29"/>
       <c r="F1196" s="24"/>
@@ -37798,10 +37798,10 @@
     </row>
     <row r="1197" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1197" s="29"/>
-      <c r="B1197" s="80" t="s">
+      <c r="B1197" s="71" t="s">
         <v>2033</v>
       </c>
-      <c r="C1197" s="81"/>
+      <c r="C1197" s="72"/>
       <c r="D1197" s="6"/>
       <c r="E1197" s="29"/>
       <c r="F1197" s="24"/>
@@ -37814,8 +37814,8 @@
     </row>
     <row r="1198" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1198" s="29"/>
-      <c r="B1198" s="82"/>
-      <c r="C1198" s="83"/>
+      <c r="B1198" s="69"/>
+      <c r="C1198" s="70"/>
       <c r="D1198" s="6"/>
       <c r="E1198" s="29"/>
       <c r="F1198" s="24"/>
@@ -38310,6 +38310,70 @@
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B213:C213"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B491:C491"/>
+    <mergeCell ref="B555:C555"/>
+    <mergeCell ref="B557:C557"/>
+    <mergeCell ref="B712:C712"/>
+    <mergeCell ref="B714:C714"/>
+    <mergeCell ref="B943:C943"/>
+    <mergeCell ref="B969:C969"/>
+    <mergeCell ref="B967:C967"/>
+    <mergeCell ref="B1087:C1087"/>
+    <mergeCell ref="B1089:C1089"/>
+    <mergeCell ref="B1082:C1082"/>
+    <mergeCell ref="B1084:C1084"/>
+    <mergeCell ref="B968:C968"/>
+    <mergeCell ref="B1196:C1196"/>
+    <mergeCell ref="B1198:C1198"/>
+    <mergeCell ref="B1197:C1197"/>
+    <mergeCell ref="B1088:C1088"/>
+    <mergeCell ref="B1083:C1083"/>
+    <mergeCell ref="B942:C942"/>
+    <mergeCell ref="B934:C934"/>
+    <mergeCell ref="B818:C818"/>
+    <mergeCell ref="B713:C713"/>
+    <mergeCell ref="B556:C556"/>
+    <mergeCell ref="B819:C819"/>
+    <mergeCell ref="B817:C817"/>
+    <mergeCell ref="B933:C933"/>
+    <mergeCell ref="B935:C935"/>
+    <mergeCell ref="B941:C941"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B23:C23"/>
@@ -38326,70 +38390,6 @@
     <mergeCell ref="B489:C489"/>
     <mergeCell ref="B185:C185"/>
     <mergeCell ref="B187:C187"/>
-    <mergeCell ref="B942:C942"/>
-    <mergeCell ref="B934:C934"/>
-    <mergeCell ref="B818:C818"/>
-    <mergeCell ref="B713:C713"/>
-    <mergeCell ref="B556:C556"/>
-    <mergeCell ref="B819:C819"/>
-    <mergeCell ref="B817:C817"/>
-    <mergeCell ref="B933:C933"/>
-    <mergeCell ref="B935:C935"/>
-    <mergeCell ref="B941:C941"/>
-    <mergeCell ref="B1196:C1196"/>
-    <mergeCell ref="B1198:C1198"/>
-    <mergeCell ref="B1197:C1197"/>
-    <mergeCell ref="B1088:C1088"/>
-    <mergeCell ref="B1083:C1083"/>
-    <mergeCell ref="B943:C943"/>
-    <mergeCell ref="B969:C969"/>
-    <mergeCell ref="B967:C967"/>
-    <mergeCell ref="B1087:C1087"/>
-    <mergeCell ref="B1089:C1089"/>
-    <mergeCell ref="B1082:C1082"/>
-    <mergeCell ref="B1084:C1084"/>
-    <mergeCell ref="B968:C968"/>
-    <mergeCell ref="B491:C491"/>
-    <mergeCell ref="B555:C555"/>
-    <mergeCell ref="B557:C557"/>
-    <mergeCell ref="B712:C712"/>
-    <mergeCell ref="B714:C714"/>
-    <mergeCell ref="B213:C213"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -38419,80 +38419,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38501,62 +38501,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38565,13 +38565,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38580,13 +38580,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38595,13 +38595,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38610,24 +38610,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38636,12 +38636,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38650,13 +38650,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38665,13 +38665,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38680,13 +38680,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38695,53 +38695,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -38750,12 +38750,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -38764,28 +38764,24 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -38801,12 +38797,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 24 Mei 2023 12:12 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -9048,6 +9048,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9059,12 +9065,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9099,13 +9099,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9420,10 +9420,10 @@
   <dimension ref="A1:M1232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D156" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D802" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D163" sqref="D163"/>
+      <selection pane="bottomRight" activeCell="D815" sqref="D815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9463,7 +9463,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="81"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
@@ -9483,7 +9483,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="82"/>
       <c r="C3" s="83"/>
-      <c r="D3" s="72"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>334</v>
@@ -9519,10 +9519,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="69" t="s">
         <v>1851</v>
       </c>
-      <c r="C5" s="74"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9535,8 +9535,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -9653,8 +9653,8 @@
     </row>
     <row r="11" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="6"/>
       <c r="E11" s="29"/>
       <c r="F11" s="24"/>
@@ -9667,10 +9667,10 @@
     </row>
     <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="69" t="s">
         <v>1850</v>
       </c>
-      <c r="C12" s="74"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="6"/>
       <c r="E12" s="29"/>
       <c r="F12" s="24"/>
@@ -9683,8 +9683,8 @@
     </row>
     <row r="13" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="70"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="6"/>
       <c r="E13" s="29"/>
       <c r="F13" s="24"/>
@@ -9765,8 +9765,8 @@
     </row>
     <row r="17" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="70"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -9779,10 +9779,10 @@
     </row>
     <row r="18" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="69" t="s">
         <v>1849</v>
       </c>
-      <c r="C18" s="74"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -9795,8 +9795,8 @@
     </row>
     <row r="19" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="6"/>
       <c r="E19" s="29"/>
       <c r="F19" s="24"/>
@@ -9871,8 +9871,8 @@
     </row>
     <row r="23" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="72"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -9901,8 +9901,8 @@
     </row>
     <row r="25" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="72"/>
       <c r="D25" s="6"/>
       <c r="E25" s="29"/>
       <c r="F25" s="24"/>
@@ -11479,8 +11479,8 @@
     </row>
     <row r="95" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="29"/>
-      <c r="B95" s="69"/>
-      <c r="C95" s="70"/>
+      <c r="B95" s="71"/>
+      <c r="C95" s="72"/>
       <c r="D95" s="6"/>
       <c r="E95" s="29"/>
       <c r="F95" s="24"/>
@@ -11493,10 +11493,10 @@
     </row>
     <row r="96" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29"/>
-      <c r="B96" s="73" t="s">
+      <c r="B96" s="69" t="s">
         <v>1870</v>
       </c>
-      <c r="C96" s="74"/>
+      <c r="C96" s="70"/>
       <c r="D96" s="6"/>
       <c r="E96" s="29"/>
       <c r="F96" s="24"/>
@@ -11509,8 +11509,8 @@
     </row>
     <row r="97" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="29"/>
-      <c r="B97" s="69"/>
-      <c r="C97" s="70"/>
+      <c r="B97" s="71"/>
+      <c r="C97" s="72"/>
       <c r="D97" s="6"/>
       <c r="E97" s="29"/>
       <c r="F97" s="24"/>
@@ -11669,8 +11669,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="71"/>
+      <c r="C104" s="72"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -11683,10 +11683,10 @@
     </row>
     <row r="105" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A105" s="29"/>
-      <c r="B105" s="73" t="s">
+      <c r="B105" s="69" t="s">
         <v>1869</v>
       </c>
-      <c r="C105" s="74"/>
+      <c r="C105" s="70"/>
       <c r="D105" s="6"/>
       <c r="E105" s="29"/>
       <c r="F105" s="24"/>
@@ -11699,8 +11699,8 @@
     </row>
     <row r="106" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="29"/>
-      <c r="B106" s="69"/>
-      <c r="C106" s="70"/>
+      <c r="B106" s="71"/>
+      <c r="C106" s="72"/>
       <c r="D106" s="6"/>
       <c r="E106" s="29"/>
       <c r="F106" s="24"/>
@@ -12205,8 +12205,8 @@
     </row>
     <row r="130" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="29"/>
-      <c r="B130" s="69"/>
-      <c r="C130" s="70"/>
+      <c r="B130" s="71"/>
+      <c r="C130" s="72"/>
       <c r="D130" s="6"/>
       <c r="E130" s="29"/>
       <c r="F130" s="24"/>
@@ -12219,10 +12219,10 @@
     </row>
     <row r="131" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A131" s="29"/>
-      <c r="B131" s="73" t="s">
+      <c r="B131" s="69" t="s">
         <v>2088</v>
       </c>
-      <c r="C131" s="74"/>
+      <c r="C131" s="70"/>
       <c r="D131" s="6"/>
       <c r="E131" s="29"/>
       <c r="F131" s="24"/>
@@ -12235,8 +12235,8 @@
     </row>
     <row r="132" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="29"/>
-      <c r="B132" s="69"/>
-      <c r="C132" s="70"/>
+      <c r="B132" s="71"/>
+      <c r="C132" s="72"/>
       <c r="D132" s="6"/>
       <c r="E132" s="29"/>
       <c r="F132" s="24"/>
@@ -12287,8 +12287,8 @@
     </row>
     <row r="135" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="29"/>
-      <c r="B135" s="69"/>
-      <c r="C135" s="70"/>
+      <c r="B135" s="71"/>
+      <c r="C135" s="72"/>
       <c r="D135" s="6"/>
       <c r="E135" s="29"/>
       <c r="F135" s="24"/>
@@ -12301,10 +12301,10 @@
     </row>
     <row r="136" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A136" s="29"/>
-      <c r="B136" s="73" t="s">
+      <c r="B136" s="69" t="s">
         <v>1867</v>
       </c>
-      <c r="C136" s="74"/>
+      <c r="C136" s="70"/>
       <c r="D136" s="6"/>
       <c r="E136" s="29"/>
       <c r="F136" s="24"/>
@@ -12317,8 +12317,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="72"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12429,8 +12429,8 @@
     </row>
     <row r="142" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="29"/>
-      <c r="B142" s="69"/>
-      <c r="C142" s="70"/>
+      <c r="B142" s="71"/>
+      <c r="C142" s="72"/>
       <c r="D142" s="6"/>
       <c r="E142" s="29"/>
       <c r="F142" s="24"/>
@@ -12443,10 +12443,10 @@
     </row>
     <row r="143" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
-      <c r="B143" s="73" t="s">
+      <c r="B143" s="69" t="s">
         <v>1868</v>
       </c>
-      <c r="C143" s="74"/>
+      <c r="C143" s="70"/>
       <c r="D143" s="6"/>
       <c r="E143" s="29"/>
       <c r="F143" s="24"/>
@@ -12459,8 +12459,8 @@
     </row>
     <row r="144" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
-      <c r="B144" s="69"/>
-      <c r="C144" s="70"/>
+      <c r="B144" s="71"/>
+      <c r="C144" s="72"/>
       <c r="D144" s="6"/>
       <c r="E144" s="29"/>
       <c r="F144" s="24"/>
@@ -12669,8 +12669,8 @@
     </row>
     <row r="154" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="29"/>
-      <c r="B154" s="69"/>
-      <c r="C154" s="70"/>
+      <c r="B154" s="71"/>
+      <c r="C154" s="72"/>
       <c r="D154" s="6"/>
       <c r="E154" s="29"/>
       <c r="F154" s="24"/>
@@ -12683,10 +12683,10 @@
     </row>
     <row r="155" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A155" s="29"/>
-      <c r="B155" s="73" t="s">
+      <c r="B155" s="69" t="s">
         <v>1866</v>
       </c>
-      <c r="C155" s="74"/>
+      <c r="C155" s="70"/>
       <c r="D155" s="6"/>
       <c r="E155" s="29"/>
       <c r="F155" s="24"/>
@@ -12699,8 +12699,8 @@
     </row>
     <row r="156" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="29"/>
-      <c r="B156" s="69"/>
-      <c r="C156" s="70"/>
+      <c r="B156" s="71"/>
+      <c r="C156" s="72"/>
       <c r="D156" s="6"/>
       <c r="E156" s="29"/>
       <c r="F156" s="24"/>
@@ -12971,8 +12971,8 @@
     </row>
     <row r="169" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="29"/>
-      <c r="B169" s="69"/>
-      <c r="C169" s="70"/>
+      <c r="B169" s="71"/>
+      <c r="C169" s="72"/>
       <c r="D169" s="6"/>
       <c r="E169" s="29"/>
       <c r="F169" s="24"/>
@@ -13085,8 +13085,8 @@
     </row>
     <row r="175" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="29"/>
-      <c r="B175" s="69"/>
-      <c r="C175" s="70"/>
+      <c r="B175" s="71"/>
+      <c r="C175" s="72"/>
       <c r="D175" s="6"/>
       <c r="E175" s="29"/>
       <c r="F175" s="24"/>
@@ -13099,10 +13099,10 @@
     </row>
     <row r="176" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A176" s="29"/>
-      <c r="B176" s="73" t="s">
+      <c r="B176" s="69" t="s">
         <v>1865</v>
       </c>
-      <c r="C176" s="74"/>
+      <c r="C176" s="70"/>
       <c r="D176" s="6"/>
       <c r="E176" s="29"/>
       <c r="F176" s="24"/>
@@ -13115,8 +13115,8 @@
     </row>
     <row r="177" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="29"/>
-      <c r="B177" s="69"/>
-      <c r="C177" s="70"/>
+      <c r="B177" s="71"/>
+      <c r="C177" s="72"/>
       <c r="D177" s="6"/>
       <c r="E177" s="29"/>
       <c r="F177" s="24"/>
@@ -13373,8 +13373,8 @@
     </row>
     <row r="189" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="29"/>
-      <c r="B189" s="69"/>
-      <c r="C189" s="70"/>
+      <c r="B189" s="71"/>
+      <c r="C189" s="72"/>
       <c r="D189" s="6"/>
       <c r="E189" s="29"/>
       <c r="F189" s="24"/>
@@ -13387,10 +13387,10 @@
     </row>
     <row r="190" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A190" s="29"/>
-      <c r="B190" s="73" t="s">
+      <c r="B190" s="69" t="s">
         <v>1863</v>
       </c>
-      <c r="C190" s="74"/>
+      <c r="C190" s="70"/>
       <c r="D190" s="6"/>
       <c r="E190" s="29"/>
       <c r="F190" s="24"/>
@@ -13403,8 +13403,8 @@
     </row>
     <row r="191" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="29"/>
-      <c r="B191" s="69"/>
-      <c r="C191" s="70"/>
+      <c r="B191" s="71"/>
+      <c r="C191" s="72"/>
       <c r="D191" s="6"/>
       <c r="E191" s="29"/>
       <c r="F191" s="24"/>
@@ -13469,8 +13469,8 @@
     </row>
     <row r="195" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="29"/>
-      <c r="B195" s="69"/>
-      <c r="C195" s="70"/>
+      <c r="B195" s="71"/>
+      <c r="C195" s="72"/>
       <c r="D195" s="6"/>
       <c r="E195" s="29"/>
       <c r="F195" s="24"/>
@@ -13483,10 +13483,10 @@
     </row>
     <row r="196" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A196" s="29"/>
-      <c r="B196" s="73" t="s">
+      <c r="B196" s="69" t="s">
         <v>1864</v>
       </c>
-      <c r="C196" s="74"/>
+      <c r="C196" s="70"/>
       <c r="D196" s="6"/>
       <c r="E196" s="29"/>
       <c r="F196" s="24"/>
@@ -13499,8 +13499,8 @@
     </row>
     <row r="197" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="29"/>
-      <c r="B197" s="69"/>
-      <c r="C197" s="70"/>
+      <c r="B197" s="71"/>
+      <c r="C197" s="72"/>
       <c r="D197" s="6"/>
       <c r="E197" s="29"/>
       <c r="F197" s="24"/>
@@ -14085,8 +14085,8 @@
     </row>
     <row r="223" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="29"/>
-      <c r="B223" s="69"/>
-      <c r="C223" s="70"/>
+      <c r="B223" s="71"/>
+      <c r="C223" s="72"/>
       <c r="D223" s="6"/>
       <c r="E223" s="29"/>
       <c r="F223" s="24"/>
@@ -14099,10 +14099,10 @@
     </row>
     <row r="224" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="73" t="s">
+      <c r="B224" s="69" t="s">
         <v>1862</v>
       </c>
-      <c r="C224" s="74"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -14115,8 +14115,8 @@
     </row>
     <row r="225" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="29"/>
-      <c r="B225" s="69"/>
-      <c r="C225" s="70"/>
+      <c r="B225" s="71"/>
+      <c r="C225" s="72"/>
       <c r="D225" s="6"/>
       <c r="E225" s="29"/>
       <c r="F225" s="24"/>
@@ -14311,8 +14311,8 @@
     </row>
     <row r="234" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="29"/>
-      <c r="B234" s="69"/>
-      <c r="C234" s="70"/>
+      <c r="B234" s="71"/>
+      <c r="C234" s="72"/>
       <c r="D234" s="6"/>
       <c r="E234" s="29"/>
       <c r="F234" s="24"/>
@@ -14325,10 +14325,10 @@
     </row>
     <row r="235" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A235" s="29"/>
-      <c r="B235" s="73" t="s">
+      <c r="B235" s="69" t="s">
         <v>1861</v>
       </c>
-      <c r="C235" s="74"/>
+      <c r="C235" s="70"/>
       <c r="D235" s="6"/>
       <c r="E235" s="29"/>
       <c r="F235" s="24"/>
@@ -14341,8 +14341,8 @@
     </row>
     <row r="236" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="29"/>
-      <c r="B236" s="69"/>
-      <c r="C236" s="70"/>
+      <c r="B236" s="71"/>
+      <c r="C236" s="72"/>
       <c r="D236" s="6"/>
       <c r="E236" s="29"/>
       <c r="F236" s="24"/>
@@ -17177,8 +17177,8 @@
     </row>
     <row r="355" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="29"/>
-      <c r="B355" s="69"/>
-      <c r="C355" s="70"/>
+      <c r="B355" s="71"/>
+      <c r="C355" s="72"/>
       <c r="D355" s="6"/>
       <c r="E355" s="29"/>
       <c r="F355" s="24"/>
@@ -17191,10 +17191,10 @@
     </row>
     <row r="356" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A356" s="29"/>
-      <c r="B356" s="73" t="s">
+      <c r="B356" s="69" t="s">
         <v>1860</v>
       </c>
-      <c r="C356" s="74"/>
+      <c r="C356" s="70"/>
       <c r="D356" s="6"/>
       <c r="E356" s="29"/>
       <c r="F356" s="24"/>
@@ -17207,8 +17207,8 @@
     </row>
     <row r="357" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="29"/>
-      <c r="B357" s="69"/>
-      <c r="C357" s="70"/>
+      <c r="B357" s="71"/>
+      <c r="C357" s="72"/>
       <c r="D357" s="6"/>
       <c r="E357" s="29"/>
       <c r="F357" s="24"/>
@@ -20833,8 +20833,8 @@
     </row>
     <row r="496" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A496" s="29"/>
-      <c r="B496" s="69"/>
-      <c r="C496" s="70"/>
+      <c r="B496" s="71"/>
+      <c r="C496" s="72"/>
       <c r="D496" s="6"/>
       <c r="E496" s="29"/>
       <c r="F496" s="24"/>
@@ -20889,8 +20889,8 @@
     </row>
     <row r="499" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A499" s="29"/>
-      <c r="B499" s="69"/>
-      <c r="C499" s="70"/>
+      <c r="B499" s="71"/>
+      <c r="C499" s="72"/>
       <c r="D499" s="6"/>
       <c r="E499" s="29"/>
       <c r="F499" s="24"/>
@@ -20903,10 +20903,10 @@
     </row>
     <row r="500" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A500" s="29"/>
-      <c r="B500" s="73" t="s">
+      <c r="B500" s="69" t="s">
         <v>1859</v>
       </c>
-      <c r="C500" s="74"/>
+      <c r="C500" s="70"/>
       <c r="D500" s="6"/>
       <c r="E500" s="29"/>
       <c r="F500" s="24"/>
@@ -20919,8 +20919,8 @@
     </row>
     <row r="501" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A501" s="29"/>
-      <c r="B501" s="69"/>
-      <c r="C501" s="70"/>
+      <c r="B501" s="71"/>
+      <c r="C501" s="72"/>
       <c r="D501" s="6"/>
       <c r="E501" s="29"/>
       <c r="F501" s="24"/>
@@ -22519,8 +22519,8 @@
     </row>
     <row r="565" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A565" s="29"/>
-      <c r="B565" s="69"/>
-      <c r="C565" s="70"/>
+      <c r="B565" s="71"/>
+      <c r="C565" s="72"/>
       <c r="D565" s="6"/>
       <c r="E565" s="29"/>
       <c r="F565" s="24"/>
@@ -22533,10 +22533,10 @@
     </row>
     <row r="566" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A566" s="29"/>
-      <c r="B566" s="73" t="s">
+      <c r="B566" s="69" t="s">
         <v>1858</v>
       </c>
-      <c r="C566" s="74"/>
+      <c r="C566" s="70"/>
       <c r="D566" s="6"/>
       <c r="E566" s="29"/>
       <c r="F566" s="24"/>
@@ -22549,8 +22549,8 @@
     </row>
     <row r="567" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A567" s="29"/>
-      <c r="B567" s="69"/>
-      <c r="C567" s="70"/>
+      <c r="B567" s="71"/>
+      <c r="C567" s="72"/>
       <c r="D567" s="6"/>
       <c r="E567" s="29"/>
       <c r="F567" s="24"/>
@@ -26373,8 +26373,8 @@
     </row>
     <row r="723" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A723" s="29"/>
-      <c r="B723" s="69"/>
-      <c r="C723" s="70"/>
+      <c r="B723" s="71"/>
+      <c r="C723" s="72"/>
       <c r="D723" s="6"/>
       <c r="E723" s="29"/>
       <c r="F723" s="24"/>
@@ -26387,10 +26387,10 @@
     </row>
     <row r="724" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A724" s="29"/>
-      <c r="B724" s="73" t="s">
+      <c r="B724" s="69" t="s">
         <v>1852</v>
       </c>
-      <c r="C724" s="74"/>
+      <c r="C724" s="70"/>
       <c r="D724" s="6"/>
       <c r="E724" s="29"/>
       <c r="F724" s="24"/>
@@ -26403,8 +26403,8 @@
     </row>
     <row r="725" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A725" s="29"/>
-      <c r="B725" s="69"/>
-      <c r="C725" s="70"/>
+      <c r="B725" s="71"/>
+      <c r="C725" s="72"/>
       <c r="D725" s="6"/>
       <c r="E725" s="29"/>
       <c r="F725" s="24"/>
@@ -28861,8 +28861,8 @@
     </row>
     <row r="828" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A828" s="29"/>
-      <c r="B828" s="69"/>
-      <c r="C828" s="70"/>
+      <c r="B828" s="71"/>
+      <c r="C828" s="72"/>
       <c r="D828" s="6"/>
       <c r="E828" s="29"/>
       <c r="F828" s="24"/>
@@ -28875,10 +28875,10 @@
     </row>
     <row r="829" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A829" s="29"/>
-      <c r="B829" s="73" t="s">
+      <c r="B829" s="69" t="s">
         <v>1853</v>
       </c>
-      <c r="C829" s="74"/>
+      <c r="C829" s="70"/>
       <c r="D829" s="6"/>
       <c r="E829" s="29"/>
       <c r="F829" s="24"/>
@@ -28891,8 +28891,8 @@
     </row>
     <row r="830" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A830" s="29"/>
-      <c r="B830" s="69"/>
-      <c r="C830" s="70"/>
+      <c r="B830" s="71"/>
+      <c r="C830" s="72"/>
       <c r="D830" s="6"/>
       <c r="E830" s="29"/>
       <c r="F830" s="24"/>
@@ -31806,8 +31806,8 @@
     </row>
     <row r="944" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A944" s="29"/>
-      <c r="B944" s="69"/>
-      <c r="C944" s="70"/>
+      <c r="B944" s="71"/>
+      <c r="C944" s="72"/>
       <c r="D944" s="6"/>
       <c r="E944" s="29"/>
       <c r="F944" s="24"/>
@@ -31820,10 +31820,10 @@
     </row>
     <row r="945" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A945" s="29"/>
-      <c r="B945" s="73" t="s">
+      <c r="B945" s="69" t="s">
         <v>1951</v>
       </c>
-      <c r="C945" s="74"/>
+      <c r="C945" s="70"/>
       <c r="D945" s="6"/>
       <c r="E945" s="29"/>
       <c r="F945" s="24"/>
@@ -31836,8 +31836,8 @@
     </row>
     <row r="946" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A946" s="29"/>
-      <c r="B946" s="69"/>
-      <c r="C946" s="70"/>
+      <c r="B946" s="71"/>
+      <c r="C946" s="72"/>
       <c r="D946" s="6"/>
       <c r="E946" s="29"/>
       <c r="F946" s="24"/>
@@ -31971,8 +31971,8 @@
     </row>
     <row r="952" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A952" s="29"/>
-      <c r="B952" s="69"/>
-      <c r="C952" s="70"/>
+      <c r="B952" s="71"/>
+      <c r="C952" s="72"/>
       <c r="D952" s="6"/>
       <c r="E952" s="29"/>
       <c r="F952" s="24"/>
@@ -31985,10 +31985,10 @@
     </row>
     <row r="953" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A953" s="29"/>
-      <c r="B953" s="73" t="s">
+      <c r="B953" s="69" t="s">
         <v>1854</v>
       </c>
-      <c r="C953" s="74"/>
+      <c r="C953" s="70"/>
       <c r="D953" s="6"/>
       <c r="E953" s="29"/>
       <c r="F953" s="24"/>
@@ -32001,8 +32001,8 @@
     </row>
     <row r="954" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A954" s="29"/>
-      <c r="B954" s="69"/>
-      <c r="C954" s="70"/>
+      <c r="B954" s="71"/>
+      <c r="C954" s="72"/>
       <c r="D954" s="6"/>
       <c r="E954" s="29"/>
       <c r="F954" s="24"/>
@@ -32525,8 +32525,8 @@
     </row>
     <row r="978" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A978" s="29"/>
-      <c r="B978" s="69"/>
-      <c r="C978" s="70"/>
+      <c r="B978" s="71"/>
+      <c r="C978" s="72"/>
       <c r="D978" s="6"/>
       <c r="E978" s="29"/>
       <c r="F978" s="24"/>
@@ -32539,10 +32539,10 @@
     </row>
     <row r="979" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A979" s="29"/>
-      <c r="B979" s="73" t="s">
+      <c r="B979" s="69" t="s">
         <v>1855</v>
       </c>
-      <c r="C979" s="74"/>
+      <c r="C979" s="70"/>
       <c r="D979" s="6"/>
       <c r="E979" s="29"/>
       <c r="F979" s="24"/>
@@ -32555,8 +32555,8 @@
     </row>
     <row r="980" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A980" s="29"/>
-      <c r="B980" s="69"/>
-      <c r="C980" s="70"/>
+      <c r="B980" s="71"/>
+      <c r="C980" s="72"/>
       <c r="D980" s="6"/>
       <c r="E980" s="29"/>
       <c r="F980" s="24"/>
@@ -35465,8 +35465,8 @@
     </row>
     <row r="1093" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1093" s="29"/>
-      <c r="B1093" s="69"/>
-      <c r="C1093" s="70"/>
+      <c r="B1093" s="71"/>
+      <c r="C1093" s="72"/>
       <c r="D1093" s="6"/>
       <c r="E1093" s="29"/>
       <c r="F1093" s="24"/>
@@ -35479,10 +35479,10 @@
     </row>
     <row r="1094" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1094" s="29"/>
-      <c r="B1094" s="73" t="s">
+      <c r="B1094" s="69" t="s">
         <v>1856</v>
       </c>
-      <c r="C1094" s="74"/>
+      <c r="C1094" s="70"/>
       <c r="D1094" s="6"/>
       <c r="E1094" s="29"/>
       <c r="F1094" s="24"/>
@@ -35495,8 +35495,8 @@
     </row>
     <row r="1095" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1095" s="29"/>
-      <c r="B1095" s="69"/>
-      <c r="C1095" s="70"/>
+      <c r="B1095" s="71"/>
+      <c r="C1095" s="72"/>
       <c r="D1095" s="6"/>
       <c r="E1095" s="29"/>
       <c r="F1095" s="24"/>
@@ -35551,8 +35551,8 @@
     </row>
     <row r="1098" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1098" s="29"/>
-      <c r="B1098" s="69"/>
-      <c r="C1098" s="70"/>
+      <c r="B1098" s="71"/>
+      <c r="C1098" s="72"/>
       <c r="D1098" s="6"/>
       <c r="E1098" s="29"/>
       <c r="F1098" s="24"/>
@@ -35565,10 +35565,10 @@
     </row>
     <row r="1099" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1099" s="29"/>
-      <c r="B1099" s="73" t="s">
+      <c r="B1099" s="69" t="s">
         <v>1857</v>
       </c>
-      <c r="C1099" s="74"/>
+      <c r="C1099" s="70"/>
       <c r="D1099" s="6"/>
       <c r="E1099" s="29"/>
       <c r="F1099" s="24"/>
@@ -35581,8 +35581,8 @@
     </row>
     <row r="1100" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1100" s="29"/>
-      <c r="B1100" s="69"/>
-      <c r="C1100" s="70"/>
+      <c r="B1100" s="71"/>
+      <c r="C1100" s="72"/>
       <c r="D1100" s="6"/>
       <c r="E1100" s="29"/>
       <c r="F1100" s="24"/>
@@ -38071,8 +38071,8 @@
     </row>
     <row r="1207" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1207" s="29"/>
-      <c r="B1207" s="69"/>
-      <c r="C1207" s="70"/>
+      <c r="B1207" s="71"/>
+      <c r="C1207" s="72"/>
       <c r="D1207" s="6"/>
       <c r="E1207" s="29"/>
       <c r="F1207" s="24"/>
@@ -38085,10 +38085,10 @@
     </row>
     <row r="1208" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1208" s="29"/>
-      <c r="B1208" s="73" t="s">
+      <c r="B1208" s="69" t="s">
         <v>2033</v>
       </c>
-      <c r="C1208" s="74"/>
+      <c r="C1208" s="70"/>
       <c r="D1208" s="6"/>
       <c r="E1208" s="29"/>
       <c r="F1208" s="24"/>
@@ -38101,8 +38101,8 @@
     </row>
     <row r="1209" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1209" s="29"/>
-      <c r="B1209" s="69"/>
-      <c r="C1209" s="70"/>
+      <c r="B1209" s="71"/>
+      <c r="C1209" s="72"/>
       <c r="D1209" s="6"/>
       <c r="E1209" s="29"/>
       <c r="F1209" s="24"/>
@@ -38597,6 +38597,75 @@
     </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B195:C195"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B191:C191"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B501:C501"/>
+    <mergeCell ref="B565:C565"/>
+    <mergeCell ref="B567:C567"/>
+    <mergeCell ref="B723:C723"/>
+    <mergeCell ref="B725:C725"/>
+    <mergeCell ref="B954:C954"/>
+    <mergeCell ref="B980:C980"/>
+    <mergeCell ref="B978:C978"/>
+    <mergeCell ref="B1098:C1098"/>
+    <mergeCell ref="B1100:C1100"/>
+    <mergeCell ref="B1093:C1093"/>
+    <mergeCell ref="B1095:C1095"/>
+    <mergeCell ref="B979:C979"/>
+    <mergeCell ref="B1207:C1207"/>
+    <mergeCell ref="B1209:C1209"/>
+    <mergeCell ref="B1208:C1208"/>
+    <mergeCell ref="B1099:C1099"/>
+    <mergeCell ref="B1094:C1094"/>
+    <mergeCell ref="B953:C953"/>
+    <mergeCell ref="B945:C945"/>
+    <mergeCell ref="B829:C829"/>
+    <mergeCell ref="B724:C724"/>
+    <mergeCell ref="B566:C566"/>
+    <mergeCell ref="B830:C830"/>
+    <mergeCell ref="B828:C828"/>
+    <mergeCell ref="B944:C944"/>
+    <mergeCell ref="B946:C946"/>
+    <mergeCell ref="B952:C952"/>
     <mergeCell ref="B500:C500"/>
     <mergeCell ref="B356:C356"/>
     <mergeCell ref="B235:C235"/>
@@ -38609,82 +38678,13 @@
     <mergeCell ref="B499:C499"/>
     <mergeCell ref="B197:C197"/>
     <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B953:C953"/>
-    <mergeCell ref="B945:C945"/>
-    <mergeCell ref="B829:C829"/>
-    <mergeCell ref="B724:C724"/>
-    <mergeCell ref="B566:C566"/>
-    <mergeCell ref="B830:C830"/>
-    <mergeCell ref="B828:C828"/>
-    <mergeCell ref="B944:C944"/>
-    <mergeCell ref="B946:C946"/>
-    <mergeCell ref="B952:C952"/>
-    <mergeCell ref="B1207:C1207"/>
-    <mergeCell ref="B1209:C1209"/>
-    <mergeCell ref="B1208:C1208"/>
-    <mergeCell ref="B1099:C1099"/>
-    <mergeCell ref="B1094:C1094"/>
-    <mergeCell ref="B954:C954"/>
-    <mergeCell ref="B980:C980"/>
-    <mergeCell ref="B978:C978"/>
-    <mergeCell ref="B1098:C1098"/>
-    <mergeCell ref="B1100:C1100"/>
-    <mergeCell ref="B1093:C1093"/>
-    <mergeCell ref="B1095:C1095"/>
-    <mergeCell ref="B979:C979"/>
-    <mergeCell ref="B501:C501"/>
-    <mergeCell ref="B565:C565"/>
-    <mergeCell ref="B567:C567"/>
-    <mergeCell ref="B723:C723"/>
-    <mergeCell ref="B725:C725"/>
     <mergeCell ref="B225:C225"/>
     <mergeCell ref="B234:C234"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B195:C195"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G14:G15 G138:G139 G141 G150:G152 G226:G232 G237:G242 G358:G362 G364:G368 G378:G380 G396 G470:G473 G811:G813 G842:G843 G957:G959 G961 G963:G967 G969:G972 G974:G975 G987:G992 G994:G996 G1005:G1006 G1012 G1067:G1069 G981:G985 G1108:G1110 G324:G327 G1181:G1184 G915:G918 G831:G833 G329:G332 G1186:G1188 G221 G198 G244:G251 G382:G387 G998:G1003 G845:G850 G192 G170:G171 G835:G840 G370:G376 G1101:G1106 G806:G809 G955 G866 G1019 G173 G178:G186 G200:G219 G1167:G1177 G1024:G1065 G871:G913 G497 G1085 F1082:G1084 G29:G37 G475:G488 G1203:G1205 G492:G494 G1089:G1091 G940:G942 G826 G93 G1096 G162:G165 G1072:G1081 G924:G938 G556:G563 G821:G824 G862:G864 G1014:G1017 G920:G922 G799:G802 G167 G868:G869 G1021:G1022 G1134:G1135 G334:G346 G815:G818 G1191:G1197 G550:G554 G765:G768 G774:G775 G770:G772 G718:G723 G734:G747 G1152:G1165 G783:G790 G749:G755 G1137:G1150 G777:G781 G762 G792:G797 G1213:G1224 G1210:G1211 G145:G148 G133 G157:G158 G692:G716 G596:G690 G568:G594 G502:G548 G490 G398:G468 G389:G394 G348:G353 G253:G322 G107:G128 G98:G102 G39:G91 G26:G27 G20:G21 G160:G161" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G14:G15 G138:G139 G141 G150:G152 G226:G232 G237:G242 G358:G362 G364:G368 G378:G380 G396 G470:G473 G811:G813 G842:G843 G957:G959 G961 G963:G967 G969:G972 G974:G975 G987:G992 G994:G996 G1005:G1006 G1012 G1067:G1069 G981:G985 G1108:G1110 G324:G327 G1181:G1184 G915:G918 G831:G833 G329:G332 G1186:G1188 G221 G198 G244:G251 G382:G387 G998:G1003 G845:G850 G192 G170:G171 G835:G840 G370:G376 G1101:G1106 G806:G809 G955 G866 G1019 G173 G178:G186 G200:G219 G1167:G1177 G1024:G1065 G871:G913 G497 G1085 F1082:G1084 G29:G37 G475:G488 G1203:G1205 G492:G494 G1089:G1091 G940:G942 G826 G93 G1096 G162:G165 G1072:G1081 G924:G938 G556:G563 G821:G824 G862:G864 G1014:G1017 G920:G922 G799:G802 G167 G868:G869 G1021:G1022 G1134:G1135 G334:G346 G815:G818 G1191:G1197 G550:G554 G718:G723 G734:G747 G1152:G1165 G782:G790 G749:G755 G1137:G1150 G777:G781 G1213:G1224 G1210:G1211 G145:G148 G133 G157:G158 G692:G716 G596:G690 G568:G594 G502:G548 G490 G398:G468 G389:G394 G348:G353 G253:G322 G107:G128 G98:G102 G39:G91 G26:G27 G20:G21 G160:G161 G762 G770:G772 G774:G775 G765:G768 G756:G761 G769 G776 G773 G763:G764 G792:G797 G791 G798 G803:G804 G819:G820" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -38709,80 +38709,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1275</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1273</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1276</v>
       </c>
@@ -38791,62 +38791,62 @@
       <c r="B9" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1274</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1277</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1265</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1283</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1297</v>
       </c>
@@ -38855,13 +38855,13 @@
       <c r="B14" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1298</v>
       </c>
@@ -38870,13 +38870,13 @@
       <c r="B15" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1284</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1296</v>
       </c>
@@ -38885,13 +38885,13 @@
       <c r="B16" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1286</v>
       </c>
@@ -38900,24 +38900,24 @@
       <c r="B17" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1290</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1295</v>
       </c>
@@ -38926,12 +38926,12 @@
       <c r="C19" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1292</v>
       </c>
@@ -38940,13 +38940,13 @@
       <c r="B20" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1301</v>
       </c>
@@ -38955,13 +38955,13 @@
       <c r="B21" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1288</v>
       </c>
@@ -38970,13 +38970,13 @@
       <c r="B22" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1294</v>
       </c>
@@ -38985,53 +38985,53 @@
       <c r="B23" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1299</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1300</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1266</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1272</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1278</v>
       </c>
@@ -39040,12 +39040,12 @@
       <c r="C27" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1270</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1279</v>
       </c>
@@ -39054,28 +39054,24 @@
       <c r="D28" s="53" t="s">
         <v>1267</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1281</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -39091,12 +39087,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 31 Oktober 2023 11:24 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -9295,6 +9295,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9306,12 +9312,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9346,13 +9346,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9710,7 +9710,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="81"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
@@ -9730,7 +9730,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="82"/>
       <c r="C3" s="83"/>
-      <c r="D3" s="72"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>332</v>
@@ -9766,10 +9766,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="69" t="s">
         <v>1849</v>
       </c>
-      <c r="C5" s="74"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9782,8 +9782,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -10010,8 +10010,8 @@
     </row>
     <row r="16" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="6"/>
       <c r="E16" s="29"/>
       <c r="F16" s="24"/>
@@ -10024,10 +10024,10 @@
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="69" t="s">
         <v>1848</v>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -10040,8 +10040,8 @@
     </row>
     <row r="18" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -10122,8 +10122,8 @@
     </row>
     <row r="22" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="6"/>
       <c r="E22" s="29"/>
       <c r="F22" s="24"/>
@@ -10136,10 +10136,10 @@
     </row>
     <row r="23" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="69" t="s">
         <v>1847</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -10152,8 +10152,8 @@
     </row>
     <row r="24" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="6"/>
       <c r="E24" s="29"/>
       <c r="F24" s="24"/>
@@ -10228,8 +10228,8 @@
     </row>
     <row r="28" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="70"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
       <c r="D28" s="6"/>
       <c r="E28" s="29"/>
       <c r="F28" s="24"/>
@@ -10258,8 +10258,8 @@
     </row>
     <row r="30" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="70"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="6"/>
       <c r="E30" s="29"/>
       <c r="F30" s="24"/>
@@ -11884,8 +11884,8 @@
     </row>
     <row r="102" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
-      <c r="B102" s="69"/>
-      <c r="C102" s="70"/>
+      <c r="B102" s="71"/>
+      <c r="C102" s="72"/>
       <c r="D102" s="6"/>
       <c r="E102" s="29"/>
       <c r="F102" s="24"/>
@@ -11898,10 +11898,10 @@
     </row>
     <row r="103" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29"/>
-      <c r="B103" s="73" t="s">
+      <c r="B103" s="69" t="s">
         <v>1868</v>
       </c>
-      <c r="C103" s="74"/>
+      <c r="C103" s="70"/>
       <c r="D103" s="6"/>
       <c r="E103" s="29"/>
       <c r="F103" s="24"/>
@@ -11914,8 +11914,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="71"/>
+      <c r="C104" s="72"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -12074,8 +12074,8 @@
     </row>
     <row r="111" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="29"/>
-      <c r="B111" s="69"/>
-      <c r="C111" s="70"/>
+      <c r="B111" s="71"/>
+      <c r="C111" s="72"/>
       <c r="D111" s="6"/>
       <c r="E111" s="29"/>
       <c r="F111" s="24"/>
@@ -12088,10 +12088,10 @@
     </row>
     <row r="112" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A112" s="29"/>
-      <c r="B112" s="73" t="s">
+      <c r="B112" s="69" t="s">
         <v>1867</v>
       </c>
-      <c r="C112" s="74"/>
+      <c r="C112" s="70"/>
       <c r="D112" s="6"/>
       <c r="E112" s="29"/>
       <c r="F112" s="24"/>
@@ -12104,8 +12104,8 @@
     </row>
     <row r="113" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="29"/>
-      <c r="B113" s="69"/>
-      <c r="C113" s="70"/>
+      <c r="B113" s="71"/>
+      <c r="C113" s="72"/>
       <c r="D113" s="6"/>
       <c r="E113" s="29"/>
       <c r="F113" s="24"/>
@@ -12610,8 +12610,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="72"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12624,10 +12624,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="73" t="s">
+      <c r="B138" s="69" t="s">
         <v>2085</v>
       </c>
-      <c r="C138" s="74"/>
+      <c r="C138" s="70"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12640,8 +12640,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="69"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="71"/>
+      <c r="C139" s="72"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12716,8 +12716,8 @@
     </row>
     <row r="143" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
-      <c r="B143" s="69"/>
-      <c r="C143" s="70"/>
+      <c r="B143" s="71"/>
+      <c r="C143" s="72"/>
       <c r="D143" s="6"/>
       <c r="E143" s="29"/>
       <c r="F143" s="24"/>
@@ -12730,10 +12730,10 @@
     </row>
     <row r="144" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
-      <c r="B144" s="73" t="s">
+      <c r="B144" s="69" t="s">
         <v>1865</v>
       </c>
-      <c r="C144" s="74"/>
+      <c r="C144" s="70"/>
       <c r="D144" s="6"/>
       <c r="E144" s="29"/>
       <c r="F144" s="24"/>
@@ -12746,8 +12746,8 @@
     </row>
     <row r="145" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
-      <c r="B145" s="69"/>
-      <c r="C145" s="70"/>
+      <c r="B145" s="71"/>
+      <c r="C145" s="72"/>
       <c r="D145" s="6"/>
       <c r="E145" s="29"/>
       <c r="F145" s="24"/>
@@ -12858,8 +12858,8 @@
     </row>
     <row r="150" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
-      <c r="B150" s="69"/>
-      <c r="C150" s="70"/>
+      <c r="B150" s="71"/>
+      <c r="C150" s="72"/>
       <c r="D150" s="6"/>
       <c r="E150" s="29"/>
       <c r="F150" s="24"/>
@@ -12872,10 +12872,10 @@
     </row>
     <row r="151" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
-      <c r="B151" s="73" t="s">
+      <c r="B151" s="69" t="s">
         <v>1866</v>
       </c>
-      <c r="C151" s="74"/>
+      <c r="C151" s="70"/>
       <c r="D151" s="6"/>
       <c r="E151" s="29"/>
       <c r="F151" s="24"/>
@@ -12888,8 +12888,8 @@
     </row>
     <row r="152" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="29"/>
-      <c r="B152" s="69"/>
-      <c r="C152" s="70"/>
+      <c r="B152" s="71"/>
+      <c r="C152" s="72"/>
       <c r="D152" s="6"/>
       <c r="E152" s="29"/>
       <c r="F152" s="24"/>
@@ -13098,8 +13098,8 @@
     </row>
     <row r="162" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
-      <c r="B162" s="69"/>
-      <c r="C162" s="70"/>
+      <c r="B162" s="71"/>
+      <c r="C162" s="72"/>
       <c r="D162" s="6"/>
       <c r="E162" s="29"/>
       <c r="F162" s="24"/>
@@ -13112,10 +13112,10 @@
     </row>
     <row r="163" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="73" t="s">
+      <c r="B163" s="69" t="s">
         <v>1864</v>
       </c>
-      <c r="C163" s="74"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -13128,8 +13128,8 @@
     </row>
     <row r="164" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="69"/>
-      <c r="C164" s="70"/>
+      <c r="B164" s="71"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -13624,8 +13624,8 @@
     </row>
     <row r="188" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="29"/>
-      <c r="B188" s="69"/>
-      <c r="C188" s="70"/>
+      <c r="B188" s="71"/>
+      <c r="C188" s="72"/>
       <c r="D188" s="6"/>
       <c r="E188" s="29"/>
       <c r="F188" s="24"/>
@@ -13638,10 +13638,10 @@
     </row>
     <row r="189" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A189" s="29"/>
-      <c r="B189" s="73" t="s">
+      <c r="B189" s="69" t="s">
         <v>2125</v>
       </c>
-      <c r="C189" s="74"/>
+      <c r="C189" s="70"/>
       <c r="D189" s="6"/>
       <c r="E189" s="29"/>
       <c r="F189" s="24"/>
@@ -13654,8 +13654,8 @@
     </row>
     <row r="190" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="29"/>
-      <c r="B190" s="69"/>
-      <c r="C190" s="70"/>
+      <c r="B190" s="71"/>
+      <c r="C190" s="72"/>
       <c r="D190" s="6"/>
       <c r="E190" s="29"/>
       <c r="F190" s="24"/>
@@ -13844,8 +13844,8 @@
     </row>
     <row r="200" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="29"/>
-      <c r="B200" s="69"/>
-      <c r="C200" s="70"/>
+      <c r="B200" s="71"/>
+      <c r="C200" s="72"/>
       <c r="D200" s="6"/>
       <c r="E200" s="29"/>
       <c r="F200" s="24"/>
@@ -13858,10 +13858,10 @@
     </row>
     <row r="201" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A201" s="29"/>
-      <c r="B201" s="73" t="s">
+      <c r="B201" s="69" t="s">
         <v>1863</v>
       </c>
-      <c r="C201" s="74"/>
+      <c r="C201" s="70"/>
       <c r="D201" s="6"/>
       <c r="E201" s="29"/>
       <c r="F201" s="24"/>
@@ -13874,8 +13874,8 @@
     </row>
     <row r="202" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="29"/>
-      <c r="B202" s="69"/>
-      <c r="C202" s="70"/>
+      <c r="B202" s="71"/>
+      <c r="C202" s="72"/>
       <c r="D202" s="6"/>
       <c r="E202" s="29"/>
       <c r="F202" s="24"/>
@@ -14132,8 +14132,8 @@
     </row>
     <row r="214" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="29"/>
-      <c r="B214" s="69"/>
-      <c r="C214" s="70"/>
+      <c r="B214" s="71"/>
+      <c r="C214" s="72"/>
       <c r="D214" s="6"/>
       <c r="E214" s="29"/>
       <c r="F214" s="24"/>
@@ -14146,10 +14146,10 @@
     </row>
     <row r="215" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A215" s="29"/>
-      <c r="B215" s="73" t="s">
+      <c r="B215" s="69" t="s">
         <v>1861</v>
       </c>
-      <c r="C215" s="74"/>
+      <c r="C215" s="70"/>
       <c r="D215" s="6"/>
       <c r="E215" s="29"/>
       <c r="F215" s="24"/>
@@ -14162,8 +14162,8 @@
     </row>
     <row r="216" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="29"/>
-      <c r="B216" s="69"/>
-      <c r="C216" s="70"/>
+      <c r="B216" s="71"/>
+      <c r="C216" s="72"/>
       <c r="D216" s="6"/>
       <c r="E216" s="29"/>
       <c r="F216" s="24"/>
@@ -14228,8 +14228,8 @@
     </row>
     <row r="220" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="29"/>
-      <c r="B220" s="69"/>
-      <c r="C220" s="70"/>
+      <c r="B220" s="71"/>
+      <c r="C220" s="72"/>
       <c r="D220" s="6"/>
       <c r="E220" s="29"/>
       <c r="F220" s="24"/>
@@ -14242,10 +14242,10 @@
     </row>
     <row r="221" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A221" s="29"/>
-      <c r="B221" s="73" t="s">
+      <c r="B221" s="69" t="s">
         <v>1862</v>
       </c>
-      <c r="C221" s="74"/>
+      <c r="C221" s="70"/>
       <c r="D221" s="6"/>
       <c r="E221" s="29"/>
       <c r="F221" s="24"/>
@@ -14258,8 +14258,8 @@
     </row>
     <row r="222" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="29"/>
-      <c r="B222" s="69"/>
-      <c r="C222" s="70"/>
+      <c r="B222" s="71"/>
+      <c r="C222" s="72"/>
       <c r="D222" s="6"/>
       <c r="E222" s="29"/>
       <c r="F222" s="24"/>
@@ -14844,8 +14844,8 @@
     </row>
     <row r="248" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="29"/>
-      <c r="B248" s="69"/>
-      <c r="C248" s="70"/>
+      <c r="B248" s="71"/>
+      <c r="C248" s="72"/>
       <c r="D248" s="6"/>
       <c r="E248" s="29"/>
       <c r="F248" s="24"/>
@@ -14858,10 +14858,10 @@
     </row>
     <row r="249" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="29"/>
-      <c r="B249" s="73" t="s">
+      <c r="B249" s="69" t="s">
         <v>1860</v>
       </c>
-      <c r="C249" s="74"/>
+      <c r="C249" s="70"/>
       <c r="D249" s="6"/>
       <c r="E249" s="29"/>
       <c r="F249" s="24"/>
@@ -14874,8 +14874,8 @@
     </row>
     <row r="250" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="29"/>
-      <c r="B250" s="69"/>
-      <c r="C250" s="70"/>
+      <c r="B250" s="71"/>
+      <c r="C250" s="72"/>
       <c r="D250" s="6"/>
       <c r="E250" s="29"/>
       <c r="F250" s="24"/>
@@ -15070,8 +15070,8 @@
     </row>
     <row r="259" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="29"/>
-      <c r="B259" s="69"/>
-      <c r="C259" s="70"/>
+      <c r="B259" s="71"/>
+      <c r="C259" s="72"/>
       <c r="D259" s="6"/>
       <c r="E259" s="29"/>
       <c r="F259" s="24"/>
@@ -15084,10 +15084,10 @@
     </row>
     <row r="260" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A260" s="29"/>
-      <c r="B260" s="73" t="s">
+      <c r="B260" s="69" t="s">
         <v>1859</v>
       </c>
-      <c r="C260" s="74"/>
+      <c r="C260" s="70"/>
       <c r="D260" s="6"/>
       <c r="E260" s="29"/>
       <c r="F260" s="24"/>
@@ -15100,8 +15100,8 @@
     </row>
     <row r="261" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="29"/>
-      <c r="B261" s="69"/>
-      <c r="C261" s="70"/>
+      <c r="B261" s="71"/>
+      <c r="C261" s="72"/>
       <c r="D261" s="6"/>
       <c r="E261" s="29"/>
       <c r="F261" s="24"/>
@@ -18070,8 +18070,8 @@
     </row>
     <row r="386" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="29"/>
-      <c r="B386" s="69"/>
-      <c r="C386" s="70"/>
+      <c r="B386" s="71"/>
+      <c r="C386" s="72"/>
       <c r="D386" s="6"/>
       <c r="E386" s="29"/>
       <c r="F386" s="24"/>
@@ -18084,10 +18084,10 @@
     </row>
     <row r="387" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A387" s="29"/>
-      <c r="B387" s="73" t="s">
+      <c r="B387" s="69" t="s">
         <v>1858</v>
       </c>
-      <c r="C387" s="74"/>
+      <c r="C387" s="70"/>
       <c r="D387" s="6"/>
       <c r="E387" s="29"/>
       <c r="F387" s="24"/>
@@ -18100,8 +18100,8 @@
     </row>
     <row r="388" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="29"/>
-      <c r="B388" s="69"/>
-      <c r="C388" s="70"/>
+      <c r="B388" s="71"/>
+      <c r="C388" s="72"/>
       <c r="D388" s="6"/>
       <c r="E388" s="29"/>
       <c r="F388" s="24"/>
@@ -21726,8 +21726,8 @@
     </row>
     <row r="527" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A527" s="29"/>
-      <c r="B527" s="69"/>
-      <c r="C527" s="70"/>
+      <c r="B527" s="71"/>
+      <c r="C527" s="72"/>
       <c r="D527" s="6"/>
       <c r="E527" s="29"/>
       <c r="F527" s="24"/>
@@ -21782,8 +21782,8 @@
     </row>
     <row r="530" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A530" s="29"/>
-      <c r="B530" s="69"/>
-      <c r="C530" s="70"/>
+      <c r="B530" s="71"/>
+      <c r="C530" s="72"/>
       <c r="D530" s="6"/>
       <c r="E530" s="29"/>
       <c r="F530" s="24"/>
@@ -21796,10 +21796,10 @@
     </row>
     <row r="531" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A531" s="29"/>
-      <c r="B531" s="73" t="s">
+      <c r="B531" s="69" t="s">
         <v>1857</v>
       </c>
-      <c r="C531" s="74"/>
+      <c r="C531" s="70"/>
       <c r="D531" s="6"/>
       <c r="E531" s="29"/>
       <c r="F531" s="24"/>
@@ -21812,8 +21812,8 @@
     </row>
     <row r="532" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A532" s="29"/>
-      <c r="B532" s="69"/>
-      <c r="C532" s="70"/>
+      <c r="B532" s="71"/>
+      <c r="C532" s="72"/>
       <c r="D532" s="6"/>
       <c r="E532" s="29"/>
       <c r="F532" s="24"/>
@@ -23436,8 +23436,8 @@
     </row>
     <row r="597" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A597" s="29"/>
-      <c r="B597" s="69"/>
-      <c r="C597" s="70"/>
+      <c r="B597" s="71"/>
+      <c r="C597" s="72"/>
       <c r="D597" s="6"/>
       <c r="E597" s="29"/>
       <c r="F597" s="24"/>
@@ -23450,10 +23450,10 @@
     </row>
     <row r="598" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A598" s="29"/>
-      <c r="B598" s="73" t="s">
+      <c r="B598" s="69" t="s">
         <v>1856</v>
       </c>
-      <c r="C598" s="74"/>
+      <c r="C598" s="70"/>
       <c r="D598" s="6"/>
       <c r="E598" s="29"/>
       <c r="F598" s="24"/>
@@ -23466,8 +23466,8 @@
     </row>
     <row r="599" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A599" s="29"/>
-      <c r="B599" s="69"/>
-      <c r="C599" s="70"/>
+      <c r="B599" s="71"/>
+      <c r="C599" s="72"/>
       <c r="D599" s="6"/>
       <c r="E599" s="29"/>
       <c r="F599" s="24"/>
@@ -27338,8 +27338,8 @@
     </row>
     <row r="757" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A757" s="29"/>
-      <c r="B757" s="69"/>
-      <c r="C757" s="70"/>
+      <c r="B757" s="71"/>
+      <c r="C757" s="72"/>
       <c r="D757" s="6"/>
       <c r="E757" s="29"/>
       <c r="F757" s="24"/>
@@ -27352,10 +27352,10 @@
     </row>
     <row r="758" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A758" s="29"/>
-      <c r="B758" s="73" t="s">
+      <c r="B758" s="69" t="s">
         <v>1850</v>
       </c>
-      <c r="C758" s="74"/>
+      <c r="C758" s="70"/>
       <c r="D758" s="6"/>
       <c r="E758" s="29"/>
       <c r="F758" s="24"/>
@@ -27368,8 +27368,8 @@
     </row>
     <row r="759" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A759" s="29"/>
-      <c r="B759" s="69"/>
-      <c r="C759" s="70"/>
+      <c r="B759" s="71"/>
+      <c r="C759" s="72"/>
       <c r="D759" s="6"/>
       <c r="E759" s="29"/>
       <c r="F759" s="24"/>
@@ -29874,8 +29874,8 @@
     </row>
     <row r="864" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A864" s="29"/>
-      <c r="B864" s="69"/>
-      <c r="C864" s="70"/>
+      <c r="B864" s="71"/>
+      <c r="C864" s="72"/>
       <c r="D864" s="6"/>
       <c r="E864" s="29"/>
       <c r="F864" s="24"/>
@@ -29888,10 +29888,10 @@
     </row>
     <row r="865" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A865" s="29"/>
-      <c r="B865" s="73" t="s">
+      <c r="B865" s="69" t="s">
         <v>1851</v>
       </c>
-      <c r="C865" s="74"/>
+      <c r="C865" s="70"/>
       <c r="D865" s="6"/>
       <c r="E865" s="29"/>
       <c r="F865" s="24"/>
@@ -29904,8 +29904,8 @@
     </row>
     <row r="866" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A866" s="29"/>
-      <c r="B866" s="69"/>
-      <c r="C866" s="70"/>
+      <c r="B866" s="71"/>
+      <c r="C866" s="72"/>
       <c r="D866" s="6"/>
       <c r="E866" s="29"/>
       <c r="F866" s="24"/>
@@ -32819,8 +32819,8 @@
     </row>
     <row r="980" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A980" s="29"/>
-      <c r="B980" s="69"/>
-      <c r="C980" s="70"/>
+      <c r="B980" s="71"/>
+      <c r="C980" s="72"/>
       <c r="D980" s="6"/>
       <c r="E980" s="29"/>
       <c r="F980" s="24"/>
@@ -32833,10 +32833,10 @@
     </row>
     <row r="981" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A981" s="29"/>
-      <c r="B981" s="73" t="s">
+      <c r="B981" s="69" t="s">
         <v>1949</v>
       </c>
-      <c r="C981" s="74"/>
+      <c r="C981" s="70"/>
       <c r="D981" s="6"/>
       <c r="E981" s="29"/>
       <c r="F981" s="24"/>
@@ -32849,8 +32849,8 @@
     </row>
     <row r="982" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A982" s="29"/>
-      <c r="B982" s="69"/>
-      <c r="C982" s="70"/>
+      <c r="B982" s="71"/>
+      <c r="C982" s="72"/>
       <c r="D982" s="6"/>
       <c r="E982" s="29"/>
       <c r="F982" s="24"/>
@@ -32984,8 +32984,8 @@
     </row>
     <row r="988" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A988" s="29"/>
-      <c r="B988" s="69"/>
-      <c r="C988" s="70"/>
+      <c r="B988" s="71"/>
+      <c r="C988" s="72"/>
       <c r="D988" s="6"/>
       <c r="E988" s="29"/>
       <c r="F988" s="24"/>
@@ -32998,10 +32998,10 @@
     </row>
     <row r="989" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A989" s="29"/>
-      <c r="B989" s="73" t="s">
+      <c r="B989" s="69" t="s">
         <v>1852</v>
       </c>
-      <c r="C989" s="74"/>
+      <c r="C989" s="70"/>
       <c r="D989" s="6"/>
       <c r="E989" s="29"/>
       <c r="F989" s="24"/>
@@ -33014,8 +33014,8 @@
     </row>
     <row r="990" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A990" s="29"/>
-      <c r="B990" s="69"/>
-      <c r="C990" s="70"/>
+      <c r="B990" s="71"/>
+      <c r="C990" s="72"/>
       <c r="D990" s="6"/>
       <c r="E990" s="29"/>
       <c r="F990" s="24"/>
@@ -33538,8 +33538,8 @@
     </row>
     <row r="1014" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1014" s="29"/>
-      <c r="B1014" s="69"/>
-      <c r="C1014" s="70"/>
+      <c r="B1014" s="71"/>
+      <c r="C1014" s="72"/>
       <c r="D1014" s="6"/>
       <c r="E1014" s="29"/>
       <c r="F1014" s="24"/>
@@ -33552,10 +33552,10 @@
     </row>
     <row r="1015" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1015" s="29"/>
-      <c r="B1015" s="73" t="s">
+      <c r="B1015" s="69" t="s">
         <v>1853</v>
       </c>
-      <c r="C1015" s="74"/>
+      <c r="C1015" s="70"/>
       <c r="D1015" s="6"/>
       <c r="E1015" s="29"/>
       <c r="F1015" s="24"/>
@@ -33568,8 +33568,8 @@
     </row>
     <row r="1016" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="29"/>
-      <c r="B1016" s="69"/>
-      <c r="C1016" s="70"/>
+      <c r="B1016" s="71"/>
+      <c r="C1016" s="72"/>
       <c r="D1016" s="6"/>
       <c r="E1016" s="29"/>
       <c r="F1016" s="24"/>
@@ -36520,8 +36520,8 @@
     </row>
     <row r="1131" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1131" s="29"/>
-      <c r="B1131" s="69"/>
-      <c r="C1131" s="70"/>
+      <c r="B1131" s="71"/>
+      <c r="C1131" s="72"/>
       <c r="D1131" s="6"/>
       <c r="E1131" s="29"/>
       <c r="F1131" s="24"/>
@@ -36534,10 +36534,10 @@
     </row>
     <row r="1132" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1132" s="29"/>
-      <c r="B1132" s="73" t="s">
+      <c r="B1132" s="69" t="s">
         <v>1854</v>
       </c>
-      <c r="C1132" s="74"/>
+      <c r="C1132" s="70"/>
       <c r="D1132" s="6"/>
       <c r="E1132" s="29"/>
       <c r="F1132" s="24"/>
@@ -36550,8 +36550,8 @@
     </row>
     <row r="1133" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1133" s="29"/>
-      <c r="B1133" s="69"/>
-      <c r="C1133" s="70"/>
+      <c r="B1133" s="71"/>
+      <c r="C1133" s="72"/>
       <c r="D1133" s="6"/>
       <c r="E1133" s="29"/>
       <c r="F1133" s="24"/>
@@ -36606,8 +36606,8 @@
     </row>
     <row r="1136" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1136" s="29"/>
-      <c r="B1136" s="69"/>
-      <c r="C1136" s="70"/>
+      <c r="B1136" s="71"/>
+      <c r="C1136" s="72"/>
       <c r="D1136" s="6"/>
       <c r="E1136" s="29"/>
       <c r="F1136" s="24"/>
@@ -36620,10 +36620,10 @@
     </row>
     <row r="1137" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1137" s="29"/>
-      <c r="B1137" s="73" t="s">
+      <c r="B1137" s="69" t="s">
         <v>1855</v>
       </c>
-      <c r="C1137" s="74"/>
+      <c r="C1137" s="70"/>
       <c r="D1137" s="6"/>
       <c r="E1137" s="29"/>
       <c r="F1137" s="24"/>
@@ -36636,8 +36636,8 @@
     </row>
     <row r="1138" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1138" s="29"/>
-      <c r="B1138" s="69"/>
-      <c r="C1138" s="70"/>
+      <c r="B1138" s="71"/>
+      <c r="C1138" s="72"/>
       <c r="D1138" s="6"/>
       <c r="E1138" s="29"/>
       <c r="F1138" s="24"/>
@@ -39274,8 +39274,8 @@
     </row>
     <row r="1252" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1252" s="29"/>
-      <c r="B1252" s="69"/>
-      <c r="C1252" s="70"/>
+      <c r="B1252" s="71"/>
+      <c r="C1252" s="72"/>
       <c r="D1252" s="6"/>
       <c r="E1252" s="29"/>
       <c r="F1252" s="24"/>
@@ -39288,10 +39288,10 @@
     </row>
     <row r="1253" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1253" s="29"/>
-      <c r="B1253" s="73" t="s">
+      <c r="B1253" s="69" t="s">
         <v>2030</v>
       </c>
-      <c r="C1253" s="74"/>
+      <c r="C1253" s="70"/>
       <c r="D1253" s="6"/>
       <c r="E1253" s="29"/>
       <c r="F1253" s="24"/>
@@ -39304,8 +39304,8 @@
     </row>
     <row r="1254" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1254" s="29"/>
-      <c r="B1254" s="69"/>
-      <c r="C1254" s="70"/>
+      <c r="B1254" s="71"/>
+      <c r="C1254" s="72"/>
       <c r="D1254" s="6"/>
       <c r="E1254" s="29"/>
       <c r="F1254" s="24"/>
@@ -39800,6 +39800,77 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B189:C189"/>
+    <mergeCell ref="B190:C190"/>
+    <mergeCell ref="B532:C532"/>
+    <mergeCell ref="B597:C597"/>
+    <mergeCell ref="B599:C599"/>
+    <mergeCell ref="B757:C757"/>
+    <mergeCell ref="B759:C759"/>
+    <mergeCell ref="B990:C990"/>
+    <mergeCell ref="B1016:C1016"/>
+    <mergeCell ref="B1014:C1014"/>
+    <mergeCell ref="B1136:C1136"/>
+    <mergeCell ref="B1138:C1138"/>
+    <mergeCell ref="B1131:C1131"/>
+    <mergeCell ref="B1133:C1133"/>
+    <mergeCell ref="B1015:C1015"/>
+    <mergeCell ref="B1252:C1252"/>
+    <mergeCell ref="B1254:C1254"/>
+    <mergeCell ref="B1253:C1253"/>
+    <mergeCell ref="B1137:C1137"/>
+    <mergeCell ref="B1132:C1132"/>
+    <mergeCell ref="B989:C989"/>
+    <mergeCell ref="B981:C981"/>
+    <mergeCell ref="B865:C865"/>
+    <mergeCell ref="B758:C758"/>
+    <mergeCell ref="B598:C598"/>
+    <mergeCell ref="B866:C866"/>
+    <mergeCell ref="B864:C864"/>
+    <mergeCell ref="B980:C980"/>
+    <mergeCell ref="B982:C982"/>
+    <mergeCell ref="B988:C988"/>
     <mergeCell ref="B531:C531"/>
     <mergeCell ref="B387:C387"/>
     <mergeCell ref="B260:C260"/>
@@ -39814,77 +39885,6 @@
     <mergeCell ref="B248:C248"/>
     <mergeCell ref="B250:C250"/>
     <mergeCell ref="B259:C259"/>
-    <mergeCell ref="B989:C989"/>
-    <mergeCell ref="B981:C981"/>
-    <mergeCell ref="B865:C865"/>
-    <mergeCell ref="B758:C758"/>
-    <mergeCell ref="B598:C598"/>
-    <mergeCell ref="B866:C866"/>
-    <mergeCell ref="B864:C864"/>
-    <mergeCell ref="B980:C980"/>
-    <mergeCell ref="B982:C982"/>
-    <mergeCell ref="B988:C988"/>
-    <mergeCell ref="B1252:C1252"/>
-    <mergeCell ref="B1254:C1254"/>
-    <mergeCell ref="B1253:C1253"/>
-    <mergeCell ref="B1137:C1137"/>
-    <mergeCell ref="B1132:C1132"/>
-    <mergeCell ref="B990:C990"/>
-    <mergeCell ref="B1016:C1016"/>
-    <mergeCell ref="B1014:C1014"/>
-    <mergeCell ref="B1136:C1136"/>
-    <mergeCell ref="B1138:C1138"/>
-    <mergeCell ref="B1131:C1131"/>
-    <mergeCell ref="B1133:C1133"/>
-    <mergeCell ref="B1015:C1015"/>
-    <mergeCell ref="B532:C532"/>
-    <mergeCell ref="B597:C597"/>
-    <mergeCell ref="B599:C599"/>
-    <mergeCell ref="B757:C757"/>
-    <mergeCell ref="B759:C759"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B188:C188"/>
-    <mergeCell ref="B189:C189"/>
-    <mergeCell ref="B190:C190"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39914,80 +39914,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1255</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1256</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1273</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1274</v>
       </c>
@@ -39996,62 +39996,62 @@
       <c r="B9" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1272</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1281</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1266</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1295</v>
       </c>
@@ -40060,13 +40060,13 @@
       <c r="B14" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1278</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1296</v>
       </c>
@@ -40075,13 +40075,13 @@
       <c r="B15" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1294</v>
       </c>
@@ -40090,13 +40090,13 @@
       <c r="B16" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1283</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1284</v>
       </c>
@@ -40105,24 +40105,24 @@
       <c r="B17" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1288</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1293</v>
       </c>
@@ -40131,12 +40131,12 @@
       <c r="C19" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1290</v>
       </c>
@@ -40145,13 +40145,13 @@
       <c r="B20" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1299</v>
       </c>
@@ -40160,13 +40160,13 @@
       <c r="B21" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1286</v>
       </c>
@@ -40175,13 +40175,13 @@
       <c r="B22" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1292</v>
       </c>
@@ -40190,53 +40190,53 @@
       <c r="B23" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1297</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1298</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1270</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1267</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1276</v>
       </c>
@@ -40245,12 +40245,12 @@
       <c r="C27" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1277</v>
       </c>
@@ -40259,28 +40259,24 @@
       <c r="D28" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1279</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -40296,12 +40292,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 15 November 2023 18:28 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -9367,6 +9367,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9378,12 +9384,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9418,13 +9418,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9739,10 +9739,10 @@
   <dimension ref="A1:M1289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D164" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D1274" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F170" sqref="F170"/>
+      <selection pane="bottomRight" activeCell="C1280" sqref="C1280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9782,7 +9782,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="81"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
@@ -9802,7 +9802,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="82"/>
       <c r="C3" s="83"/>
-      <c r="D3" s="72"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>332</v>
@@ -9838,10 +9838,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="69" t="s">
         <v>1849</v>
       </c>
-      <c r="C5" s="74"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -9854,8 +9854,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -10082,8 +10082,8 @@
     </row>
     <row r="16" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="6"/>
       <c r="E16" s="29"/>
       <c r="F16" s="24"/>
@@ -10096,10 +10096,10 @@
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="69" t="s">
         <v>1848</v>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -10112,8 +10112,8 @@
     </row>
     <row r="18" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -10194,8 +10194,8 @@
     </row>
     <row r="22" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="6"/>
       <c r="E22" s="29"/>
       <c r="F22" s="24"/>
@@ -10208,10 +10208,10 @@
     </row>
     <row r="23" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="69" t="s">
         <v>1847</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -10224,8 +10224,8 @@
     </row>
     <row r="24" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="6"/>
       <c r="E24" s="29"/>
       <c r="F24" s="24"/>
@@ -10300,8 +10300,8 @@
     </row>
     <row r="28" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="70"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
       <c r="D28" s="6"/>
       <c r="E28" s="29"/>
       <c r="F28" s="24"/>
@@ -10330,8 +10330,8 @@
     </row>
     <row r="30" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="70"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="6"/>
       <c r="E30" s="29"/>
       <c r="F30" s="24"/>
@@ -11956,8 +11956,8 @@
     </row>
     <row r="102" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
-      <c r="B102" s="69"/>
-      <c r="C102" s="70"/>
+      <c r="B102" s="71"/>
+      <c r="C102" s="72"/>
       <c r="D102" s="6"/>
       <c r="E102" s="29"/>
       <c r="F102" s="24"/>
@@ -11970,10 +11970,10 @@
     </row>
     <row r="103" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29"/>
-      <c r="B103" s="73" t="s">
+      <c r="B103" s="69" t="s">
         <v>1868</v>
       </c>
-      <c r="C103" s="74"/>
+      <c r="C103" s="70"/>
       <c r="D103" s="6"/>
       <c r="E103" s="29"/>
       <c r="F103" s="24"/>
@@ -11986,8 +11986,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="71"/>
+      <c r="C104" s="72"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -12146,8 +12146,8 @@
     </row>
     <row r="111" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="29"/>
-      <c r="B111" s="69"/>
-      <c r="C111" s="70"/>
+      <c r="B111" s="71"/>
+      <c r="C111" s="72"/>
       <c r="D111" s="6"/>
       <c r="E111" s="29"/>
       <c r="F111" s="24"/>
@@ -12160,10 +12160,10 @@
     </row>
     <row r="112" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A112" s="29"/>
-      <c r="B112" s="73" t="s">
+      <c r="B112" s="69" t="s">
         <v>1867</v>
       </c>
-      <c r="C112" s="74"/>
+      <c r="C112" s="70"/>
       <c r="D112" s="6"/>
       <c r="E112" s="29"/>
       <c r="F112" s="24"/>
@@ -12176,8 +12176,8 @@
     </row>
     <row r="113" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="29"/>
-      <c r="B113" s="69"/>
-      <c r="C113" s="70"/>
+      <c r="B113" s="71"/>
+      <c r="C113" s="72"/>
       <c r="D113" s="6"/>
       <c r="E113" s="29"/>
       <c r="F113" s="24"/>
@@ -12682,8 +12682,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="72"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12696,10 +12696,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="73" t="s">
+      <c r="B138" s="69" t="s">
         <v>2085</v>
       </c>
-      <c r="C138" s="74"/>
+      <c r="C138" s="70"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12712,8 +12712,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="69"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="71"/>
+      <c r="C139" s="72"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12788,8 +12788,8 @@
     </row>
     <row r="143" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
-      <c r="B143" s="69"/>
-      <c r="C143" s="70"/>
+      <c r="B143" s="71"/>
+      <c r="C143" s="72"/>
       <c r="D143" s="6"/>
       <c r="E143" s="29"/>
       <c r="F143" s="24"/>
@@ -12802,10 +12802,10 @@
     </row>
     <row r="144" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
-      <c r="B144" s="73" t="s">
+      <c r="B144" s="69" t="s">
         <v>1865</v>
       </c>
-      <c r="C144" s="74"/>
+      <c r="C144" s="70"/>
       <c r="D144" s="6"/>
       <c r="E144" s="29"/>
       <c r="F144" s="24"/>
@@ -12818,8 +12818,8 @@
     </row>
     <row r="145" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
-      <c r="B145" s="69"/>
-      <c r="C145" s="70"/>
+      <c r="B145" s="71"/>
+      <c r="C145" s="72"/>
       <c r="D145" s="6"/>
       <c r="E145" s="29"/>
       <c r="F145" s="24"/>
@@ -12930,8 +12930,8 @@
     </row>
     <row r="150" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
-      <c r="B150" s="69"/>
-      <c r="C150" s="70"/>
+      <c r="B150" s="71"/>
+      <c r="C150" s="72"/>
       <c r="D150" s="6"/>
       <c r="E150" s="29"/>
       <c r="F150" s="24"/>
@@ -12944,10 +12944,10 @@
     </row>
     <row r="151" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
-      <c r="B151" s="73" t="s">
+      <c r="B151" s="69" t="s">
         <v>1866</v>
       </c>
-      <c r="C151" s="74"/>
+      <c r="C151" s="70"/>
       <c r="D151" s="6"/>
       <c r="E151" s="29"/>
       <c r="F151" s="24"/>
@@ -12960,8 +12960,8 @@
     </row>
     <row r="152" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="29"/>
-      <c r="B152" s="69"/>
-      <c r="C152" s="70"/>
+      <c r="B152" s="71"/>
+      <c r="C152" s="72"/>
       <c r="D152" s="6"/>
       <c r="E152" s="29"/>
       <c r="F152" s="24"/>
@@ -13170,8 +13170,8 @@
     </row>
     <row r="162" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
-      <c r="B162" s="69"/>
-      <c r="C162" s="70"/>
+      <c r="B162" s="71"/>
+      <c r="C162" s="72"/>
       <c r="D162" s="6"/>
       <c r="E162" s="29"/>
       <c r="F162" s="24"/>
@@ -13184,10 +13184,10 @@
     </row>
     <row r="163" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="73" t="s">
+      <c r="B163" s="69" t="s">
         <v>1864</v>
       </c>
-      <c r="C163" s="74"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -13200,8 +13200,8 @@
     </row>
     <row r="164" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="69"/>
-      <c r="C164" s="70"/>
+      <c r="B164" s="71"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -13792,8 +13792,8 @@
     </row>
     <row r="192" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="29"/>
-      <c r="B192" s="69"/>
-      <c r="C192" s="70"/>
+      <c r="B192" s="71"/>
+      <c r="C192" s="72"/>
       <c r="D192" s="6"/>
       <c r="E192" s="29"/>
       <c r="F192" s="24"/>
@@ -13806,10 +13806,10 @@
     </row>
     <row r="193" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A193" s="29"/>
-      <c r="B193" s="73" t="s">
+      <c r="B193" s="69" t="s">
         <v>2125</v>
       </c>
-      <c r="C193" s="74"/>
+      <c r="C193" s="70"/>
       <c r="D193" s="6"/>
       <c r="E193" s="29"/>
       <c r="F193" s="24"/>
@@ -13822,8 +13822,8 @@
     </row>
     <row r="194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="29"/>
-      <c r="B194" s="69"/>
-      <c r="C194" s="70"/>
+      <c r="B194" s="71"/>
+      <c r="C194" s="72"/>
       <c r="D194" s="6"/>
       <c r="E194" s="29"/>
       <c r="F194" s="24"/>
@@ -14012,8 +14012,8 @@
     </row>
     <row r="204" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="29"/>
-      <c r="B204" s="69"/>
-      <c r="C204" s="70"/>
+      <c r="B204" s="71"/>
+      <c r="C204" s="72"/>
       <c r="D204" s="6"/>
       <c r="E204" s="29"/>
       <c r="F204" s="24"/>
@@ -14026,10 +14026,10 @@
     </row>
     <row r="205" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A205" s="29"/>
-      <c r="B205" s="73" t="s">
+      <c r="B205" s="69" t="s">
         <v>1863</v>
       </c>
-      <c r="C205" s="74"/>
+      <c r="C205" s="70"/>
       <c r="D205" s="6"/>
       <c r="E205" s="29"/>
       <c r="F205" s="24"/>
@@ -14042,8 +14042,8 @@
     </row>
     <row r="206" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="29"/>
-      <c r="B206" s="69"/>
-      <c r="C206" s="70"/>
+      <c r="B206" s="71"/>
+      <c r="C206" s="72"/>
       <c r="D206" s="6"/>
       <c r="E206" s="29"/>
       <c r="F206" s="24"/>
@@ -14300,8 +14300,8 @@
     </row>
     <row r="218" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="29"/>
-      <c r="B218" s="69"/>
-      <c r="C218" s="70"/>
+      <c r="B218" s="71"/>
+      <c r="C218" s="72"/>
       <c r="D218" s="6"/>
       <c r="E218" s="29"/>
       <c r="F218" s="24"/>
@@ -14314,10 +14314,10 @@
     </row>
     <row r="219" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A219" s="29"/>
-      <c r="B219" s="73" t="s">
+      <c r="B219" s="69" t="s">
         <v>1861</v>
       </c>
-      <c r="C219" s="74"/>
+      <c r="C219" s="70"/>
       <c r="D219" s="6"/>
       <c r="E219" s="29"/>
       <c r="F219" s="24"/>
@@ -14330,8 +14330,8 @@
     </row>
     <row r="220" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="29"/>
-      <c r="B220" s="69"/>
-      <c r="C220" s="70"/>
+      <c r="B220" s="71"/>
+      <c r="C220" s="72"/>
       <c r="D220" s="6"/>
       <c r="E220" s="29"/>
       <c r="F220" s="24"/>
@@ -14396,8 +14396,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="69"/>
-      <c r="C224" s="70"/>
+      <c r="B224" s="71"/>
+      <c r="C224" s="72"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -14410,10 +14410,10 @@
     </row>
     <row r="225" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A225" s="29"/>
-      <c r="B225" s="73" t="s">
+      <c r="B225" s="69" t="s">
         <v>1862</v>
       </c>
-      <c r="C225" s="74"/>
+      <c r="C225" s="70"/>
       <c r="D225" s="6"/>
       <c r="E225" s="29"/>
       <c r="F225" s="24"/>
@@ -14426,8 +14426,8 @@
     </row>
     <row r="226" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="29"/>
-      <c r="B226" s="69"/>
-      <c r="C226" s="70"/>
+      <c r="B226" s="71"/>
+      <c r="C226" s="72"/>
       <c r="D226" s="6"/>
       <c r="E226" s="29"/>
       <c r="F226" s="24"/>
@@ -15012,8 +15012,8 @@
     </row>
     <row r="252" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="29"/>
-      <c r="B252" s="69"/>
-      <c r="C252" s="70"/>
+      <c r="B252" s="71"/>
+      <c r="C252" s="72"/>
       <c r="D252" s="6"/>
       <c r="E252" s="29"/>
       <c r="F252" s="24"/>
@@ -15026,10 +15026,10 @@
     </row>
     <row r="253" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="29"/>
-      <c r="B253" s="73" t="s">
+      <c r="B253" s="69" t="s">
         <v>1860</v>
       </c>
-      <c r="C253" s="74"/>
+      <c r="C253" s="70"/>
       <c r="D253" s="6"/>
       <c r="E253" s="29"/>
       <c r="F253" s="24"/>
@@ -15042,8 +15042,8 @@
     </row>
     <row r="254" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="29"/>
-      <c r="B254" s="69"/>
-      <c r="C254" s="70"/>
+      <c r="B254" s="71"/>
+      <c r="C254" s="72"/>
       <c r="D254" s="6"/>
       <c r="E254" s="29"/>
       <c r="F254" s="24"/>
@@ -15238,8 +15238,8 @@
     </row>
     <row r="263" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="29"/>
-      <c r="B263" s="69"/>
-      <c r="C263" s="70"/>
+      <c r="B263" s="71"/>
+      <c r="C263" s="72"/>
       <c r="D263" s="6"/>
       <c r="E263" s="29"/>
       <c r="F263" s="24"/>
@@ -15252,10 +15252,10 @@
     </row>
     <row r="264" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A264" s="29"/>
-      <c r="B264" s="73" t="s">
+      <c r="B264" s="69" t="s">
         <v>1859</v>
       </c>
-      <c r="C264" s="74"/>
+      <c r="C264" s="70"/>
       <c r="D264" s="6"/>
       <c r="E264" s="29"/>
       <c r="F264" s="24"/>
@@ -15268,8 +15268,8 @@
     </row>
     <row r="265" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="29"/>
-      <c r="B265" s="69"/>
-      <c r="C265" s="70"/>
+      <c r="B265" s="71"/>
+      <c r="C265" s="72"/>
       <c r="D265" s="6"/>
       <c r="E265" s="29"/>
       <c r="F265" s="24"/>
@@ -18312,8 +18312,8 @@
     </row>
     <row r="393" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="29"/>
-      <c r="B393" s="69"/>
-      <c r="C393" s="70"/>
+      <c r="B393" s="71"/>
+      <c r="C393" s="72"/>
       <c r="D393" s="6"/>
       <c r="E393" s="29"/>
       <c r="F393" s="24"/>
@@ -18326,10 +18326,10 @@
     </row>
     <row r="394" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A394" s="29"/>
-      <c r="B394" s="73" t="s">
+      <c r="B394" s="69" t="s">
         <v>1858</v>
       </c>
-      <c r="C394" s="74"/>
+      <c r="C394" s="70"/>
       <c r="D394" s="6"/>
       <c r="E394" s="29"/>
       <c r="F394" s="24"/>
@@ -18342,8 +18342,8 @@
     </row>
     <row r="395" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="29"/>
-      <c r="B395" s="69"/>
-      <c r="C395" s="70"/>
+      <c r="B395" s="71"/>
+      <c r="C395" s="72"/>
       <c r="D395" s="6"/>
       <c r="E395" s="29"/>
       <c r="F395" s="24"/>
@@ -21968,8 +21968,8 @@
     </row>
     <row r="534" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A534" s="29"/>
-      <c r="B534" s="69"/>
-      <c r="C534" s="70"/>
+      <c r="B534" s="71"/>
+      <c r="C534" s="72"/>
       <c r="D534" s="6"/>
       <c r="E534" s="29"/>
       <c r="F534" s="24"/>
@@ -22024,8 +22024,8 @@
     </row>
     <row r="537" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A537" s="29"/>
-      <c r="B537" s="69"/>
-      <c r="C537" s="70"/>
+      <c r="B537" s="71"/>
+      <c r="C537" s="72"/>
       <c r="D537" s="6"/>
       <c r="E537" s="29"/>
       <c r="F537" s="24"/>
@@ -22038,10 +22038,10 @@
     </row>
     <row r="538" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A538" s="29"/>
-      <c r="B538" s="73" t="s">
+      <c r="B538" s="69" t="s">
         <v>1857</v>
       </c>
-      <c r="C538" s="74"/>
+      <c r="C538" s="70"/>
       <c r="D538" s="6"/>
       <c r="E538" s="29"/>
       <c r="F538" s="24"/>
@@ -22054,8 +22054,8 @@
     </row>
     <row r="539" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A539" s="29"/>
-      <c r="B539" s="69"/>
-      <c r="C539" s="70"/>
+      <c r="B539" s="71"/>
+      <c r="C539" s="72"/>
       <c r="D539" s="6"/>
       <c r="E539" s="29"/>
       <c r="F539" s="24"/>
@@ -23678,8 +23678,8 @@
     </row>
     <row r="604" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A604" s="29"/>
-      <c r="B604" s="69"/>
-      <c r="C604" s="70"/>
+      <c r="B604" s="71"/>
+      <c r="C604" s="72"/>
       <c r="D604" s="6"/>
       <c r="E604" s="29"/>
       <c r="F604" s="24"/>
@@ -23692,10 +23692,10 @@
     </row>
     <row r="605" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A605" s="29"/>
-      <c r="B605" s="73" t="s">
+      <c r="B605" s="69" t="s">
         <v>1856</v>
       </c>
-      <c r="C605" s="74"/>
+      <c r="C605" s="70"/>
       <c r="D605" s="6"/>
       <c r="E605" s="29"/>
       <c r="F605" s="24"/>
@@ -23708,8 +23708,8 @@
     </row>
     <row r="606" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A606" s="29"/>
-      <c r="B606" s="69"/>
-      <c r="C606" s="70"/>
+      <c r="B606" s="71"/>
+      <c r="C606" s="72"/>
       <c r="D606" s="6"/>
       <c r="E606" s="29"/>
       <c r="F606" s="24"/>
@@ -27580,8 +27580,8 @@
     </row>
     <row r="764" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A764" s="29"/>
-      <c r="B764" s="69"/>
-      <c r="C764" s="70"/>
+      <c r="B764" s="71"/>
+      <c r="C764" s="72"/>
       <c r="D764" s="6"/>
       <c r="E764" s="29"/>
       <c r="F764" s="24"/>
@@ -27594,10 +27594,10 @@
     </row>
     <row r="765" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A765" s="29"/>
-      <c r="B765" s="73" t="s">
+      <c r="B765" s="69" t="s">
         <v>1850</v>
       </c>
-      <c r="C765" s="74"/>
+      <c r="C765" s="70"/>
       <c r="D765" s="6"/>
       <c r="E765" s="29"/>
       <c r="F765" s="24"/>
@@ -27610,8 +27610,8 @@
     </row>
     <row r="766" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A766" s="29"/>
-      <c r="B766" s="69"/>
-      <c r="C766" s="70"/>
+      <c r="B766" s="71"/>
+      <c r="C766" s="72"/>
       <c r="D766" s="6"/>
       <c r="E766" s="29"/>
       <c r="F766" s="24"/>
@@ -30116,8 +30116,8 @@
     </row>
     <row r="871" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A871" s="29"/>
-      <c r="B871" s="69"/>
-      <c r="C871" s="70"/>
+      <c r="B871" s="71"/>
+      <c r="C871" s="72"/>
       <c r="D871" s="6"/>
       <c r="E871" s="29"/>
       <c r="F871" s="24"/>
@@ -30130,10 +30130,10 @@
     </row>
     <row r="872" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A872" s="29"/>
-      <c r="B872" s="73" t="s">
+      <c r="B872" s="69" t="s">
         <v>1851</v>
       </c>
-      <c r="C872" s="74"/>
+      <c r="C872" s="70"/>
       <c r="D872" s="6"/>
       <c r="E872" s="29"/>
       <c r="F872" s="24"/>
@@ -30146,8 +30146,8 @@
     </row>
     <row r="873" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A873" s="29"/>
-      <c r="B873" s="69"/>
-      <c r="C873" s="70"/>
+      <c r="B873" s="71"/>
+      <c r="C873" s="72"/>
       <c r="D873" s="6"/>
       <c r="E873" s="29"/>
       <c r="F873" s="24"/>
@@ -33061,8 +33061,8 @@
     </row>
     <row r="987" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A987" s="29"/>
-      <c r="B987" s="69"/>
-      <c r="C987" s="70"/>
+      <c r="B987" s="71"/>
+      <c r="C987" s="72"/>
       <c r="D987" s="6"/>
       <c r="E987" s="29"/>
       <c r="F987" s="24"/>
@@ -33075,10 +33075,10 @@
     </row>
     <row r="988" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A988" s="29"/>
-      <c r="B988" s="73" t="s">
+      <c r="B988" s="69" t="s">
         <v>1949</v>
       </c>
-      <c r="C988" s="74"/>
+      <c r="C988" s="70"/>
       <c r="D988" s="6"/>
       <c r="E988" s="29"/>
       <c r="F988" s="24"/>
@@ -33091,8 +33091,8 @@
     </row>
     <row r="989" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A989" s="29"/>
-      <c r="B989" s="69"/>
-      <c r="C989" s="70"/>
+      <c r="B989" s="71"/>
+      <c r="C989" s="72"/>
       <c r="D989" s="6"/>
       <c r="E989" s="29"/>
       <c r="F989" s="24"/>
@@ -33226,8 +33226,8 @@
     </row>
     <row r="995" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A995" s="29"/>
-      <c r="B995" s="69"/>
-      <c r="C995" s="70"/>
+      <c r="B995" s="71"/>
+      <c r="C995" s="72"/>
       <c r="D995" s="6"/>
       <c r="E995" s="29"/>
       <c r="F995" s="24"/>
@@ -33240,10 +33240,10 @@
     </row>
     <row r="996" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A996" s="29"/>
-      <c r="B996" s="73" t="s">
+      <c r="B996" s="69" t="s">
         <v>1852</v>
       </c>
-      <c r="C996" s="74"/>
+      <c r="C996" s="70"/>
       <c r="D996" s="6"/>
       <c r="E996" s="29"/>
       <c r="F996" s="24"/>
@@ -33256,8 +33256,8 @@
     </row>
     <row r="997" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A997" s="29"/>
-      <c r="B997" s="69"/>
-      <c r="C997" s="70"/>
+      <c r="B997" s="71"/>
+      <c r="C997" s="72"/>
       <c r="D997" s="6"/>
       <c r="E997" s="29"/>
       <c r="F997" s="24"/>
@@ -33780,8 +33780,8 @@
     </row>
     <row r="1021" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1021" s="29"/>
-      <c r="B1021" s="69"/>
-      <c r="C1021" s="70"/>
+      <c r="B1021" s="71"/>
+      <c r="C1021" s="72"/>
       <c r="D1021" s="6"/>
       <c r="E1021" s="29"/>
       <c r="F1021" s="24"/>
@@ -33794,10 +33794,10 @@
     </row>
     <row r="1022" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1022" s="29"/>
-      <c r="B1022" s="73" t="s">
+      <c r="B1022" s="69" t="s">
         <v>1853</v>
       </c>
-      <c r="C1022" s="74"/>
+      <c r="C1022" s="70"/>
       <c r="D1022" s="6"/>
       <c r="E1022" s="29"/>
       <c r="F1022" s="24"/>
@@ -33810,8 +33810,8 @@
     </row>
     <row r="1023" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1023" s="29"/>
-      <c r="B1023" s="69"/>
-      <c r="C1023" s="70"/>
+      <c r="B1023" s="71"/>
+      <c r="C1023" s="72"/>
       <c r="D1023" s="6"/>
       <c r="E1023" s="29"/>
       <c r="F1023" s="24"/>
@@ -36762,8 +36762,8 @@
     </row>
     <row r="1138" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1138" s="29"/>
-      <c r="B1138" s="69"/>
-      <c r="C1138" s="70"/>
+      <c r="B1138" s="71"/>
+      <c r="C1138" s="72"/>
       <c r="D1138" s="6"/>
       <c r="E1138" s="29"/>
       <c r="F1138" s="24"/>
@@ -36776,10 +36776,10 @@
     </row>
     <row r="1139" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1139" s="29"/>
-      <c r="B1139" s="73" t="s">
+      <c r="B1139" s="69" t="s">
         <v>1854</v>
       </c>
-      <c r="C1139" s="74"/>
+      <c r="C1139" s="70"/>
       <c r="D1139" s="6"/>
       <c r="E1139" s="29"/>
       <c r="F1139" s="24"/>
@@ -36792,8 +36792,8 @@
     </row>
     <row r="1140" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1140" s="29"/>
-      <c r="B1140" s="69"/>
-      <c r="C1140" s="70"/>
+      <c r="B1140" s="71"/>
+      <c r="C1140" s="72"/>
       <c r="D1140" s="6"/>
       <c r="E1140" s="29"/>
       <c r="F1140" s="24"/>
@@ -36848,8 +36848,8 @@
     </row>
     <row r="1143" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1143" s="29"/>
-      <c r="B1143" s="69"/>
-      <c r="C1143" s="70"/>
+      <c r="B1143" s="71"/>
+      <c r="C1143" s="72"/>
       <c r="D1143" s="6"/>
       <c r="E1143" s="29"/>
       <c r="F1143" s="24"/>
@@ -36862,10 +36862,10 @@
     </row>
     <row r="1144" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1144" s="29"/>
-      <c r="B1144" s="73" t="s">
+      <c r="B1144" s="69" t="s">
         <v>1855</v>
       </c>
-      <c r="C1144" s="74"/>
+      <c r="C1144" s="70"/>
       <c r="D1144" s="6"/>
       <c r="E1144" s="29"/>
       <c r="F1144" s="24"/>
@@ -36878,8 +36878,8 @@
     </row>
     <row r="1145" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1145" s="29"/>
-      <c r="B1145" s="69"/>
-      <c r="C1145" s="70"/>
+      <c r="B1145" s="71"/>
+      <c r="C1145" s="72"/>
       <c r="D1145" s="6"/>
       <c r="E1145" s="29"/>
       <c r="F1145" s="24"/>
@@ -39632,8 +39632,8 @@
     </row>
     <row r="1264" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1264" s="29"/>
-      <c r="B1264" s="69"/>
-      <c r="C1264" s="70"/>
+      <c r="B1264" s="71"/>
+      <c r="C1264" s="72"/>
       <c r="D1264" s="6"/>
       <c r="E1264" s="29"/>
       <c r="F1264" s="24"/>
@@ -39646,10 +39646,10 @@
     </row>
     <row r="1265" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1265" s="29"/>
-      <c r="B1265" s="73" t="s">
+      <c r="B1265" s="69" t="s">
         <v>2030</v>
       </c>
-      <c r="C1265" s="74"/>
+      <c r="C1265" s="70"/>
       <c r="D1265" s="6"/>
       <c r="E1265" s="29"/>
       <c r="F1265" s="24"/>
@@ -39662,8 +39662,8 @@
     </row>
     <row r="1266" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1266" s="29"/>
-      <c r="B1266" s="69"/>
-      <c r="C1266" s="70"/>
+      <c r="B1266" s="71"/>
+      <c r="C1266" s="72"/>
       <c r="D1266" s="6"/>
       <c r="E1266" s="29"/>
       <c r="F1266" s="24"/>
@@ -40158,6 +40158,77 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B539:C539"/>
+    <mergeCell ref="B604:C604"/>
+    <mergeCell ref="B606:C606"/>
+    <mergeCell ref="B764:C764"/>
+    <mergeCell ref="B766:C766"/>
+    <mergeCell ref="B997:C997"/>
+    <mergeCell ref="B1023:C1023"/>
+    <mergeCell ref="B1021:C1021"/>
+    <mergeCell ref="B1143:C1143"/>
+    <mergeCell ref="B1145:C1145"/>
+    <mergeCell ref="B1138:C1138"/>
+    <mergeCell ref="B1140:C1140"/>
+    <mergeCell ref="B1022:C1022"/>
+    <mergeCell ref="B1264:C1264"/>
+    <mergeCell ref="B1266:C1266"/>
+    <mergeCell ref="B1265:C1265"/>
+    <mergeCell ref="B1144:C1144"/>
+    <mergeCell ref="B1139:C1139"/>
+    <mergeCell ref="B996:C996"/>
+    <mergeCell ref="B988:C988"/>
+    <mergeCell ref="B872:C872"/>
+    <mergeCell ref="B765:C765"/>
+    <mergeCell ref="B605:C605"/>
+    <mergeCell ref="B873:C873"/>
+    <mergeCell ref="B871:C871"/>
+    <mergeCell ref="B987:C987"/>
+    <mergeCell ref="B989:C989"/>
+    <mergeCell ref="B995:C995"/>
     <mergeCell ref="B538:C538"/>
     <mergeCell ref="B394:C394"/>
     <mergeCell ref="B264:C264"/>
@@ -40172,77 +40243,6 @@
     <mergeCell ref="B252:C252"/>
     <mergeCell ref="B254:C254"/>
     <mergeCell ref="B263:C263"/>
-    <mergeCell ref="B996:C996"/>
-    <mergeCell ref="B988:C988"/>
-    <mergeCell ref="B872:C872"/>
-    <mergeCell ref="B765:C765"/>
-    <mergeCell ref="B605:C605"/>
-    <mergeCell ref="B873:C873"/>
-    <mergeCell ref="B871:C871"/>
-    <mergeCell ref="B987:C987"/>
-    <mergeCell ref="B989:C989"/>
-    <mergeCell ref="B995:C995"/>
-    <mergeCell ref="B1264:C1264"/>
-    <mergeCell ref="B1266:C1266"/>
-    <mergeCell ref="B1265:C1265"/>
-    <mergeCell ref="B1144:C1144"/>
-    <mergeCell ref="B1139:C1139"/>
-    <mergeCell ref="B997:C997"/>
-    <mergeCell ref="B1023:C1023"/>
-    <mergeCell ref="B1021:C1021"/>
-    <mergeCell ref="B1143:C1143"/>
-    <mergeCell ref="B1145:C1145"/>
-    <mergeCell ref="B1138:C1138"/>
-    <mergeCell ref="B1140:C1140"/>
-    <mergeCell ref="B1022:C1022"/>
-    <mergeCell ref="B539:C539"/>
-    <mergeCell ref="B604:C604"/>
-    <mergeCell ref="B606:C606"/>
-    <mergeCell ref="B764:C764"/>
-    <mergeCell ref="B766:C766"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40272,80 +40272,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1255</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1256</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1273</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1274</v>
       </c>
@@ -40354,62 +40354,62 @@
       <c r="B9" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1272</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1263</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1281</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1266</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1295</v>
       </c>
@@ -40418,13 +40418,13 @@
       <c r="B14" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1278</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1296</v>
       </c>
@@ -40433,13 +40433,13 @@
       <c r="B15" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1282</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1294</v>
       </c>
@@ -40448,13 +40448,13 @@
       <c r="B16" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1283</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1284</v>
       </c>
@@ -40463,24 +40463,24 @@
       <c r="B17" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1288</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1293</v>
       </c>
@@ -40489,12 +40489,12 @@
       <c r="C19" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1290</v>
       </c>
@@ -40503,13 +40503,13 @@
       <c r="B20" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1291</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1299</v>
       </c>
@@ -40518,13 +40518,13 @@
       <c r="B21" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1286</v>
       </c>
@@ -40533,13 +40533,13 @@
       <c r="B22" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1292</v>
       </c>
@@ -40548,53 +40548,53 @@
       <c r="B23" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1297</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1298</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1270</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1267</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1276</v>
       </c>
@@ -40603,12 +40603,12 @@
       <c r="C27" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1277</v>
       </c>
@@ -40617,28 +40617,24 @@
       <c r="D28" s="53" t="s">
         <v>1265</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1279</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -40654,12 +40650,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 25 Januari 2023 16:00 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4457" uniqueCount="2239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="2242">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8850,6 +8850,15 @@
   </si>
   <si>
     <t>Menyimpan Data Baru Log Jalur WorkFlow Dokumen Bisnis</t>
+  </si>
+  <si>
+    <t>transaction.update.taxation.setTransactionTaxDetail</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Perincian Pajak Transaksi</t>
+  </si>
+  <si>
+    <t>1.0000.0000002</t>
   </si>
 </sst>
 </file>
@@ -9517,12 +9526,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9534,6 +9537,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9568,13 +9577,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9886,13 +9895,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1315"/>
+  <dimension ref="A1:M1316"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D1275" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F1284" sqref="F1284"/>
+      <selection pane="bottomRight" activeCell="G1289" sqref="G1289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -9932,7 +9941,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="81"/>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="71" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
@@ -9952,7 +9961,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="82"/>
       <c r="C3" s="83"/>
-      <c r="D3" s="74"/>
+      <c r="D3" s="72"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>332</v>
@@ -9988,10 +9997,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="73" t="s">
         <v>1823</v>
       </c>
-      <c r="C5" s="70"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -10004,8 +10013,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="72"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -10232,8 +10241,8 @@
     </row>
     <row r="16" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="72"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="6"/>
       <c r="E16" s="29"/>
       <c r="F16" s="24"/>
@@ -10246,10 +10255,10 @@
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="73" t="s">
         <v>1822</v>
       </c>
-      <c r="C17" s="70"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -10262,8 +10271,8 @@
     </row>
     <row r="18" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="72"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -10344,8 +10353,8 @@
     </row>
     <row r="22" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="6"/>
       <c r="E22" s="29"/>
       <c r="F22" s="24"/>
@@ -10358,10 +10367,10 @@
     </row>
     <row r="23" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="73" t="s">
         <v>1821</v>
       </c>
-      <c r="C23" s="70"/>
+      <c r="C23" s="74"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -10374,8 +10383,8 @@
     </row>
     <row r="24" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="6"/>
       <c r="E24" s="29"/>
       <c r="F24" s="24"/>
@@ -10450,8 +10459,8 @@
     </row>
     <row r="28" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
-      <c r="B28" s="71"/>
-      <c r="C28" s="72"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="70"/>
       <c r="D28" s="6"/>
       <c r="E28" s="29"/>
       <c r="F28" s="24"/>
@@ -10480,8 +10489,8 @@
     </row>
     <row r="30" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="72"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="70"/>
       <c r="D30" s="6"/>
       <c r="E30" s="29"/>
       <c r="F30" s="24"/>
@@ -12106,8 +12115,8 @@
     </row>
     <row r="102" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
-      <c r="B102" s="71"/>
-      <c r="C102" s="72"/>
+      <c r="B102" s="69"/>
+      <c r="C102" s="70"/>
       <c r="D102" s="6"/>
       <c r="E102" s="29"/>
       <c r="F102" s="24"/>
@@ -12120,10 +12129,10 @@
     </row>
     <row r="103" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29"/>
-      <c r="B103" s="69" t="s">
+      <c r="B103" s="73" t="s">
         <v>1842</v>
       </c>
-      <c r="C103" s="70"/>
+      <c r="C103" s="74"/>
       <c r="D103" s="6"/>
       <c r="E103" s="29"/>
       <c r="F103" s="24"/>
@@ -12136,8 +12145,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="71"/>
-      <c r="C104" s="72"/>
+      <c r="B104" s="69"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -12296,8 +12305,8 @@
     </row>
     <row r="111" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="29"/>
-      <c r="B111" s="71"/>
-      <c r="C111" s="72"/>
+      <c r="B111" s="69"/>
+      <c r="C111" s="70"/>
       <c r="D111" s="6"/>
       <c r="E111" s="29"/>
       <c r="F111" s="24"/>
@@ -12310,10 +12319,10 @@
     </row>
     <row r="112" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A112" s="29"/>
-      <c r="B112" s="69" t="s">
+      <c r="B112" s="73" t="s">
         <v>1841</v>
       </c>
-      <c r="C112" s="70"/>
+      <c r="C112" s="74"/>
       <c r="D112" s="6"/>
       <c r="E112" s="29"/>
       <c r="F112" s="24"/>
@@ -12326,8 +12335,8 @@
     </row>
     <row r="113" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="29"/>
-      <c r="B113" s="71"/>
-      <c r="C113" s="72"/>
+      <c r="B113" s="69"/>
+      <c r="C113" s="70"/>
       <c r="D113" s="6"/>
       <c r="E113" s="29"/>
       <c r="F113" s="24"/>
@@ -12832,8 +12841,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="71"/>
-      <c r="C137" s="72"/>
+      <c r="B137" s="69"/>
+      <c r="C137" s="70"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12846,10 +12855,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="69" t="s">
+      <c r="B138" s="73" t="s">
         <v>2055</v>
       </c>
-      <c r="C138" s="70"/>
+      <c r="C138" s="74"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12862,8 +12871,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="71"/>
-      <c r="C139" s="72"/>
+      <c r="B139" s="69"/>
+      <c r="C139" s="70"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -12938,8 +12947,8 @@
     </row>
     <row r="143" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
-      <c r="B143" s="71"/>
-      <c r="C143" s="72"/>
+      <c r="B143" s="69"/>
+      <c r="C143" s="70"/>
       <c r="D143" s="6"/>
       <c r="E143" s="29"/>
       <c r="F143" s="24"/>
@@ -12952,10 +12961,10 @@
     </row>
     <row r="144" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
-      <c r="B144" s="69" t="s">
+      <c r="B144" s="73" t="s">
         <v>1839</v>
       </c>
-      <c r="C144" s="70"/>
+      <c r="C144" s="74"/>
       <c r="D144" s="6"/>
       <c r="E144" s="29"/>
       <c r="F144" s="24"/>
@@ -12968,8 +12977,8 @@
     </row>
     <row r="145" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
-      <c r="B145" s="71"/>
-      <c r="C145" s="72"/>
+      <c r="B145" s="69"/>
+      <c r="C145" s="70"/>
       <c r="D145" s="6"/>
       <c r="E145" s="29"/>
       <c r="F145" s="24"/>
@@ -13080,8 +13089,8 @@
     </row>
     <row r="150" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
-      <c r="B150" s="71"/>
-      <c r="C150" s="72"/>
+      <c r="B150" s="69"/>
+      <c r="C150" s="70"/>
       <c r="D150" s="6"/>
       <c r="E150" s="29"/>
       <c r="F150" s="24"/>
@@ -13094,10 +13103,10 @@
     </row>
     <row r="151" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
-      <c r="B151" s="69" t="s">
+      <c r="B151" s="73" t="s">
         <v>1840</v>
       </c>
-      <c r="C151" s="70"/>
+      <c r="C151" s="74"/>
       <c r="D151" s="6"/>
       <c r="E151" s="29"/>
       <c r="F151" s="24"/>
@@ -13110,8 +13119,8 @@
     </row>
     <row r="152" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="29"/>
-      <c r="B152" s="71"/>
-      <c r="C152" s="72"/>
+      <c r="B152" s="69"/>
+      <c r="C152" s="70"/>
       <c r="D152" s="6"/>
       <c r="E152" s="29"/>
       <c r="F152" s="24"/>
@@ -13320,8 +13329,8 @@
     </row>
     <row r="162" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
-      <c r="B162" s="71"/>
-      <c r="C162" s="72"/>
+      <c r="B162" s="69"/>
+      <c r="C162" s="70"/>
       <c r="D162" s="6"/>
       <c r="E162" s="29"/>
       <c r="F162" s="24"/>
@@ -13334,10 +13343,10 @@
     </row>
     <row r="163" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="69" t="s">
+      <c r="B163" s="73" t="s">
         <v>1838</v>
       </c>
-      <c r="C163" s="70"/>
+      <c r="C163" s="74"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -13350,8 +13359,8 @@
     </row>
     <row r="164" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="71"/>
-      <c r="C164" s="72"/>
+      <c r="B164" s="69"/>
+      <c r="C164" s="70"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -13942,8 +13951,8 @@
     </row>
     <row r="192" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="29"/>
-      <c r="B192" s="71"/>
-      <c r="C192" s="72"/>
+      <c r="B192" s="69"/>
+      <c r="C192" s="70"/>
       <c r="D192" s="6"/>
       <c r="E192" s="29"/>
       <c r="F192" s="24"/>
@@ -13956,10 +13965,10 @@
     </row>
     <row r="193" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A193" s="29"/>
-      <c r="B193" s="69" t="s">
+      <c r="B193" s="73" t="s">
         <v>2095</v>
       </c>
-      <c r="C193" s="70"/>
+      <c r="C193" s="74"/>
       <c r="D193" s="6"/>
       <c r="E193" s="29"/>
       <c r="F193" s="24"/>
@@ -13972,8 +13981,8 @@
     </row>
     <row r="194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="29"/>
-      <c r="B194" s="71"/>
-      <c r="C194" s="72"/>
+      <c r="B194" s="69"/>
+      <c r="C194" s="70"/>
       <c r="D194" s="6"/>
       <c r="E194" s="29"/>
       <c r="F194" s="24"/>
@@ -14162,8 +14171,8 @@
     </row>
     <row r="204" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="29"/>
-      <c r="B204" s="71"/>
-      <c r="C204" s="72"/>
+      <c r="B204" s="69"/>
+      <c r="C204" s="70"/>
       <c r="D204" s="6"/>
       <c r="E204" s="29"/>
       <c r="F204" s="24"/>
@@ -14176,10 +14185,10 @@
     </row>
     <row r="205" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A205" s="29"/>
-      <c r="B205" s="69" t="s">
+      <c r="B205" s="73" t="s">
         <v>1837</v>
       </c>
-      <c r="C205" s="70"/>
+      <c r="C205" s="74"/>
       <c r="D205" s="6"/>
       <c r="E205" s="29"/>
       <c r="F205" s="24"/>
@@ -14192,8 +14201,8 @@
     </row>
     <row r="206" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="29"/>
-      <c r="B206" s="71"/>
-      <c r="C206" s="72"/>
+      <c r="B206" s="69"/>
+      <c r="C206" s="70"/>
       <c r="D206" s="6"/>
       <c r="E206" s="29"/>
       <c r="F206" s="24"/>
@@ -14450,8 +14459,8 @@
     </row>
     <row r="218" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="29"/>
-      <c r="B218" s="71"/>
-      <c r="C218" s="72"/>
+      <c r="B218" s="69"/>
+      <c r="C218" s="70"/>
       <c r="D218" s="6"/>
       <c r="E218" s="29"/>
       <c r="F218" s="24"/>
@@ -14464,10 +14473,10 @@
     </row>
     <row r="219" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A219" s="29"/>
-      <c r="B219" s="69" t="s">
+      <c r="B219" s="73" t="s">
         <v>1835</v>
       </c>
-      <c r="C219" s="70"/>
+      <c r="C219" s="74"/>
       <c r="D219" s="6"/>
       <c r="E219" s="29"/>
       <c r="F219" s="24"/>
@@ -14480,8 +14489,8 @@
     </row>
     <row r="220" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="29"/>
-      <c r="B220" s="71"/>
-      <c r="C220" s="72"/>
+      <c r="B220" s="69"/>
+      <c r="C220" s="70"/>
       <c r="D220" s="6"/>
       <c r="E220" s="29"/>
       <c r="F220" s="24"/>
@@ -14546,8 +14555,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="71"/>
-      <c r="C224" s="72"/>
+      <c r="B224" s="69"/>
+      <c r="C224" s="70"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -14560,10 +14569,10 @@
     </row>
     <row r="225" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A225" s="29"/>
-      <c r="B225" s="69" t="s">
+      <c r="B225" s="73" t="s">
         <v>1836</v>
       </c>
-      <c r="C225" s="70"/>
+      <c r="C225" s="74"/>
       <c r="D225" s="6"/>
       <c r="E225" s="29"/>
       <c r="F225" s="24"/>
@@ -14576,8 +14585,8 @@
     </row>
     <row r="226" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="29"/>
-      <c r="B226" s="71"/>
-      <c r="C226" s="72"/>
+      <c r="B226" s="69"/>
+      <c r="C226" s="70"/>
       <c r="D226" s="6"/>
       <c r="E226" s="29"/>
       <c r="F226" s="24"/>
@@ -15162,8 +15171,8 @@
     </row>
     <row r="252" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="29"/>
-      <c r="B252" s="71"/>
-      <c r="C252" s="72"/>
+      <c r="B252" s="69"/>
+      <c r="C252" s="70"/>
       <c r="D252" s="6"/>
       <c r="E252" s="29"/>
       <c r="F252" s="24"/>
@@ -15176,10 +15185,10 @@
     </row>
     <row r="253" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="29"/>
-      <c r="B253" s="69" t="s">
+      <c r="B253" s="73" t="s">
         <v>1834</v>
       </c>
-      <c r="C253" s="70"/>
+      <c r="C253" s="74"/>
       <c r="D253" s="6"/>
       <c r="E253" s="29"/>
       <c r="F253" s="24"/>
@@ -15192,8 +15201,8 @@
     </row>
     <row r="254" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="29"/>
-      <c r="B254" s="71"/>
-      <c r="C254" s="72"/>
+      <c r="B254" s="69"/>
+      <c r="C254" s="70"/>
       <c r="D254" s="6"/>
       <c r="E254" s="29"/>
       <c r="F254" s="24"/>
@@ -15388,8 +15397,8 @@
     </row>
     <row r="263" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="29"/>
-      <c r="B263" s="71"/>
-      <c r="C263" s="72"/>
+      <c r="B263" s="69"/>
+      <c r="C263" s="70"/>
       <c r="D263" s="6"/>
       <c r="E263" s="29"/>
       <c r="F263" s="24"/>
@@ -15402,10 +15411,10 @@
     </row>
     <row r="264" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A264" s="29"/>
-      <c r="B264" s="69" t="s">
+      <c r="B264" s="73" t="s">
         <v>1833</v>
       </c>
-      <c r="C264" s="70"/>
+      <c r="C264" s="74"/>
       <c r="D264" s="6"/>
       <c r="E264" s="29"/>
       <c r="F264" s="24"/>
@@ -15418,8 +15427,8 @@
     </row>
     <row r="265" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="29"/>
-      <c r="B265" s="71"/>
-      <c r="C265" s="72"/>
+      <c r="B265" s="69"/>
+      <c r="C265" s="70"/>
       <c r="D265" s="6"/>
       <c r="E265" s="29"/>
       <c r="F265" s="24"/>
@@ -18644,8 +18653,8 @@
     </row>
     <row r="401" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="29"/>
-      <c r="B401" s="71"/>
-      <c r="C401" s="72"/>
+      <c r="B401" s="69"/>
+      <c r="C401" s="70"/>
       <c r="D401" s="6"/>
       <c r="E401" s="29"/>
       <c r="F401" s="24"/>
@@ -18658,10 +18667,10 @@
     </row>
     <row r="402" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A402" s="29"/>
-      <c r="B402" s="69" t="s">
+      <c r="B402" s="73" t="s">
         <v>1832</v>
       </c>
-      <c r="C402" s="70"/>
+      <c r="C402" s="74"/>
       <c r="D402" s="6"/>
       <c r="E402" s="29"/>
       <c r="F402" s="24"/>
@@ -18674,8 +18683,8 @@
     </row>
     <row r="403" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="29"/>
-      <c r="B403" s="71"/>
-      <c r="C403" s="72"/>
+      <c r="B403" s="69"/>
+      <c r="C403" s="70"/>
       <c r="D403" s="6"/>
       <c r="E403" s="29"/>
       <c r="F403" s="24"/>
@@ -22412,8 +22421,8 @@
     </row>
     <row r="546" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A546" s="29"/>
-      <c r="B546" s="71"/>
-      <c r="C546" s="72"/>
+      <c r="B546" s="69"/>
+      <c r="C546" s="70"/>
       <c r="D546" s="6"/>
       <c r="E546" s="29"/>
       <c r="F546" s="24"/>
@@ -22468,8 +22477,8 @@
     </row>
     <row r="549" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A549" s="29"/>
-      <c r="B549" s="71"/>
-      <c r="C549" s="72"/>
+      <c r="B549" s="69"/>
+      <c r="C549" s="70"/>
       <c r="D549" s="6"/>
       <c r="E549" s="29"/>
       <c r="F549" s="24"/>
@@ -22482,10 +22491,10 @@
     </row>
     <row r="550" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A550" s="29"/>
-      <c r="B550" s="69" t="s">
+      <c r="B550" s="73" t="s">
         <v>1831</v>
       </c>
-      <c r="C550" s="70"/>
+      <c r="C550" s="74"/>
       <c r="D550" s="6"/>
       <c r="E550" s="29"/>
       <c r="F550" s="24"/>
@@ -22498,8 +22507,8 @@
     </row>
     <row r="551" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A551" s="29"/>
-      <c r="B551" s="71"/>
-      <c r="C551" s="72"/>
+      <c r="B551" s="69"/>
+      <c r="C551" s="70"/>
       <c r="D551" s="6"/>
       <c r="E551" s="29"/>
       <c r="F551" s="24"/>
@@ -24122,8 +24131,8 @@
     </row>
     <row r="616" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A616" s="29"/>
-      <c r="B616" s="71"/>
-      <c r="C616" s="72"/>
+      <c r="B616" s="69"/>
+      <c r="C616" s="70"/>
       <c r="D616" s="6"/>
       <c r="E616" s="29"/>
       <c r="F616" s="24"/>
@@ -24136,10 +24145,10 @@
     </row>
     <row r="617" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A617" s="29"/>
-      <c r="B617" s="69" t="s">
+      <c r="B617" s="73" t="s">
         <v>1830</v>
       </c>
-      <c r="C617" s="70"/>
+      <c r="C617" s="74"/>
       <c r="D617" s="6"/>
       <c r="E617" s="29"/>
       <c r="F617" s="24"/>
@@ -24152,8 +24161,8 @@
     </row>
     <row r="618" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A618" s="29"/>
-      <c r="B618" s="71"/>
-      <c r="C618" s="72"/>
+      <c r="B618" s="69"/>
+      <c r="C618" s="70"/>
       <c r="D618" s="6"/>
       <c r="E618" s="29"/>
       <c r="F618" s="24"/>
@@ -28042,8 +28051,8 @@
     </row>
     <row r="777" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A777" s="29"/>
-      <c r="B777" s="71"/>
-      <c r="C777" s="72"/>
+      <c r="B777" s="69"/>
+      <c r="C777" s="70"/>
       <c r="D777" s="6"/>
       <c r="E777" s="29"/>
       <c r="F777" s="24"/>
@@ -28056,10 +28065,10 @@
     </row>
     <row r="778" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A778" s="29"/>
-      <c r="B778" s="69" t="s">
+      <c r="B778" s="73" t="s">
         <v>1824</v>
       </c>
-      <c r="C778" s="70"/>
+      <c r="C778" s="74"/>
       <c r="D778" s="6"/>
       <c r="E778" s="29"/>
       <c r="F778" s="24"/>
@@ -28072,8 +28081,8 @@
     </row>
     <row r="779" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A779" s="29"/>
-      <c r="B779" s="71"/>
-      <c r="C779" s="72"/>
+      <c r="B779" s="69"/>
+      <c r="C779" s="70"/>
       <c r="D779" s="6"/>
       <c r="E779" s="29"/>
       <c r="F779" s="24"/>
@@ -30626,8 +30635,8 @@
     </row>
     <row r="886" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A886" s="29"/>
-      <c r="B886" s="71"/>
-      <c r="C886" s="72"/>
+      <c r="B886" s="69"/>
+      <c r="C886" s="70"/>
       <c r="D886" s="6"/>
       <c r="E886" s="29"/>
       <c r="F886" s="24"/>
@@ -30640,10 +30649,10 @@
     </row>
     <row r="887" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A887" s="29"/>
-      <c r="B887" s="69" t="s">
+      <c r="B887" s="73" t="s">
         <v>1825</v>
       </c>
-      <c r="C887" s="70"/>
+      <c r="C887" s="74"/>
       <c r="D887" s="6"/>
       <c r="E887" s="29"/>
       <c r="F887" s="24"/>
@@ -30656,8 +30665,8 @@
     </row>
     <row r="888" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A888" s="29"/>
-      <c r="B888" s="71"/>
-      <c r="C888" s="72"/>
+      <c r="B888" s="69"/>
+      <c r="C888" s="70"/>
       <c r="D888" s="6"/>
       <c r="E888" s="29"/>
       <c r="F888" s="24"/>
@@ -33571,8 +33580,8 @@
     </row>
     <row r="1002" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1002" s="29"/>
-      <c r="B1002" s="71"/>
-      <c r="C1002" s="72"/>
+      <c r="B1002" s="69"/>
+      <c r="C1002" s="70"/>
       <c r="D1002" s="6"/>
       <c r="E1002" s="29"/>
       <c r="F1002" s="24"/>
@@ -33585,10 +33594,10 @@
     </row>
     <row r="1003" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1003" s="29"/>
-      <c r="B1003" s="69" t="s">
+      <c r="B1003" s="73" t="s">
         <v>1923</v>
       </c>
-      <c r="C1003" s="70"/>
+      <c r="C1003" s="74"/>
       <c r="D1003" s="6"/>
       <c r="E1003" s="29"/>
       <c r="F1003" s="24"/>
@@ -33601,8 +33610,8 @@
     </row>
     <row r="1004" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1004" s="29"/>
-      <c r="B1004" s="71"/>
-      <c r="C1004" s="72"/>
+      <c r="B1004" s="69"/>
+      <c r="C1004" s="70"/>
       <c r="D1004" s="6"/>
       <c r="E1004" s="29"/>
       <c r="F1004" s="24"/>
@@ -33736,8 +33745,8 @@
     </row>
     <row r="1010" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1010" s="29"/>
-      <c r="B1010" s="71"/>
-      <c r="C1010" s="72"/>
+      <c r="B1010" s="69"/>
+      <c r="C1010" s="70"/>
       <c r="D1010" s="6"/>
       <c r="E1010" s="29"/>
       <c r="F1010" s="24"/>
@@ -33750,10 +33759,10 @@
     </row>
     <row r="1011" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1011" s="29"/>
-      <c r="B1011" s="69" t="s">
+      <c r="B1011" s="73" t="s">
         <v>1826</v>
       </c>
-      <c r="C1011" s="70"/>
+      <c r="C1011" s="74"/>
       <c r="D1011" s="6"/>
       <c r="E1011" s="29"/>
       <c r="F1011" s="24"/>
@@ -33766,8 +33775,8 @@
     </row>
     <row r="1012" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1012" s="29"/>
-      <c r="B1012" s="71"/>
-      <c r="C1012" s="72"/>
+      <c r="B1012" s="69"/>
+      <c r="C1012" s="70"/>
       <c r="D1012" s="6"/>
       <c r="E1012" s="29"/>
       <c r="F1012" s="24"/>
@@ -34290,8 +34299,8 @@
     </row>
     <row r="1036" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1036" s="29"/>
-      <c r="B1036" s="71"/>
-      <c r="C1036" s="72"/>
+      <c r="B1036" s="69"/>
+      <c r="C1036" s="70"/>
       <c r="D1036" s="6"/>
       <c r="E1036" s="29"/>
       <c r="F1036" s="24"/>
@@ -34304,10 +34313,10 @@
     </row>
     <row r="1037" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1037" s="29"/>
-      <c r="B1037" s="69" t="s">
+      <c r="B1037" s="73" t="s">
         <v>1827</v>
       </c>
-      <c r="C1037" s="70"/>
+      <c r="C1037" s="74"/>
       <c r="D1037" s="6"/>
       <c r="E1037" s="29"/>
       <c r="F1037" s="24"/>
@@ -34320,8 +34329,8 @@
     </row>
     <row r="1038" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1038" s="29"/>
-      <c r="B1038" s="71"/>
-      <c r="C1038" s="72"/>
+      <c r="B1038" s="69"/>
+      <c r="C1038" s="70"/>
       <c r="D1038" s="6"/>
       <c r="E1038" s="29"/>
       <c r="F1038" s="24"/>
@@ -37384,8 +37393,8 @@
     </row>
     <row r="1157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1157" s="29"/>
-      <c r="B1157" s="71"/>
-      <c r="C1157" s="72"/>
+      <c r="B1157" s="69"/>
+      <c r="C1157" s="70"/>
       <c r="D1157" s="6"/>
       <c r="E1157" s="29"/>
       <c r="F1157" s="24"/>
@@ -37398,10 +37407,10 @@
     </row>
     <row r="1158" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1158" s="29"/>
-      <c r="B1158" s="69" t="s">
+      <c r="B1158" s="73" t="s">
         <v>1828</v>
       </c>
-      <c r="C1158" s="70"/>
+      <c r="C1158" s="74"/>
       <c r="D1158" s="6"/>
       <c r="E1158" s="29"/>
       <c r="F1158" s="24"/>
@@ -37414,8 +37423,8 @@
     </row>
     <row r="1159" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1159" s="29"/>
-      <c r="B1159" s="71"/>
-      <c r="C1159" s="72"/>
+      <c r="B1159" s="69"/>
+      <c r="C1159" s="70"/>
       <c r="D1159" s="6"/>
       <c r="E1159" s="29"/>
       <c r="F1159" s="24"/>
@@ -37470,8 +37479,8 @@
     </row>
     <row r="1162" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1162" s="29"/>
-      <c r="B1162" s="71"/>
-      <c r="C1162" s="72"/>
+      <c r="B1162" s="69"/>
+      <c r="C1162" s="70"/>
       <c r="D1162" s="6"/>
       <c r="E1162" s="29"/>
       <c r="F1162" s="24"/>
@@ -37484,10 +37493,10 @@
     </row>
     <row r="1163" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1163" s="29"/>
-      <c r="B1163" s="69" t="s">
+      <c r="B1163" s="73" t="s">
         <v>1829</v>
       </c>
-      <c r="C1163" s="70"/>
+      <c r="C1163" s="74"/>
       <c r="D1163" s="6"/>
       <c r="E1163" s="29"/>
       <c r="F1163" s="24"/>
@@ -37500,8 +37509,8 @@
     </row>
     <row r="1164" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1164" s="29"/>
-      <c r="B1164" s="71"/>
-      <c r="C1164" s="72"/>
+      <c r="B1164" s="69"/>
+      <c r="C1164" s="70"/>
       <c r="D1164" s="6"/>
       <c r="E1164" s="29"/>
       <c r="F1164" s="24"/>
@@ -40408,37 +40417,45 @@
     </row>
     <row r="1289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1289" s="29"/>
-      <c r="B1289" s="57"/>
-      <c r="C1289" s="54"/>
-      <c r="D1289" s="3"/>
+      <c r="B1289" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1289" s="54" t="s">
+        <v>2239</v>
+      </c>
+      <c r="D1289" s="3" t="s">
+        <v>2240</v>
+      </c>
       <c r="E1289" s="29"/>
-      <c r="F1289" s="23"/>
-      <c r="G1289" s="44"/>
+      <c r="F1289" s="23">
+        <v>44732</v>
+      </c>
+      <c r="G1289" s="44" t="s">
+        <v>2241</v>
+      </c>
       <c r="H1289" s="29"/>
       <c r="I1289" s="23"/>
       <c r="J1289" s="13"/>
       <c r="K1289" s="14"/>
       <c r="L1289" s="29"/>
     </row>
-    <row r="1290" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1290" s="29"/>
-      <c r="B1290" s="71"/>
-      <c r="C1290" s="72"/>
-      <c r="D1290" s="6"/>
+      <c r="B1290" s="57"/>
+      <c r="C1290" s="54"/>
+      <c r="D1290" s="3"/>
       <c r="E1290" s="29"/>
-      <c r="F1290" s="24"/>
-      <c r="G1290" s="45"/>
+      <c r="F1290" s="23"/>
+      <c r="G1290" s="44"/>
       <c r="H1290" s="29"/>
-      <c r="I1290" s="24"/>
-      <c r="J1290" s="15"/>
-      <c r="K1290" s="16"/>
+      <c r="I1290" s="23"/>
+      <c r="J1290" s="13"/>
+      <c r="K1290" s="14"/>
       <c r="L1290" s="29"/>
     </row>
-    <row r="1291" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1291" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1291" s="29"/>
-      <c r="B1291" s="69" t="s">
-        <v>2004</v>
-      </c>
+      <c r="B1291" s="69"/>
       <c r="C1291" s="70"/>
       <c r="D1291" s="6"/>
       <c r="E1291" s="29"/>
@@ -40450,10 +40467,12 @@
       <c r="K1291" s="16"/>
       <c r="L1291" s="29"/>
     </row>
-    <row r="1292" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1292" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1292" s="29"/>
-      <c r="B1292" s="71"/>
-      <c r="C1292" s="72"/>
+      <c r="B1292" s="73" t="s">
+        <v>2004</v>
+      </c>
+      <c r="C1292" s="74"/>
       <c r="D1292" s="6"/>
       <c r="E1292" s="29"/>
       <c r="F1292" s="24"/>
@@ -40464,28 +40483,18 @@
       <c r="K1292" s="16"/>
       <c r="L1292" s="29"/>
     </row>
-    <row r="1293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1293" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1293" s="29"/>
-      <c r="B1293" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1293" s="54" t="s">
-        <v>1998</v>
-      </c>
-      <c r="D1293" s="3" t="s">
-        <v>2002</v>
-      </c>
+      <c r="B1293" s="69"/>
+      <c r="C1293" s="70"/>
+      <c r="D1293" s="6"/>
       <c r="E1293" s="29"/>
-      <c r="F1293" s="23">
-        <v>44971</v>
-      </c>
-      <c r="G1293" s="44" t="s">
-        <v>588</v>
-      </c>
+      <c r="F1293" s="24"/>
+      <c r="G1293" s="45"/>
       <c r="H1293" s="29"/>
-      <c r="I1293" s="23"/>
-      <c r="J1293" s="13"/>
-      <c r="K1293" s="14"/>
+      <c r="I1293" s="24"/>
+      <c r="J1293" s="15"/>
+      <c r="K1293" s="16"/>
       <c r="L1293" s="29"/>
     </row>
     <row r="1294" spans="1:12" x14ac:dyDescent="0.25">
@@ -40494,10 +40503,10 @@
         <v>2014</v>
       </c>
       <c r="C1294" s="54" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="D1294" s="3" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="E1294" s="29"/>
       <c r="F1294" s="23">
@@ -40518,14 +40527,14 @@
         <v>2014</v>
       </c>
       <c r="C1295" s="54" t="s">
-        <v>2041</v>
+        <v>1999</v>
       </c>
       <c r="D1295" s="3" t="s">
-        <v>2042</v>
+        <v>2001</v>
       </c>
       <c r="E1295" s="29"/>
       <c r="F1295" s="23">
-        <v>45001</v>
+        <v>44971</v>
       </c>
       <c r="G1295" s="44" t="s">
         <v>588</v>
@@ -40542,14 +40551,14 @@
         <v>2014</v>
       </c>
       <c r="C1296" s="54" t="s">
-        <v>2007</v>
+        <v>2041</v>
       </c>
       <c r="D1296" s="3" t="s">
-        <v>2008</v>
+        <v>2042</v>
       </c>
       <c r="E1296" s="29"/>
       <c r="F1296" s="23">
-        <v>44971</v>
+        <v>45001</v>
       </c>
       <c r="G1296" s="44" t="s">
         <v>588</v>
@@ -40566,14 +40575,14 @@
         <v>2014</v>
       </c>
       <c r="C1297" s="54" t="s">
-        <v>2031</v>
+        <v>2007</v>
       </c>
       <c r="D1297" s="3" t="s">
-        <v>2038</v>
+        <v>2008</v>
       </c>
       <c r="E1297" s="29"/>
       <c r="F1297" s="23">
-        <v>44992</v>
+        <v>44971</v>
       </c>
       <c r="G1297" s="44" t="s">
         <v>588</v>
@@ -40590,10 +40599,10 @@
         <v>2014</v>
       </c>
       <c r="C1298" s="54" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="D1298" s="3" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="E1298" s="29"/>
       <c r="F1298" s="23">
@@ -40614,10 +40623,10 @@
         <v>2014</v>
       </c>
       <c r="C1299" s="54" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D1299" s="3" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="E1299" s="29"/>
       <c r="F1299" s="23">
@@ -40638,10 +40647,10 @@
         <v>2014</v>
       </c>
       <c r="C1300" s="54" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="D1300" s="3" t="s">
-        <v>2036</v>
+        <v>2040</v>
       </c>
       <c r="E1300" s="29"/>
       <c r="F1300" s="23">
@@ -40662,10 +40671,10 @@
         <v>2014</v>
       </c>
       <c r="C1301" s="54" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D1301" s="3" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="E1301" s="29"/>
       <c r="F1301" s="23">
@@ -40680,61 +40689,61 @@
       <c r="K1301" s="14"/>
       <c r="L1301" s="29"/>
     </row>
-    <row r="1302" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1302" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1302" s="29"/>
-      <c r="B1302" s="59"/>
-      <c r="C1302" s="64"/>
-      <c r="D1302" s="7"/>
+      <c r="B1302" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1302" s="54" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D1302" s="3" t="s">
+        <v>2037</v>
+      </c>
       <c r="E1302" s="29"/>
-      <c r="F1302" s="26"/>
-      <c r="G1302" s="46"/>
+      <c r="F1302" s="23">
+        <v>44992</v>
+      </c>
+      <c r="G1302" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1302" s="29"/>
-      <c r="I1302" s="26"/>
-      <c r="J1302" s="17"/>
-      <c r="K1302" s="18"/>
+      <c r="I1302" s="23"/>
+      <c r="J1302" s="13"/>
+      <c r="K1302" s="14"/>
       <c r="L1302" s="29"/>
     </row>
-    <row r="1303" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1303" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1303" s="29"/>
-      <c r="B1303" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1303" s="54" t="s">
-        <v>2000</v>
-      </c>
-      <c r="D1303" s="3" t="s">
-        <v>2003</v>
-      </c>
+      <c r="B1303" s="59"/>
+      <c r="C1303" s="64"/>
+      <c r="D1303" s="7"/>
       <c r="E1303" s="29"/>
-      <c r="F1303" s="23">
-        <v>44987</v>
-      </c>
-      <c r="G1303" s="44" t="s">
-        <v>2013</v>
-      </c>
+      <c r="F1303" s="26"/>
+      <c r="G1303" s="46"/>
       <c r="H1303" s="29"/>
-      <c r="I1303" s="23"/>
-      <c r="J1303" s="13"/>
-      <c r="K1303" s="14"/>
+      <c r="I1303" s="26"/>
+      <c r="J1303" s="17"/>
+      <c r="K1303" s="18"/>
       <c r="L1303" s="29"/>
     </row>
-    <row r="1304" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1304" s="29"/>
       <c r="B1304" s="56" t="s">
         <v>2014</v>
       </c>
       <c r="C1304" s="54" t="s">
-        <v>2029</v>
+        <v>2000</v>
       </c>
       <c r="D1304" s="3" t="s">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="E1304" s="29"/>
       <c r="F1304" s="23">
         <v>44987</v>
       </c>
       <c r="G1304" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1304" s="29"/>
       <c r="I1304" s="23"/>
@@ -40748,17 +40757,17 @@
         <v>2014</v>
       </c>
       <c r="C1305" s="54" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D1305" s="3" t="s">
-        <v>2005</v>
+        <v>2012</v>
       </c>
       <c r="E1305" s="29"/>
       <c r="F1305" s="23">
         <v>44987</v>
       </c>
       <c r="G1305" s="44" t="s">
-        <v>2013</v>
+        <v>588</v>
       </c>
       <c r="H1305" s="29"/>
       <c r="I1305" s="23"/>
@@ -40772,17 +40781,17 @@
         <v>2014</v>
       </c>
       <c r="C1306" s="54" t="s">
-        <v>2015</v>
+        <v>2030</v>
       </c>
       <c r="D1306" s="3" t="s">
-        <v>2028</v>
+        <v>2005</v>
       </c>
       <c r="E1306" s="29"/>
       <c r="F1306" s="23">
         <v>44987</v>
       </c>
       <c r="G1306" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1306" s="29"/>
       <c r="I1306" s="23"/>
@@ -40790,20 +40799,20 @@
       <c r="K1306" s="14"/>
       <c r="L1306" s="29"/>
     </row>
-    <row r="1307" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1307" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1307" s="29"/>
       <c r="B1307" s="56" t="s">
         <v>2014</v>
       </c>
       <c r="C1307" s="54" t="s">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="D1307" s="3" t="s">
-        <v>2009</v>
+        <v>2028</v>
       </c>
       <c r="E1307" s="29"/>
       <c r="F1307" s="23">
-        <v>44972</v>
+        <v>44987</v>
       </c>
       <c r="G1307" s="44" t="s">
         <v>588</v>
@@ -40814,42 +40823,42 @@
       <c r="K1307" s="14"/>
       <c r="L1307" s="29"/>
     </row>
-    <row r="1308" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1308" s="29"/>
-      <c r="B1308" s="59"/>
-      <c r="C1308" s="64"/>
-      <c r="D1308" s="7"/>
+      <c r="B1308" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1308" s="54" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D1308" s="3" t="s">
+        <v>2009</v>
+      </c>
       <c r="E1308" s="29"/>
-      <c r="F1308" s="26"/>
-      <c r="G1308" s="46"/>
+      <c r="F1308" s="23">
+        <v>44972</v>
+      </c>
+      <c r="G1308" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1308" s="29"/>
-      <c r="I1308" s="26"/>
-      <c r="J1308" s="17"/>
-      <c r="K1308" s="18"/>
+      <c r="I1308" s="23"/>
+      <c r="J1308" s="13"/>
+      <c r="K1308" s="14"/>
       <c r="L1308" s="29"/>
     </row>
-    <row r="1309" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1309" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1309" s="29"/>
-      <c r="B1309" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1309" s="54" t="s">
-        <v>2044</v>
-      </c>
-      <c r="D1309" s="3" t="s">
-        <v>2046</v>
-      </c>
+      <c r="B1309" s="59"/>
+      <c r="C1309" s="64"/>
+      <c r="D1309" s="7"/>
       <c r="E1309" s="29"/>
-      <c r="F1309" s="23">
-        <v>45002</v>
-      </c>
-      <c r="G1309" s="44" t="s">
-        <v>588</v>
-      </c>
+      <c r="F1309" s="26"/>
+      <c r="G1309" s="46"/>
       <c r="H1309" s="29"/>
-      <c r="I1309" s="23"/>
-      <c r="J1309" s="13"/>
-      <c r="K1309" s="14"/>
+      <c r="I1309" s="26"/>
+      <c r="J1309" s="17"/>
+      <c r="K1309" s="18"/>
       <c r="L1309" s="29"/>
     </row>
     <row r="1310" spans="1:12" x14ac:dyDescent="0.25">
@@ -40858,10 +40867,10 @@
         <v>2014</v>
       </c>
       <c r="C1310" s="54" t="s">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="D1310" s="3" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="E1310" s="29"/>
       <c r="F1310" s="23">
@@ -40882,14 +40891,14 @@
         <v>2014</v>
       </c>
       <c r="C1311" s="54" t="s">
-        <v>2047</v>
+        <v>2043</v>
       </c>
       <c r="D1311" s="3" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
       <c r="E1311" s="29"/>
       <c r="F1311" s="23">
-        <v>45005</v>
+        <v>45002</v>
       </c>
       <c r="G1311" s="44" t="s">
         <v>588</v>
@@ -40900,83 +40909,120 @@
       <c r="K1311" s="14"/>
       <c r="L1311" s="29"/>
     </row>
-    <row r="1312" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1312" s="29"/>
-      <c r="B1312" s="60"/>
-      <c r="C1312" s="67"/>
-      <c r="D1312" s="5"/>
+      <c r="B1312" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1312" s="54" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D1312" s="3" t="s">
+        <v>2048</v>
+      </c>
       <c r="E1312" s="29"/>
-      <c r="F1312" s="27"/>
-      <c r="G1312" s="47"/>
+      <c r="F1312" s="23">
+        <v>45005</v>
+      </c>
+      <c r="G1312" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1312" s="29"/>
-      <c r="I1312" s="27"/>
-      <c r="J1312" s="19"/>
-      <c r="K1312" s="20"/>
+      <c r="I1312" s="23"/>
+      <c r="J1312" s="13"/>
+      <c r="K1312" s="14"/>
       <c r="L1312" s="29"/>
     </row>
-    <row r="1313" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1313" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1313" s="29"/>
-      <c r="B1313" s="55"/>
-      <c r="C1313" s="62"/>
-      <c r="D1313" s="32"/>
+      <c r="B1313" s="60"/>
+      <c r="C1313" s="67"/>
+      <c r="D1313" s="5"/>
       <c r="E1313" s="29"/>
-      <c r="F1313" s="33"/>
-      <c r="G1313" s="41"/>
+      <c r="F1313" s="27"/>
+      <c r="G1313" s="47"/>
       <c r="H1313" s="29"/>
-      <c r="I1313" s="33"/>
-      <c r="J1313" s="34"/>
-      <c r="K1313" s="34"/>
+      <c r="I1313" s="27"/>
+      <c r="J1313" s="19"/>
+      <c r="K1313" s="20"/>
       <c r="L1313" s="29"/>
     </row>
-    <row r="1315" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1315" s="29"/>
-      <c r="B1315" s="55"/>
-      <c r="C1315" s="54" t="s">
+    <row r="1314" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1314" s="29"/>
+      <c r="B1314" s="55"/>
+      <c r="C1314" s="62"/>
+      <c r="D1314" s="32"/>
+      <c r="E1314" s="29"/>
+      <c r="F1314" s="33"/>
+      <c r="G1314" s="41"/>
+      <c r="H1314" s="29"/>
+      <c r="I1314" s="33"/>
+      <c r="J1314" s="34"/>
+      <c r="K1314" s="34"/>
+      <c r="L1314" s="29"/>
+    </row>
+    <row r="1316" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1316" s="29"/>
+      <c r="B1316" s="55"/>
+      <c r="C1316" s="54" t="s">
         <v>362</v>
       </c>
-      <c r="D1315" s="3" t="s">
+      <c r="D1316" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="E1315" s="29"/>
-      <c r="F1315" s="23"/>
-      <c r="G1315" s="44"/>
-      <c r="H1315" s="29"/>
-      <c r="I1315" s="23"/>
-      <c r="J1315" s="13"/>
-      <c r="K1315" s="14"/>
-      <c r="L1315" s="29"/>
+      <c r="E1316" s="29"/>
+      <c r="F1316" s="23"/>
+      <c r="G1316" s="44"/>
+      <c r="H1316" s="29"/>
+      <c r="I1316" s="23"/>
+      <c r="J1316" s="13"/>
+      <c r="K1316" s="14"/>
+      <c r="L1316" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B550:C550"/>
+    <mergeCell ref="B402:C402"/>
+    <mergeCell ref="B264:C264"/>
+    <mergeCell ref="B253:C253"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B265:C265"/>
+    <mergeCell ref="B401:C401"/>
+    <mergeCell ref="B403:C403"/>
+    <mergeCell ref="B546:C546"/>
+    <mergeCell ref="B549:C549"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="B252:C252"/>
+    <mergeCell ref="B254:C254"/>
+    <mergeCell ref="B263:C263"/>
+    <mergeCell ref="B1011:C1011"/>
+    <mergeCell ref="B1003:C1003"/>
+    <mergeCell ref="B887:C887"/>
+    <mergeCell ref="B778:C778"/>
+    <mergeCell ref="B617:C617"/>
+    <mergeCell ref="B888:C888"/>
+    <mergeCell ref="B886:C886"/>
+    <mergeCell ref="B1002:C1002"/>
+    <mergeCell ref="B1004:C1004"/>
+    <mergeCell ref="B1010:C1010"/>
+    <mergeCell ref="B1291:C1291"/>
+    <mergeCell ref="B1293:C1293"/>
+    <mergeCell ref="B1292:C1292"/>
+    <mergeCell ref="B1163:C1163"/>
+    <mergeCell ref="B1158:C1158"/>
+    <mergeCell ref="B1012:C1012"/>
+    <mergeCell ref="B1038:C1038"/>
+    <mergeCell ref="B1036:C1036"/>
+    <mergeCell ref="B1162:C1162"/>
+    <mergeCell ref="B1164:C1164"/>
+    <mergeCell ref="B1157:C1157"/>
+    <mergeCell ref="B1159:C1159"/>
+    <mergeCell ref="B1037:C1037"/>
+    <mergeCell ref="B551:C551"/>
+    <mergeCell ref="B616:C616"/>
+    <mergeCell ref="B618:C618"/>
+    <mergeCell ref="B777:C777"/>
+    <mergeCell ref="B779:C779"/>
     <mergeCell ref="B224:C224"/>
     <mergeCell ref="B152:C152"/>
     <mergeCell ref="B162:C162"/>
@@ -40991,53 +41037,40 @@
     <mergeCell ref="B192:C192"/>
     <mergeCell ref="B193:C193"/>
     <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B551:C551"/>
-    <mergeCell ref="B616:C616"/>
-    <mergeCell ref="B618:C618"/>
-    <mergeCell ref="B777:C777"/>
-    <mergeCell ref="B779:C779"/>
-    <mergeCell ref="B1012:C1012"/>
-    <mergeCell ref="B1038:C1038"/>
-    <mergeCell ref="B1036:C1036"/>
-    <mergeCell ref="B1162:C1162"/>
-    <mergeCell ref="B1164:C1164"/>
-    <mergeCell ref="B1157:C1157"/>
-    <mergeCell ref="B1159:C1159"/>
-    <mergeCell ref="B1037:C1037"/>
-    <mergeCell ref="B1290:C1290"/>
-    <mergeCell ref="B1292:C1292"/>
-    <mergeCell ref="B1291:C1291"/>
-    <mergeCell ref="B1163:C1163"/>
-    <mergeCell ref="B1158:C1158"/>
-    <mergeCell ref="B1011:C1011"/>
-    <mergeCell ref="B1003:C1003"/>
-    <mergeCell ref="B887:C887"/>
-    <mergeCell ref="B778:C778"/>
-    <mergeCell ref="B617:C617"/>
-    <mergeCell ref="B888:C888"/>
-    <mergeCell ref="B886:C886"/>
-    <mergeCell ref="B1002:C1002"/>
-    <mergeCell ref="B1004:C1004"/>
-    <mergeCell ref="B1010:C1010"/>
-    <mergeCell ref="B550:C550"/>
-    <mergeCell ref="B402:C402"/>
-    <mergeCell ref="B264:C264"/>
-    <mergeCell ref="B253:C253"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B265:C265"/>
-    <mergeCell ref="B401:C401"/>
-    <mergeCell ref="B403:C403"/>
-    <mergeCell ref="B546:C546"/>
-    <mergeCell ref="B549:C549"/>
-    <mergeCell ref="B226:C226"/>
-    <mergeCell ref="B252:C252"/>
-    <mergeCell ref="B254:C254"/>
-    <mergeCell ref="B263:C263"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G19:G20 G146:G147 G149 G158:G160 G255:G261 G268:G273 G404:G408 G410:G414 G424:G426 G446 G520:G523 G869:G871 G900:G901 G1015:G1017 G1019 G1021:G1025 G1027:G1030 G1032:G1033 G1047:G1052 G1054:G1056 G1065:G1066 G1076 G1131:G1133 G1039:G1043 G1174:G1175 G367:G370 G1262:G1265 G973:G976 G889:G891 G372:G375 G1267:G1269 G250 G227 G282:G285 G428:G433 G1058:G1063 G903:G908 G221 G195:G196 G893:G898 G416:G422 G1167:G1172 G864:G867 G1013 G924 G1083 G198 G207:G215 G229:G248 G1248:G1258 G1088:G1129 G929:G971 G547 G1149 F1146:G1148 G34:G42 G525:G538 G1286:G1288 G542:G544 G1153:G1155 G998:G1000 G884 G100 G1160 G1136:G1145 G982:G996 G920:G922 G1078:G1081 G978:G980 G190 G926:G927 G1085:G1086 G1215:G1216 G377:G389 G1272:G1278 G600:G604 G772:G777 G1233:G1246 G1218:G1231 G1296:G1307 G1293:G1294 G153:G156 G140 G173 G746:G770 G669:G744 G639:G646 G552:G598 G540 G448:G518 G435:G440 G397:G399 G311:G365 G114:G135 G105:G109 G31:G32 G25:G26 G183:G188 G873:G882 G180:G181 G165:G166 G790:G862 G44:G98 G606:G614 G11:G14 G279 G287:G288 G648:G651 G290 G297:G298 G293 G168 G275:G276 G619:G637 G300:G302 G654:G664 G392:G393" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G19:G20 G146:G147 G149 G158:G160 G255:G261 G268:G273 G404:G408 G410:G414 G424:G426 G446 G520:G523 G869:G871 G900:G901 G1015:G1017 G1019 G1021:G1025 G1027:G1030 G1032:G1033 G1047:G1052 G1054:G1056 G1065:G1066 G1076 G1131:G1133 G1039:G1043 G1174:G1175 G367:G370 G1262:G1265 G973:G976 G889:G891 G372:G375 G1267:G1269 G250 G227 G282:G285 G428:G433 G1058:G1063 G903:G908 G221 G195:G196 G893:G898 G416:G422 G1167:G1172 G864:G867 G1013 G924 G1083 G198 G207:G215 G229:G248 G1248:G1258 G1088:G1129 G929:G971 G547 G1149 F1146:G1148 G34:G42 G525:G538 G1286:G1288 G542:G544 G1153:G1155 G998:G1000 G884 G100 G1160 G1136:G1145 G982:G996 G920:G922 G1078:G1081 G978:G980 G190 G926:G927 G1085:G1086 G1215:G1216 G377:G389 G1272:G1278 G600:G604 G772:G777 G1233:G1246 G1218:G1231 G1297:G1308 G1294:G1295 G153:G156 G140 G173 G746:G770 G669:G744 G639:G646 G552:G598 G540 G448:G518 G435:G440 G397:G399 G311:G365 G114:G135 G105:G109 G31:G32 G25:G26 G183:G188 G873:G882 G180:G181 G165:G166 G790:G862 G44:G98 G606:G614 G11:G14 G279 G287:G288 G648:G651 G290 G297:G298 G293 G168 G275:G276 G619:G637 G300:G302 G654:G664 G392:G393" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -41062,80 +41095,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="88" t="s">
         <v>1253</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="88" t="s">
         <v>1254</v>
       </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="88" t="s">
         <v>1255</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="88" t="s">
         <v>1256</v>
       </c>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="88" t="s">
         <v>1257</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="88" t="s">
         <v>1258</v>
       </c>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="88" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="87" t="s">
         <v>1271</v>
       </c>
-      <c r="I7" s="88"/>
+      <c r="I7" s="87"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="86" t="s">
         <v>1269</v>
       </c>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="I8" s="52" t="s">
         <v>1272</v>
       </c>
@@ -41144,62 +41177,62 @@
       <c r="B9" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="86" t="s">
         <v>1270</v>
       </c>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
       <c r="I9" s="52" t="s">
         <v>1273</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="88" t="s">
         <v>1259</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="88" t="s">
         <v>1260</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="88" t="s">
         <v>1261</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="88" t="s">
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="87" t="s">
         <v>1279</v>
       </c>
-      <c r="I12" s="88"/>
+      <c r="I12" s="87"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
       <c r="I13" s="52" t="s">
         <v>1293</v>
       </c>
@@ -41208,13 +41241,13 @@
       <c r="B14" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="86" t="s">
         <v>1276</v>
       </c>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
       <c r="I14" s="52" t="s">
         <v>1294</v>
       </c>
@@ -41223,13 +41256,13 @@
       <c r="B15" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="86" t="s">
         <v>1280</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
       <c r="I15" s="52" t="s">
         <v>1292</v>
       </c>
@@ -41238,13 +41271,13 @@
       <c r="B16" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C16" s="87" t="s">
+      <c r="C16" s="86" t="s">
         <v>1281</v>
       </c>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
       <c r="I16" s="52" t="s">
         <v>1282</v>
       </c>
@@ -41253,24 +41286,24 @@
       <c r="B17" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C17" s="87" t="s">
+      <c r="C17" s="86" t="s">
         <v>1285</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="86" t="s">
         <v>1286</v>
       </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
       <c r="I18" s="52" t="s">
         <v>1291</v>
       </c>
@@ -41279,12 +41312,12 @@
       <c r="C19" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="86" t="s">
         <v>1287</v>
       </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
       <c r="I19" s="52" t="s">
         <v>1288</v>
       </c>
@@ -41293,13 +41326,13 @@
       <c r="B20" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C20" s="87" t="s">
+      <c r="C20" s="86" t="s">
         <v>1289</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
       <c r="I20" s="52" t="s">
         <v>1297</v>
       </c>
@@ -41308,13 +41341,13 @@
       <c r="B21" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="86" t="s">
         <v>1283</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
       <c r="I21" s="52" t="s">
         <v>1284</v>
       </c>
@@ -41323,13 +41356,13 @@
       <c r="B22" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="86" t="s">
         <v>1278</v>
       </c>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
       <c r="I22" s="52" t="s">
         <v>1290</v>
       </c>
@@ -41338,53 +41371,53 @@
       <c r="B23" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="86" t="s">
         <v>1295</v>
       </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
       <c r="I23" s="52" t="s">
         <v>1296</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="88" t="s">
         <v>1262</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="88" t="s">
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="87" t="s">
         <v>1268</v>
       </c>
-      <c r="I24" s="88"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="86" t="s">
         <v>1267</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="86" t="s">
         <v>1265</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
       <c r="I26" s="52" t="s">
         <v>1274</v>
       </c>
@@ -41393,12 +41426,12 @@
       <c r="C27" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="86" t="s">
         <v>1266</v>
       </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
       <c r="I27" s="52" t="s">
         <v>1275</v>
       </c>
@@ -41407,24 +41440,28 @@
       <c r="D28" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="E28" s="87" t="s">
+      <c r="E28" s="86" t="s">
         <v>1277</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -41440,16 +41477,12 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Pertanggal 25 Januari 2023 16:59 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="2242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4501" uniqueCount="2262">
   <si>
     <t>transaction.update.master.setBloodAglutinogenType</t>
   </si>
@@ -8859,6 +8859,66 @@
   </si>
   <si>
     <t>1.0000.0000002</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setDeliveryOrder</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Pesanan Pengiriman (DO)</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setDeliveryOrderDetail</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Perincian Pesanan Pengiriman</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Pemilihan Pesanan (OP)</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setOrderPicking</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setOrderPickingDetail</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Perincian Pemilihan Pesanan</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setOrderPickingRequisition</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setOrderPickingRequisitionDetail</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Permintaan Pemilihan Pesanan (OPR)</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Perincian Permintaan Pemilihan Pesanan</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setPurchaseOrderAdditionalCost</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Biaya Tambahan Pesanan Pembelian</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setPurchaseOrderPaymentTerm</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setPurchaseOrderPaymentTermDetail</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Termin Pembayaran Pesanan Pembelian</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Perincian Termin Pembayaran Pesanan Pembelian</t>
+  </si>
+  <si>
+    <t>transaction.update.supplyChain.setSupplier</t>
+  </si>
+  <si>
+    <t>Memutakhirkan Data Pemasok</t>
   </si>
 </sst>
 </file>
@@ -9895,13 +9955,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1316"/>
+  <dimension ref="A1:M1326"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D1275" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D1278" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G1289" sqref="G1289"/>
+      <selection pane="bottomRight" activeCell="D1286" sqref="D1286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -40040,7 +40100,7 @@
       </c>
       <c r="E1272" s="29"/>
       <c r="F1272" s="23">
-        <v>44663</v>
+        <v>44621</v>
       </c>
       <c r="G1272" s="44" t="s">
         <v>588</v>
@@ -40057,14 +40117,14 @@
         <v>2014</v>
       </c>
       <c r="C1273" s="54" t="s">
-        <v>1071</v>
+        <v>2242</v>
       </c>
       <c r="D1273" s="3" t="s">
-        <v>1075</v>
+        <v>2243</v>
       </c>
       <c r="E1273" s="29"/>
       <c r="F1273" s="23">
-        <v>44624</v>
+        <v>44630</v>
       </c>
       <c r="G1273" s="44" t="s">
         <v>588</v>
@@ -40081,14 +40141,14 @@
         <v>2014</v>
       </c>
       <c r="C1274" s="54" t="s">
-        <v>1072</v>
+        <v>2244</v>
       </c>
       <c r="D1274" s="3" t="s">
-        <v>1076</v>
+        <v>2245</v>
       </c>
       <c r="E1274" s="29"/>
       <c r="F1274" s="23">
-        <v>44624</v>
+        <v>44630</v>
       </c>
       <c r="G1274" s="44" t="s">
         <v>588</v>
@@ -40105,14 +40165,14 @@
         <v>2014</v>
       </c>
       <c r="C1275" s="54" t="s">
-        <v>1073</v>
+        <v>2247</v>
       </c>
       <c r="D1275" s="3" t="s">
-        <v>1077</v>
+        <v>2246</v>
       </c>
       <c r="E1275" s="29"/>
       <c r="F1275" s="23">
-        <v>44624</v>
+        <v>45302</v>
       </c>
       <c r="G1275" s="44" t="s">
         <v>588</v>
@@ -40129,14 +40189,14 @@
         <v>2014</v>
       </c>
       <c r="C1276" s="54" t="s">
-        <v>1074</v>
+        <v>2248</v>
       </c>
       <c r="D1276" s="3" t="s">
-        <v>1078</v>
+        <v>2249</v>
       </c>
       <c r="E1276" s="29"/>
       <c r="F1276" s="23">
-        <v>44624</v>
+        <v>45301</v>
       </c>
       <c r="G1276" s="44" t="s">
         <v>588</v>
@@ -40153,14 +40213,14 @@
         <v>2014</v>
       </c>
       <c r="C1277" s="54" t="s">
-        <v>1039</v>
+        <v>2250</v>
       </c>
       <c r="D1277" s="3" t="s">
-        <v>1041</v>
+        <v>2252</v>
       </c>
       <c r="E1277" s="29"/>
       <c r="F1277" s="23">
-        <v>44621</v>
+        <v>45302</v>
       </c>
       <c r="G1277" s="44" t="s">
         <v>588</v>
@@ -40177,14 +40237,14 @@
         <v>2014</v>
       </c>
       <c r="C1278" s="54" t="s">
-        <v>1040</v>
+        <v>2251</v>
       </c>
       <c r="D1278" s="3" t="s">
-        <v>1042</v>
+        <v>2253</v>
       </c>
       <c r="E1278" s="29"/>
       <c r="F1278" s="23">
-        <v>44621</v>
+        <v>45293</v>
       </c>
       <c r="G1278" s="44" t="s">
         <v>588</v>
@@ -40195,18 +40255,28 @@
       <c r="K1278" s="14"/>
       <c r="L1278" s="29"/>
     </row>
-    <row r="1279" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1279" s="29"/>
-      <c r="B1279" s="59"/>
-      <c r="C1279" s="64"/>
-      <c r="D1279" s="7"/>
+      <c r="B1279" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1279" s="54" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D1279" s="3" t="s">
+        <v>1075</v>
+      </c>
       <c r="E1279" s="29"/>
-      <c r="F1279" s="26"/>
-      <c r="G1279" s="46"/>
+      <c r="F1279" s="23">
+        <v>44831</v>
+      </c>
+      <c r="G1279" s="44" t="s">
+        <v>2241</v>
+      </c>
       <c r="H1279" s="29"/>
-      <c r="I1279" s="26"/>
-      <c r="J1279" s="17"/>
-      <c r="K1279" s="18"/>
+      <c r="I1279" s="23"/>
+      <c r="J1279" s="13"/>
+      <c r="K1279" s="14"/>
       <c r="L1279" s="29"/>
     </row>
     <row r="1280" spans="1:12" x14ac:dyDescent="0.25">
@@ -40215,14 +40285,14 @@
         <v>2014</v>
       </c>
       <c r="C1280" s="54" t="s">
-        <v>2234</v>
+        <v>2254</v>
       </c>
       <c r="D1280" s="3" t="s">
-        <v>2235</v>
+        <v>2255</v>
       </c>
       <c r="E1280" s="29"/>
       <c r="F1280" s="23">
-        <v>45316</v>
+        <v>44732</v>
       </c>
       <c r="G1280" s="44" t="s">
         <v>588</v>
@@ -40239,14 +40309,14 @@
         <v>2014</v>
       </c>
       <c r="C1281" s="54" t="s">
-        <v>2232</v>
+        <v>1072</v>
       </c>
       <c r="D1281" s="3" t="s">
-        <v>2010</v>
+        <v>1076</v>
       </c>
       <c r="E1281" s="29"/>
       <c r="F1281" s="23">
-        <v>44985</v>
+        <v>44630</v>
       </c>
       <c r="G1281" s="44" t="s">
         <v>588</v>
@@ -40263,17 +40333,17 @@
         <v>2014</v>
       </c>
       <c r="C1282" s="54" t="s">
-        <v>2233</v>
+        <v>2256</v>
       </c>
       <c r="D1282" s="3" t="s">
-        <v>2023</v>
+        <v>2258</v>
       </c>
       <c r="E1282" s="29"/>
       <c r="F1282" s="23">
-        <v>44988</v>
+        <v>44732</v>
       </c>
       <c r="G1282" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1282" s="29"/>
       <c r="I1282" s="23"/>
@@ -40287,17 +40357,17 @@
         <v>2014</v>
       </c>
       <c r="C1283" s="54" t="s">
-        <v>2236</v>
+        <v>2257</v>
       </c>
       <c r="D1283" s="3" t="s">
-        <v>2237</v>
+        <v>2259</v>
       </c>
       <c r="E1283" s="29"/>
       <c r="F1283" s="23">
-        <v>44991</v>
+        <v>45051</v>
       </c>
       <c r="G1283" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1283" s="29"/>
       <c r="I1283" s="23"/>
@@ -40311,17 +40381,17 @@
         <v>2014</v>
       </c>
       <c r="C1284" s="54" t="s">
-        <v>2016</v>
+        <v>1073</v>
       </c>
       <c r="D1284" s="3" t="s">
-        <v>2017</v>
+        <v>1077</v>
       </c>
       <c r="E1284" s="29"/>
       <c r="F1284" s="23">
-        <v>44987</v>
+        <v>44831</v>
       </c>
       <c r="G1284" s="44" t="s">
-        <v>588</v>
+        <v>2241</v>
       </c>
       <c r="H1284" s="29"/>
       <c r="I1284" s="23"/>
@@ -40329,18 +40399,28 @@
       <c r="K1284" s="14"/>
       <c r="L1284" s="29"/>
     </row>
-    <row r="1285" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1285" s="29"/>
-      <c r="B1285" s="59"/>
-      <c r="C1285" s="64"/>
-      <c r="D1285" s="7"/>
+      <c r="B1285" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1285" s="54" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D1285" s="3" t="s">
+        <v>1078</v>
+      </c>
       <c r="E1285" s="29"/>
-      <c r="F1285" s="26"/>
-      <c r="G1285" s="46"/>
+      <c r="F1285" s="23">
+        <v>44644</v>
+      </c>
+      <c r="G1285" s="44" t="s">
+        <v>2013</v>
+      </c>
       <c r="H1285" s="29"/>
-      <c r="I1285" s="26"/>
-      <c r="J1285" s="17"/>
-      <c r="K1285" s="18"/>
+      <c r="I1285" s="23"/>
+      <c r="J1285" s="13"/>
+      <c r="K1285" s="14"/>
       <c r="L1285" s="29"/>
     </row>
     <row r="1286" spans="1:12" x14ac:dyDescent="0.25">
@@ -40349,14 +40429,14 @@
         <v>2014</v>
       </c>
       <c r="C1286" s="54" t="s">
-        <v>1223</v>
+        <v>2260</v>
       </c>
       <c r="D1286" s="3" t="s">
-        <v>1225</v>
+        <v>2261</v>
       </c>
       <c r="E1286" s="29"/>
       <c r="F1286" s="23">
-        <v>44635</v>
+        <v>44627</v>
       </c>
       <c r="G1286" s="44" t="s">
         <v>588</v>
@@ -40373,14 +40453,14 @@
         <v>2014</v>
       </c>
       <c r="C1287" s="54" t="s">
-        <v>1224</v>
+        <v>1039</v>
       </c>
       <c r="D1287" s="3" t="s">
-        <v>1226</v>
+        <v>1041</v>
       </c>
       <c r="E1287" s="29"/>
       <c r="F1287" s="23">
-        <v>44635</v>
+        <v>44621</v>
       </c>
       <c r="G1287" s="44" t="s">
         <v>588</v>
@@ -40397,14 +40477,14 @@
         <v>2014</v>
       </c>
       <c r="C1288" s="54" t="s">
-        <v>1227</v>
+        <v>1040</v>
       </c>
       <c r="D1288" s="3" t="s">
-        <v>1228</v>
+        <v>1042</v>
       </c>
       <c r="E1288" s="29"/>
       <c r="F1288" s="23">
-        <v>44636</v>
+        <v>44621</v>
       </c>
       <c r="G1288" s="44" t="s">
         <v>588</v>
@@ -40415,86 +40495,114 @@
       <c r="K1288" s="14"/>
       <c r="L1288" s="29"/>
     </row>
-    <row r="1289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1289" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1289" s="29"/>
-      <c r="B1289" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1289" s="54" t="s">
-        <v>2239</v>
-      </c>
-      <c r="D1289" s="3" t="s">
-        <v>2240</v>
-      </c>
+      <c r="B1289" s="59"/>
+      <c r="C1289" s="64"/>
+      <c r="D1289" s="7"/>
       <c r="E1289" s="29"/>
-      <c r="F1289" s="23">
-        <v>44732</v>
-      </c>
-      <c r="G1289" s="44" t="s">
-        <v>2241</v>
-      </c>
+      <c r="F1289" s="26"/>
+      <c r="G1289" s="46"/>
       <c r="H1289" s="29"/>
-      <c r="I1289" s="23"/>
-      <c r="J1289" s="13"/>
-      <c r="K1289" s="14"/>
+      <c r="I1289" s="26"/>
+      <c r="J1289" s="17"/>
+      <c r="K1289" s="18"/>
       <c r="L1289" s="29"/>
     </row>
     <row r="1290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1290" s="29"/>
-      <c r="B1290" s="57"/>
-      <c r="C1290" s="54"/>
-      <c r="D1290" s="3"/>
+      <c r="B1290" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1290" s="54" t="s">
+        <v>2234</v>
+      </c>
+      <c r="D1290" s="3" t="s">
+        <v>2235</v>
+      </c>
       <c r="E1290" s="29"/>
-      <c r="F1290" s="23"/>
-      <c r="G1290" s="44"/>
+      <c r="F1290" s="23">
+        <v>45316</v>
+      </c>
+      <c r="G1290" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1290" s="29"/>
       <c r="I1290" s="23"/>
       <c r="J1290" s="13"/>
       <c r="K1290" s="14"/>
       <c r="L1290" s="29"/>
     </row>
-    <row r="1291" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1291" s="29"/>
-      <c r="B1291" s="69"/>
-      <c r="C1291" s="70"/>
-      <c r="D1291" s="6"/>
+      <c r="B1291" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1291" s="54" t="s">
+        <v>2232</v>
+      </c>
+      <c r="D1291" s="3" t="s">
+        <v>2010</v>
+      </c>
       <c r="E1291" s="29"/>
-      <c r="F1291" s="24"/>
-      <c r="G1291" s="45"/>
+      <c r="F1291" s="23">
+        <v>44985</v>
+      </c>
+      <c r="G1291" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1291" s="29"/>
-      <c r="I1291" s="24"/>
-      <c r="J1291" s="15"/>
-      <c r="K1291" s="16"/>
+      <c r="I1291" s="23"/>
+      <c r="J1291" s="13"/>
+      <c r="K1291" s="14"/>
       <c r="L1291" s="29"/>
     </row>
-    <row r="1292" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1292" s="29"/>
-      <c r="B1292" s="73" t="s">
-        <v>2004</v>
-      </c>
-      <c r="C1292" s="74"/>
-      <c r="D1292" s="6"/>
+      <c r="B1292" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1292" s="54" t="s">
+        <v>2233</v>
+      </c>
+      <c r="D1292" s="3" t="s">
+        <v>2023</v>
+      </c>
       <c r="E1292" s="29"/>
-      <c r="F1292" s="24"/>
-      <c r="G1292" s="45"/>
+      <c r="F1292" s="23">
+        <v>44988</v>
+      </c>
+      <c r="G1292" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1292" s="29"/>
-      <c r="I1292" s="24"/>
-      <c r="J1292" s="15"/>
-      <c r="K1292" s="16"/>
+      <c r="I1292" s="23"/>
+      <c r="J1292" s="13"/>
+      <c r="K1292" s="14"/>
       <c r="L1292" s="29"/>
     </row>
-    <row r="1293" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1293" s="29"/>
-      <c r="B1293" s="69"/>
-      <c r="C1293" s="70"/>
-      <c r="D1293" s="6"/>
+      <c r="B1293" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1293" s="54" t="s">
+        <v>2236</v>
+      </c>
+      <c r="D1293" s="3" t="s">
+        <v>2237</v>
+      </c>
       <c r="E1293" s="29"/>
-      <c r="F1293" s="24"/>
-      <c r="G1293" s="45"/>
+      <c r="F1293" s="23">
+        <v>44991</v>
+      </c>
+      <c r="G1293" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1293" s="29"/>
-      <c r="I1293" s="24"/>
-      <c r="J1293" s="15"/>
-      <c r="K1293" s="16"/>
+      <c r="I1293" s="23"/>
+      <c r="J1293" s="13"/>
+      <c r="K1293" s="14"/>
       <c r="L1293" s="29"/>
     </row>
     <row r="1294" spans="1:12" x14ac:dyDescent="0.25">
@@ -40503,14 +40611,14 @@
         <v>2014</v>
       </c>
       <c r="C1294" s="54" t="s">
-        <v>1998</v>
+        <v>2016</v>
       </c>
       <c r="D1294" s="3" t="s">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="E1294" s="29"/>
       <c r="F1294" s="23">
-        <v>44971</v>
+        <v>44987</v>
       </c>
       <c r="G1294" s="44" t="s">
         <v>588</v>
@@ -40521,28 +40629,18 @@
       <c r="K1294" s="14"/>
       <c r="L1294" s="29"/>
     </row>
-    <row r="1295" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1295" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1295" s="29"/>
-      <c r="B1295" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1295" s="54" t="s">
-        <v>1999</v>
-      </c>
-      <c r="D1295" s="3" t="s">
-        <v>2001</v>
-      </c>
+      <c r="B1295" s="59"/>
+      <c r="C1295" s="64"/>
+      <c r="D1295" s="7"/>
       <c r="E1295" s="29"/>
-      <c r="F1295" s="23">
-        <v>44971</v>
-      </c>
-      <c r="G1295" s="44" t="s">
-        <v>588</v>
-      </c>
+      <c r="F1295" s="26"/>
+      <c r="G1295" s="46"/>
       <c r="H1295" s="29"/>
-      <c r="I1295" s="23"/>
-      <c r="J1295" s="13"/>
-      <c r="K1295" s="14"/>
+      <c r="I1295" s="26"/>
+      <c r="J1295" s="17"/>
+      <c r="K1295" s="18"/>
       <c r="L1295" s="29"/>
     </row>
     <row r="1296" spans="1:12" x14ac:dyDescent="0.25">
@@ -40551,14 +40649,14 @@
         <v>2014</v>
       </c>
       <c r="C1296" s="54" t="s">
-        <v>2041</v>
+        <v>1223</v>
       </c>
       <c r="D1296" s="3" t="s">
-        <v>2042</v>
+        <v>1225</v>
       </c>
       <c r="E1296" s="29"/>
       <c r="F1296" s="23">
-        <v>45001</v>
+        <v>44635</v>
       </c>
       <c r="G1296" s="44" t="s">
         <v>588</v>
@@ -40575,14 +40673,14 @@
         <v>2014</v>
       </c>
       <c r="C1297" s="54" t="s">
-        <v>2007</v>
+        <v>1224</v>
       </c>
       <c r="D1297" s="3" t="s">
-        <v>2008</v>
+        <v>1226</v>
       </c>
       <c r="E1297" s="29"/>
       <c r="F1297" s="23">
-        <v>44971</v>
+        <v>44635</v>
       </c>
       <c r="G1297" s="44" t="s">
         <v>588</v>
@@ -40599,14 +40697,14 @@
         <v>2014</v>
       </c>
       <c r="C1298" s="54" t="s">
-        <v>2031</v>
+        <v>1227</v>
       </c>
       <c r="D1298" s="3" t="s">
-        <v>2038</v>
+        <v>1228</v>
       </c>
       <c r="E1298" s="29"/>
       <c r="F1298" s="23">
-        <v>44992</v>
+        <v>44636</v>
       </c>
       <c r="G1298" s="44" t="s">
         <v>588</v>
@@ -40623,17 +40721,17 @@
         <v>2014</v>
       </c>
       <c r="C1299" s="54" t="s">
-        <v>2032</v>
+        <v>2239</v>
       </c>
       <c r="D1299" s="3" t="s">
-        <v>2039</v>
+        <v>2240</v>
       </c>
       <c r="E1299" s="29"/>
       <c r="F1299" s="23">
-        <v>44992</v>
+        <v>44732</v>
       </c>
       <c r="G1299" s="44" t="s">
-        <v>588</v>
+        <v>2241</v>
       </c>
       <c r="H1299" s="29"/>
       <c r="I1299" s="23"/>
@@ -40643,88 +40741,60 @@
     </row>
     <row r="1300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1300" s="29"/>
-      <c r="B1300" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1300" s="54" t="s">
-        <v>2033</v>
-      </c>
-      <c r="D1300" s="3" t="s">
-        <v>2040</v>
-      </c>
+      <c r="B1300" s="57"/>
+      <c r="C1300" s="54"/>
+      <c r="D1300" s="3"/>
       <c r="E1300" s="29"/>
-      <c r="F1300" s="23">
-        <v>44992</v>
-      </c>
-      <c r="G1300" s="44" t="s">
-        <v>588</v>
-      </c>
+      <c r="F1300" s="23"/>
+      <c r="G1300" s="44"/>
       <c r="H1300" s="29"/>
       <c r="I1300" s="23"/>
       <c r="J1300" s="13"/>
       <c r="K1300" s="14"/>
       <c r="L1300" s="29"/>
     </row>
-    <row r="1301" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1301" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1301" s="29"/>
-      <c r="B1301" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1301" s="54" t="s">
-        <v>2034</v>
-      </c>
-      <c r="D1301" s="3" t="s">
-        <v>2036</v>
-      </c>
+      <c r="B1301" s="69"/>
+      <c r="C1301" s="70"/>
+      <c r="D1301" s="6"/>
       <c r="E1301" s="29"/>
-      <c r="F1301" s="23">
-        <v>44992</v>
-      </c>
-      <c r="G1301" s="44" t="s">
-        <v>588</v>
-      </c>
+      <c r="F1301" s="24"/>
+      <c r="G1301" s="45"/>
       <c r="H1301" s="29"/>
-      <c r="I1301" s="23"/>
-      <c r="J1301" s="13"/>
-      <c r="K1301" s="14"/>
+      <c r="I1301" s="24"/>
+      <c r="J1301" s="15"/>
+      <c r="K1301" s="16"/>
       <c r="L1301" s="29"/>
     </row>
-    <row r="1302" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1302" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1302" s="29"/>
-      <c r="B1302" s="56" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C1302" s="54" t="s">
-        <v>2035</v>
-      </c>
-      <c r="D1302" s="3" t="s">
-        <v>2037</v>
-      </c>
+      <c r="B1302" s="73" t="s">
+        <v>2004</v>
+      </c>
+      <c r="C1302" s="74"/>
+      <c r="D1302" s="6"/>
       <c r="E1302" s="29"/>
-      <c r="F1302" s="23">
-        <v>44992</v>
-      </c>
-      <c r="G1302" s="44" t="s">
-        <v>588</v>
-      </c>
+      <c r="F1302" s="24"/>
+      <c r="G1302" s="45"/>
       <c r="H1302" s="29"/>
-      <c r="I1302" s="23"/>
-      <c r="J1302" s="13"/>
-      <c r="K1302" s="14"/>
+      <c r="I1302" s="24"/>
+      <c r="J1302" s="15"/>
+      <c r="K1302" s="16"/>
       <c r="L1302" s="29"/>
     </row>
-    <row r="1303" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1303" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1303" s="29"/>
-      <c r="B1303" s="59"/>
-      <c r="C1303" s="64"/>
-      <c r="D1303" s="7"/>
+      <c r="B1303" s="69"/>
+      <c r="C1303" s="70"/>
+      <c r="D1303" s="6"/>
       <c r="E1303" s="29"/>
-      <c r="F1303" s="26"/>
-      <c r="G1303" s="46"/>
+      <c r="F1303" s="24"/>
+      <c r="G1303" s="45"/>
       <c r="H1303" s="29"/>
-      <c r="I1303" s="26"/>
-      <c r="J1303" s="17"/>
-      <c r="K1303" s="18"/>
+      <c r="I1303" s="24"/>
+      <c r="J1303" s="15"/>
+      <c r="K1303" s="16"/>
       <c r="L1303" s="29"/>
     </row>
     <row r="1304" spans="1:12" x14ac:dyDescent="0.25">
@@ -40733,17 +40803,17 @@
         <v>2014</v>
       </c>
       <c r="C1304" s="54" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="D1304" s="3" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="E1304" s="29"/>
       <c r="F1304" s="23">
-        <v>44987</v>
+        <v>44971</v>
       </c>
       <c r="G1304" s="44" t="s">
-        <v>2013</v>
+        <v>588</v>
       </c>
       <c r="H1304" s="29"/>
       <c r="I1304" s="23"/>
@@ -40751,20 +40821,20 @@
       <c r="K1304" s="14"/>
       <c r="L1304" s="29"/>
     </row>
-    <row r="1305" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1305" s="29"/>
       <c r="B1305" s="56" t="s">
         <v>2014</v>
       </c>
       <c r="C1305" s="54" t="s">
-        <v>2029</v>
+        <v>1999</v>
       </c>
       <c r="D1305" s="3" t="s">
-        <v>2012</v>
+        <v>2001</v>
       </c>
       <c r="E1305" s="29"/>
       <c r="F1305" s="23">
-        <v>44987</v>
+        <v>44971</v>
       </c>
       <c r="G1305" s="44" t="s">
         <v>588</v>
@@ -40775,23 +40845,23 @@
       <c r="K1305" s="14"/>
       <c r="L1305" s="29"/>
     </row>
-    <row r="1306" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1306" s="29"/>
       <c r="B1306" s="56" t="s">
         <v>2014</v>
       </c>
       <c r="C1306" s="54" t="s">
-        <v>2030</v>
+        <v>2041</v>
       </c>
       <c r="D1306" s="3" t="s">
-        <v>2005</v>
+        <v>2042</v>
       </c>
       <c r="E1306" s="29"/>
       <c r="F1306" s="23">
-        <v>44987</v>
+        <v>45001</v>
       </c>
       <c r="G1306" s="44" t="s">
-        <v>2013</v>
+        <v>588</v>
       </c>
       <c r="H1306" s="29"/>
       <c r="I1306" s="23"/>
@@ -40799,20 +40869,20 @@
       <c r="K1306" s="14"/>
       <c r="L1306" s="29"/>
     </row>
-    <row r="1307" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1307" s="29"/>
       <c r="B1307" s="56" t="s">
         <v>2014</v>
       </c>
       <c r="C1307" s="54" t="s">
-        <v>2015</v>
+        <v>2007</v>
       </c>
       <c r="D1307" s="3" t="s">
-        <v>2028</v>
+        <v>2008</v>
       </c>
       <c r="E1307" s="29"/>
       <c r="F1307" s="23">
-        <v>44987</v>
+        <v>44971</v>
       </c>
       <c r="G1307" s="44" t="s">
         <v>588</v>
@@ -40829,14 +40899,14 @@
         <v>2014</v>
       </c>
       <c r="C1308" s="54" t="s">
-        <v>2006</v>
+        <v>2031</v>
       </c>
       <c r="D1308" s="3" t="s">
-        <v>2009</v>
+        <v>2038</v>
       </c>
       <c r="E1308" s="29"/>
       <c r="F1308" s="23">
-        <v>44972</v>
+        <v>44992</v>
       </c>
       <c r="G1308" s="44" t="s">
         <v>588</v>
@@ -40847,18 +40917,28 @@
       <c r="K1308" s="14"/>
       <c r="L1308" s="29"/>
     </row>
-    <row r="1309" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1309" s="29"/>
-      <c r="B1309" s="59"/>
-      <c r="C1309" s="64"/>
-      <c r="D1309" s="7"/>
+      <c r="B1309" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1309" s="54" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D1309" s="3" t="s">
+        <v>2039</v>
+      </c>
       <c r="E1309" s="29"/>
-      <c r="F1309" s="26"/>
-      <c r="G1309" s="46"/>
+      <c r="F1309" s="23">
+        <v>44992</v>
+      </c>
+      <c r="G1309" s="44" t="s">
+        <v>588</v>
+      </c>
       <c r="H1309" s="29"/>
-      <c r="I1309" s="26"/>
-      <c r="J1309" s="17"/>
-      <c r="K1309" s="18"/>
+      <c r="I1309" s="23"/>
+      <c r="J1309" s="13"/>
+      <c r="K1309" s="14"/>
       <c r="L1309" s="29"/>
     </row>
     <row r="1310" spans="1:12" x14ac:dyDescent="0.25">
@@ -40867,14 +40947,14 @@
         <v>2014</v>
       </c>
       <c r="C1310" s="54" t="s">
-        <v>2044</v>
+        <v>2033</v>
       </c>
       <c r="D1310" s="3" t="s">
-        <v>2046</v>
+        <v>2040</v>
       </c>
       <c r="E1310" s="29"/>
       <c r="F1310" s="23">
-        <v>45002</v>
+        <v>44992</v>
       </c>
       <c r="G1310" s="44" t="s">
         <v>588</v>
@@ -40891,14 +40971,14 @@
         <v>2014</v>
       </c>
       <c r="C1311" s="54" t="s">
-        <v>2043</v>
+        <v>2034</v>
       </c>
       <c r="D1311" s="3" t="s">
-        <v>2045</v>
+        <v>2036</v>
       </c>
       <c r="E1311" s="29"/>
       <c r="F1311" s="23">
-        <v>45002</v>
+        <v>44992</v>
       </c>
       <c r="G1311" s="44" t="s">
         <v>588</v>
@@ -40915,14 +40995,14 @@
         <v>2014</v>
       </c>
       <c r="C1312" s="54" t="s">
-        <v>2047</v>
+        <v>2035</v>
       </c>
       <c r="D1312" s="3" t="s">
-        <v>2048</v>
+        <v>2037</v>
       </c>
       <c r="E1312" s="29"/>
       <c r="F1312" s="23">
-        <v>45005</v>
+        <v>44992</v>
       </c>
       <c r="G1312" s="44" t="s">
         <v>588</v>
@@ -40933,51 +41013,271 @@
       <c r="K1312" s="14"/>
       <c r="L1312" s="29"/>
     </row>
-    <row r="1313" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1313" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1313" s="29"/>
-      <c r="B1313" s="60"/>
-      <c r="C1313" s="67"/>
-      <c r="D1313" s="5"/>
+      <c r="B1313" s="59"/>
+      <c r="C1313" s="64"/>
+      <c r="D1313" s="7"/>
       <c r="E1313" s="29"/>
-      <c r="F1313" s="27"/>
-      <c r="G1313" s="47"/>
+      <c r="F1313" s="26"/>
+      <c r="G1313" s="46"/>
       <c r="H1313" s="29"/>
-      <c r="I1313" s="27"/>
-      <c r="J1313" s="19"/>
-      <c r="K1313" s="20"/>
+      <c r="I1313" s="26"/>
+      <c r="J1313" s="17"/>
+      <c r="K1313" s="18"/>
       <c r="L1313" s="29"/>
     </row>
-    <row r="1314" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1314" s="29"/>
-      <c r="B1314" s="55"/>
-      <c r="C1314" s="62"/>
-      <c r="D1314" s="32"/>
+      <c r="B1314" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1314" s="54" t="s">
+        <v>2000</v>
+      </c>
+      <c r="D1314" s="3" t="s">
+        <v>2003</v>
+      </c>
       <c r="E1314" s="29"/>
-      <c r="F1314" s="33"/>
-      <c r="G1314" s="41"/>
+      <c r="F1314" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1314" s="44" t="s">
+        <v>2013</v>
+      </c>
       <c r="H1314" s="29"/>
-      <c r="I1314" s="33"/>
-      <c r="J1314" s="34"/>
-      <c r="K1314" s="34"/>
+      <c r="I1314" s="23"/>
+      <c r="J1314" s="13"/>
+      <c r="K1314" s="14"/>
       <c r="L1314" s="29"/>
     </row>
-    <row r="1316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1315" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1315" s="29"/>
+      <c r="B1315" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1315" s="54" t="s">
+        <v>2029</v>
+      </c>
+      <c r="D1315" s="3" t="s">
+        <v>2012</v>
+      </c>
+      <c r="E1315" s="29"/>
+      <c r="F1315" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1315" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1315" s="29"/>
+      <c r="I1315" s="23"/>
+      <c r="J1315" s="13"/>
+      <c r="K1315" s="14"/>
+      <c r="L1315" s="29"/>
+    </row>
+    <row r="1316" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1316" s="29"/>
-      <c r="B1316" s="55"/>
+      <c r="B1316" s="56" t="s">
+        <v>2014</v>
+      </c>
       <c r="C1316" s="54" t="s">
-        <v>362</v>
+        <v>2030</v>
       </c>
       <c r="D1316" s="3" t="s">
-        <v>363</v>
+        <v>2005</v>
       </c>
       <c r="E1316" s="29"/>
-      <c r="F1316" s="23"/>
-      <c r="G1316" s="44"/>
+      <c r="F1316" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1316" s="44" t="s">
+        <v>2013</v>
+      </c>
       <c r="H1316" s="29"/>
       <c r="I1316" s="23"/>
       <c r="J1316" s="13"/>
       <c r="K1316" s="14"/>
       <c r="L1316" s="29"/>
+    </row>
+    <row r="1317" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1317" s="29"/>
+      <c r="B1317" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1317" s="54" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D1317" s="3" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E1317" s="29"/>
+      <c r="F1317" s="23">
+        <v>44987</v>
+      </c>
+      <c r="G1317" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1317" s="29"/>
+      <c r="I1317" s="23"/>
+      <c r="J1317" s="13"/>
+      <c r="K1317" s="14"/>
+      <c r="L1317" s="29"/>
+    </row>
+    <row r="1318" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1318" s="29"/>
+      <c r="B1318" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1318" s="54" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D1318" s="3" t="s">
+        <v>2009</v>
+      </c>
+      <c r="E1318" s="29"/>
+      <c r="F1318" s="23">
+        <v>44972</v>
+      </c>
+      <c r="G1318" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1318" s="29"/>
+      <c r="I1318" s="23"/>
+      <c r="J1318" s="13"/>
+      <c r="K1318" s="14"/>
+      <c r="L1318" s="29"/>
+    </row>
+    <row r="1319" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1319" s="29"/>
+      <c r="B1319" s="59"/>
+      <c r="C1319" s="64"/>
+      <c r="D1319" s="7"/>
+      <c r="E1319" s="29"/>
+      <c r="F1319" s="26"/>
+      <c r="G1319" s="46"/>
+      <c r="H1319" s="29"/>
+      <c r="I1319" s="26"/>
+      <c r="J1319" s="17"/>
+      <c r="K1319" s="18"/>
+      <c r="L1319" s="29"/>
+    </row>
+    <row r="1320" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1320" s="29"/>
+      <c r="B1320" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1320" s="54" t="s">
+        <v>2044</v>
+      </c>
+      <c r="D1320" s="3" t="s">
+        <v>2046</v>
+      </c>
+      <c r="E1320" s="29"/>
+      <c r="F1320" s="23">
+        <v>45002</v>
+      </c>
+      <c r="G1320" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1320" s="29"/>
+      <c r="I1320" s="23"/>
+      <c r="J1320" s="13"/>
+      <c r="K1320" s="14"/>
+      <c r="L1320" s="29"/>
+    </row>
+    <row r="1321" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1321" s="29"/>
+      <c r="B1321" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1321" s="54" t="s">
+        <v>2043</v>
+      </c>
+      <c r="D1321" s="3" t="s">
+        <v>2045</v>
+      </c>
+      <c r="E1321" s="29"/>
+      <c r="F1321" s="23">
+        <v>45002</v>
+      </c>
+      <c r="G1321" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1321" s="29"/>
+      <c r="I1321" s="23"/>
+      <c r="J1321" s="13"/>
+      <c r="K1321" s="14"/>
+      <c r="L1321" s="29"/>
+    </row>
+    <row r="1322" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1322" s="29"/>
+      <c r="B1322" s="56" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C1322" s="54" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D1322" s="3" t="s">
+        <v>2048</v>
+      </c>
+      <c r="E1322" s="29"/>
+      <c r="F1322" s="23">
+        <v>45005</v>
+      </c>
+      <c r="G1322" s="44" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1322" s="29"/>
+      <c r="I1322" s="23"/>
+      <c r="J1322" s="13"/>
+      <c r="K1322" s="14"/>
+      <c r="L1322" s="29"/>
+    </row>
+    <row r="1323" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1323" s="29"/>
+      <c r="B1323" s="60"/>
+      <c r="C1323" s="67"/>
+      <c r="D1323" s="5"/>
+      <c r="E1323" s="29"/>
+      <c r="F1323" s="27"/>
+      <c r="G1323" s="47"/>
+      <c r="H1323" s="29"/>
+      <c r="I1323" s="27"/>
+      <c r="J1323" s="19"/>
+      <c r="K1323" s="20"/>
+      <c r="L1323" s="29"/>
+    </row>
+    <row r="1324" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1324" s="29"/>
+      <c r="B1324" s="55"/>
+      <c r="C1324" s="62"/>
+      <c r="D1324" s="32"/>
+      <c r="E1324" s="29"/>
+      <c r="F1324" s="33"/>
+      <c r="G1324" s="41"/>
+      <c r="H1324" s="29"/>
+      <c r="I1324" s="33"/>
+      <c r="J1324" s="34"/>
+      <c r="K1324" s="34"/>
+      <c r="L1324" s="29"/>
+    </row>
+    <row r="1326" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1326" s="29"/>
+      <c r="B1326" s="55"/>
+      <c r="C1326" s="54" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1326" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1326" s="29"/>
+      <c r="F1326" s="23"/>
+      <c r="G1326" s="44"/>
+      <c r="H1326" s="29"/>
+      <c r="I1326" s="23"/>
+      <c r="J1326" s="13"/>
+      <c r="K1326" s="14"/>
+      <c r="L1326" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="85">
@@ -41005,9 +41305,9 @@
     <mergeCell ref="B1002:C1002"/>
     <mergeCell ref="B1004:C1004"/>
     <mergeCell ref="B1010:C1010"/>
-    <mergeCell ref="B1291:C1291"/>
-    <mergeCell ref="B1293:C1293"/>
-    <mergeCell ref="B1292:C1292"/>
+    <mergeCell ref="B1301:C1301"/>
+    <mergeCell ref="B1303:C1303"/>
+    <mergeCell ref="B1302:C1302"/>
     <mergeCell ref="B1163:C1163"/>
     <mergeCell ref="B1158:C1158"/>
     <mergeCell ref="B1012:C1012"/>
@@ -41070,7 +41370,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G19:G20 G146:G147 G149 G158:G160 G255:G261 G268:G273 G404:G408 G410:G414 G424:G426 G446 G520:G523 G869:G871 G900:G901 G1015:G1017 G1019 G1021:G1025 G1027:G1030 G1032:G1033 G1047:G1052 G1054:G1056 G1065:G1066 G1076 G1131:G1133 G1039:G1043 G1174:G1175 G367:G370 G1262:G1265 G973:G976 G889:G891 G372:G375 G1267:G1269 G250 G227 G282:G285 G428:G433 G1058:G1063 G903:G908 G221 G195:G196 G893:G898 G416:G422 G1167:G1172 G864:G867 G1013 G924 G1083 G198 G207:G215 G229:G248 G1248:G1258 G1088:G1129 G929:G971 G547 G1149 F1146:G1148 G34:G42 G525:G538 G1286:G1288 G542:G544 G1153:G1155 G998:G1000 G884 G100 G1160 G1136:G1145 G982:G996 G920:G922 G1078:G1081 G978:G980 G190 G926:G927 G1085:G1086 G1215:G1216 G377:G389 G1272:G1278 G600:G604 G772:G777 G1233:G1246 G1218:G1231 G1297:G1308 G1294:G1295 G153:G156 G140 G173 G746:G770 G669:G744 G639:G646 G552:G598 G540 G448:G518 G435:G440 G397:G399 G311:G365 G114:G135 G105:G109 G31:G32 G25:G26 G183:G188 G873:G882 G180:G181 G165:G166 G790:G862 G44:G98 G606:G614 G11:G14 G279 G287:G288 G648:G651 G290 G297:G298 G293 G168 G275:G276 G619:G637 G300:G302 G654:G664 G392:G393" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G19:G20 G146:G147 G149 G158:G160 G255:G261 G268:G273 G404:G408 G410:G414 G424:G426 G446 G520:G523 G869:G871 G900:G901 G1015:G1017 G1019 G1021:G1025 G1027:G1030 G1032:G1033 G1047:G1052 G1054:G1056 G1065:G1066 G1076 G1131:G1133 G1039:G1043 G1174:G1175 G367:G370 G1262:G1265 G973:G976 G889:G891 G372:G375 G1267:G1269 G250 G227 G282:G285 G428:G433 G1058:G1063 G903:G908 G221 G195:G196 G893:G898 G416:G422 G1167:G1172 G864:G867 G1013 G924 G1083 G198 G207:G215 G229:G248 G1248:G1258 G1088:G1129 G929:G971 G547 G1149 F1146:G1148 G34:G42 G525:G538 G1296:G1298 G542:G544 G1153:G1155 G998:G1000 G884 G100 G1160 G1136:G1145 G982:G996 G920:G922 G1078:G1081 G978:G980 G190 G926:G927 G1085:G1086 G1215:G1216 G377:G389 G1287:G1288 G600:G604 G772:G777 G1233:G1246 G1218:G1231 G1307:G1318 G1304:G1305 G153:G156 G140 G173 G746:G770 G669:G744 G639:G646 G552:G598 G540 G448:G518 G435:G440 G397:G399 G311:G365 G114:G135 G105:G109 G31:G32 G25:G26 G183:G188 G873:G882 G180:G181 G165:G166 G790:G862 G44:G98 G606:G614 G11:G14 G279 G287:G288 G648:G651 G290 G297:G298 G293 G168 G275:G276 G619:G637 G300:G302 G654:G664 G392:G393 G1272 G1281" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Pertanggal 25 Januari 2023 17:11 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - API/API-Catalogue.xlsx
@@ -9586,6 +9586,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -9597,12 +9603,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -9637,13 +9637,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9958,10 +9958,10 @@
   <dimension ref="A1:M1326"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D1278" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D1260" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D1286" sqref="D1286"/>
+      <selection pane="bottomRight" activeCell="F1271" sqref="F1271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -10001,7 +10001,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="81"/>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="73" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="29"/>
@@ -10021,7 +10021,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="82"/>
       <c r="C3" s="83"/>
-      <c r="D3" s="72"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="30"/>
       <c r="F3" s="35" t="s">
         <v>332</v>
@@ -10057,10 +10057,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="69" t="s">
         <v>1823</v>
       </c>
-      <c r="C5" s="74"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="6"/>
       <c r="E5" s="29"/>
       <c r="F5" s="24"/>
@@ -10073,8 +10073,8 @@
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="6"/>
       <c r="E6" s="29"/>
       <c r="F6" s="24"/>
@@ -10301,8 +10301,8 @@
     </row>
     <row r="16" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="70"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="72"/>
       <c r="D16" s="6"/>
       <c r="E16" s="29"/>
       <c r="F16" s="24"/>
@@ -10315,10 +10315,10 @@
     </row>
     <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="69" t="s">
         <v>1822</v>
       </c>
-      <c r="C17" s="74"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="6"/>
       <c r="E17" s="29"/>
       <c r="F17" s="24"/>
@@ -10331,8 +10331,8 @@
     </row>
     <row r="18" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="6"/>
       <c r="E18" s="29"/>
       <c r="F18" s="24"/>
@@ -10413,8 +10413,8 @@
     </row>
     <row r="22" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="6"/>
       <c r="E22" s="29"/>
       <c r="F22" s="24"/>
@@ -10427,10 +10427,10 @@
     </row>
     <row r="23" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="69" t="s">
         <v>1821</v>
       </c>
-      <c r="C23" s="74"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="6"/>
       <c r="E23" s="29"/>
       <c r="F23" s="24"/>
@@ -10443,8 +10443,8 @@
     </row>
     <row r="24" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="6"/>
       <c r="E24" s="29"/>
       <c r="F24" s="24"/>
@@ -10519,8 +10519,8 @@
     </row>
     <row r="28" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="70"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
       <c r="D28" s="6"/>
       <c r="E28" s="29"/>
       <c r="F28" s="24"/>
@@ -10549,8 +10549,8 @@
     </row>
     <row r="30" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="70"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="6"/>
       <c r="E30" s="29"/>
       <c r="F30" s="24"/>
@@ -12175,8 +12175,8 @@
     </row>
     <row r="102" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29"/>
-      <c r="B102" s="69"/>
-      <c r="C102" s="70"/>
+      <c r="B102" s="71"/>
+      <c r="C102" s="72"/>
       <c r="D102" s="6"/>
       <c r="E102" s="29"/>
       <c r="F102" s="24"/>
@@ -12189,10 +12189,10 @@
     </row>
     <row r="103" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29"/>
-      <c r="B103" s="73" t="s">
+      <c r="B103" s="69" t="s">
         <v>1842</v>
       </c>
-      <c r="C103" s="74"/>
+      <c r="C103" s="70"/>
       <c r="D103" s="6"/>
       <c r="E103" s="29"/>
       <c r="F103" s="24"/>
@@ -12205,8 +12205,8 @@
     </row>
     <row r="104" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="29"/>
-      <c r="B104" s="69"/>
-      <c r="C104" s="70"/>
+      <c r="B104" s="71"/>
+      <c r="C104" s="72"/>
       <c r="D104" s="6"/>
       <c r="E104" s="29"/>
       <c r="F104" s="24"/>
@@ -12365,8 +12365,8 @@
     </row>
     <row r="111" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="29"/>
-      <c r="B111" s="69"/>
-      <c r="C111" s="70"/>
+      <c r="B111" s="71"/>
+      <c r="C111" s="72"/>
       <c r="D111" s="6"/>
       <c r="E111" s="29"/>
       <c r="F111" s="24"/>
@@ -12379,10 +12379,10 @@
     </row>
     <row r="112" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A112" s="29"/>
-      <c r="B112" s="73" t="s">
+      <c r="B112" s="69" t="s">
         <v>1841</v>
       </c>
-      <c r="C112" s="74"/>
+      <c r="C112" s="70"/>
       <c r="D112" s="6"/>
       <c r="E112" s="29"/>
       <c r="F112" s="24"/>
@@ -12395,8 +12395,8 @@
     </row>
     <row r="113" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="29"/>
-      <c r="B113" s="69"/>
-      <c r="C113" s="70"/>
+      <c r="B113" s="71"/>
+      <c r="C113" s="72"/>
       <c r="D113" s="6"/>
       <c r="E113" s="29"/>
       <c r="F113" s="24"/>
@@ -12901,8 +12901,8 @@
     </row>
     <row r="137" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="29"/>
-      <c r="B137" s="69"/>
-      <c r="C137" s="70"/>
+      <c r="B137" s="71"/>
+      <c r="C137" s="72"/>
       <c r="D137" s="6"/>
       <c r="E137" s="29"/>
       <c r="F137" s="24"/>
@@ -12915,10 +12915,10 @@
     </row>
     <row r="138" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A138" s="29"/>
-      <c r="B138" s="73" t="s">
+      <c r="B138" s="69" t="s">
         <v>2055</v>
       </c>
-      <c r="C138" s="74"/>
+      <c r="C138" s="70"/>
       <c r="D138" s="6"/>
       <c r="E138" s="29"/>
       <c r="F138" s="24"/>
@@ -12931,8 +12931,8 @@
     </row>
     <row r="139" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="29"/>
-      <c r="B139" s="69"/>
-      <c r="C139" s="70"/>
+      <c r="B139" s="71"/>
+      <c r="C139" s="72"/>
       <c r="D139" s="6"/>
       <c r="E139" s="29"/>
       <c r="F139" s="24"/>
@@ -13007,8 +13007,8 @@
     </row>
     <row r="143" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="29"/>
-      <c r="B143" s="69"/>
-      <c r="C143" s="70"/>
+      <c r="B143" s="71"/>
+      <c r="C143" s="72"/>
       <c r="D143" s="6"/>
       <c r="E143" s="29"/>
       <c r="F143" s="24"/>
@@ -13021,10 +13021,10 @@
     </row>
     <row r="144" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A144" s="29"/>
-      <c r="B144" s="73" t="s">
+      <c r="B144" s="69" t="s">
         <v>1839</v>
       </c>
-      <c r="C144" s="74"/>
+      <c r="C144" s="70"/>
       <c r="D144" s="6"/>
       <c r="E144" s="29"/>
       <c r="F144" s="24"/>
@@ -13037,8 +13037,8 @@
     </row>
     <row r="145" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="29"/>
-      <c r="B145" s="69"/>
-      <c r="C145" s="70"/>
+      <c r="B145" s="71"/>
+      <c r="C145" s="72"/>
       <c r="D145" s="6"/>
       <c r="E145" s="29"/>
       <c r="F145" s="24"/>
@@ -13149,8 +13149,8 @@
     </row>
     <row r="150" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="29"/>
-      <c r="B150" s="69"/>
-      <c r="C150" s="70"/>
+      <c r="B150" s="71"/>
+      <c r="C150" s="72"/>
       <c r="D150" s="6"/>
       <c r="E150" s="29"/>
       <c r="F150" s="24"/>
@@ -13163,10 +13163,10 @@
     </row>
     <row r="151" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A151" s="29"/>
-      <c r="B151" s="73" t="s">
+      <c r="B151" s="69" t="s">
         <v>1840</v>
       </c>
-      <c r="C151" s="74"/>
+      <c r="C151" s="70"/>
       <c r="D151" s="6"/>
       <c r="E151" s="29"/>
       <c r="F151" s="24"/>
@@ -13179,8 +13179,8 @@
     </row>
     <row r="152" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="29"/>
-      <c r="B152" s="69"/>
-      <c r="C152" s="70"/>
+      <c r="B152" s="71"/>
+      <c r="C152" s="72"/>
       <c r="D152" s="6"/>
       <c r="E152" s="29"/>
       <c r="F152" s="24"/>
@@ -13389,8 +13389,8 @@
     </row>
     <row r="162" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
-      <c r="B162" s="69"/>
-      <c r="C162" s="70"/>
+      <c r="B162" s="71"/>
+      <c r="C162" s="72"/>
       <c r="D162" s="6"/>
       <c r="E162" s="29"/>
       <c r="F162" s="24"/>
@@ -13403,10 +13403,10 @@
     </row>
     <row r="163" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
-      <c r="B163" s="73" t="s">
+      <c r="B163" s="69" t="s">
         <v>1838</v>
       </c>
-      <c r="C163" s="74"/>
+      <c r="C163" s="70"/>
       <c r="D163" s="6"/>
       <c r="E163" s="29"/>
       <c r="F163" s="24"/>
@@ -13419,8 +13419,8 @@
     </row>
     <row r="164" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
-      <c r="B164" s="69"/>
-      <c r="C164" s="70"/>
+      <c r="B164" s="71"/>
+      <c r="C164" s="72"/>
       <c r="D164" s="6"/>
       <c r="E164" s="29"/>
       <c r="F164" s="24"/>
@@ -14011,8 +14011,8 @@
     </row>
     <row r="192" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="29"/>
-      <c r="B192" s="69"/>
-      <c r="C192" s="70"/>
+      <c r="B192" s="71"/>
+      <c r="C192" s="72"/>
       <c r="D192" s="6"/>
       <c r="E192" s="29"/>
       <c r="F192" s="24"/>
@@ -14025,10 +14025,10 @@
     </row>
     <row r="193" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A193" s="29"/>
-      <c r="B193" s="73" t="s">
+      <c r="B193" s="69" t="s">
         <v>2095</v>
       </c>
-      <c r="C193" s="74"/>
+      <c r="C193" s="70"/>
       <c r="D193" s="6"/>
       <c r="E193" s="29"/>
       <c r="F193" s="24"/>
@@ -14041,8 +14041,8 @@
     </row>
     <row r="194" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="29"/>
-      <c r="B194" s="69"/>
-      <c r="C194" s="70"/>
+      <c r="B194" s="71"/>
+      <c r="C194" s="72"/>
       <c r="D194" s="6"/>
       <c r="E194" s="29"/>
       <c r="F194" s="24"/>
@@ -14231,8 +14231,8 @@
     </row>
     <row r="204" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="29"/>
-      <c r="B204" s="69"/>
-      <c r="C204" s="70"/>
+      <c r="B204" s="71"/>
+      <c r="C204" s="72"/>
       <c r="D204" s="6"/>
       <c r="E204" s="29"/>
       <c r="F204" s="24"/>
@@ -14245,10 +14245,10 @@
     </row>
     <row r="205" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A205" s="29"/>
-      <c r="B205" s="73" t="s">
+      <c r="B205" s="69" t="s">
         <v>1837</v>
       </c>
-      <c r="C205" s="74"/>
+      <c r="C205" s="70"/>
       <c r="D205" s="6"/>
       <c r="E205" s="29"/>
       <c r="F205" s="24"/>
@@ -14261,8 +14261,8 @@
     </row>
     <row r="206" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="29"/>
-      <c r="B206" s="69"/>
-      <c r="C206" s="70"/>
+      <c r="B206" s="71"/>
+      <c r="C206" s="72"/>
       <c r="D206" s="6"/>
       <c r="E206" s="29"/>
       <c r="F206" s="24"/>
@@ -14519,8 +14519,8 @@
     </row>
     <row r="218" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="29"/>
-      <c r="B218" s="69"/>
-      <c r="C218" s="70"/>
+      <c r="B218" s="71"/>
+      <c r="C218" s="72"/>
       <c r="D218" s="6"/>
       <c r="E218" s="29"/>
       <c r="F218" s="24"/>
@@ -14533,10 +14533,10 @@
     </row>
     <row r="219" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A219" s="29"/>
-      <c r="B219" s="73" t="s">
+      <c r="B219" s="69" t="s">
         <v>1835</v>
       </c>
-      <c r="C219" s="74"/>
+      <c r="C219" s="70"/>
       <c r="D219" s="6"/>
       <c r="E219" s="29"/>
       <c r="F219" s="24"/>
@@ -14549,8 +14549,8 @@
     </row>
     <row r="220" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="29"/>
-      <c r="B220" s="69"/>
-      <c r="C220" s="70"/>
+      <c r="B220" s="71"/>
+      <c r="C220" s="72"/>
       <c r="D220" s="6"/>
       <c r="E220" s="29"/>
       <c r="F220" s="24"/>
@@ -14615,8 +14615,8 @@
     </row>
     <row r="224" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="29"/>
-      <c r="B224" s="69"/>
-      <c r="C224" s="70"/>
+      <c r="B224" s="71"/>
+      <c r="C224" s="72"/>
       <c r="D224" s="6"/>
       <c r="E224" s="29"/>
       <c r="F224" s="24"/>
@@ -14629,10 +14629,10 @@
     </row>
     <row r="225" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A225" s="29"/>
-      <c r="B225" s="73" t="s">
+      <c r="B225" s="69" t="s">
         <v>1836</v>
       </c>
-      <c r="C225" s="74"/>
+      <c r="C225" s="70"/>
       <c r="D225" s="6"/>
       <c r="E225" s="29"/>
       <c r="F225" s="24"/>
@@ -14645,8 +14645,8 @@
     </row>
     <row r="226" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="29"/>
-      <c r="B226" s="69"/>
-      <c r="C226" s="70"/>
+      <c r="B226" s="71"/>
+      <c r="C226" s="72"/>
       <c r="D226" s="6"/>
       <c r="E226" s="29"/>
       <c r="F226" s="24"/>
@@ -15231,8 +15231,8 @@
     </row>
     <row r="252" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="29"/>
-      <c r="B252" s="69"/>
-      <c r="C252" s="70"/>
+      <c r="B252" s="71"/>
+      <c r="C252" s="72"/>
       <c r="D252" s="6"/>
       <c r="E252" s="29"/>
       <c r="F252" s="24"/>
@@ -15245,10 +15245,10 @@
     </row>
     <row r="253" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="29"/>
-      <c r="B253" s="73" t="s">
+      <c r="B253" s="69" t="s">
         <v>1834</v>
       </c>
-      <c r="C253" s="74"/>
+      <c r="C253" s="70"/>
       <c r="D253" s="6"/>
       <c r="E253" s="29"/>
       <c r="F253" s="24"/>
@@ -15261,8 +15261,8 @@
     </row>
     <row r="254" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="29"/>
-      <c r="B254" s="69"/>
-      <c r="C254" s="70"/>
+      <c r="B254" s="71"/>
+      <c r="C254" s="72"/>
       <c r="D254" s="6"/>
       <c r="E254" s="29"/>
       <c r="F254" s="24"/>
@@ -15457,8 +15457,8 @@
     </row>
     <row r="263" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="29"/>
-      <c r="B263" s="69"/>
-      <c r="C263" s="70"/>
+      <c r="B263" s="71"/>
+      <c r="C263" s="72"/>
       <c r="D263" s="6"/>
       <c r="E263" s="29"/>
       <c r="F263" s="24"/>
@@ -15471,10 +15471,10 @@
     </row>
     <row r="264" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A264" s="29"/>
-      <c r="B264" s="73" t="s">
+      <c r="B264" s="69" t="s">
         <v>1833</v>
       </c>
-      <c r="C264" s="74"/>
+      <c r="C264" s="70"/>
       <c r="D264" s="6"/>
       <c r="E264" s="29"/>
       <c r="F264" s="24"/>
@@ -15487,8 +15487,8 @@
     </row>
     <row r="265" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="29"/>
-      <c r="B265" s="69"/>
-      <c r="C265" s="70"/>
+      <c r="B265" s="71"/>
+      <c r="C265" s="72"/>
       <c r="D265" s="6"/>
       <c r="E265" s="29"/>
       <c r="F265" s="24"/>
@@ -18713,8 +18713,8 @@
     </row>
     <row r="401" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="29"/>
-      <c r="B401" s="69"/>
-      <c r="C401" s="70"/>
+      <c r="B401" s="71"/>
+      <c r="C401" s="72"/>
       <c r="D401" s="6"/>
       <c r="E401" s="29"/>
       <c r="F401" s="24"/>
@@ -18727,10 +18727,10 @@
     </row>
     <row r="402" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A402" s="29"/>
-      <c r="B402" s="73" t="s">
+      <c r="B402" s="69" t="s">
         <v>1832</v>
       </c>
-      <c r="C402" s="74"/>
+      <c r="C402" s="70"/>
       <c r="D402" s="6"/>
       <c r="E402" s="29"/>
       <c r="F402" s="24"/>
@@ -18743,8 +18743,8 @@
     </row>
     <row r="403" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="29"/>
-      <c r="B403" s="69"/>
-      <c r="C403" s="70"/>
+      <c r="B403" s="71"/>
+      <c r="C403" s="72"/>
       <c r="D403" s="6"/>
       <c r="E403" s="29"/>
       <c r="F403" s="24"/>
@@ -22481,8 +22481,8 @@
     </row>
     <row r="546" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A546" s="29"/>
-      <c r="B546" s="69"/>
-      <c r="C546" s="70"/>
+      <c r="B546" s="71"/>
+      <c r="C546" s="72"/>
       <c r="D546" s="6"/>
       <c r="E546" s="29"/>
       <c r="F546" s="24"/>
@@ -22537,8 +22537,8 @@
     </row>
     <row r="549" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A549" s="29"/>
-      <c r="B549" s="69"/>
-      <c r="C549" s="70"/>
+      <c r="B549" s="71"/>
+      <c r="C549" s="72"/>
       <c r="D549" s="6"/>
       <c r="E549" s="29"/>
       <c r="F549" s="24"/>
@@ -22551,10 +22551,10 @@
     </row>
     <row r="550" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A550" s="29"/>
-      <c r="B550" s="73" t="s">
+      <c r="B550" s="69" t="s">
         <v>1831</v>
       </c>
-      <c r="C550" s="74"/>
+      <c r="C550" s="70"/>
       <c r="D550" s="6"/>
       <c r="E550" s="29"/>
       <c r="F550" s="24"/>
@@ -22567,8 +22567,8 @@
     </row>
     <row r="551" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A551" s="29"/>
-      <c r="B551" s="69"/>
-      <c r="C551" s="70"/>
+      <c r="B551" s="71"/>
+      <c r="C551" s="72"/>
       <c r="D551" s="6"/>
       <c r="E551" s="29"/>
       <c r="F551" s="24"/>
@@ -24191,8 +24191,8 @@
     </row>
     <row r="616" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A616" s="29"/>
-      <c r="B616" s="69"/>
-      <c r="C616" s="70"/>
+      <c r="B616" s="71"/>
+      <c r="C616" s="72"/>
       <c r="D616" s="6"/>
       <c r="E616" s="29"/>
       <c r="F616" s="24"/>
@@ -24205,10 +24205,10 @@
     </row>
     <row r="617" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A617" s="29"/>
-      <c r="B617" s="73" t="s">
+      <c r="B617" s="69" t="s">
         <v>1830</v>
       </c>
-      <c r="C617" s="74"/>
+      <c r="C617" s="70"/>
       <c r="D617" s="6"/>
       <c r="E617" s="29"/>
       <c r="F617" s="24"/>
@@ -24221,8 +24221,8 @@
     </row>
     <row r="618" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A618" s="29"/>
-      <c r="B618" s="69"/>
-      <c r="C618" s="70"/>
+      <c r="B618" s="71"/>
+      <c r="C618" s="72"/>
       <c r="D618" s="6"/>
       <c r="E618" s="29"/>
       <c r="F618" s="24"/>
@@ -28111,8 +28111,8 @@
     </row>
     <row r="777" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A777" s="29"/>
-      <c r="B777" s="69"/>
-      <c r="C777" s="70"/>
+      <c r="B777" s="71"/>
+      <c r="C777" s="72"/>
       <c r="D777" s="6"/>
       <c r="E777" s="29"/>
       <c r="F777" s="24"/>
@@ -28125,10 +28125,10 @@
     </row>
     <row r="778" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A778" s="29"/>
-      <c r="B778" s="73" t="s">
+      <c r="B778" s="69" t="s">
         <v>1824</v>
       </c>
-      <c r="C778" s="74"/>
+      <c r="C778" s="70"/>
       <c r="D778" s="6"/>
       <c r="E778" s="29"/>
       <c r="F778" s="24"/>
@@ -28141,8 +28141,8 @@
     </row>
     <row r="779" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A779" s="29"/>
-      <c r="B779" s="69"/>
-      <c r="C779" s="70"/>
+      <c r="B779" s="71"/>
+      <c r="C779" s="72"/>
       <c r="D779" s="6"/>
       <c r="E779" s="29"/>
       <c r="F779" s="24"/>
@@ -30695,8 +30695,8 @@
     </row>
     <row r="886" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A886" s="29"/>
-      <c r="B886" s="69"/>
-      <c r="C886" s="70"/>
+      <c r="B886" s="71"/>
+      <c r="C886" s="72"/>
       <c r="D886" s="6"/>
       <c r="E886" s="29"/>
       <c r="F886" s="24"/>
@@ -30709,10 +30709,10 @@
     </row>
     <row r="887" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A887" s="29"/>
-      <c r="B887" s="73" t="s">
+      <c r="B887" s="69" t="s">
         <v>1825</v>
       </c>
-      <c r="C887" s="74"/>
+      <c r="C887" s="70"/>
       <c r="D887" s="6"/>
       <c r="E887" s="29"/>
       <c r="F887" s="24"/>
@@ -30725,8 +30725,8 @@
     </row>
     <row r="888" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A888" s="29"/>
-      <c r="B888" s="69"/>
-      <c r="C888" s="70"/>
+      <c r="B888" s="71"/>
+      <c r="C888" s="72"/>
       <c r="D888" s="6"/>
       <c r="E888" s="29"/>
       <c r="F888" s="24"/>
@@ -33640,8 +33640,8 @@
     </row>
     <row r="1002" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1002" s="29"/>
-      <c r="B1002" s="69"/>
-      <c r="C1002" s="70"/>
+      <c r="B1002" s="71"/>
+      <c r="C1002" s="72"/>
       <c r="D1002" s="6"/>
       <c r="E1002" s="29"/>
       <c r="F1002" s="24"/>
@@ -33654,10 +33654,10 @@
     </row>
     <row r="1003" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1003" s="29"/>
-      <c r="B1003" s="73" t="s">
+      <c r="B1003" s="69" t="s">
         <v>1923</v>
       </c>
-      <c r="C1003" s="74"/>
+      <c r="C1003" s="70"/>
       <c r="D1003" s="6"/>
       <c r="E1003" s="29"/>
       <c r="F1003" s="24"/>
@@ -33670,8 +33670,8 @@
     </row>
     <row r="1004" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1004" s="29"/>
-      <c r="B1004" s="69"/>
-      <c r="C1004" s="70"/>
+      <c r="B1004" s="71"/>
+      <c r="C1004" s="72"/>
       <c r="D1004" s="6"/>
       <c r="E1004" s="29"/>
       <c r="F1004" s="24"/>
@@ -33805,8 +33805,8 @@
     </row>
     <row r="1010" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1010" s="29"/>
-      <c r="B1010" s="69"/>
-      <c r="C1010" s="70"/>
+      <c r="B1010" s="71"/>
+      <c r="C1010" s="72"/>
       <c r="D1010" s="6"/>
       <c r="E1010" s="29"/>
       <c r="F1010" s="24"/>
@@ -33819,10 +33819,10 @@
     </row>
     <row r="1011" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1011" s="29"/>
-      <c r="B1011" s="73" t="s">
+      <c r="B1011" s="69" t="s">
         <v>1826</v>
       </c>
-      <c r="C1011" s="74"/>
+      <c r="C1011" s="70"/>
       <c r="D1011" s="6"/>
       <c r="E1011" s="29"/>
       <c r="F1011" s="24"/>
@@ -33835,8 +33835,8 @@
     </row>
     <row r="1012" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1012" s="29"/>
-      <c r="B1012" s="69"/>
-      <c r="C1012" s="70"/>
+      <c r="B1012" s="71"/>
+      <c r="C1012" s="72"/>
       <c r="D1012" s="6"/>
       <c r="E1012" s="29"/>
       <c r="F1012" s="24"/>
@@ -34359,8 +34359,8 @@
     </row>
     <row r="1036" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1036" s="29"/>
-      <c r="B1036" s="69"/>
-      <c r="C1036" s="70"/>
+      <c r="B1036" s="71"/>
+      <c r="C1036" s="72"/>
       <c r="D1036" s="6"/>
       <c r="E1036" s="29"/>
       <c r="F1036" s="24"/>
@@ -34373,10 +34373,10 @@
     </row>
     <row r="1037" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1037" s="29"/>
-      <c r="B1037" s="73" t="s">
+      <c r="B1037" s="69" t="s">
         <v>1827</v>
       </c>
-      <c r="C1037" s="74"/>
+      <c r="C1037" s="70"/>
       <c r="D1037" s="6"/>
       <c r="E1037" s="29"/>
       <c r="F1037" s="24"/>
@@ -34389,8 +34389,8 @@
     </row>
     <row r="1038" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1038" s="29"/>
-      <c r="B1038" s="69"/>
-      <c r="C1038" s="70"/>
+      <c r="B1038" s="71"/>
+      <c r="C1038" s="72"/>
       <c r="D1038" s="6"/>
       <c r="E1038" s="29"/>
       <c r="F1038" s="24"/>
@@ -37453,8 +37453,8 @@
     </row>
     <row r="1157" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1157" s="29"/>
-      <c r="B1157" s="69"/>
-      <c r="C1157" s="70"/>
+      <c r="B1157" s="71"/>
+      <c r="C1157" s="72"/>
       <c r="D1157" s="6"/>
       <c r="E1157" s="29"/>
       <c r="F1157" s="24"/>
@@ -37467,10 +37467,10 @@
     </row>
     <row r="1158" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1158" s="29"/>
-      <c r="B1158" s="73" t="s">
+      <c r="B1158" s="69" t="s">
         <v>1828</v>
       </c>
-      <c r="C1158" s="74"/>
+      <c r="C1158" s="70"/>
       <c r="D1158" s="6"/>
       <c r="E1158" s="29"/>
       <c r="F1158" s="24"/>
@@ -37483,8 +37483,8 @@
     </row>
     <row r="1159" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1159" s="29"/>
-      <c r="B1159" s="69"/>
-      <c r="C1159" s="70"/>
+      <c r="B1159" s="71"/>
+      <c r="C1159" s="72"/>
       <c r="D1159" s="6"/>
       <c r="E1159" s="29"/>
       <c r="F1159" s="24"/>
@@ -37539,8 +37539,8 @@
     </row>
     <row r="1162" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1162" s="29"/>
-      <c r="B1162" s="69"/>
-      <c r="C1162" s="70"/>
+      <c r="B1162" s="71"/>
+      <c r="C1162" s="72"/>
       <c r="D1162" s="6"/>
       <c r="E1162" s="29"/>
       <c r="F1162" s="24"/>
@@ -37553,10 +37553,10 @@
     </row>
     <row r="1163" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1163" s="29"/>
-      <c r="B1163" s="73" t="s">
+      <c r="B1163" s="69" t="s">
         <v>1829</v>
       </c>
-      <c r="C1163" s="74"/>
+      <c r="C1163" s="70"/>
       <c r="D1163" s="6"/>
       <c r="E1163" s="29"/>
       <c r="F1163" s="24"/>
@@ -37569,8 +37569,8 @@
     </row>
     <row r="1164" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1164" s="29"/>
-      <c r="B1164" s="69"/>
-      <c r="C1164" s="70"/>
+      <c r="B1164" s="71"/>
+      <c r="C1164" s="72"/>
       <c r="D1164" s="6"/>
       <c r="E1164" s="29"/>
       <c r="F1164" s="24"/>
@@ -39990,10 +39990,10 @@
       </c>
       <c r="E1267" s="29"/>
       <c r="F1267" s="23">
-        <v>44384</v>
+        <v>44831</v>
       </c>
       <c r="G1267" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1267" s="29"/>
       <c r="I1267" s="23"/>
@@ -40014,10 +40014,10 @@
       </c>
       <c r="E1268" s="29"/>
       <c r="F1268" s="23">
-        <v>44384</v>
+        <v>44831</v>
       </c>
       <c r="G1268" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1268" s="29"/>
       <c r="I1268" s="23"/>
@@ -40038,10 +40038,10 @@
       </c>
       <c r="E1269" s="29"/>
       <c r="F1269" s="23">
-        <v>44384</v>
+        <v>44831</v>
       </c>
       <c r="G1269" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1269" s="29"/>
       <c r="I1269" s="23"/>
@@ -40062,10 +40062,10 @@
       </c>
       <c r="E1270" s="29"/>
       <c r="F1270" s="23">
-        <v>44711</v>
+        <v>44831</v>
       </c>
       <c r="G1270" s="44" t="s">
-        <v>588</v>
+        <v>2013</v>
       </c>
       <c r="H1270" s="29"/>
       <c r="I1270" s="23"/>
@@ -40755,8 +40755,8 @@
     </row>
     <row r="1301" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1301" s="29"/>
-      <c r="B1301" s="69"/>
-      <c r="C1301" s="70"/>
+      <c r="B1301" s="71"/>
+      <c r="C1301" s="72"/>
       <c r="D1301" s="6"/>
       <c r="E1301" s="29"/>
       <c r="F1301" s="24"/>
@@ -40769,10 +40769,10 @@
     </row>
     <row r="1302" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1302" s="29"/>
-      <c r="B1302" s="73" t="s">
+      <c r="B1302" s="69" t="s">
         <v>2004</v>
       </c>
-      <c r="C1302" s="74"/>
+      <c r="C1302" s="70"/>
       <c r="D1302" s="6"/>
       <c r="E1302" s="29"/>
       <c r="F1302" s="24"/>
@@ -40785,8 +40785,8 @@
     </row>
     <row r="1303" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1303" s="29"/>
-      <c r="B1303" s="69"/>
-      <c r="C1303" s="70"/>
+      <c r="B1303" s="71"/>
+      <c r="C1303" s="72"/>
       <c r="D1303" s="6"/>
       <c r="E1303" s="29"/>
       <c r="F1303" s="24"/>
@@ -41281,6 +41281,77 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B224:C224"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B194:C194"/>
+    <mergeCell ref="B551:C551"/>
+    <mergeCell ref="B616:C616"/>
+    <mergeCell ref="B618:C618"/>
+    <mergeCell ref="B777:C777"/>
+    <mergeCell ref="B779:C779"/>
+    <mergeCell ref="B1012:C1012"/>
+    <mergeCell ref="B1038:C1038"/>
+    <mergeCell ref="B1036:C1036"/>
+    <mergeCell ref="B1162:C1162"/>
+    <mergeCell ref="B1164:C1164"/>
+    <mergeCell ref="B1157:C1157"/>
+    <mergeCell ref="B1159:C1159"/>
+    <mergeCell ref="B1037:C1037"/>
+    <mergeCell ref="B1301:C1301"/>
+    <mergeCell ref="B1303:C1303"/>
+    <mergeCell ref="B1302:C1302"/>
+    <mergeCell ref="B1163:C1163"/>
+    <mergeCell ref="B1158:C1158"/>
+    <mergeCell ref="B1011:C1011"/>
+    <mergeCell ref="B1003:C1003"/>
+    <mergeCell ref="B887:C887"/>
+    <mergeCell ref="B778:C778"/>
+    <mergeCell ref="B617:C617"/>
+    <mergeCell ref="B888:C888"/>
+    <mergeCell ref="B886:C886"/>
+    <mergeCell ref="B1002:C1002"/>
+    <mergeCell ref="B1004:C1004"/>
+    <mergeCell ref="B1010:C1010"/>
     <mergeCell ref="B550:C550"/>
     <mergeCell ref="B402:C402"/>
     <mergeCell ref="B264:C264"/>
@@ -41295,82 +41366,11 @@
     <mergeCell ref="B252:C252"/>
     <mergeCell ref="B254:C254"/>
     <mergeCell ref="B263:C263"/>
-    <mergeCell ref="B1011:C1011"/>
-    <mergeCell ref="B1003:C1003"/>
-    <mergeCell ref="B887:C887"/>
-    <mergeCell ref="B778:C778"/>
-    <mergeCell ref="B617:C617"/>
-    <mergeCell ref="B888:C888"/>
-    <mergeCell ref="B886:C886"/>
-    <mergeCell ref="B1002:C1002"/>
-    <mergeCell ref="B1004:C1004"/>
-    <mergeCell ref="B1010:C1010"/>
-    <mergeCell ref="B1301:C1301"/>
-    <mergeCell ref="B1303:C1303"/>
-    <mergeCell ref="B1302:C1302"/>
-    <mergeCell ref="B1163:C1163"/>
-    <mergeCell ref="B1158:C1158"/>
-    <mergeCell ref="B1012:C1012"/>
-    <mergeCell ref="B1038:C1038"/>
-    <mergeCell ref="B1036:C1036"/>
-    <mergeCell ref="B1162:C1162"/>
-    <mergeCell ref="B1164:C1164"/>
-    <mergeCell ref="B1157:C1157"/>
-    <mergeCell ref="B1159:C1159"/>
-    <mergeCell ref="B1037:C1037"/>
-    <mergeCell ref="B551:C551"/>
-    <mergeCell ref="B616:C616"/>
-    <mergeCell ref="B618:C618"/>
-    <mergeCell ref="B777:C777"/>
-    <mergeCell ref="B779:C779"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B194:C194"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7:G9 G19:G20 G146:G147 G149 G158:G160 G255:G261 G268:G273 G404:G408 G410:G414 G424:G426 G446 G520:G523 G869:G871 G900:G901 G1015:G1017 G1019 G1021:G1025 G1027:G1030 G1032:G1033 G1047:G1052 G1054:G1056 G1065:G1066 G1076 G1131:G1133 G1039:G1043 G1174:G1175 G367:G370 G1262:G1265 G973:G976 G889:G891 G372:G375 G1267:G1269 G250 G227 G282:G285 G428:G433 G1058:G1063 G903:G908 G221 G195:G196 G893:G898 G416:G422 G1167:G1172 G864:G867 G1013 G924 G1083 G198 G207:G215 G229:G248 G1248:G1258 G1088:G1129 G929:G971 G547 G1149 F1146:G1148 G34:G42 G525:G538 G1296:G1298 G542:G544 G1153:G1155 G998:G1000 G884 G100 G1160 G1136:G1145 G982:G996 G920:G922 G1078:G1081 G978:G980 G190 G926:G927 G1085:G1086 G1215:G1216 G377:G389 G1287:G1288 G600:G604 G772:G777 G1233:G1246 G1218:G1231 G1307:G1318 G1304:G1305 G153:G156 G140 G173 G746:G770 G669:G744 G639:G646 G552:G598 G540 G448:G518 G435:G440 G397:G399 G311:G365 G114:G135 G105:G109 G31:G32 G25:G26 G183:G188 G873:G882 G180:G181 G165:G166 G790:G862 G44:G98 G606:G614 G11:G14 G279 G287:G288 G648:G651 G290 G297:G298 G293 G168 G275:G276 G619:G637 G300:G302 G654:G664 G392:G393 G1272 G1281" numberStoredAsText="1"/>
+    <ignoredError sqref="G7:G9 G19:G20 G146:G147 G149 G158:G160 G255:G261 G268:G273 G404:G408 G410:G414 G424:G426 G446 G520:G523 G869:G871 G900:G901 G1015:G1017 G1019 G1021:G1025 G1027:G1030 G1032:G1033 G1047:G1052 G1054:G1056 G1065:G1066 G1076 G1131:G1133 G1039:G1043 G1174:G1175 G367:G370 G1262:G1265 G973:G976 G889:G891 G372:G375 G250 G227 G282:G285 G428:G433 G1058:G1063 G903:G908 G221 G195:G196 G893:G898 G416:G422 G1167:G1172 G864:G867 G1013 G924 G1083 G198 G207:G215 G229:G248 G1248:G1258 G1088:G1129 G929:G971 G547 G1149 F1146:G1148 G34:G42 G525:G538 G1296:G1298 G542:G544 G1153:G1155 G998:G1000 G884 G100 G1160 G1136:G1145 G982:G996 G920:G922 G1078:G1081 G978:G980 G190 G926:G927 G1085:G1086 G1215:G1216 G377:G389 G1287:G1288 G600:G604 G772:G777 G1233:G1246 G1218:G1231 G1307:G1318 G1304:G1305 G153:G156 G140 G173 G746:G770 G669:G744 G639:G646 G552:G598 G540 G448:G518 G435:G440 G397:G399 G311:G365 G114:G135 G105:G109 G31:G32 G25:G26 G183:G188 G873:G882 G180:G181 G165:G166 G790:G862 G44:G98 G606:G614 G11:G14 G279 G287:G288 G648:G651 G290 G297:G298 G293 G168 G275:G276 G619:G637 G300:G302 G654:G664 G392:G393 G1272 G1281" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -41395,80 +41395,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="86" t="s">
         <v>1253</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="86" t="s">
         <v>1254</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="86" t="s">
         <v>1255</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="86" t="s">
         <v>1256</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="86" t="s">
         <v>1257</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="87" t="s">
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="88" t="s">
         <v>1271</v>
       </c>
-      <c r="I7" s="87"/>
+      <c r="I7" s="88"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="87" t="s">
         <v>1269</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
       <c r="I8" s="52" t="s">
         <v>1272</v>
       </c>
@@ -41477,62 +41477,62 @@
       <c r="B9" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="87" t="s">
         <v>1270</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
       <c r="I9" s="52" t="s">
         <v>1273</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="86" t="s">
         <v>1259</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="86" t="s">
         <v>1261</v>
       </c>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="87" t="s">
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="88" t="s">
         <v>1279</v>
       </c>
-      <c r="I12" s="87"/>
+      <c r="I12" s="88"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="87" t="s">
         <v>1264</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
       <c r="I13" s="52" t="s">
         <v>1293</v>
       </c>
@@ -41541,13 +41541,13 @@
       <c r="B14" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="87" t="s">
         <v>1276</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
       <c r="I14" s="52" t="s">
         <v>1294</v>
       </c>
@@ -41556,13 +41556,13 @@
       <c r="B15" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="87" t="s">
         <v>1280</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
       <c r="I15" s="52" t="s">
         <v>1292</v>
       </c>
@@ -41571,13 +41571,13 @@
       <c r="B16" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="87" t="s">
         <v>1281</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
       <c r="I16" s="52" t="s">
         <v>1282</v>
       </c>
@@ -41586,24 +41586,24 @@
       <c r="B17" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="87" t="s">
         <v>1285</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="87" t="s">
         <v>1286</v>
       </c>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
       <c r="I18" s="52" t="s">
         <v>1291</v>
       </c>
@@ -41612,12 +41612,12 @@
       <c r="C19" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="87" t="s">
         <v>1287</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
       <c r="I19" s="52" t="s">
         <v>1288</v>
       </c>
@@ -41626,13 +41626,13 @@
       <c r="B20" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="87" t="s">
         <v>1289</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
       <c r="I20" s="52" t="s">
         <v>1297</v>
       </c>
@@ -41641,13 +41641,13 @@
       <c r="B21" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="87" t="s">
         <v>1283</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
       <c r="I21" s="52" t="s">
         <v>1284</v>
       </c>
@@ -41656,13 +41656,13 @@
       <c r="B22" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="87" t="s">
         <v>1278</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
       <c r="I22" s="52" t="s">
         <v>1290</v>
       </c>
@@ -41671,53 +41671,53 @@
       <c r="B23" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="87" t="s">
         <v>1295</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="87"/>
+      <c r="F23" s="87"/>
+      <c r="G23" s="87"/>
       <c r="I23" s="52" t="s">
         <v>1296</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>1262</v>
       </c>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="87" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="88" t="s">
         <v>1268</v>
       </c>
-      <c r="I24" s="87"/>
+      <c r="I24" s="88"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C25" s="87" t="s">
         <v>1267</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="87" t="s">
         <v>1265</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
       <c r="I26" s="52" t="s">
         <v>1274</v>
       </c>
@@ -41726,12 +41726,12 @@
       <c r="C27" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="87" t="s">
         <v>1266</v>
       </c>
-      <c r="E27" s="86"/>
-      <c r="F27" s="86"/>
-      <c r="G27" s="86"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="52" t="s">
         <v>1275</v>
       </c>
@@ -41740,28 +41740,24 @@
       <c r="D28" s="53" t="s">
         <v>1263</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="87" t="s">
         <v>1277</v>
       </c>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B24:G24"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C22:G22"/>
@@ -41777,12 +41773,16 @@
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>